<commit_message>
review distance to compliance sheet
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368" firstSheet="11" activeTab="11"/>
+    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="579">
   <si>
     <t>Acronym</t>
   </si>
@@ -2231,6 +2231,9 @@
   <si>
     <t>Number of breaches</t>
   </si>
+  <si>
+    <t>Wastewater Distance To Target (DTT) Big cities</t>
+  </si>
 </sst>
 </file>
 
@@ -5466,6 +5469,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5554,6 +5561,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5590,9 +5636,6 @@
     <xf numFmtId="3" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5641,113 +5684,113 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5755,36 +5798,6 @@
     <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5797,6 +5810,18 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -5806,23 +5831,11 @@
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5852,6 +5865,39 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -5879,38 +5925,11 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5931,101 +5950,85 @@
     <xf numFmtId="3" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6338,7 +6341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6634,10 +6637,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F62"/>
+  <dimension ref="B2:F81"/>
   <sheetViews>
-    <sheetView topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6658,8 +6661,8 @@
       <c r="B3" s="325" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="906"/>
-      <c r="D3" s="906"/>
+      <c r="C3" s="910"/>
+      <c r="D3" s="910"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C4" s="326"/>
@@ -6692,10 +6695,10 @@
       <c r="D10" s="333" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="907" t="s">
+      <c r="E10" s="911" t="s">
         <v>574</v>
       </c>
-      <c r="F10" s="908"/>
+      <c r="F10" s="912"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="334" t="s">
@@ -6846,10 +6849,10 @@
       <c r="D30" s="344" t="s">
         <v>316</v>
       </c>
-      <c r="E30" s="907" t="s">
+      <c r="E30" s="911" t="s">
         <v>574</v>
       </c>
-      <c r="F30" s="908"/>
+      <c r="F30" s="912"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="334" t="s">
@@ -6997,10 +7000,10 @@
       <c r="D49" s="344" t="s">
         <v>316</v>
       </c>
-      <c r="E49" s="907" t="s">
+      <c r="E49" s="911" t="s">
         <v>574</v>
       </c>
-      <c r="F49" s="908"/>
+      <c r="F49" s="912"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="334" t="s">
@@ -7123,13 +7126,165 @@
       <c r="E62" s="370"/>
       <c r="F62" s="354"/>
     </row>
+    <row r="65" spans="2:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="B65" s="328" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="B66" s="329"/>
+      <c r="C66" s="329"/>
+      <c r="D66" s="330" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D67" s="331"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B68" s="515" t="s">
+        <v>491</v>
+      </c>
+      <c r="C68" s="332" t="s">
+        <v>283</v>
+      </c>
+      <c r="D68" s="344" t="s">
+        <v>316</v>
+      </c>
+      <c r="E68" s="911" t="s">
+        <v>574</v>
+      </c>
+      <c r="F68" s="912"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B69" s="516" t="s">
+        <v>277</v>
+      </c>
+      <c r="C69" s="335" t="s">
+        <v>191</v>
+      </c>
+      <c r="D69" s="345" t="s">
+        <v>520</v>
+      </c>
+      <c r="E69" s="517" t="s">
+        <v>521</v>
+      </c>
+      <c r="F69" s="518" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B70" s="338" t="s">
+        <v>437</v>
+      </c>
+      <c r="C70" s="347"/>
+      <c r="D70" s="355">
+        <v>100</v>
+      </c>
+      <c r="E70" s="355"/>
+      <c r="F70" s="352"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" s="339" t="s">
+        <v>318</v>
+      </c>
+      <c r="C71" s="348"/>
+      <c r="D71" s="356"/>
+      <c r="E71" s="375"/>
+      <c r="F71" s="376"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="363" t="s">
+        <v>319</v>
+      </c>
+      <c r="C72" s="364"/>
+      <c r="D72" s="365"/>
+      <c r="E72" s="377"/>
+      <c r="F72" s="378"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B73" s="340"/>
+      <c r="C73" s="349"/>
+      <c r="D73" s="357"/>
+      <c r="E73" s="358"/>
+      <c r="F73" s="353"/>
+    </row>
+    <row r="74" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B74" s="341" t="s">
+        <v>571</v>
+      </c>
+      <c r="C74" s="350"/>
+      <c r="D74" s="359"/>
+      <c r="E74" s="359"/>
+      <c r="F74" s="354"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75" s="339" t="s">
+        <v>568</v>
+      </c>
+      <c r="C75" s="348"/>
+      <c r="D75" s="356"/>
+      <c r="E75" s="356"/>
+      <c r="F75" s="353"/>
+    </row>
+    <row r="76" spans="2:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B76" s="379" t="s">
+        <v>320</v>
+      </c>
+      <c r="C76" s="367"/>
+      <c r="D76" s="365"/>
+      <c r="E76" s="365"/>
+      <c r="F76" s="354"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" s="342"/>
+      <c r="C77" s="351"/>
+      <c r="D77" s="360"/>
+      <c r="E77" s="360"/>
+      <c r="F77" s="353"/>
+    </row>
+    <row r="78" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B78" s="341" t="s">
+        <v>572</v>
+      </c>
+      <c r="C78" s="350"/>
+      <c r="D78" s="361"/>
+      <c r="E78" s="361"/>
+      <c r="F78" s="354"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" s="339" t="s">
+        <v>568</v>
+      </c>
+      <c r="C79" s="348"/>
+      <c r="D79" s="356"/>
+      <c r="E79" s="356"/>
+      <c r="F79" s="353"/>
+    </row>
+    <row r="80" spans="2:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B80" s="380" t="s">
+        <v>320</v>
+      </c>
+      <c r="C80" s="348"/>
+      <c r="D80" s="356"/>
+      <c r="E80" s="356"/>
+      <c r="F80" s="353"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B81" s="373"/>
+      <c r="C81" s="369"/>
+      <c r="D81" s="374"/>
+      <c r="E81" s="370"/>
+      <c r="F81" s="354"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E68:F68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7169,8 +7324,8 @@
       </c>
       <c r="C2" s="385"/>
       <c r="D2" s="385"/>
-      <c r="E2" s="904"/>
-      <c r="F2" s="904"/>
+      <c r="E2" s="901"/>
+      <c r="F2" s="901"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="384"/>
@@ -7202,13 +7357,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="382"/>
-      <c r="B6" s="905" t="s">
+      <c r="B6" s="902" t="s">
         <v>492</v>
       </c>
-      <c r="C6" s="905"/>
-      <c r="D6" s="905"/>
-      <c r="E6" s="905"/>
-      <c r="F6" s="905"/>
+      <c r="C6" s="902"/>
+      <c r="D6" s="902"/>
+      <c r="E6" s="902"/>
+      <c r="F6" s="902"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="382"/>
@@ -7223,14 +7378,14 @@
       <c r="B8" s="411" t="s">
         <v>526</v>
       </c>
-      <c r="C8" s="909" t="s">
+      <c r="C8" s="913" t="s">
         <v>282</v>
       </c>
-      <c r="D8" s="910"/>
-      <c r="E8" s="909" t="s">
+      <c r="D8" s="914"/>
+      <c r="E8" s="913" t="s">
         <v>283</v>
       </c>
-      <c r="F8" s="910"/>
+      <c r="F8" s="914"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="382"/>
@@ -7366,11 +7521,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="382"/>
-      <c r="B22" s="899"/>
-      <c r="C22" s="899"/>
-      <c r="D22" s="899"/>
-      <c r="E22" s="899"/>
-      <c r="F22" s="899"/>
+      <c r="B22" s="907"/>
+      <c r="C22" s="907"/>
+      <c r="D22" s="907"/>
+      <c r="E22" s="907"/>
+      <c r="F22" s="907"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="382"/>
@@ -7392,7 +7547,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="382"/>
-      <c r="B25" s="975" t="s">
+      <c r="B25" s="787" t="s">
         <v>569</v>
       </c>
       <c r="C25" s="383"/>
@@ -7402,7 +7557,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="382"/>
-      <c r="B26" s="975" t="s">
+      <c r="B26" s="787" t="s">
         <v>570</v>
       </c>
       <c r="C26" s="383"/>
@@ -7427,7 +7582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
@@ -7441,13 +7596,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="911" t="s">
+      <c r="B2" s="915" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="912" t="s">
+      <c r="C2" s="916" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="912" t="s">
+      <c r="D2" s="916" t="s">
         <v>214</v>
       </c>
       <c r="E2" s="436" t="s">
@@ -7482,9 +7637,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="911"/>
-      <c r="C3" s="913"/>
-      <c r="D3" s="913"/>
+      <c r="B3" s="915"/>
+      <c r="C3" s="917"/>
+      <c r="D3" s="917"/>
       <c r="E3" s="451" t="s">
         <v>334</v>
       </c>
@@ -7517,7 +7672,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="914" t="s">
+      <c r="B4" s="918" t="s">
         <v>337</v>
       </c>
       <c r="C4" s="437" t="s">
@@ -7536,7 +7691,7 @@
       <c r="N4" s="439"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="914"/>
+      <c r="B5" s="918"/>
       <c r="C5" s="437" t="s">
         <v>129</v>
       </c>
@@ -7553,7 +7708,7 @@
       <c r="N5" s="439"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="915"/>
+      <c r="B6" s="919"/>
       <c r="C6" s="447" t="s">
         <v>327</v>
       </c>
@@ -7648,10 +7803,10 @@
   <dimension ref="A1:Y55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="Q5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T1" sqref="T1:Y1"/>
+      <selection pane="bottomRight" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7667,43 +7822,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="928" t="s">
+      <c r="A1" s="923" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="929"/>
+      <c r="B1" s="924"/>
       <c r="C1" s="467"/>
-      <c r="D1" s="919" t="s">
+      <c r="D1" s="934" t="s">
         <v>338</v>
       </c>
-      <c r="E1" s="920"/>
-      <c r="F1" s="920"/>
-      <c r="G1" s="920"/>
-      <c r="H1" s="920"/>
-      <c r="I1" s="921"/>
-      <c r="J1" s="930" t="s">
+      <c r="E1" s="935"/>
+      <c r="F1" s="935"/>
+      <c r="G1" s="935"/>
+      <c r="H1" s="935"/>
+      <c r="I1" s="936"/>
+      <c r="J1" s="925" t="s">
         <v>339</v>
       </c>
-      <c r="K1" s="931"/>
-      <c r="L1" s="931"/>
-      <c r="M1" s="931"/>
-      <c r="N1" s="932"/>
-      <c r="O1" s="933" t="s">
+      <c r="K1" s="926"/>
+      <c r="L1" s="926"/>
+      <c r="M1" s="926"/>
+      <c r="N1" s="927"/>
+      <c r="O1" s="928" t="s">
         <v>340</v>
       </c>
-      <c r="P1" s="934"/>
-      <c r="Q1" s="935"/>
+      <c r="P1" s="929"/>
+      <c r="Q1" s="930"/>
       <c r="R1" s="454" t="s">
         <v>116</v>
       </c>
       <c r="S1" s="455"/>
-      <c r="T1" s="927" t="s">
+      <c r="T1" s="922" t="s">
         <v>537</v>
       </c>
-      <c r="U1" s="927"/>
-      <c r="V1" s="927"/>
-      <c r="W1" s="927"/>
-      <c r="X1" s="927"/>
-      <c r="Y1" s="927"/>
+      <c r="U1" s="922"/>
+      <c r="V1" s="922"/>
+      <c r="W1" s="922"/>
+      <c r="X1" s="922"/>
+      <c r="Y1" s="922"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="457" t="s">
@@ -7715,18 +7870,18 @@
       <c r="C2" s="458" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="924" t="s">
+      <c r="D2" s="939" t="s">
         <v>342</v>
       </c>
-      <c r="E2" s="923"/>
-      <c r="F2" s="923" t="s">
+      <c r="E2" s="938"/>
+      <c r="F2" s="938" t="s">
         <v>343</v>
       </c>
-      <c r="G2" s="923"/>
-      <c r="H2" s="922" t="s">
+      <c r="G2" s="938"/>
+      <c r="H2" s="937" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="922"/>
+      <c r="I2" s="937"/>
       <c r="J2" s="459">
         <v>0</v>
       </c>
@@ -7757,18 +7912,18 @@
       <c r="S2" s="699" t="s">
         <v>127</v>
       </c>
-      <c r="T2" s="925" t="s">
+      <c r="T2" s="920" t="s">
         <v>504</v>
       </c>
-      <c r="U2" s="925"/>
-      <c r="V2" s="926" t="s">
+      <c r="U2" s="920"/>
+      <c r="V2" s="921" t="s">
         <v>523</v>
       </c>
-      <c r="W2" s="926"/>
-      <c r="X2" s="926" t="s">
+      <c r="W2" s="921"/>
+      <c r="X2" s="921" t="s">
         <v>524</v>
       </c>
-      <c r="Y2" s="926"/>
+      <c r="Y2" s="921"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="462"/>
@@ -7794,13 +7949,13 @@
       <c r="I3" s="683" t="s">
         <v>105</v>
       </c>
-      <c r="J3" s="916" t="s">
+      <c r="J3" s="931" t="s">
         <v>349</v>
       </c>
-      <c r="K3" s="917"/>
-      <c r="L3" s="917"/>
-      <c r="M3" s="917"/>
-      <c r="N3" s="918"/>
+      <c r="K3" s="932"/>
+      <c r="L3" s="932"/>
+      <c r="M3" s="932"/>
+      <c r="N3" s="933"/>
       <c r="O3" s="470"/>
       <c r="P3" s="470"/>
       <c r="Q3" s="470"/>
@@ -9029,6 +9184,11 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:X4"/>
   <mergeCells count="12">
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -9036,11 +9196,6 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9080,25 +9235,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="845" t="s">
+      <c r="A1" s="818" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="846"/>
-      <c r="C1" s="846"/>
-      <c r="D1" s="846"/>
-      <c r="E1" s="846"/>
-      <c r="F1" s="846"/>
+      <c r="B1" s="819"/>
+      <c r="C1" s="819"/>
+      <c r="D1" s="819"/>
+      <c r="E1" s="819"/>
+      <c r="F1" s="819"/>
       <c r="G1" s="484"/>
-      <c r="H1" s="939" t="s">
+      <c r="H1" s="945" t="s">
         <v>205</v>
       </c>
-      <c r="I1" s="940"/>
-      <c r="J1" s="940"/>
+      <c r="I1" s="946"/>
+      <c r="J1" s="946"/>
       <c r="K1" s="486"/>
       <c r="L1" s="476"/>
       <c r="M1" s="486"/>
       <c r="N1" s="477"/>
-      <c r="O1" s="937" t="s">
+      <c r="O1" s="943" t="s">
         <v>351</v>
       </c>
       <c r="P1" s="478"/>
@@ -9110,26 +9265,26 @@
       <c r="T1" s="476"/>
       <c r="U1" s="486"/>
       <c r="V1" s="477"/>
-      <c r="W1" s="937" t="s">
+      <c r="W1" s="943" t="s">
         <v>353</v>
       </c>
       <c r="X1" s="478"/>
-      <c r="Y1" s="941" t="s">
+      <c r="Y1" s="947" t="s">
         <v>354</v>
       </c>
-      <c r="Z1" s="941"/>
-      <c r="AA1" s="941"/>
-      <c r="AB1" s="941"/>
-      <c r="AC1" s="941"/>
-      <c r="AD1" s="942"/>
-      <c r="AE1" s="937" t="s">
+      <c r="Z1" s="947"/>
+      <c r="AA1" s="947"/>
+      <c r="AB1" s="947"/>
+      <c r="AC1" s="947"/>
+      <c r="AD1" s="948"/>
+      <c r="AE1" s="943" t="s">
         <v>355</v>
       </c>
-      <c r="AF1" s="936" t="s">
+      <c r="AF1" s="942" t="s">
         <v>522</v>
       </c>
-      <c r="AG1" s="927"/>
-      <c r="AH1" s="927"/>
+      <c r="AG1" s="922"/>
+      <c r="AH1" s="922"/>
       <c r="AI1" s="706"/>
       <c r="AJ1" s="706"/>
       <c r="AK1" s="706"/>
@@ -9188,56 +9343,56 @@
       <c r="C2" s="485" t="s">
         <v>357</v>
       </c>
-      <c r="D2" s="944" t="s">
+      <c r="D2" s="941" t="s">
         <v>527</v>
       </c>
-      <c r="E2" s="944"/>
-      <c r="F2" s="944" t="s">
+      <c r="E2" s="941"/>
+      <c r="F2" s="941" t="s">
         <v>528</v>
       </c>
-      <c r="G2" s="944"/>
+      <c r="G2" s="941"/>
       <c r="H2" s="480"/>
-      <c r="I2" s="943" t="s">
+      <c r="I2" s="940" t="s">
         <v>224</v>
       </c>
-      <c r="J2" s="943"/>
-      <c r="K2" s="943" t="s">
+      <c r="J2" s="940"/>
+      <c r="K2" s="940" t="s">
         <v>225</v>
       </c>
-      <c r="L2" s="943"/>
-      <c r="M2" s="943" t="s">
+      <c r="L2" s="940"/>
+      <c r="M2" s="940" t="s">
         <v>226</v>
       </c>
-      <c r="N2" s="945"/>
-      <c r="O2" s="938"/>
+      <c r="N2" s="949"/>
+      <c r="O2" s="944"/>
       <c r="P2" s="481"/>
-      <c r="Q2" s="943" t="s">
+      <c r="Q2" s="940" t="s">
         <v>224</v>
       </c>
-      <c r="R2" s="943"/>
-      <c r="S2" s="943" t="s">
+      <c r="R2" s="940"/>
+      <c r="S2" s="940" t="s">
         <v>225</v>
       </c>
-      <c r="T2" s="943"/>
-      <c r="U2" s="943" t="s">
+      <c r="T2" s="940"/>
+      <c r="U2" s="940" t="s">
         <v>226</v>
       </c>
-      <c r="V2" s="945"/>
-      <c r="W2" s="938"/>
+      <c r="V2" s="949"/>
+      <c r="W2" s="944"/>
       <c r="X2" s="481"/>
-      <c r="Y2" s="943" t="s">
+      <c r="Y2" s="940" t="s">
         <v>224</v>
       </c>
-      <c r="Z2" s="943"/>
-      <c r="AA2" s="943" t="s">
+      <c r="Z2" s="940"/>
+      <c r="AA2" s="940" t="s">
         <v>225</v>
       </c>
-      <c r="AB2" s="943"/>
-      <c r="AC2" s="943" t="s">
+      <c r="AB2" s="940"/>
+      <c r="AC2" s="940" t="s">
         <v>226</v>
       </c>
-      <c r="AD2" s="945"/>
-      <c r="AE2" s="938"/>
+      <c r="AD2" s="949"/>
+      <c r="AE2" s="944"/>
       <c r="AF2" s="700" t="s">
         <v>504</v>
       </c>
@@ -10123,6 +10278,8 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:AH4"/>
   <mergeCells count="18">
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="AF1:AH1"/>
@@ -10139,8 +10296,6 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="Y2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10355,9 +10510,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="964"/>
-      <c r="B1" s="835"/>
-      <c r="C1" s="835"/>
+      <c r="A1" s="950"/>
+      <c r="B1" s="849"/>
+      <c r="C1" s="849"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="759"/>
@@ -10372,13 +10527,13 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="968" t="s">
+      <c r="A3" s="958" t="s">
         <v>383</v>
       </c>
-      <c r="B3" s="970" t="s">
+      <c r="B3" s="960" t="s">
         <v>493</v>
       </c>
-      <c r="C3" s="971"/>
+      <c r="C3" s="961"/>
       <c r="D3" s="956" t="s">
         <v>494</v>
       </c>
@@ -10397,14 +10552,14 @@
       <c r="K3" s="739"/>
       <c r="L3" s="739"/>
       <c r="N3" s="724"/>
-      <c r="O3" s="953" t="s">
+      <c r="O3" s="972" t="s">
         <v>384</v>
       </c>
-      <c r="P3" s="953"/>
-      <c r="Q3" s="953" t="s">
+      <c r="P3" s="972"/>
+      <c r="Q3" s="972" t="s">
         <v>385</v>
       </c>
-      <c r="R3" s="953"/>
+      <c r="R3" s="972"/>
       <c r="S3" s="724"/>
       <c r="T3" s="732" t="s">
         <v>386</v>
@@ -10412,7 +10567,7 @@
       <c r="U3" s="724"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="969"/>
+      <c r="A4" s="959"/>
       <c r="B4" s="524" t="s">
         <v>387</v>
       </c>
@@ -10671,14 +10826,14 @@
       <c r="K10" s="739"/>
       <c r="L10" s="739"/>
       <c r="N10" s="732"/>
-      <c r="O10" s="953" t="s">
+      <c r="O10" s="972" t="s">
         <v>387</v>
       </c>
-      <c r="P10" s="953"/>
-      <c r="Q10" s="953" t="s">
+      <c r="P10" s="972"/>
+      <c r="Q10" s="972" t="s">
         <v>394</v>
       </c>
-      <c r="R10" s="953"/>
+      <c r="R10" s="972"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I11" s="757" t="str">
@@ -10742,7 +10897,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="968" t="s">
+      <c r="A13" s="958" t="s">
         <v>395</v>
       </c>
       <c r="B13" s="523" t="str">
@@ -10788,7 +10943,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="969"/>
+      <c r="A14" s="959"/>
       <c r="B14" s="526" t="s">
         <v>388</v>
       </c>
@@ -10918,34 +11073,34 @@
       <c r="A21" s="514" t="s">
         <v>400</v>
       </c>
-      <c r="B21" s="958" t="s">
+      <c r="B21" s="973" t="s">
         <v>549</v>
       </c>
-      <c r="C21" s="959"/>
-      <c r="D21" s="959"/>
-      <c r="E21" s="959"/>
-      <c r="F21" s="959"/>
-      <c r="G21" s="959"/>
+      <c r="C21" s="974"/>
+      <c r="D21" s="974"/>
+      <c r="E21" s="974"/>
+      <c r="F21" s="974"/>
+      <c r="G21" s="974"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="528" t="s">
         <v>364</v>
       </c>
-      <c r="B22" s="960" t="str">
+      <c r="B22" s="962" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="961"/>
-      <c r="D22" s="960" t="str">
+      <c r="C22" s="963"/>
+      <c r="D22" s="962" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="961"/>
-      <c r="F22" s="960" t="str">
+      <c r="E22" s="963"/>
+      <c r="F22" s="962" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="961"/>
+      <c r="G22" s="963"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="529"/>
@@ -11372,11 +11527,11 @@
       <c r="A41" s="531" t="s">
         <v>410</v>
       </c>
-      <c r="B41" s="966" t="str">
+      <c r="B41" s="952" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="967"/>
+      <c r="C41" s="953"/>
       <c r="D41" s="954" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
@@ -11600,11 +11755,11 @@
       <c r="F53" s="729" t="s">
         <v>555</v>
       </c>
-      <c r="H53" s="946" t="s">
+      <c r="H53" s="975" t="s">
         <v>542</v>
       </c>
-      <c r="I53" s="946"/>
-      <c r="J53" s="946"/>
+      <c r="I53" s="975"/>
+      <c r="J53" s="975"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="720" t="s">
@@ -11774,11 +11929,11 @@
       <c r="F63" s="729" t="s">
         <v>555</v>
       </c>
-      <c r="H63" s="946" t="s">
+      <c r="H63" s="975" t="s">
         <v>556</v>
       </c>
-      <c r="I63" s="946"/>
-      <c r="J63" s="946"/>
+      <c r="I63" s="975"/>
+      <c r="J63" s="975"/>
       <c r="L63" s="727"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -11965,12 +12120,12 @@
       <c r="A74" s="637" t="s">
         <v>409</v>
       </c>
-      <c r="B74" s="965" t="s">
+      <c r="B74" s="951" t="s">
         <v>495</v>
       </c>
-      <c r="C74" s="965"/>
-      <c r="D74" s="965"/>
-      <c r="E74" s="965"/>
+      <c r="C74" s="951"/>
+      <c r="D74" s="951"/>
+      <c r="E74" s="951"/>
       <c r="I74" s="728"/>
       <c r="J74" s="728"/>
       <c r="K74" s="728"/>
@@ -12286,36 +12441,36 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="951" t="str">
+      <c r="B85" s="966" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="952"/>
-      <c r="D85" s="951" t="str">
+      <c r="C85" s="967"/>
+      <c r="D85" s="966" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="952"/>
-      <c r="F85" s="951" t="str">
+      <c r="E85" s="967"/>
+      <c r="F85" s="966" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="952"/>
+      <c r="G85" s="967"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="515"/>
-      <c r="B86" s="907" t="s">
+      <c r="B86" s="911" t="s">
         <v>317</v>
       </c>
-      <c r="C86" s="908"/>
-      <c r="D86" s="907" t="s">
+      <c r="C86" s="912"/>
+      <c r="D86" s="911" t="s">
         <v>317</v>
       </c>
-      <c r="E86" s="908"/>
-      <c r="F86" s="907" t="s">
+      <c r="E86" s="912"/>
+      <c r="F86" s="911" t="s">
         <v>317</v>
       </c>
-      <c r="G86" s="908"/>
+      <c r="G86" s="912"/>
       <c r="N86" s="732" t="s">
         <v>436</v>
       </c>
@@ -12596,36 +12751,36 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="951" t="str">
+      <c r="B101" s="966" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="952"/>
-      <c r="D101" s="951" t="str">
+      <c r="C101" s="967"/>
+      <c r="D101" s="966" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="952"/>
-      <c r="F101" s="951" t="str">
+      <c r="E101" s="967"/>
+      <c r="F101" s="966" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="952"/>
+      <c r="G101" s="967"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="515"/>
-      <c r="B102" s="907" t="s">
+      <c r="B102" s="911" t="s">
         <v>317</v>
       </c>
-      <c r="C102" s="908"/>
-      <c r="D102" s="907" t="s">
+      <c r="C102" s="912"/>
+      <c r="D102" s="911" t="s">
         <v>317</v>
       </c>
-      <c r="E102" s="908"/>
-      <c r="F102" s="907" t="s">
+      <c r="E102" s="912"/>
+      <c r="F102" s="911" t="s">
         <v>317</v>
       </c>
-      <c r="G102" s="908"/>
+      <c r="G102" s="912"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="516" t="s">
@@ -12906,36 +13061,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="947" t="str">
+      <c r="B116" s="968" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="948"/>
-      <c r="D116" s="947" t="str">
+      <c r="C116" s="969"/>
+      <c r="D116" s="968" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="948"/>
-      <c r="F116" s="947" t="str">
+      <c r="E116" s="969"/>
+      <c r="F116" s="968" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="948"/>
+      <c r="G116" s="969"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="554"/>
-      <c r="B117" s="949" t="s">
+      <c r="B117" s="970" t="s">
         <v>317</v>
       </c>
-      <c r="C117" s="950"/>
-      <c r="D117" s="949" t="s">
+      <c r="C117" s="971"/>
+      <c r="D117" s="970" t="s">
         <v>317</v>
       </c>
-      <c r="E117" s="950"/>
-      <c r="F117" s="949" t="s">
+      <c r="E117" s="971"/>
+      <c r="F117" s="970" t="s">
         <v>317</v>
       </c>
-      <c r="G117" s="950"/>
+      <c r="G117" s="971"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="555" t="s">
@@ -13238,12 +13393,12 @@
       <c r="A129" s="558" t="s">
         <v>395</v>
       </c>
-      <c r="B129" s="962" t="str">
+      <c r="B129" s="964" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="963"/>
-      <c r="D129" s="963"/>
+      <c r="C129" s="965"/>
+      <c r="D129" s="965"/>
       <c r="N129" s="732" t="s">
         <v>436</v>
       </c>
@@ -14019,16 +14174,22 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="39">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -14042,22 +14203,16 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17391,7 +17546,7 @@
       <c r="A1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="972" t="s">
+      <c r="D1" s="786" t="s">
         <v>109</v>
       </c>
       <c r="E1" s="5"/>
@@ -17452,62 +17607,62 @@
       <c r="AP3" s="7"/>
     </row>
     <row r="4" spans="1:42" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="786" t="s">
+      <c r="A4" s="788" t="s">
         <v>552</v>
       </c>
-      <c r="B4" s="787"/>
-      <c r="C4" s="787"/>
-      <c r="D4" s="787"/>
-      <c r="E4" s="788"/>
-      <c r="F4" s="788"/>
-      <c r="G4" s="788"/>
-      <c r="H4" s="788"/>
-      <c r="I4" s="788"/>
-      <c r="J4" s="788"/>
-      <c r="K4" s="788"/>
-      <c r="L4" s="788"/>
-      <c r="M4" s="788"/>
-      <c r="N4" s="788"/>
-      <c r="O4" s="788"/>
-      <c r="P4" s="788"/>
-      <c r="Q4" s="788"/>
-      <c r="R4" s="788"/>
-      <c r="S4" s="788"/>
-      <c r="T4" s="788"/>
-      <c r="U4" s="788"/>
-      <c r="V4" s="788"/>
-      <c r="W4" s="788"/>
-      <c r="X4" s="788"/>
-      <c r="Y4" s="788"/>
-      <c r="Z4" s="788"/>
-      <c r="AA4" s="788"/>
-      <c r="AB4" s="788"/>
-      <c r="AC4" s="788"/>
-      <c r="AD4" s="788"/>
-      <c r="AE4" s="788"/>
-      <c r="AF4" s="788"/>
-      <c r="AG4" s="788"/>
-      <c r="AH4" s="788"/>
-      <c r="AI4" s="788"/>
-      <c r="AJ4" s="788"/>
-      <c r="AK4" s="788"/>
-      <c r="AL4" s="788"/>
-      <c r="AM4" s="788"/>
-      <c r="AN4" s="788"/>
-      <c r="AO4" s="788"/>
-      <c r="AP4" s="788"/>
+      <c r="B4" s="789"/>
+      <c r="C4" s="789"/>
+      <c r="D4" s="789"/>
+      <c r="E4" s="790"/>
+      <c r="F4" s="790"/>
+      <c r="G4" s="790"/>
+      <c r="H4" s="790"/>
+      <c r="I4" s="790"/>
+      <c r="J4" s="790"/>
+      <c r="K4" s="790"/>
+      <c r="L4" s="790"/>
+      <c r="M4" s="790"/>
+      <c r="N4" s="790"/>
+      <c r="O4" s="790"/>
+      <c r="P4" s="790"/>
+      <c r="Q4" s="790"/>
+      <c r="R4" s="790"/>
+      <c r="S4" s="790"/>
+      <c r="T4" s="790"/>
+      <c r="U4" s="790"/>
+      <c r="V4" s="790"/>
+      <c r="W4" s="790"/>
+      <c r="X4" s="790"/>
+      <c r="Y4" s="790"/>
+      <c r="Z4" s="790"/>
+      <c r="AA4" s="790"/>
+      <c r="AB4" s="790"/>
+      <c r="AC4" s="790"/>
+      <c r="AD4" s="790"/>
+      <c r="AE4" s="790"/>
+      <c r="AF4" s="790"/>
+      <c r="AG4" s="790"/>
+      <c r="AH4" s="790"/>
+      <c r="AI4" s="790"/>
+      <c r="AJ4" s="790"/>
+      <c r="AK4" s="790"/>
+      <c r="AL4" s="790"/>
+      <c r="AM4" s="790"/>
+      <c r="AN4" s="790"/>
+      <c r="AO4" s="790"/>
+      <c r="AP4" s="790"/>
     </row>
     <row r="5" spans="1:42" s="8" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="789" t="s">
+      <c r="A5" s="791" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="789" t="s">
+      <c r="B5" s="791" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="789" t="s">
+      <c r="C5" s="791" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="789" t="s">
+      <c r="D5" s="791" t="s">
         <v>63</v>
       </c>
       <c r="E5" s="13" t="s">
@@ -17567,10 +17722,10 @@
       <c r="W5" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="X5" s="791" t="s">
+      <c r="X5" s="793" t="s">
         <v>83</v>
       </c>
-      <c r="Y5" s="791" t="s">
+      <c r="Y5" s="793" t="s">
         <v>84</v>
       </c>
       <c r="Z5" s="17" t="s">
@@ -17600,7 +17755,7 @@
       <c r="AH5" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="AI5" s="791" t="s">
+      <c r="AI5" s="793" t="s">
         <v>93</v>
       </c>
       <c r="AJ5" s="17" t="s">
@@ -17609,27 +17764,27 @@
       <c r="AK5" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="AL5" s="789" t="s">
+      <c r="AL5" s="791" t="s">
         <v>96</v>
       </c>
-      <c r="AM5" s="789" t="s">
+      <c r="AM5" s="791" t="s">
         <v>97</v>
       </c>
-      <c r="AN5" s="789" t="s">
+      <c r="AN5" s="791" t="s">
         <v>98</v>
       </c>
-      <c r="AO5" s="789" t="s">
+      <c r="AO5" s="791" t="s">
         <v>99</v>
       </c>
-      <c r="AP5" s="789" t="s">
+      <c r="AP5" s="791" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:42" s="10" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="790"/>
-      <c r="B6" s="790"/>
-      <c r="C6" s="790"/>
-      <c r="D6" s="790"/>
+      <c r="A6" s="792"/>
+      <c r="B6" s="792"/>
+      <c r="C6" s="792"/>
+      <c r="D6" s="792"/>
       <c r="E6" s="15" t="s">
         <v>101</v>
       </c>
@@ -17687,8 +17842,8 @@
       <c r="W6" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="X6" s="792"/>
-      <c r="Y6" s="792"/>
+      <c r="X6" s="794"/>
+      <c r="Y6" s="794"/>
       <c r="Z6" s="10" t="s">
         <v>102</v>
       </c>
@@ -17716,18 +17871,18 @@
       <c r="AH6" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="AI6" s="792"/>
+      <c r="AI6" s="794"/>
       <c r="AJ6" s="10" t="s">
         <v>102</v>
       </c>
       <c r="AK6" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="AL6" s="790"/>
-      <c r="AM6" s="790"/>
-      <c r="AN6" s="790"/>
-      <c r="AO6" s="790"/>
-      <c r="AP6" s="790"/>
+      <c r="AL6" s="792"/>
+      <c r="AM6" s="792"/>
+      <c r="AN6" s="792"/>
+      <c r="AO6" s="792"/>
+      <c r="AP6" s="792"/>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.3">
       <c r="AD7" s="9"/>
@@ -57893,36 +58048,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="772" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="801"/>
-      <c r="B1" s="801"/>
-      <c r="C1" s="801"/>
-      <c r="D1" s="802"/>
-      <c r="E1" s="803"/>
-      <c r="F1" s="803"/>
-      <c r="G1" s="804"/>
-      <c r="H1" s="805"/>
-      <c r="I1" s="805"/>
-      <c r="J1" s="806"/>
-      <c r="K1" s="807"/>
-      <c r="L1" s="807"/>
-      <c r="M1" s="808"/>
-      <c r="N1" s="809"/>
-      <c r="O1" s="809"/>
-      <c r="P1" s="810"/>
-      <c r="Q1" s="811"/>
-      <c r="R1" s="811"/>
-      <c r="S1" s="793"/>
-      <c r="T1" s="794"/>
-      <c r="U1" s="794"/>
-      <c r="V1" s="795"/>
-      <c r="W1" s="796"/>
-      <c r="X1" s="796"/>
-      <c r="Y1" s="797"/>
-      <c r="Z1" s="798"/>
-      <c r="AA1" s="798"/>
-      <c r="AB1" s="799"/>
-      <c r="AC1" s="800"/>
-      <c r="AD1" s="800"/>
+      <c r="A1" s="803"/>
+      <c r="B1" s="803"/>
+      <c r="C1" s="803"/>
+      <c r="D1" s="804"/>
+      <c r="E1" s="805"/>
+      <c r="F1" s="805"/>
+      <c r="G1" s="806"/>
+      <c r="H1" s="807"/>
+      <c r="I1" s="807"/>
+      <c r="J1" s="808"/>
+      <c r="K1" s="809"/>
+      <c r="L1" s="809"/>
+      <c r="M1" s="810"/>
+      <c r="N1" s="811"/>
+      <c r="O1" s="811"/>
+      <c r="P1" s="812"/>
+      <c r="Q1" s="813"/>
+      <c r="R1" s="813"/>
+      <c r="S1" s="795"/>
+      <c r="T1" s="796"/>
+      <c r="U1" s="796"/>
+      <c r="V1" s="797"/>
+      <c r="W1" s="798"/>
+      <c r="X1" s="798"/>
+      <c r="Y1" s="799"/>
+      <c r="Z1" s="800"/>
+      <c r="AA1" s="800"/>
+      <c r="AB1" s="801"/>
+      <c r="AC1" s="802"/>
+      <c r="AD1" s="802"/>
     </row>
     <row r="2" spans="1:30" s="771" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="761"/>
@@ -57997,10 +58152,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="58.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="812" t="s">
+      <c r="A1" s="814" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="814" t="s">
+      <c r="B1" s="816" t="s">
         <v>61</v>
       </c>
       <c r="C1" s="682" t="s">
@@ -58050,8 +58205,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="813"/>
-      <c r="B2" s="815"/>
+      <c r="A2" s="815"/>
+      <c r="B2" s="817"/>
       <c r="C2" s="10" t="s">
         <v>102</v>
       </c>
@@ -58215,123 +58370,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="673" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="845" t="s">
+      <c r="A1" s="818" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="846"/>
-      <c r="C1" s="846"/>
-      <c r="D1" s="846"/>
-      <c r="E1" s="846"/>
-      <c r="F1" s="846"/>
-      <c r="G1" s="846"/>
-      <c r="H1" s="847" t="s">
+      <c r="B1" s="819"/>
+      <c r="C1" s="819"/>
+      <c r="D1" s="819"/>
+      <c r="E1" s="819"/>
+      <c r="F1" s="819"/>
+      <c r="G1" s="819"/>
+      <c r="H1" s="820" t="s">
         <v>504</v>
       </c>
-      <c r="I1" s="848"/>
-      <c r="J1" s="848"/>
-      <c r="K1" s="848"/>
-      <c r="L1" s="848"/>
-      <c r="M1" s="849"/>
-      <c r="N1" s="850" t="s">
+      <c r="I1" s="821"/>
+      <c r="J1" s="821"/>
+      <c r="K1" s="821"/>
+      <c r="L1" s="821"/>
+      <c r="M1" s="822"/>
+      <c r="N1" s="823" t="s">
         <v>117</v>
       </c>
-      <c r="O1" s="828"/>
-      <c r="P1" s="828"/>
-      <c r="Q1" s="828"/>
-      <c r="R1" s="828"/>
-      <c r="S1" s="828"/>
-      <c r="T1" s="828"/>
-      <c r="U1" s="828"/>
-      <c r="V1" s="851" t="s">
+      <c r="O1" s="824"/>
+      <c r="P1" s="824"/>
+      <c r="Q1" s="824"/>
+      <c r="R1" s="824"/>
+      <c r="S1" s="824"/>
+      <c r="T1" s="824"/>
+      <c r="U1" s="824"/>
+      <c r="V1" s="825" t="s">
         <v>118</v>
       </c>
-      <c r="W1" s="852"/>
-      <c r="X1" s="853"/>
-      <c r="Y1" s="853"/>
-      <c r="Z1" s="854"/>
-      <c r="AA1" s="855" t="s">
+      <c r="W1" s="826"/>
+      <c r="X1" s="827"/>
+      <c r="Y1" s="827"/>
+      <c r="Z1" s="828"/>
+      <c r="AA1" s="829" t="s">
         <v>119</v>
       </c>
-      <c r="AB1" s="856"/>
-      <c r="AC1" s="856"/>
-      <c r="AD1" s="856"/>
-      <c r="AE1" s="856"/>
-      <c r="AF1" s="856"/>
-      <c r="AG1" s="856"/>
-      <c r="AH1" s="856"/>
-      <c r="AI1" s="856"/>
-      <c r="AJ1" s="856"/>
-      <c r="AK1" s="856"/>
-      <c r="AL1" s="856"/>
-      <c r="AM1" s="856"/>
+      <c r="AB1" s="830"/>
+      <c r="AC1" s="830"/>
+      <c r="AD1" s="830"/>
+      <c r="AE1" s="830"/>
+      <c r="AF1" s="830"/>
+      <c r="AG1" s="830"/>
+      <c r="AH1" s="830"/>
+      <c r="AI1" s="830"/>
+      <c r="AJ1" s="830"/>
+      <c r="AK1" s="830"/>
+      <c r="AL1" s="830"/>
+      <c r="AM1" s="830"/>
       <c r="AN1" s="53"/>
       <c r="AO1" s="54"/>
-      <c r="AP1" s="827" t="s">
+      <c r="AP1" s="842" t="s">
         <v>120</v>
       </c>
-      <c r="AQ1" s="828"/>
-      <c r="AR1" s="828"/>
-      <c r="AS1" s="828"/>
-      <c r="AT1" s="828"/>
-      <c r="AU1" s="828"/>
-      <c r="AV1" s="828"/>
-      <c r="AW1" s="829"/>
-      <c r="AX1" s="836" t="s">
+      <c r="AQ1" s="824"/>
+      <c r="AR1" s="824"/>
+      <c r="AS1" s="824"/>
+      <c r="AT1" s="824"/>
+      <c r="AU1" s="824"/>
+      <c r="AV1" s="824"/>
+      <c r="AW1" s="843"/>
+      <c r="AX1" s="850" t="s">
         <v>121</v>
       </c>
-      <c r="AY1" s="837"/>
-      <c r="AZ1" s="837"/>
-      <c r="BA1" s="837"/>
-      <c r="BB1" s="837"/>
-      <c r="BC1" s="838"/>
-      <c r="BD1" s="839" t="s">
+      <c r="AY1" s="851"/>
+      <c r="AZ1" s="851"/>
+      <c r="BA1" s="851"/>
+      <c r="BB1" s="851"/>
+      <c r="BC1" s="852"/>
+      <c r="BD1" s="853" t="s">
         <v>122</v>
       </c>
-      <c r="BE1" s="840"/>
-      <c r="BF1" s="840"/>
-      <c r="BG1" s="840"/>
-      <c r="BH1" s="840"/>
-      <c r="BI1" s="841"/>
-      <c r="BJ1" s="842" t="s">
+      <c r="BE1" s="854"/>
+      <c r="BF1" s="854"/>
+      <c r="BG1" s="854"/>
+      <c r="BH1" s="854"/>
+      <c r="BI1" s="855"/>
+      <c r="BJ1" s="856" t="s">
         <v>123</v>
       </c>
-      <c r="BK1" s="843"/>
-      <c r="BL1" s="843"/>
-      <c r="BM1" s="843"/>
-      <c r="BN1" s="843"/>
-      <c r="BO1" s="843"/>
-      <c r="BP1" s="844"/>
-      <c r="BQ1" s="816" t="s">
+      <c r="BK1" s="857"/>
+      <c r="BL1" s="857"/>
+      <c r="BM1" s="857"/>
+      <c r="BN1" s="857"/>
+      <c r="BO1" s="857"/>
+      <c r="BP1" s="858"/>
+      <c r="BQ1" s="831" t="s">
         <v>124</v>
       </c>
-      <c r="BR1" s="817"/>
-      <c r="BS1" s="817"/>
-      <c r="BT1" s="817"/>
-      <c r="BU1" s="817"/>
-      <c r="BV1" s="817"/>
+      <c r="BR1" s="832"/>
+      <c r="BS1" s="832"/>
+      <c r="BT1" s="832"/>
+      <c r="BU1" s="832"/>
+      <c r="BV1" s="832"/>
       <c r="BW1" s="54"/>
       <c r="BX1" s="55"/>
-      <c r="BY1" s="818" t="s">
+      <c r="BY1" s="833" t="s">
         <v>125</v>
       </c>
-      <c r="BZ1" s="819"/>
-      <c r="CA1" s="819"/>
-      <c r="CB1" s="819"/>
-      <c r="CC1" s="819"/>
-      <c r="CD1" s="819"/>
-      <c r="CE1" s="819"/>
-      <c r="CF1" s="820"/>
-      <c r="CG1" s="820"/>
-      <c r="CH1" s="820"/>
-      <c r="CI1" s="820"/>
-      <c r="CJ1" s="820"/>
-      <c r="CK1" s="820"/>
-      <c r="CL1" s="820"/>
-      <c r="CM1" s="820"/>
-      <c r="CN1" s="820"/>
-      <c r="CO1" s="820"/>
-      <c r="CP1" s="820"/>
-      <c r="CQ1" s="820"/>
+      <c r="BZ1" s="834"/>
+      <c r="CA1" s="834"/>
+      <c r="CB1" s="834"/>
+      <c r="CC1" s="834"/>
+      <c r="CD1" s="834"/>
+      <c r="CE1" s="834"/>
+      <c r="CF1" s="835"/>
+      <c r="CG1" s="835"/>
+      <c r="CH1" s="835"/>
+      <c r="CI1" s="835"/>
+      <c r="CJ1" s="835"/>
+      <c r="CK1" s="835"/>
+      <c r="CL1" s="835"/>
+      <c r="CM1" s="835"/>
+      <c r="CN1" s="835"/>
+      <c r="CO1" s="835"/>
+      <c r="CP1" s="835"/>
+      <c r="CQ1" s="835"/>
     </row>
     <row r="2" spans="1:95" s="673" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
@@ -58355,18 +58510,18 @@
       <c r="G2" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="821" t="s">
+      <c r="H2" s="836" t="s">
         <v>505</v>
       </c>
-      <c r="I2" s="822"/>
-      <c r="J2" s="822" t="s">
+      <c r="I2" s="837"/>
+      <c r="J2" s="837" t="s">
         <v>133</v>
       </c>
-      <c r="K2" s="822"/>
-      <c r="L2" s="822" t="s">
+      <c r="K2" s="837"/>
+      <c r="L2" s="837" t="s">
         <v>134</v>
       </c>
-      <c r="M2" s="823"/>
+      <c r="M2" s="838"/>
       <c r="N2" s="58" t="s">
         <v>126</v>
       </c>
@@ -58475,36 +58630,36 @@
       <c r="AW2" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="AX2" s="824" t="s">
+      <c r="AX2" s="839" t="s">
         <v>161</v>
       </c>
-      <c r="AY2" s="825"/>
-      <c r="AZ2" s="825"/>
-      <c r="BA2" s="825" t="s">
+      <c r="AY2" s="840"/>
+      <c r="AZ2" s="840"/>
+      <c r="BA2" s="840" t="s">
         <v>162</v>
       </c>
-      <c r="BB2" s="825"/>
-      <c r="BC2" s="826"/>
-      <c r="BD2" s="830" t="s">
+      <c r="BB2" s="840"/>
+      <c r="BC2" s="841"/>
+      <c r="BD2" s="844" t="s">
         <v>161</v>
       </c>
-      <c r="BE2" s="831"/>
-      <c r="BF2" s="831"/>
-      <c r="BG2" s="831" t="s">
+      <c r="BE2" s="845"/>
+      <c r="BF2" s="845"/>
+      <c r="BG2" s="845" t="s">
         <v>162</v>
       </c>
-      <c r="BH2" s="831"/>
-      <c r="BI2" s="832"/>
-      <c r="BJ2" s="833" t="s">
+      <c r="BH2" s="845"/>
+      <c r="BI2" s="846"/>
+      <c r="BJ2" s="847" t="s">
         <v>161</v>
       </c>
-      <c r="BK2" s="834"/>
-      <c r="BL2" s="834"/>
-      <c r="BM2" s="834" t="s">
+      <c r="BK2" s="848"/>
+      <c r="BL2" s="848"/>
+      <c r="BM2" s="848" t="s">
         <v>162</v>
       </c>
-      <c r="BN2" s="835"/>
-      <c r="BO2" s="835"/>
+      <c r="BN2" s="849"/>
+      <c r="BO2" s="849"/>
       <c r="BP2" s="70" t="s">
         <v>163</v>
       </c>
@@ -59137,11 +59292,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -59157,6 +59307,11 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -59239,127 +59394,127 @@
         <v>203</v>
       </c>
       <c r="L1" s="146"/>
-      <c r="M1" s="880" t="s">
+      <c r="M1" s="859" t="s">
         <v>204</v>
       </c>
-      <c r="N1" s="973" t="s">
+      <c r="N1" s="860" t="s">
         <v>564</v>
       </c>
-      <c r="O1" s="974"/>
-      <c r="P1" s="974"/>
-      <c r="Q1" s="974"/>
-      <c r="R1" s="883" t="s">
+      <c r="O1" s="861"/>
+      <c r="P1" s="861"/>
+      <c r="Q1" s="861"/>
+      <c r="R1" s="862" t="s">
         <v>504</v>
       </c>
-      <c r="S1" s="876"/>
-      <c r="T1" s="876"/>
-      <c r="U1" s="876"/>
-      <c r="V1" s="876"/>
-      <c r="W1" s="876"/>
-      <c r="X1" s="884"/>
-      <c r="Y1" s="870" t="s">
+      <c r="S1" s="863"/>
+      <c r="T1" s="863"/>
+      <c r="U1" s="863"/>
+      <c r="V1" s="863"/>
+      <c r="W1" s="863"/>
+      <c r="X1" s="864"/>
+      <c r="Y1" s="865" t="s">
         <v>512</v>
       </c>
-      <c r="Z1" s="840"/>
-      <c r="AA1" s="885" t="s">
+      <c r="Z1" s="854"/>
+      <c r="AA1" s="868" t="s">
         <v>205</v>
       </c>
-      <c r="AB1" s="858" t="s">
+      <c r="AB1" s="879" t="s">
         <v>206</v>
       </c>
-      <c r="AC1" s="872" t="s">
+      <c r="AC1" s="875" t="s">
         <v>207</v>
       </c>
-      <c r="AD1" s="873"/>
-      <c r="AE1" s="873"/>
-      <c r="AF1" s="874"/>
-      <c r="AG1" s="875" t="s">
+      <c r="AD1" s="876"/>
+      <c r="AE1" s="876"/>
+      <c r="AF1" s="877"/>
+      <c r="AG1" s="878" t="s">
         <v>208</v>
       </c>
-      <c r="AH1" s="876"/>
-      <c r="AI1" s="876"/>
-      <c r="AJ1" s="876"/>
-      <c r="AK1" s="876"/>
-      <c r="AL1" s="876"/>
-      <c r="AM1" s="876"/>
-      <c r="AN1" s="876"/>
-      <c r="AO1" s="858" t="s">
+      <c r="AH1" s="863"/>
+      <c r="AI1" s="863"/>
+      <c r="AJ1" s="863"/>
+      <c r="AK1" s="863"/>
+      <c r="AL1" s="863"/>
+      <c r="AM1" s="863"/>
+      <c r="AN1" s="863"/>
+      <c r="AO1" s="879" t="s">
         <v>209</v>
       </c>
-      <c r="AP1" s="870" t="s">
+      <c r="AP1" s="865" t="s">
         <v>511</v>
       </c>
-      <c r="AQ1" s="840"/>
-      <c r="AR1" s="840"/>
-      <c r="AS1" s="841"/>
-      <c r="AT1" s="878" t="s">
+      <c r="AQ1" s="854"/>
+      <c r="AR1" s="854"/>
+      <c r="AS1" s="855"/>
+      <c r="AT1" s="882" t="s">
         <v>210</v>
       </c>
-      <c r="AU1" s="879"/>
-      <c r="AV1" s="879"/>
-      <c r="AW1" s="879"/>
-      <c r="AX1" s="879"/>
-      <c r="AY1" s="879"/>
-      <c r="AZ1" s="879"/>
-      <c r="BA1" s="879"/>
-      <c r="BB1" s="879"/>
-      <c r="BC1" s="879"/>
-      <c r="BD1" s="879"/>
-      <c r="BE1" s="879"/>
-      <c r="BF1" s="879"/>
-      <c r="BG1" s="879"/>
-      <c r="BH1" s="879"/>
-      <c r="BI1" s="879"/>
-      <c r="BJ1" s="879"/>
-      <c r="BK1" s="879"/>
-      <c r="BL1" s="879"/>
-      <c r="BM1" s="879"/>
-      <c r="BN1" s="879"/>
-      <c r="BO1" s="879"/>
-      <c r="BP1" s="879"/>
-      <c r="BQ1" s="879"/>
-      <c r="BR1" s="879"/>
-      <c r="BS1" s="879"/>
-      <c r="BT1" s="879"/>
-      <c r="BU1" s="879"/>
-      <c r="BV1" s="879"/>
-      <c r="BW1" s="858" t="s">
+      <c r="AU1" s="883"/>
+      <c r="AV1" s="883"/>
+      <c r="AW1" s="883"/>
+      <c r="AX1" s="883"/>
+      <c r="AY1" s="883"/>
+      <c r="AZ1" s="883"/>
+      <c r="BA1" s="883"/>
+      <c r="BB1" s="883"/>
+      <c r="BC1" s="883"/>
+      <c r="BD1" s="883"/>
+      <c r="BE1" s="883"/>
+      <c r="BF1" s="883"/>
+      <c r="BG1" s="883"/>
+      <c r="BH1" s="883"/>
+      <c r="BI1" s="883"/>
+      <c r="BJ1" s="883"/>
+      <c r="BK1" s="883"/>
+      <c r="BL1" s="883"/>
+      <c r="BM1" s="883"/>
+      <c r="BN1" s="883"/>
+      <c r="BO1" s="883"/>
+      <c r="BP1" s="883"/>
+      <c r="BQ1" s="883"/>
+      <c r="BR1" s="883"/>
+      <c r="BS1" s="883"/>
+      <c r="BT1" s="883"/>
+      <c r="BU1" s="883"/>
+      <c r="BV1" s="883"/>
+      <c r="BW1" s="879" t="s">
         <v>211</v>
       </c>
-      <c r="BX1" s="870" t="s">
+      <c r="BX1" s="865" t="s">
         <v>510</v>
       </c>
-      <c r="BY1" s="840"/>
-      <c r="BZ1" s="840"/>
-      <c r="CA1" s="841"/>
-      <c r="CB1" s="869" t="s">
+      <c r="BY1" s="854"/>
+      <c r="BZ1" s="854"/>
+      <c r="CA1" s="855"/>
+      <c r="CB1" s="891" t="s">
         <v>529</v>
       </c>
-      <c r="CC1" s="871" t="s">
+      <c r="CC1" s="873" t="s">
         <v>119</v>
       </c>
-      <c r="CD1" s="871"/>
-      <c r="CE1" s="871"/>
-      <c r="CF1" s="871"/>
-      <c r="CG1" s="871"/>
-      <c r="CH1" s="871"/>
-      <c r="CI1" s="871"/>
-      <c r="CJ1" s="871"/>
-      <c r="CK1" s="871"/>
-      <c r="CL1" s="871"/>
-      <c r="CM1" s="871"/>
-      <c r="CN1" s="871"/>
+      <c r="CD1" s="873"/>
+      <c r="CE1" s="873"/>
+      <c r="CF1" s="873"/>
+      <c r="CG1" s="873"/>
+      <c r="CH1" s="873"/>
+      <c r="CI1" s="873"/>
+      <c r="CJ1" s="873"/>
+      <c r="CK1" s="873"/>
+      <c r="CL1" s="873"/>
+      <c r="CM1" s="873"/>
+      <c r="CN1" s="873"/>
       <c r="CO1" s="147"/>
-      <c r="CP1" s="857" t="s">
+      <c r="CP1" s="887" t="s">
         <v>124</v>
       </c>
-      <c r="CQ1" s="828"/>
-      <c r="CR1" s="828"/>
-      <c r="CS1" s="828"/>
-      <c r="CT1" s="828"/>
-      <c r="CU1" s="828"/>
-      <c r="CV1" s="828"/>
-      <c r="CW1" s="829"/>
+      <c r="CQ1" s="824"/>
+      <c r="CR1" s="824"/>
+      <c r="CS1" s="824"/>
+      <c r="CT1" s="824"/>
+      <c r="CU1" s="824"/>
+      <c r="CV1" s="824"/>
+      <c r="CW1" s="843"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="148" t="s">
@@ -59398,7 +59553,7 @@
       <c r="L2" s="152" t="s">
         <v>127</v>
       </c>
-      <c r="M2" s="880"/>
+      <c r="M2" s="859"/>
       <c r="N2" s="153" t="s">
         <v>216</v>
       </c>
@@ -59414,22 +59569,22 @@
       <c r="R2" s="158" t="s">
         <v>219</v>
       </c>
-      <c r="S2" s="887" t="s">
+      <c r="S2" s="870" t="s">
         <v>505</v>
       </c>
-      <c r="T2" s="835"/>
-      <c r="U2" s="888" t="s">
+      <c r="T2" s="849"/>
+      <c r="U2" s="871" t="s">
         <v>133</v>
       </c>
-      <c r="V2" s="888"/>
-      <c r="W2" s="888" t="s">
+      <c r="V2" s="871"/>
+      <c r="W2" s="871" t="s">
         <v>134</v>
       </c>
-      <c r="X2" s="889"/>
-      <c r="Y2" s="864"/>
-      <c r="Z2" s="865"/>
-      <c r="AA2" s="886"/>
-      <c r="AB2" s="859"/>
+      <c r="X2" s="872"/>
+      <c r="Y2" s="866"/>
+      <c r="Z2" s="867"/>
+      <c r="AA2" s="869"/>
+      <c r="AB2" s="880"/>
       <c r="AC2" s="154" t="s">
         <v>220</v>
       </c>
@@ -59442,81 +59597,81 @@
       <c r="AF2" s="154" t="s">
         <v>223</v>
       </c>
-      <c r="AG2" s="877" t="s">
+      <c r="AG2" s="881" t="s">
         <v>224</v>
       </c>
-      <c r="AH2" s="862"/>
-      <c r="AI2" s="862" t="s">
+      <c r="AH2" s="874"/>
+      <c r="AI2" s="874" t="s">
         <v>225</v>
       </c>
-      <c r="AJ2" s="862"/>
-      <c r="AK2" s="862" t="s">
+      <c r="AJ2" s="874"/>
+      <c r="AK2" s="874" t="s">
         <v>226</v>
       </c>
-      <c r="AL2" s="862"/>
+      <c r="AL2" s="874"/>
       <c r="AM2" s="155" t="s">
         <v>227</v>
       </c>
       <c r="AN2" s="155" t="s">
         <v>228</v>
       </c>
-      <c r="AO2" s="859"/>
-      <c r="AP2" s="864" t="s">
+      <c r="AO2" s="880"/>
+      <c r="AP2" s="866" t="s">
         <v>229</v>
       </c>
-      <c r="AQ2" s="865"/>
-      <c r="AR2" s="866" t="s">
+      <c r="AQ2" s="867"/>
+      <c r="AR2" s="884" t="s">
         <v>230</v>
       </c>
-      <c r="AS2" s="867"/>
-      <c r="AT2" s="862" t="s">
+      <c r="AS2" s="885"/>
+      <c r="AT2" s="874" t="s">
         <v>231</v>
       </c>
-      <c r="AU2" s="862"/>
-      <c r="AV2" s="863" t="s">
+      <c r="AU2" s="874"/>
+      <c r="AV2" s="886" t="s">
         <v>232</v>
       </c>
-      <c r="AW2" s="863"/>
-      <c r="AX2" s="863" t="s">
+      <c r="AW2" s="886"/>
+      <c r="AX2" s="886" t="s">
         <v>233</v>
       </c>
-      <c r="AY2" s="863"/>
+      <c r="AY2" s="886"/>
       <c r="AZ2" s="155" t="s">
         <v>234</v>
       </c>
       <c r="BA2" s="155" t="s">
         <v>235</v>
       </c>
-      <c r="BB2" s="862" t="s">
+      <c r="BB2" s="874" t="s">
         <v>236</v>
       </c>
-      <c r="BC2" s="862"/>
-      <c r="BD2" s="863" t="s">
+      <c r="BC2" s="874"/>
+      <c r="BD2" s="886" t="s">
         <v>237</v>
       </c>
-      <c r="BE2" s="863"/>
-      <c r="BF2" s="863" t="s">
+      <c r="BE2" s="886"/>
+      <c r="BF2" s="886" t="s">
         <v>238</v>
       </c>
-      <c r="BG2" s="863"/>
+      <c r="BG2" s="886"/>
       <c r="BH2" s="155" t="s">
         <v>239</v>
       </c>
       <c r="BI2" s="155" t="s">
         <v>240</v>
       </c>
-      <c r="BJ2" s="862" t="s">
+      <c r="BJ2" s="874" t="s">
         <v>241</v>
       </c>
-      <c r="BK2" s="862"/>
-      <c r="BL2" s="863" t="s">
+      <c r="BK2" s="874"/>
+      <c r="BL2" s="886" t="s">
         <v>242</v>
       </c>
-      <c r="BM2" s="863"/>
-      <c r="BN2" s="863" t="s">
+      <c r="BM2" s="886"/>
+      <c r="BN2" s="886" t="s">
         <v>243</v>
       </c>
-      <c r="BO2" s="863"/>
+      <c r="BO2" s="886"/>
       <c r="BP2" s="155" t="s">
         <v>244</v>
       </c>
@@ -59538,16 +59693,16 @@
       <c r="BV2" s="155" t="s">
         <v>250</v>
       </c>
-      <c r="BW2" s="859"/>
-      <c r="BX2" s="864" t="s">
+      <c r="BW2" s="880"/>
+      <c r="BX2" s="866" t="s">
         <v>229</v>
       </c>
-      <c r="BY2" s="865"/>
-      <c r="BZ2" s="866" t="s">
+      <c r="BY2" s="867"/>
+      <c r="BZ2" s="884" t="s">
         <v>230</v>
       </c>
-      <c r="CA2" s="867"/>
-      <c r="CB2" s="869"/>
+      <c r="CA2" s="885"/>
+      <c r="CB2" s="891"/>
       <c r="CC2" s="139" t="s">
         <v>142</v>
       </c>
@@ -59587,22 +59742,22 @@
       <c r="CO2" s="141" t="s">
         <v>513</v>
       </c>
-      <c r="CP2" s="868" t="s">
+      <c r="CP2" s="890" t="s">
         <v>252</v>
       </c>
-      <c r="CQ2" s="860"/>
-      <c r="CR2" s="860" t="s">
+      <c r="CQ2" s="888"/>
+      <c r="CR2" s="888" t="s">
         <v>253</v>
       </c>
-      <c r="CS2" s="860"/>
-      <c r="CT2" s="860" t="s">
+      <c r="CS2" s="888"/>
+      <c r="CT2" s="888" t="s">
         <v>254</v>
       </c>
-      <c r="CU2" s="860"/>
-      <c r="CV2" s="860" t="s">
+      <c r="CU2" s="888"/>
+      <c r="CV2" s="888" t="s">
         <v>255</v>
       </c>
-      <c r="CW2" s="861"/>
+      <c r="CW2" s="889"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="169"/>
@@ -60467,29 +60622,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="39">
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="CC1:CN1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AN1"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
     <mergeCell ref="CP1:CW1"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="CV2:CW2"/>
@@ -60506,6 +60638,29 @@
     <mergeCell ref="CT2:CU2"/>
     <mergeCell ref="CB1:CB2"/>
     <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CC1:CN1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AN1"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -60548,105 +60703,110 @@
       <c r="K1" s="145"/>
       <c r="L1" s="146"/>
       <c r="M1" s="713"/>
-      <c r="N1" s="881"/>
-      <c r="O1" s="882"/>
-      <c r="P1" s="882"/>
-      <c r="Q1" s="882"/>
-      <c r="R1" s="883"/>
-      <c r="S1" s="876"/>
-      <c r="T1" s="876"/>
-      <c r="U1" s="876"/>
-      <c r="V1" s="876"/>
-      <c r="W1" s="876"/>
-      <c r="X1" s="884"/>
-      <c r="Y1" s="870"/>
-      <c r="Z1" s="840"/>
+      <c r="N1" s="895"/>
+      <c r="O1" s="896"/>
+      <c r="P1" s="896"/>
+      <c r="Q1" s="896"/>
+      <c r="R1" s="862"/>
+      <c r="S1" s="863"/>
+      <c r="T1" s="863"/>
+      <c r="U1" s="863"/>
+      <c r="V1" s="863"/>
+      <c r="W1" s="863"/>
+      <c r="X1" s="864"/>
+      <c r="Y1" s="865"/>
+      <c r="Z1" s="854"/>
       <c r="AA1" s="714"/>
       <c r="AB1" s="712"/>
-      <c r="AC1" s="872"/>
-      <c r="AD1" s="873"/>
-      <c r="AE1" s="873"/>
-      <c r="AF1" s="874"/>
-      <c r="AG1" s="875"/>
-      <c r="AH1" s="876"/>
-      <c r="AI1" s="876"/>
-      <c r="AJ1" s="876"/>
-      <c r="AK1" s="876"/>
-      <c r="AL1" s="876"/>
-      <c r="AM1" s="876"/>
-      <c r="AN1" s="876"/>
+      <c r="AC1" s="875"/>
+      <c r="AD1" s="876"/>
+      <c r="AE1" s="876"/>
+      <c r="AF1" s="877"/>
+      <c r="AG1" s="878"/>
+      <c r="AH1" s="863"/>
+      <c r="AI1" s="863"/>
+      <c r="AJ1" s="863"/>
+      <c r="AK1" s="863"/>
+      <c r="AL1" s="863"/>
+      <c r="AM1" s="863"/>
+      <c r="AN1" s="863"/>
       <c r="AO1" s="712"/>
-      <c r="AP1" s="870"/>
-      <c r="AQ1" s="840"/>
-      <c r="AR1" s="840"/>
-      <c r="AS1" s="841"/>
-      <c r="AT1" s="878"/>
-      <c r="AU1" s="879"/>
-      <c r="AV1" s="879"/>
-      <c r="AW1" s="879"/>
-      <c r="AX1" s="879"/>
-      <c r="AY1" s="879"/>
-      <c r="AZ1" s="879"/>
-      <c r="BA1" s="879"/>
-      <c r="BB1" s="879"/>
-      <c r="BC1" s="879"/>
-      <c r="BD1" s="879"/>
-      <c r="BE1" s="879"/>
-      <c r="BF1" s="879"/>
-      <c r="BG1" s="879"/>
-      <c r="BH1" s="879"/>
-      <c r="BI1" s="879"/>
-      <c r="BJ1" s="879"/>
-      <c r="BK1" s="879"/>
-      <c r="BL1" s="879"/>
-      <c r="BM1" s="879"/>
-      <c r="BN1" s="879"/>
-      <c r="BO1" s="879"/>
-      <c r="BP1" s="879"/>
-      <c r="BQ1" s="879"/>
-      <c r="BR1" s="879"/>
-      <c r="BS1" s="879"/>
-      <c r="BT1" s="879"/>
-      <c r="BU1" s="879"/>
-      <c r="BV1" s="879"/>
+      <c r="AP1" s="865"/>
+      <c r="AQ1" s="854"/>
+      <c r="AR1" s="854"/>
+      <c r="AS1" s="855"/>
+      <c r="AT1" s="882"/>
+      <c r="AU1" s="883"/>
+      <c r="AV1" s="883"/>
+      <c r="AW1" s="883"/>
+      <c r="AX1" s="883"/>
+      <c r="AY1" s="883"/>
+      <c r="AZ1" s="883"/>
+      <c r="BA1" s="883"/>
+      <c r="BB1" s="883"/>
+      <c r="BC1" s="883"/>
+      <c r="BD1" s="883"/>
+      <c r="BE1" s="883"/>
+      <c r="BF1" s="883"/>
+      <c r="BG1" s="883"/>
+      <c r="BH1" s="883"/>
+      <c r="BI1" s="883"/>
+      <c r="BJ1" s="883"/>
+      <c r="BK1" s="883"/>
+      <c r="BL1" s="883"/>
+      <c r="BM1" s="883"/>
+      <c r="BN1" s="883"/>
+      <c r="BO1" s="883"/>
+      <c r="BP1" s="883"/>
+      <c r="BQ1" s="883"/>
+      <c r="BR1" s="883"/>
+      <c r="BS1" s="883"/>
+      <c r="BT1" s="883"/>
+      <c r="BU1" s="883"/>
+      <c r="BV1" s="883"/>
       <c r="BW1" s="712"/>
-      <c r="BX1" s="870"/>
-      <c r="BY1" s="840"/>
-      <c r="BZ1" s="840"/>
-      <c r="CA1" s="841"/>
-      <c r="CB1" s="871"/>
-      <c r="CC1" s="871"/>
-      <c r="CD1" s="871"/>
-      <c r="CE1" s="871"/>
-      <c r="CF1" s="871"/>
-      <c r="CG1" s="871"/>
-      <c r="CH1" s="871"/>
-      <c r="CI1" s="871"/>
-      <c r="CJ1" s="871"/>
-      <c r="CK1" s="871"/>
-      <c r="CL1" s="871"/>
-      <c r="CM1" s="871"/>
+      <c r="BX1" s="865"/>
+      <c r="BY1" s="854"/>
+      <c r="BZ1" s="854"/>
+      <c r="CA1" s="855"/>
+      <c r="CB1" s="873"/>
+      <c r="CC1" s="873"/>
+      <c r="CD1" s="873"/>
+      <c r="CE1" s="873"/>
+      <c r="CF1" s="873"/>
+      <c r="CG1" s="873"/>
+      <c r="CH1" s="873"/>
+      <c r="CI1" s="873"/>
+      <c r="CJ1" s="873"/>
+      <c r="CK1" s="873"/>
+      <c r="CL1" s="873"/>
+      <c r="CM1" s="873"/>
       <c r="CN1" s="711"/>
-      <c r="CO1" s="857"/>
-      <c r="CP1" s="828"/>
-      <c r="CQ1" s="828"/>
-      <c r="CR1" s="828"/>
-      <c r="CS1" s="828"/>
-      <c r="CT1" s="828"/>
-      <c r="CU1" s="828"/>
-      <c r="CV1" s="829"/>
-      <c r="CW1" s="890"/>
-      <c r="CX1" s="891"/>
-      <c r="CY1" s="891"/>
-      <c r="CZ1" s="892"/>
-      <c r="DA1" s="891"/>
-      <c r="DB1" s="891"/>
-      <c r="DC1" s="892"/>
-      <c r="DD1" s="891"/>
-      <c r="DE1" s="891"/>
+      <c r="CO1" s="887"/>
+      <c r="CP1" s="824"/>
+      <c r="CQ1" s="824"/>
+      <c r="CR1" s="824"/>
+      <c r="CS1" s="824"/>
+      <c r="CT1" s="824"/>
+      <c r="CU1" s="824"/>
+      <c r="CV1" s="843"/>
+      <c r="CW1" s="892"/>
+      <c r="CX1" s="893"/>
+      <c r="CY1" s="893"/>
+      <c r="CZ1" s="894"/>
+      <c r="DA1" s="893"/>
+      <c r="DB1" s="893"/>
+      <c r="DC1" s="894"/>
+      <c r="DD1" s="893"/>
+      <c r="DE1" s="893"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="CZ1:DB1"/>
     <mergeCell ref="DC1:DE1"/>
@@ -60655,11 +60815,6 @@
     <mergeCell ref="AG1:AN1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CB1:CM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -60682,12 +60837,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="895" t="s">
+      <c r="A1" s="899" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="896"/>
-      <c r="C1" s="896"/>
-      <c r="D1" s="893" t="s">
+      <c r="B1" s="900"/>
+      <c r="C1" s="900"/>
+      <c r="D1" s="897" t="s">
         <v>258</v>
       </c>
     </row>
@@ -60701,7 +60856,7 @@
       <c r="C2" s="474" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="894"/>
+      <c r="D2" s="898"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="465"/>
@@ -60789,10 +60944,10 @@
       <c r="B2" s="204" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="904" t="s">
+      <c r="C2" s="901" t="s">
         <v>276</v>
       </c>
-      <c r="D2" s="904"/>
+      <c r="D2" s="901"/>
       <c r="E2" s="202"/>
       <c r="F2" s="202"/>
       <c r="G2" s="202"/>
@@ -60917,32 +61072,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="201"/>
-      <c r="B7" s="905" t="s">
+      <c r="B7" s="902" t="s">
         <v>488</v>
       </c>
-      <c r="C7" s="905"/>
-      <c r="D7" s="905"/>
+      <c r="C7" s="902"/>
+      <c r="D7" s="902"/>
       <c r="E7" s="202"/>
       <c r="F7" s="202"/>
       <c r="G7" s="202"/>
       <c r="H7" s="202"/>
       <c r="I7" s="202"/>
-      <c r="J7" s="905" t="s">
+      <c r="J7" s="902" t="s">
         <v>487</v>
       </c>
-      <c r="K7" s="905"/>
-      <c r="L7" s="905"/>
+      <c r="K7" s="902"/>
+      <c r="L7" s="902"/>
       <c r="M7" s="202"/>
       <c r="N7" s="202"/>
       <c r="O7" s="202"/>
       <c r="P7" s="203" t="s">
         <v>280</v>
       </c>
-      <c r="Q7" s="905" t="s">
+      <c r="Q7" s="902" t="s">
         <v>488</v>
       </c>
-      <c r="R7" s="905"/>
-      <c r="S7" s="905"/>
+      <c r="R7" s="902"/>
+      <c r="S7" s="902"/>
       <c r="T7" s="202"/>
       <c r="U7" s="216" t="s">
         <v>281</v>
@@ -60976,41 +61131,41 @@
       <c r="B9" s="217" t="s">
         <v>490</v>
       </c>
-      <c r="C9" s="900" t="s">
+      <c r="C9" s="903" t="s">
         <v>282</v>
       </c>
-      <c r="D9" s="901"/>
-      <c r="E9" s="900" t="s">
+      <c r="D9" s="904"/>
+      <c r="E9" s="903" t="s">
         <v>283</v>
       </c>
-      <c r="F9" s="901"/>
+      <c r="F9" s="904"/>
       <c r="G9" s="202"/>
       <c r="H9" s="202"/>
       <c r="I9" s="202"/>
       <c r="J9" s="217" t="s">
         <v>490</v>
       </c>
-      <c r="K9" s="900" t="s">
+      <c r="K9" s="903" t="s">
         <v>282</v>
       </c>
-      <c r="L9" s="901"/>
-      <c r="M9" s="900" t="s">
+      <c r="L9" s="904"/>
+      <c r="M9" s="903" t="s">
         <v>283</v>
       </c>
-      <c r="N9" s="901"/>
+      <c r="N9" s="904"/>
       <c r="O9" s="202"/>
       <c r="P9" s="202"/>
       <c r="Q9" s="217" t="s">
         <v>490</v>
       </c>
-      <c r="R9" s="900" t="s">
+      <c r="R9" s="903" t="s">
         <v>282</v>
       </c>
-      <c r="S9" s="901"/>
-      <c r="T9" s="900" t="s">
+      <c r="S9" s="904"/>
+      <c r="T9" s="903" t="s">
         <v>283</v>
       </c>
-      <c r="U9" s="901"/>
+      <c r="U9" s="904"/>
     </row>
     <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="201"/>
@@ -61072,10 +61227,10 @@
       </c>
       <c r="C11" s="222"/>
       <c r="D11" s="222"/>
-      <c r="E11" s="897" t="s">
+      <c r="E11" s="905" t="s">
         <v>287</v>
       </c>
-      <c r="F11" s="898"/>
+      <c r="F11" s="906"/>
       <c r="G11" s="223"/>
       <c r="H11" s="223"/>
       <c r="I11" s="223"/>
@@ -61084,10 +61239,10 @@
       </c>
       <c r="K11" s="202"/>
       <c r="L11" s="202"/>
-      <c r="M11" s="902" t="s">
+      <c r="M11" s="908" t="s">
         <v>287</v>
       </c>
-      <c r="N11" s="903"/>
+      <c r="N11" s="909"/>
       <c r="O11" s="223"/>
       <c r="P11" s="223"/>
       <c r="Q11" s="221" t="s">
@@ -61095,10 +61250,10 @@
       </c>
       <c r="R11" s="222"/>
       <c r="S11" s="222"/>
-      <c r="T11" s="897" t="s">
+      <c r="T11" s="905" t="s">
         <v>287</v>
       </c>
-      <c r="U11" s="898"/>
+      <c r="U11" s="906"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="201"/>
@@ -61333,10 +61488,10 @@
       </c>
       <c r="C20" s="303"/>
       <c r="D20" s="250"/>
-      <c r="E20" s="897" t="s">
+      <c r="E20" s="905" t="s">
         <v>294</v>
       </c>
-      <c r="F20" s="898"/>
+      <c r="F20" s="906"/>
       <c r="G20" s="231"/>
       <c r="H20" s="231"/>
       <c r="I20" s="202"/>
@@ -61345,10 +61500,10 @@
       </c>
       <c r="K20" s="303"/>
       <c r="L20" s="250"/>
-      <c r="M20" s="897" t="s">
+      <c r="M20" s="905" t="s">
         <v>294</v>
       </c>
-      <c r="N20" s="898"/>
+      <c r="N20" s="906"/>
       <c r="O20" s="241"/>
       <c r="P20" s="241"/>
       <c r="Q20" s="221" t="s">
@@ -61356,10 +61511,10 @@
       </c>
       <c r="R20" s="303"/>
       <c r="S20" s="250"/>
-      <c r="T20" s="897" t="s">
+      <c r="T20" s="905" t="s">
         <v>294</v>
       </c>
-      <c r="U20" s="898"/>
+      <c r="U20" s="906"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="201"/>
@@ -61623,10 +61778,10 @@
       </c>
       <c r="C30" s="303"/>
       <c r="D30" s="250"/>
-      <c r="E30" s="897" t="s">
+      <c r="E30" s="905" t="s">
         <v>294</v>
       </c>
-      <c r="F30" s="898"/>
+      <c r="F30" s="906"/>
       <c r="G30" s="231"/>
       <c r="H30" s="231"/>
       <c r="I30" s="202"/>
@@ -61635,10 +61790,10 @@
       </c>
       <c r="K30" s="303"/>
       <c r="L30" s="250"/>
-      <c r="M30" s="897" t="s">
+      <c r="M30" s="905" t="s">
         <v>294</v>
       </c>
-      <c r="N30" s="898"/>
+      <c r="N30" s="906"/>
       <c r="O30" s="241"/>
       <c r="P30" s="241"/>
       <c r="Q30" s="221" t="s">
@@ -61646,10 +61801,10 @@
       </c>
       <c r="R30" s="303"/>
       <c r="S30" s="250"/>
-      <c r="T30" s="897" t="s">
+      <c r="T30" s="905" t="s">
         <v>294</v>
       </c>
-      <c r="U30" s="898"/>
+      <c r="U30" s="906"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="263"/>
@@ -61988,11 +62143,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="201"/>
-      <c r="B42" s="899"/>
-      <c r="C42" s="899"/>
-      <c r="D42" s="899"/>
-      <c r="E42" s="899"/>
-      <c r="F42" s="899"/>
+      <c r="B42" s="907"/>
+      <c r="C42" s="907"/>
+      <c r="D42" s="907"/>
+      <c r="E42" s="907"/>
+      <c r="F42" s="907"/>
       <c r="G42" s="241"/>
       <c r="H42" s="202"/>
       <c r="I42" s="241"/>
@@ -62137,15 +62292,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="20">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -62157,6 +62303,15 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
drupal update and add a table for art 5.4 in summary legal comp sheet
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368" activeTab="4"/>
+    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="600">
   <si>
     <t>Acronym</t>
   </si>
@@ -2272,9 +2272,6 @@
     <t>This sheet presents at country level aggregated values for waste water collection and treatment situation when for each level of treatment respectively equipment is in place and performance = pass. This is different from sheet summary legal compliance which considers all rules of the Directive.</t>
   </si>
   <si>
-    <t>SA/CSA applying Art. 5</t>
-  </si>
-  <si>
     <t>NR (reference: wastewater load connected to collecting system)</t>
   </si>
   <si>
@@ -2291,6 +2288,12 @@
   </si>
   <si>
     <t>Compliance of treatment plant under pending deadline</t>
+  </si>
+  <si>
+    <t>SA/CSA applying Art. 5.2,3</t>
+  </si>
+  <si>
+    <t>SA/CSA applying Art. 5.4</t>
   </si>
 </sst>
 </file>
@@ -5740,45 +5743,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -5813,6 +5777,9 @@
     <xf numFmtId="3" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5861,6 +5828,111 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5873,21 +5945,9 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5903,62 +5963,11 @@
     <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5969,12 +5978,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5987,32 +5990,32 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6042,6 +6045,33 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6075,31 +6105,10 @@
     <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6121,15 +6130,61 @@
     <xf numFmtId="3" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6142,18 +6197,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6165,46 +6208,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6518,9 +6521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7052,7 +7053,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="820" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C19" s="821"/>
       <c r="D19" s="823"/>
@@ -7088,7 +7089,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="804" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C23" s="363"/>
       <c r="D23" s="362"/>
@@ -7210,7 +7211,7 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="816" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C39" s="817"/>
       <c r="D39" s="823"/>
@@ -7246,7 +7247,7 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="816" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C43" s="360"/>
       <c r="D43" s="355"/>
@@ -7365,7 +7366,7 @@
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="815" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C58" s="817"/>
       <c r="D58" s="823"/>
@@ -7401,7 +7402,7 @@
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="804" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C62" s="360"/>
       <c r="D62" s="364"/>
@@ -7520,7 +7521,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="815" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C77" s="817"/>
       <c r="D77" s="823"/>
@@ -7556,7 +7557,7 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" s="804" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C81" s="360"/>
       <c r="D81" s="364"/>
@@ -7610,8 +7611,8 @@
       </c>
       <c r="C2" s="373"/>
       <c r="D2" s="373"/>
-      <c r="E2" s="919"/>
-      <c r="F2" s="919"/>
+      <c r="E2" s="926"/>
+      <c r="F2" s="926"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="372"/>
@@ -7643,13 +7644,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="370"/>
-      <c r="B6" s="920" t="s">
+      <c r="B6" s="927" t="s">
         <v>452</v>
       </c>
-      <c r="C6" s="920"/>
-      <c r="D6" s="920"/>
-      <c r="E6" s="920"/>
-      <c r="F6" s="920"/>
+      <c r="C6" s="927"/>
+      <c r="D6" s="927"/>
+      <c r="E6" s="927"/>
+      <c r="F6" s="927"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="370"/>
@@ -7807,11 +7808,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="370"/>
-      <c r="B22" s="925"/>
-      <c r="C22" s="925"/>
-      <c r="D22" s="925"/>
-      <c r="E22" s="925"/>
-      <c r="F22" s="925"/>
+      <c r="B22" s="921"/>
+      <c r="C22" s="921"/>
+      <c r="D22" s="921"/>
+      <c r="E22" s="921"/>
+      <c r="F22" s="921"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="370"/>
@@ -8108,43 +8109,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="941" t="s">
+      <c r="A1" s="950" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="942"/>
+      <c r="B1" s="951"/>
       <c r="C1" s="455"/>
-      <c r="D1" s="952" t="s">
+      <c r="D1" s="941" t="s">
         <v>300</v>
       </c>
-      <c r="E1" s="953"/>
-      <c r="F1" s="953"/>
-      <c r="G1" s="953"/>
-      <c r="H1" s="953"/>
-      <c r="I1" s="954"/>
-      <c r="J1" s="943" t="s">
+      <c r="E1" s="942"/>
+      <c r="F1" s="942"/>
+      <c r="G1" s="942"/>
+      <c r="H1" s="942"/>
+      <c r="I1" s="943"/>
+      <c r="J1" s="952" t="s">
         <v>301</v>
       </c>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
-      <c r="M1" s="944"/>
-      <c r="N1" s="945"/>
-      <c r="O1" s="946" t="s">
+      <c r="K1" s="953"/>
+      <c r="L1" s="953"/>
+      <c r="M1" s="953"/>
+      <c r="N1" s="954"/>
+      <c r="O1" s="955" t="s">
         <v>302</v>
       </c>
-      <c r="P1" s="947"/>
-      <c r="Q1" s="948"/>
+      <c r="P1" s="956"/>
+      <c r="Q1" s="957"/>
       <c r="R1" s="442" t="s">
         <v>81</v>
       </c>
       <c r="S1" s="443"/>
-      <c r="T1" s="940" t="s">
+      <c r="T1" s="949" t="s">
         <v>496</v>
       </c>
-      <c r="U1" s="940"/>
-      <c r="V1" s="940"/>
-      <c r="W1" s="940"/>
-      <c r="X1" s="940"/>
-      <c r="Y1" s="940"/>
+      <c r="U1" s="949"/>
+      <c r="V1" s="949"/>
+      <c r="W1" s="949"/>
+      <c r="X1" s="949"/>
+      <c r="Y1" s="949"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="445" t="s">
@@ -8156,18 +8157,18 @@
       <c r="C2" s="446" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="957" t="s">
+      <c r="D2" s="946" t="s">
         <v>304</v>
       </c>
-      <c r="E2" s="956"/>
-      <c r="F2" s="956" t="s">
+      <c r="E2" s="945"/>
+      <c r="F2" s="945" t="s">
         <v>305</v>
       </c>
-      <c r="G2" s="956"/>
-      <c r="H2" s="955" t="s">
+      <c r="G2" s="945"/>
+      <c r="H2" s="944" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="955"/>
+      <c r="I2" s="944"/>
       <c r="J2" s="447">
         <v>0</v>
       </c>
@@ -8198,18 +8199,18 @@
       <c r="S2" s="682" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="938" t="s">
+      <c r="T2" s="947" t="s">
         <v>464</v>
       </c>
-      <c r="U2" s="938"/>
-      <c r="V2" s="939" t="s">
+      <c r="U2" s="947"/>
+      <c r="V2" s="948" t="s">
         <v>482</v>
       </c>
-      <c r="W2" s="939"/>
-      <c r="X2" s="939" t="s">
+      <c r="W2" s="948"/>
+      <c r="X2" s="948" t="s">
         <v>483</v>
       </c>
-      <c r="Y2" s="939"/>
+      <c r="Y2" s="948"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="450"/>
@@ -8235,13 +8236,13 @@
       <c r="I3" s="666" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="949" t="s">
+      <c r="J3" s="938" t="s">
         <v>311</v>
       </c>
-      <c r="K3" s="950"/>
-      <c r="L3" s="950"/>
-      <c r="M3" s="950"/>
-      <c r="N3" s="951"/>
+      <c r="K3" s="939"/>
+      <c r="L3" s="939"/>
+      <c r="M3" s="939"/>
+      <c r="N3" s="940"/>
       <c r="O3" s="458"/>
       <c r="P3" s="458"/>
       <c r="Q3" s="458"/>
@@ -9470,11 +9471,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:X4"/>
   <mergeCells count="12">
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -9482,6 +9478,11 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9521,25 +9522,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="836" t="s">
+      <c r="A1" s="865" t="s">
         <v>312</v>
       </c>
-      <c r="B1" s="837"/>
-      <c r="C1" s="837"/>
-      <c r="D1" s="837"/>
-      <c r="E1" s="837"/>
-      <c r="F1" s="837"/>
+      <c r="B1" s="866"/>
+      <c r="C1" s="866"/>
+      <c r="D1" s="866"/>
+      <c r="E1" s="866"/>
+      <c r="F1" s="866"/>
       <c r="G1" s="472"/>
-      <c r="H1" s="961" t="s">
+      <c r="H1" s="963" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="962"/>
-      <c r="J1" s="962"/>
+      <c r="I1" s="964"/>
+      <c r="J1" s="964"/>
       <c r="K1" s="474"/>
       <c r="L1" s="464"/>
       <c r="M1" s="474"/>
       <c r="N1" s="465"/>
-      <c r="O1" s="959" t="s">
+      <c r="O1" s="961" t="s">
         <v>313</v>
       </c>
       <c r="P1" s="466"/>
@@ -9551,26 +9552,26 @@
       <c r="T1" s="464"/>
       <c r="U1" s="474"/>
       <c r="V1" s="465"/>
-      <c r="W1" s="959" t="s">
+      <c r="W1" s="961" t="s">
         <v>315</v>
       </c>
       <c r="X1" s="466"/>
-      <c r="Y1" s="963" t="s">
+      <c r="Y1" s="965" t="s">
         <v>316</v>
       </c>
-      <c r="Z1" s="963"/>
-      <c r="AA1" s="963"/>
-      <c r="AB1" s="963"/>
-      <c r="AC1" s="963"/>
-      <c r="AD1" s="964"/>
-      <c r="AE1" s="959" t="s">
+      <c r="Z1" s="965"/>
+      <c r="AA1" s="965"/>
+      <c r="AB1" s="965"/>
+      <c r="AC1" s="965"/>
+      <c r="AD1" s="966"/>
+      <c r="AE1" s="961" t="s">
         <v>317</v>
       </c>
-      <c r="AF1" s="958" t="s">
+      <c r="AF1" s="960" t="s">
         <v>481</v>
       </c>
-      <c r="AG1" s="940"/>
-      <c r="AH1" s="940"/>
+      <c r="AG1" s="949"/>
+      <c r="AH1" s="949"/>
       <c r="AI1" s="689"/>
       <c r="AJ1" s="689"/>
       <c r="AK1" s="689"/>
@@ -9629,56 +9630,56 @@
       <c r="C2" s="473" t="s">
         <v>319</v>
       </c>
-      <c r="D2" s="966" t="s">
+      <c r="D2" s="959" t="s">
         <v>486</v>
       </c>
-      <c r="E2" s="966"/>
-      <c r="F2" s="966" t="s">
+      <c r="E2" s="959"/>
+      <c r="F2" s="959" t="s">
         <v>487</v>
       </c>
-      <c r="G2" s="966"/>
+      <c r="G2" s="959"/>
       <c r="H2" s="468"/>
-      <c r="I2" s="965" t="s">
+      <c r="I2" s="958" t="s">
         <v>188</v>
       </c>
-      <c r="J2" s="965"/>
-      <c r="K2" s="965" t="s">
+      <c r="J2" s="958"/>
+      <c r="K2" s="958" t="s">
         <v>189</v>
       </c>
-      <c r="L2" s="965"/>
-      <c r="M2" s="965" t="s">
+      <c r="L2" s="958"/>
+      <c r="M2" s="958" t="s">
         <v>190</v>
       </c>
       <c r="N2" s="967"/>
-      <c r="O2" s="960"/>
+      <c r="O2" s="962"/>
       <c r="P2" s="469"/>
-      <c r="Q2" s="965" t="s">
+      <c r="Q2" s="958" t="s">
         <v>188</v>
       </c>
-      <c r="R2" s="965"/>
-      <c r="S2" s="965" t="s">
+      <c r="R2" s="958"/>
+      <c r="S2" s="958" t="s">
         <v>189</v>
       </c>
-      <c r="T2" s="965"/>
-      <c r="U2" s="965" t="s">
+      <c r="T2" s="958"/>
+      <c r="U2" s="958" t="s">
         <v>190</v>
       </c>
       <c r="V2" s="967"/>
-      <c r="W2" s="960"/>
+      <c r="W2" s="962"/>
       <c r="X2" s="469"/>
-      <c r="Y2" s="965" t="s">
+      <c r="Y2" s="958" t="s">
         <v>188</v>
       </c>
-      <c r="Z2" s="965"/>
-      <c r="AA2" s="965" t="s">
+      <c r="Z2" s="958"/>
+      <c r="AA2" s="958" t="s">
         <v>189</v>
       </c>
-      <c r="AB2" s="965"/>
-      <c r="AC2" s="965" t="s">
+      <c r="AB2" s="958"/>
+      <c r="AC2" s="958" t="s">
         <v>190</v>
       </c>
       <c r="AD2" s="967"/>
-      <c r="AE2" s="960"/>
+      <c r="AE2" s="962"/>
       <c r="AF2" s="683" t="s">
         <v>464</v>
       </c>
@@ -10564,6 +10565,8 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:AH4"/>
   <mergeCells count="18">
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="AF1:AH1"/>
@@ -10580,8 +10583,6 @@
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="Y2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10796,9 +10797,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="968"/>
-      <c r="B1" s="867"/>
-      <c r="C1" s="867"/>
+      <c r="A1" s="986"/>
+      <c r="B1" s="855"/>
+      <c r="C1" s="855"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="742"/>
@@ -10813,21 +10814,21 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="976" t="s">
+      <c r="A3" s="990" t="s">
         <v>345</v>
       </c>
-      <c r="B3" s="978" t="s">
+      <c r="B3" s="992" t="s">
         <v>453</v>
       </c>
-      <c r="C3" s="979"/>
-      <c r="D3" s="974" t="s">
+      <c r="C3" s="993"/>
+      <c r="D3" s="978" t="s">
         <v>454</v>
       </c>
-      <c r="E3" s="975"/>
-      <c r="F3" s="974" t="s">
+      <c r="E3" s="979"/>
+      <c r="F3" s="978" t="s">
         <v>489</v>
       </c>
-      <c r="G3" s="975"/>
+      <c r="G3" s="979"/>
       <c r="I3" s="740" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
@@ -10838,14 +10839,14 @@
       <c r="K3" s="722"/>
       <c r="L3" s="722"/>
       <c r="N3" s="707"/>
-      <c r="O3" s="990" t="s">
+      <c r="O3" s="975" t="s">
         <v>346</v>
       </c>
-      <c r="P3" s="990"/>
-      <c r="Q3" s="990" t="s">
+      <c r="P3" s="975"/>
+      <c r="Q3" s="975" t="s">
         <v>347</v>
       </c>
-      <c r="R3" s="990"/>
+      <c r="R3" s="975"/>
       <c r="S3" s="707"/>
       <c r="T3" s="715" t="s">
         <v>348</v>
@@ -10853,7 +10854,7 @@
       <c r="U3" s="707"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="977"/>
+      <c r="A4" s="991"/>
       <c r="B4" s="512" t="s">
         <v>349</v>
       </c>
@@ -11112,14 +11113,14 @@
       <c r="K10" s="722"/>
       <c r="L10" s="722"/>
       <c r="N10" s="715"/>
-      <c r="O10" s="990" t="s">
+      <c r="O10" s="975" t="s">
         <v>349</v>
       </c>
-      <c r="P10" s="990"/>
-      <c r="Q10" s="990" t="s">
+      <c r="P10" s="975"/>
+      <c r="Q10" s="975" t="s">
         <v>356</v>
       </c>
-      <c r="R10" s="990"/>
+      <c r="R10" s="975"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I11" s="740" t="str">
@@ -11183,7 +11184,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="976" t="s">
+      <c r="A13" s="990" t="s">
         <v>357</v>
       </c>
       <c r="B13" s="511" t="str">
@@ -11229,7 +11230,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="977"/>
+      <c r="A14" s="991"/>
       <c r="B14" s="514" t="s">
         <v>350</v>
       </c>
@@ -11359,34 +11360,34 @@
       <c r="A21" s="502" t="s">
         <v>362</v>
       </c>
-      <c r="B21" s="991" t="s">
+      <c r="B21" s="980" t="s">
         <v>508</v>
       </c>
-      <c r="C21" s="992"/>
-      <c r="D21" s="992"/>
-      <c r="E21" s="992"/>
-      <c r="F21" s="992"/>
-      <c r="G21" s="992"/>
+      <c r="C21" s="981"/>
+      <c r="D21" s="981"/>
+      <c r="E21" s="981"/>
+      <c r="F21" s="981"/>
+      <c r="G21" s="981"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="516" t="s">
         <v>326</v>
       </c>
-      <c r="B22" s="980" t="str">
+      <c r="B22" s="982" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="981"/>
-      <c r="D22" s="980" t="str">
+      <c r="C22" s="983"/>
+      <c r="D22" s="982" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="981"/>
-      <c r="F22" s="980" t="str">
+      <c r="E22" s="983"/>
+      <c r="F22" s="982" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="981"/>
+      <c r="G22" s="983"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="517"/>
@@ -11813,21 +11814,21 @@
       <c r="A41" s="519" t="s">
         <v>372</v>
       </c>
-      <c r="B41" s="970" t="str">
+      <c r="B41" s="988" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="971"/>
-      <c r="D41" s="972" t="str">
+      <c r="C41" s="989"/>
+      <c r="D41" s="976" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="973"/>
-      <c r="F41" s="972" t="str">
+      <c r="E41" s="977"/>
+      <c r="F41" s="976" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G41" s="973"/>
+      <c r="G41" s="977"/>
       <c r="N41" s="707"/>
       <c r="O41" s="734" t="s">
         <v>458</v>
@@ -12041,11 +12042,11 @@
       <c r="F53" s="712" t="s">
         <v>514</v>
       </c>
-      <c r="H53" s="993" t="s">
+      <c r="H53" s="968" t="s">
         <v>501</v>
       </c>
-      <c r="I53" s="993"/>
-      <c r="J53" s="993"/>
+      <c r="I53" s="968"/>
+      <c r="J53" s="968"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="703" t="s">
@@ -12215,11 +12216,11 @@
       <c r="F63" s="712" t="s">
         <v>514</v>
       </c>
-      <c r="H63" s="993" t="s">
+      <c r="H63" s="968" t="s">
         <v>515</v>
       </c>
-      <c r="I63" s="993"/>
-      <c r="J63" s="993"/>
+      <c r="I63" s="968"/>
+      <c r="J63" s="968"/>
       <c r="L63" s="710"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -12406,12 +12407,12 @@
       <c r="A74" s="623" t="s">
         <v>371</v>
       </c>
-      <c r="B74" s="969" t="s">
+      <c r="B74" s="987" t="s">
         <v>455</v>
       </c>
-      <c r="C74" s="969"/>
-      <c r="D74" s="969"/>
-      <c r="E74" s="969"/>
+      <c r="C74" s="987"/>
+      <c r="D74" s="987"/>
+      <c r="E74" s="987"/>
       <c r="I74" s="711"/>
       <c r="J74" s="711"/>
       <c r="K74" s="711"/>
@@ -12727,21 +12728,21 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="984" t="str">
+      <c r="B85" s="973" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="985"/>
-      <c r="D85" s="984" t="str">
+      <c r="C85" s="974"/>
+      <c r="D85" s="973" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="985"/>
-      <c r="F85" s="984" t="str">
+      <c r="E85" s="974"/>
+      <c r="F85" s="973" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="985"/>
+      <c r="G85" s="974"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="503"/>
@@ -13037,21 +13038,21 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="984" t="str">
+      <c r="B101" s="973" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="985"/>
-      <c r="D101" s="984" t="str">
+      <c r="C101" s="974"/>
+      <c r="D101" s="973" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="985"/>
-      <c r="F101" s="984" t="str">
+      <c r="E101" s="974"/>
+      <c r="F101" s="973" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="985"/>
+      <c r="G101" s="974"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="503"/>
@@ -13347,36 +13348,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="986" t="str">
+      <c r="B116" s="969" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="987"/>
-      <c r="D116" s="986" t="str">
+      <c r="C116" s="970"/>
+      <c r="D116" s="969" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="987"/>
-      <c r="F116" s="986" t="str">
+      <c r="E116" s="970"/>
+      <c r="F116" s="969" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="987"/>
+      <c r="G116" s="970"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="542"/>
-      <c r="B117" s="988" t="s">
+      <c r="B117" s="971" t="s">
         <v>279</v>
       </c>
-      <c r="C117" s="989"/>
-      <c r="D117" s="988" t="s">
+      <c r="C117" s="972"/>
+      <c r="D117" s="971" t="s">
         <v>279</v>
       </c>
-      <c r="E117" s="989"/>
-      <c r="F117" s="988" t="s">
+      <c r="E117" s="972"/>
+      <c r="F117" s="971" t="s">
         <v>279</v>
       </c>
-      <c r="G117" s="989"/>
+      <c r="G117" s="972"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="543" t="s">
@@ -13679,12 +13680,12 @@
       <c r="A129" s="546" t="s">
         <v>357</v>
       </c>
-      <c r="B129" s="982" t="str">
+      <c r="B129" s="984" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="983"/>
-      <c r="D129" s="983"/>
+      <c r="C129" s="985"/>
+      <c r="D129" s="985"/>
       <c r="N129" s="715" t="s">
         <v>398</v>
       </c>
@@ -13906,7 +13907,7 @@
     </row>
     <row r="150" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="556" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B150" s="556" t="s">
         <v>73</v>
@@ -13925,7 +13926,7 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" s="556" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B151" s="556" t="s">
         <v>73</v>
@@ -14460,22 +14461,16 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="39">
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -14489,16 +14484,22 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17948,7 +17949,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="797" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D5" s="828" t="s">
         <v>27</v>
@@ -58624,7 +58625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CQ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="AW5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -58652,123 +58653,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="658" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="836" t="s">
+      <c r="A1" s="865" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="837"/>
-      <c r="C1" s="837"/>
-      <c r="D1" s="837"/>
-      <c r="E1" s="837"/>
-      <c r="F1" s="837"/>
-      <c r="G1" s="837"/>
-      <c r="H1" s="838" t="s">
+      <c r="B1" s="866"/>
+      <c r="C1" s="866"/>
+      <c r="D1" s="866"/>
+      <c r="E1" s="866"/>
+      <c r="F1" s="866"/>
+      <c r="G1" s="866"/>
+      <c r="H1" s="867" t="s">
         <v>464</v>
       </c>
-      <c r="I1" s="839"/>
-      <c r="J1" s="839"/>
-      <c r="K1" s="839"/>
-      <c r="L1" s="839"/>
-      <c r="M1" s="840"/>
-      <c r="N1" s="841" t="s">
+      <c r="I1" s="868"/>
+      <c r="J1" s="868"/>
+      <c r="K1" s="868"/>
+      <c r="L1" s="868"/>
+      <c r="M1" s="869"/>
+      <c r="N1" s="870" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="842"/>
-      <c r="P1" s="842"/>
-      <c r="Q1" s="842"/>
-      <c r="R1" s="842"/>
-      <c r="S1" s="842"/>
-      <c r="T1" s="842"/>
-      <c r="U1" s="842"/>
-      <c r="V1" s="843" t="s">
+      <c r="O1" s="848"/>
+      <c r="P1" s="848"/>
+      <c r="Q1" s="848"/>
+      <c r="R1" s="848"/>
+      <c r="S1" s="848"/>
+      <c r="T1" s="848"/>
+      <c r="U1" s="848"/>
+      <c r="V1" s="871" t="s">
         <v>83</v>
       </c>
-      <c r="W1" s="844"/>
-      <c r="X1" s="845"/>
-      <c r="Y1" s="845"/>
-      <c r="Z1" s="846"/>
-      <c r="AA1" s="847" t="s">
+      <c r="W1" s="872"/>
+      <c r="X1" s="873"/>
+      <c r="Y1" s="873"/>
+      <c r="Z1" s="874"/>
+      <c r="AA1" s="875" t="s">
         <v>84</v>
       </c>
-      <c r="AB1" s="848"/>
-      <c r="AC1" s="848"/>
-      <c r="AD1" s="848"/>
-      <c r="AE1" s="848"/>
-      <c r="AF1" s="848"/>
-      <c r="AG1" s="848"/>
-      <c r="AH1" s="848"/>
-      <c r="AI1" s="848"/>
-      <c r="AJ1" s="848"/>
-      <c r="AK1" s="848"/>
-      <c r="AL1" s="848"/>
-      <c r="AM1" s="848"/>
+      <c r="AB1" s="876"/>
+      <c r="AC1" s="876"/>
+      <c r="AD1" s="876"/>
+      <c r="AE1" s="876"/>
+      <c r="AF1" s="876"/>
+      <c r="AG1" s="876"/>
+      <c r="AH1" s="876"/>
+      <c r="AI1" s="876"/>
+      <c r="AJ1" s="876"/>
+      <c r="AK1" s="876"/>
+      <c r="AL1" s="876"/>
+      <c r="AM1" s="876"/>
       <c r="AN1" s="52"/>
       <c r="AO1" s="53"/>
-      <c r="AP1" s="860" t="s">
+      <c r="AP1" s="847" t="s">
         <v>85</v>
       </c>
-      <c r="AQ1" s="842"/>
-      <c r="AR1" s="842"/>
-      <c r="AS1" s="842"/>
-      <c r="AT1" s="842"/>
-      <c r="AU1" s="842"/>
-      <c r="AV1" s="842"/>
-      <c r="AW1" s="861"/>
-      <c r="AX1" s="868" t="s">
-        <v>598</v>
-      </c>
-      <c r="AY1" s="869"/>
-      <c r="AZ1" s="869"/>
-      <c r="BA1" s="869"/>
-      <c r="BB1" s="869"/>
-      <c r="BC1" s="870"/>
-      <c r="BD1" s="871" t="s">
+      <c r="AQ1" s="848"/>
+      <c r="AR1" s="848"/>
+      <c r="AS1" s="848"/>
+      <c r="AT1" s="848"/>
+      <c r="AU1" s="848"/>
+      <c r="AV1" s="848"/>
+      <c r="AW1" s="849"/>
+      <c r="AX1" s="856" t="s">
+        <v>597</v>
+      </c>
+      <c r="AY1" s="857"/>
+      <c r="AZ1" s="857"/>
+      <c r="BA1" s="857"/>
+      <c r="BB1" s="857"/>
+      <c r="BC1" s="858"/>
+      <c r="BD1" s="859" t="s">
         <v>86</v>
       </c>
-      <c r="BE1" s="872"/>
-      <c r="BF1" s="872"/>
-      <c r="BG1" s="872"/>
-      <c r="BH1" s="872"/>
-      <c r="BI1" s="873"/>
-      <c r="BJ1" s="874" t="s">
+      <c r="BE1" s="860"/>
+      <c r="BF1" s="860"/>
+      <c r="BG1" s="860"/>
+      <c r="BH1" s="860"/>
+      <c r="BI1" s="861"/>
+      <c r="BJ1" s="862" t="s">
         <v>87</v>
       </c>
-      <c r="BK1" s="875"/>
-      <c r="BL1" s="875"/>
-      <c r="BM1" s="875"/>
-      <c r="BN1" s="875"/>
-      <c r="BO1" s="875"/>
-      <c r="BP1" s="876"/>
-      <c r="BQ1" s="849" t="s">
+      <c r="BK1" s="863"/>
+      <c r="BL1" s="863"/>
+      <c r="BM1" s="863"/>
+      <c r="BN1" s="863"/>
+      <c r="BO1" s="863"/>
+      <c r="BP1" s="864"/>
+      <c r="BQ1" s="836" t="s">
         <v>88</v>
       </c>
-      <c r="BR1" s="850"/>
-      <c r="BS1" s="850"/>
-      <c r="BT1" s="850"/>
-      <c r="BU1" s="850"/>
-      <c r="BV1" s="850"/>
+      <c r="BR1" s="837"/>
+      <c r="BS1" s="837"/>
+      <c r="BT1" s="837"/>
+      <c r="BU1" s="837"/>
+      <c r="BV1" s="837"/>
       <c r="BW1" s="53"/>
       <c r="BX1" s="54"/>
-      <c r="BY1" s="851" t="s">
+      <c r="BY1" s="838" t="s">
         <v>89</v>
       </c>
-      <c r="BZ1" s="852"/>
-      <c r="CA1" s="852"/>
-      <c r="CB1" s="852"/>
-      <c r="CC1" s="852"/>
-      <c r="CD1" s="852"/>
-      <c r="CE1" s="852"/>
-      <c r="CF1" s="853"/>
-      <c r="CG1" s="853"/>
-      <c r="CH1" s="853"/>
-      <c r="CI1" s="853"/>
-      <c r="CJ1" s="853"/>
-      <c r="CK1" s="853"/>
-      <c r="CL1" s="853"/>
-      <c r="CM1" s="853"/>
-      <c r="CN1" s="853"/>
-      <c r="CO1" s="853"/>
-      <c r="CP1" s="853"/>
-      <c r="CQ1" s="853"/>
+      <c r="BZ1" s="839"/>
+      <c r="CA1" s="839"/>
+      <c r="CB1" s="839"/>
+      <c r="CC1" s="839"/>
+      <c r="CD1" s="839"/>
+      <c r="CE1" s="839"/>
+      <c r="CF1" s="840"/>
+      <c r="CG1" s="840"/>
+      <c r="CH1" s="840"/>
+      <c r="CI1" s="840"/>
+      <c r="CJ1" s="840"/>
+      <c r="CK1" s="840"/>
+      <c r="CL1" s="840"/>
+      <c r="CM1" s="840"/>
+      <c r="CN1" s="840"/>
+      <c r="CO1" s="840"/>
+      <c r="CP1" s="840"/>
+      <c r="CQ1" s="840"/>
     </row>
     <row r="2" spans="1:95" s="658" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -58792,18 +58793,18 @@
       <c r="G2" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="854" t="s">
+      <c r="H2" s="841" t="s">
         <v>465</v>
       </c>
-      <c r="I2" s="855"/>
-      <c r="J2" s="855" t="s">
+      <c r="I2" s="842"/>
+      <c r="J2" s="842" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="855"/>
-      <c r="L2" s="855" t="s">
+      <c r="K2" s="842"/>
+      <c r="L2" s="842" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="856"/>
+      <c r="M2" s="843"/>
       <c r="N2" s="57" t="s">
         <v>90</v>
       </c>
@@ -58912,36 +58913,36 @@
       <c r="AW2" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="AX2" s="857" t="s">
+      <c r="AX2" s="844" t="s">
         <v>125</v>
       </c>
-      <c r="AY2" s="858"/>
-      <c r="AZ2" s="858"/>
-      <c r="BA2" s="858" t="s">
+      <c r="AY2" s="845"/>
+      <c r="AZ2" s="845"/>
+      <c r="BA2" s="845" t="s">
         <v>126</v>
       </c>
-      <c r="BB2" s="858"/>
-      <c r="BC2" s="859"/>
-      <c r="BD2" s="862" t="s">
+      <c r="BB2" s="845"/>
+      <c r="BC2" s="846"/>
+      <c r="BD2" s="850" t="s">
         <v>125</v>
       </c>
-      <c r="BE2" s="863"/>
-      <c r="BF2" s="863"/>
-      <c r="BG2" s="863" t="s">
+      <c r="BE2" s="851"/>
+      <c r="BF2" s="851"/>
+      <c r="BG2" s="851" t="s">
         <v>126</v>
       </c>
-      <c r="BH2" s="863"/>
-      <c r="BI2" s="864"/>
-      <c r="BJ2" s="865" t="s">
+      <c r="BH2" s="851"/>
+      <c r="BI2" s="852"/>
+      <c r="BJ2" s="853" t="s">
         <v>125</v>
       </c>
-      <c r="BK2" s="866"/>
-      <c r="BL2" s="866"/>
-      <c r="BM2" s="866" t="s">
+      <c r="BK2" s="854"/>
+      <c r="BL2" s="854"/>
+      <c r="BM2" s="854" t="s">
         <v>126</v>
       </c>
-      <c r="BN2" s="867"/>
-      <c r="BO2" s="867"/>
+      <c r="BN2" s="855"/>
+      <c r="BO2" s="855"/>
       <c r="BP2" s="69" t="s">
         <v>127</v>
       </c>
@@ -59574,6 +59575,11 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -59589,11 +59595,6 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -59676,100 +59677,100 @@
         <v>167</v>
       </c>
       <c r="L1" s="145"/>
-      <c r="M1" s="877" t="s">
+      <c r="M1" s="900" t="s">
         <v>168</v>
       </c>
-      <c r="N1" s="878" t="s">
+      <c r="N1" s="901" t="s">
         <v>523</v>
       </c>
-      <c r="O1" s="879"/>
-      <c r="P1" s="879"/>
-      <c r="Q1" s="879"/>
-      <c r="R1" s="880" t="s">
+      <c r="O1" s="902"/>
+      <c r="P1" s="902"/>
+      <c r="Q1" s="902"/>
+      <c r="R1" s="903" t="s">
         <v>464</v>
       </c>
-      <c r="S1" s="881"/>
-      <c r="T1" s="881"/>
-      <c r="U1" s="881"/>
-      <c r="V1" s="881"/>
-      <c r="W1" s="881"/>
-      <c r="X1" s="882"/>
-      <c r="Y1" s="883" t="s">
+      <c r="S1" s="896"/>
+      <c r="T1" s="896"/>
+      <c r="U1" s="896"/>
+      <c r="V1" s="896"/>
+      <c r="W1" s="896"/>
+      <c r="X1" s="904"/>
+      <c r="Y1" s="890" t="s">
         <v>472</v>
       </c>
-      <c r="Z1" s="872"/>
-      <c r="AA1" s="886" t="s">
+      <c r="Z1" s="860"/>
+      <c r="AA1" s="905" t="s">
         <v>169</v>
       </c>
-      <c r="AB1" s="897" t="s">
+      <c r="AB1" s="878" t="s">
         <v>170</v>
       </c>
-      <c r="AC1" s="893" t="s">
+      <c r="AC1" s="892" t="s">
         <v>171</v>
       </c>
-      <c r="AD1" s="894"/>
-      <c r="AE1" s="894"/>
-      <c r="AF1" s="895"/>
-      <c r="AG1" s="896" t="s">
+      <c r="AD1" s="893"/>
+      <c r="AE1" s="893"/>
+      <c r="AF1" s="894"/>
+      <c r="AG1" s="895" t="s">
         <v>172</v>
       </c>
-      <c r="AH1" s="881"/>
-      <c r="AI1" s="881"/>
-      <c r="AJ1" s="881"/>
-      <c r="AK1" s="881"/>
-      <c r="AL1" s="881"/>
-      <c r="AM1" s="881"/>
-      <c r="AN1" s="881"/>
-      <c r="AO1" s="897" t="s">
+      <c r="AH1" s="896"/>
+      <c r="AI1" s="896"/>
+      <c r="AJ1" s="896"/>
+      <c r="AK1" s="896"/>
+      <c r="AL1" s="896"/>
+      <c r="AM1" s="896"/>
+      <c r="AN1" s="896"/>
+      <c r="AO1" s="878" t="s">
         <v>173</v>
       </c>
-      <c r="AP1" s="883" t="s">
+      <c r="AP1" s="890" t="s">
         <v>471</v>
       </c>
-      <c r="AQ1" s="872"/>
-      <c r="AR1" s="872"/>
-      <c r="AS1" s="873"/>
-      <c r="AT1" s="900" t="s">
+      <c r="AQ1" s="860"/>
+      <c r="AR1" s="860"/>
+      <c r="AS1" s="861"/>
+      <c r="AT1" s="898" t="s">
         <v>174</v>
       </c>
-      <c r="AU1" s="901"/>
-      <c r="AV1" s="901"/>
-      <c r="AW1" s="901"/>
-      <c r="AX1" s="901"/>
-      <c r="AY1" s="901"/>
-      <c r="AZ1" s="901"/>
-      <c r="BA1" s="901"/>
-      <c r="BB1" s="901"/>
-      <c r="BC1" s="901"/>
-      <c r="BD1" s="901"/>
-      <c r="BE1" s="901"/>
-      <c r="BF1" s="901"/>
-      <c r="BG1" s="901"/>
-      <c r="BH1" s="901"/>
-      <c r="BI1" s="901"/>
-      <c r="BJ1" s="901"/>
-      <c r="BK1" s="901"/>
-      <c r="BL1" s="901"/>
-      <c r="BM1" s="901"/>
-      <c r="BN1" s="901"/>
-      <c r="BO1" s="901"/>
-      <c r="BP1" s="901"/>
-      <c r="BQ1" s="901"/>
-      <c r="BR1" s="901"/>
-      <c r="BS1" s="901"/>
-      <c r="BT1" s="901"/>
-      <c r="BU1" s="901"/>
-      <c r="BV1" s="901"/>
-      <c r="BW1" s="897" t="s">
+      <c r="AU1" s="899"/>
+      <c r="AV1" s="899"/>
+      <c r="AW1" s="899"/>
+      <c r="AX1" s="899"/>
+      <c r="AY1" s="899"/>
+      <c r="AZ1" s="899"/>
+      <c r="BA1" s="899"/>
+      <c r="BB1" s="899"/>
+      <c r="BC1" s="899"/>
+      <c r="BD1" s="899"/>
+      <c r="BE1" s="899"/>
+      <c r="BF1" s="899"/>
+      <c r="BG1" s="899"/>
+      <c r="BH1" s="899"/>
+      <c r="BI1" s="899"/>
+      <c r="BJ1" s="899"/>
+      <c r="BK1" s="899"/>
+      <c r="BL1" s="899"/>
+      <c r="BM1" s="899"/>
+      <c r="BN1" s="899"/>
+      <c r="BO1" s="899"/>
+      <c r="BP1" s="899"/>
+      <c r="BQ1" s="899"/>
+      <c r="BR1" s="899"/>
+      <c r="BS1" s="899"/>
+      <c r="BT1" s="899"/>
+      <c r="BU1" s="899"/>
+      <c r="BV1" s="899"/>
+      <c r="BW1" s="878" t="s">
         <v>175</v>
       </c>
-      <c r="BX1" s="883" t="s">
+      <c r="BX1" s="890" t="s">
         <v>470</v>
       </c>
-      <c r="BY1" s="872"/>
-      <c r="BZ1" s="872"/>
-      <c r="CA1" s="873"/>
-      <c r="CB1" s="909" t="s">
+      <c r="BY1" s="860"/>
+      <c r="BZ1" s="860"/>
+      <c r="CA1" s="861"/>
+      <c r="CB1" s="889" t="s">
         <v>488</v>
       </c>
       <c r="CC1" s="891" t="s">
@@ -59787,16 +59788,16 @@
       <c r="CM1" s="891"/>
       <c r="CN1" s="891"/>
       <c r="CO1" s="146"/>
-      <c r="CP1" s="905" t="s">
+      <c r="CP1" s="877" t="s">
         <v>88</v>
       </c>
-      <c r="CQ1" s="842"/>
-      <c r="CR1" s="842"/>
-      <c r="CS1" s="842"/>
-      <c r="CT1" s="842"/>
-      <c r="CU1" s="842"/>
-      <c r="CV1" s="842"/>
-      <c r="CW1" s="861"/>
+      <c r="CQ1" s="848"/>
+      <c r="CR1" s="848"/>
+      <c r="CS1" s="848"/>
+      <c r="CT1" s="848"/>
+      <c r="CU1" s="848"/>
+      <c r="CV1" s="848"/>
+      <c r="CW1" s="849"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="147" t="s">
@@ -59835,7 +59836,7 @@
       <c r="L2" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="M2" s="877"/>
+      <c r="M2" s="900"/>
       <c r="N2" s="152" t="s">
         <v>180</v>
       </c>
@@ -59851,22 +59852,22 @@
       <c r="R2" s="157" t="s">
         <v>183</v>
       </c>
-      <c r="S2" s="888" t="s">
+      <c r="S2" s="907" t="s">
         <v>465</v>
       </c>
-      <c r="T2" s="867"/>
-      <c r="U2" s="889" t="s">
+      <c r="T2" s="855"/>
+      <c r="U2" s="908" t="s">
         <v>97</v>
       </c>
-      <c r="V2" s="889"/>
-      <c r="W2" s="889" t="s">
+      <c r="V2" s="908"/>
+      <c r="W2" s="908" t="s">
         <v>98</v>
       </c>
-      <c r="X2" s="890"/>
+      <c r="X2" s="909"/>
       <c r="Y2" s="884"/>
       <c r="Z2" s="885"/>
-      <c r="AA2" s="887"/>
-      <c r="AB2" s="898"/>
+      <c r="AA2" s="906"/>
+      <c r="AB2" s="879"/>
       <c r="AC2" s="153" t="s">
         <v>184</v>
       </c>
@@ -59879,81 +59880,81 @@
       <c r="AF2" s="153" t="s">
         <v>187</v>
       </c>
-      <c r="AG2" s="899" t="s">
+      <c r="AG2" s="897" t="s">
         <v>188</v>
       </c>
-      <c r="AH2" s="892"/>
-      <c r="AI2" s="892" t="s">
+      <c r="AH2" s="882"/>
+      <c r="AI2" s="882" t="s">
         <v>189</v>
       </c>
-      <c r="AJ2" s="892"/>
-      <c r="AK2" s="892" t="s">
+      <c r="AJ2" s="882"/>
+      <c r="AK2" s="882" t="s">
         <v>190</v>
       </c>
-      <c r="AL2" s="892"/>
+      <c r="AL2" s="882"/>
       <c r="AM2" s="154" t="s">
         <v>191</v>
       </c>
       <c r="AN2" s="154" t="s">
         <v>192</v>
       </c>
-      <c r="AO2" s="898"/>
+      <c r="AO2" s="879"/>
       <c r="AP2" s="884" t="s">
         <v>193</v>
       </c>
       <c r="AQ2" s="885"/>
-      <c r="AR2" s="902" t="s">
+      <c r="AR2" s="886" t="s">
         <v>194</v>
       </c>
-      <c r="AS2" s="903"/>
-      <c r="AT2" s="892" t="s">
+      <c r="AS2" s="887"/>
+      <c r="AT2" s="882" t="s">
         <v>195</v>
       </c>
-      <c r="AU2" s="892"/>
-      <c r="AV2" s="904" t="s">
+      <c r="AU2" s="882"/>
+      <c r="AV2" s="883" t="s">
         <v>196</v>
       </c>
-      <c r="AW2" s="904"/>
-      <c r="AX2" s="904" t="s">
+      <c r="AW2" s="883"/>
+      <c r="AX2" s="883" t="s">
         <v>197</v>
       </c>
-      <c r="AY2" s="904"/>
+      <c r="AY2" s="883"/>
       <c r="AZ2" s="154" t="s">
         <v>198</v>
       </c>
       <c r="BA2" s="154" t="s">
         <v>199</v>
       </c>
-      <c r="BB2" s="892" t="s">
+      <c r="BB2" s="882" t="s">
         <v>200</v>
       </c>
-      <c r="BC2" s="892"/>
-      <c r="BD2" s="904" t="s">
+      <c r="BC2" s="882"/>
+      <c r="BD2" s="883" t="s">
         <v>201</v>
       </c>
-      <c r="BE2" s="904"/>
-      <c r="BF2" s="904" t="s">
+      <c r="BE2" s="883"/>
+      <c r="BF2" s="883" t="s">
         <v>202</v>
       </c>
-      <c r="BG2" s="904"/>
+      <c r="BG2" s="883"/>
       <c r="BH2" s="154" t="s">
         <v>203</v>
       </c>
       <c r="BI2" s="154" t="s">
         <v>204</v>
       </c>
-      <c r="BJ2" s="892" t="s">
+      <c r="BJ2" s="882" t="s">
         <v>205</v>
       </c>
-      <c r="BK2" s="892"/>
-      <c r="BL2" s="904" t="s">
+      <c r="BK2" s="882"/>
+      <c r="BL2" s="883" t="s">
         <v>206</v>
       </c>
-      <c r="BM2" s="904"/>
-      <c r="BN2" s="904" t="s">
+      <c r="BM2" s="883"/>
+      <c r="BN2" s="883" t="s">
         <v>207</v>
       </c>
-      <c r="BO2" s="904"/>
+      <c r="BO2" s="883"/>
       <c r="BP2" s="154" t="s">
         <v>208</v>
       </c>
@@ -59975,16 +59976,16 @@
       <c r="BV2" s="154" t="s">
         <v>214</v>
       </c>
-      <c r="BW2" s="898"/>
+      <c r="BW2" s="879"/>
       <c r="BX2" s="884" t="s">
         <v>193</v>
       </c>
       <c r="BY2" s="885"/>
-      <c r="BZ2" s="902" t="s">
+      <c r="BZ2" s="886" t="s">
         <v>194</v>
       </c>
-      <c r="CA2" s="903"/>
-      <c r="CB2" s="909"/>
+      <c r="CA2" s="887"/>
+      <c r="CB2" s="889"/>
       <c r="CC2" s="138" t="s">
         <v>106</v>
       </c>
@@ -60024,22 +60025,22 @@
       <c r="CO2" s="140" t="s">
         <v>473</v>
       </c>
-      <c r="CP2" s="908" t="s">
+      <c r="CP2" s="888" t="s">
         <v>216</v>
       </c>
-      <c r="CQ2" s="906"/>
-      <c r="CR2" s="906" t="s">
+      <c r="CQ2" s="880"/>
+      <c r="CR2" s="880" t="s">
         <v>217</v>
       </c>
-      <c r="CS2" s="906"/>
-      <c r="CT2" s="906" t="s">
+      <c r="CS2" s="880"/>
+      <c r="CT2" s="880" t="s">
         <v>218</v>
       </c>
-      <c r="CU2" s="906"/>
-      <c r="CV2" s="906" t="s">
+      <c r="CU2" s="880"/>
+      <c r="CV2" s="880" t="s">
         <v>219</v>
       </c>
-      <c r="CW2" s="907"/>
+      <c r="CW2" s="881"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="168"/>
@@ -60904,6 +60905,29 @@
     </sortState>
   </autoFilter>
   <mergeCells count="39">
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="CC1:CN1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AN1"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
     <mergeCell ref="CP1:CW1"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="CV2:CW2"/>
@@ -60920,29 +60944,6 @@
     <mergeCell ref="CT2:CU2"/>
     <mergeCell ref="CB1:CB2"/>
     <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CC1:CN1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AN1"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -60985,72 +60986,72 @@
       <c r="K1" s="144"/>
       <c r="L1" s="145"/>
       <c r="M1" s="696"/>
-      <c r="N1" s="913"/>
-      <c r="O1" s="914"/>
-      <c r="P1" s="914"/>
-      <c r="Q1" s="914"/>
-      <c r="R1" s="880"/>
-      <c r="S1" s="881"/>
-      <c r="T1" s="881"/>
-      <c r="U1" s="881"/>
-      <c r="V1" s="881"/>
-      <c r="W1" s="881"/>
-      <c r="X1" s="882"/>
-      <c r="Y1" s="883"/>
-      <c r="Z1" s="872"/>
+      <c r="N1" s="910"/>
+      <c r="O1" s="911"/>
+      <c r="P1" s="911"/>
+      <c r="Q1" s="911"/>
+      <c r="R1" s="903"/>
+      <c r="S1" s="896"/>
+      <c r="T1" s="896"/>
+      <c r="U1" s="896"/>
+      <c r="V1" s="896"/>
+      <c r="W1" s="896"/>
+      <c r="X1" s="904"/>
+      <c r="Y1" s="890"/>
+      <c r="Z1" s="860"/>
       <c r="AA1" s="697"/>
       <c r="AB1" s="695"/>
-      <c r="AC1" s="893"/>
-      <c r="AD1" s="894"/>
-      <c r="AE1" s="894"/>
-      <c r="AF1" s="895"/>
-      <c r="AG1" s="896"/>
-      <c r="AH1" s="881"/>
-      <c r="AI1" s="881"/>
-      <c r="AJ1" s="881"/>
-      <c r="AK1" s="881"/>
-      <c r="AL1" s="881"/>
-      <c r="AM1" s="881"/>
-      <c r="AN1" s="881"/>
+      <c r="AC1" s="892"/>
+      <c r="AD1" s="893"/>
+      <c r="AE1" s="893"/>
+      <c r="AF1" s="894"/>
+      <c r="AG1" s="895"/>
+      <c r="AH1" s="896"/>
+      <c r="AI1" s="896"/>
+      <c r="AJ1" s="896"/>
+      <c r="AK1" s="896"/>
+      <c r="AL1" s="896"/>
+      <c r="AM1" s="896"/>
+      <c r="AN1" s="896"/>
       <c r="AO1" s="695"/>
-      <c r="AP1" s="883"/>
-      <c r="AQ1" s="872"/>
-      <c r="AR1" s="872"/>
-      <c r="AS1" s="873"/>
-      <c r="AT1" s="900"/>
-      <c r="AU1" s="901"/>
-      <c r="AV1" s="901"/>
-      <c r="AW1" s="901"/>
-      <c r="AX1" s="901"/>
-      <c r="AY1" s="901"/>
-      <c r="AZ1" s="901"/>
-      <c r="BA1" s="901"/>
-      <c r="BB1" s="901"/>
-      <c r="BC1" s="901"/>
-      <c r="BD1" s="901"/>
-      <c r="BE1" s="901"/>
-      <c r="BF1" s="901"/>
-      <c r="BG1" s="901"/>
-      <c r="BH1" s="901"/>
-      <c r="BI1" s="901"/>
-      <c r="BJ1" s="901"/>
-      <c r="BK1" s="901"/>
-      <c r="BL1" s="901"/>
-      <c r="BM1" s="901"/>
-      <c r="BN1" s="901"/>
-      <c r="BO1" s="901"/>
-      <c r="BP1" s="901"/>
-      <c r="BQ1" s="901"/>
-      <c r="BR1" s="901"/>
-      <c r="BS1" s="901"/>
-      <c r="BT1" s="901"/>
-      <c r="BU1" s="901"/>
-      <c r="BV1" s="901"/>
+      <c r="AP1" s="890"/>
+      <c r="AQ1" s="860"/>
+      <c r="AR1" s="860"/>
+      <c r="AS1" s="861"/>
+      <c r="AT1" s="898"/>
+      <c r="AU1" s="899"/>
+      <c r="AV1" s="899"/>
+      <c r="AW1" s="899"/>
+      <c r="AX1" s="899"/>
+      <c r="AY1" s="899"/>
+      <c r="AZ1" s="899"/>
+      <c r="BA1" s="899"/>
+      <c r="BB1" s="899"/>
+      <c r="BC1" s="899"/>
+      <c r="BD1" s="899"/>
+      <c r="BE1" s="899"/>
+      <c r="BF1" s="899"/>
+      <c r="BG1" s="899"/>
+      <c r="BH1" s="899"/>
+      <c r="BI1" s="899"/>
+      <c r="BJ1" s="899"/>
+      <c r="BK1" s="899"/>
+      <c r="BL1" s="899"/>
+      <c r="BM1" s="899"/>
+      <c r="BN1" s="899"/>
+      <c r="BO1" s="899"/>
+      <c r="BP1" s="899"/>
+      <c r="BQ1" s="899"/>
+      <c r="BR1" s="899"/>
+      <c r="BS1" s="899"/>
+      <c r="BT1" s="899"/>
+      <c r="BU1" s="899"/>
+      <c r="BV1" s="899"/>
       <c r="BW1" s="695"/>
-      <c r="BX1" s="883"/>
-      <c r="BY1" s="872"/>
-      <c r="BZ1" s="872"/>
-      <c r="CA1" s="873"/>
+      <c r="BX1" s="890"/>
+      <c r="BY1" s="860"/>
+      <c r="BZ1" s="860"/>
+      <c r="CA1" s="861"/>
       <c r="CB1" s="891"/>
       <c r="CC1" s="891"/>
       <c r="CD1" s="891"/>
@@ -61064,31 +61065,26 @@
       <c r="CL1" s="891"/>
       <c r="CM1" s="891"/>
       <c r="CN1" s="694"/>
-      <c r="CO1" s="905"/>
-      <c r="CP1" s="842"/>
-      <c r="CQ1" s="842"/>
-      <c r="CR1" s="842"/>
-      <c r="CS1" s="842"/>
-      <c r="CT1" s="842"/>
-      <c r="CU1" s="842"/>
-      <c r="CV1" s="861"/>
-      <c r="CW1" s="910"/>
-      <c r="CX1" s="911"/>
-      <c r="CY1" s="911"/>
-      <c r="CZ1" s="912"/>
-      <c r="DA1" s="911"/>
-      <c r="DB1" s="911"/>
-      <c r="DC1" s="912"/>
-      <c r="DD1" s="911"/>
-      <c r="DE1" s="911"/>
+      <c r="CO1" s="877"/>
+      <c r="CP1" s="848"/>
+      <c r="CQ1" s="848"/>
+      <c r="CR1" s="848"/>
+      <c r="CS1" s="848"/>
+      <c r="CT1" s="848"/>
+      <c r="CU1" s="848"/>
+      <c r="CV1" s="849"/>
+      <c r="CW1" s="912"/>
+      <c r="CX1" s="913"/>
+      <c r="CY1" s="913"/>
+      <c r="CZ1" s="914"/>
+      <c r="DA1" s="913"/>
+      <c r="DB1" s="913"/>
+      <c r="DC1" s="914"/>
+      <c r="DD1" s="913"/>
+      <c r="DE1" s="913"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="CZ1:DB1"/>
     <mergeCell ref="DC1:DE1"/>
@@ -61097,6 +61093,11 @@
     <mergeCell ref="AG1:AN1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CB1:CM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -61177,11 +61178,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U47"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -61192,9 +61191,11 @@
     <col min="13" max="13" width="15.77734375" customWidth="1"/>
     <col min="17" max="17" width="34.21875" customWidth="1"/>
     <col min="20" max="20" width="16.77734375" customWidth="1"/>
+    <col min="24" max="24" width="34.21875" customWidth="1"/>
+    <col min="27" max="27" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="200"/>
       <c r="B1" s="201" t="s">
         <v>238</v>
@@ -61220,16 +61221,23 @@
       <c r="S1" s="201"/>
       <c r="T1" s="201"/>
       <c r="U1" s="201"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V1" s="372"/>
+      <c r="W1" s="372"/>
+      <c r="X1" s="372"/>
+      <c r="Y1" s="372"/>
+      <c r="Z1" s="372"/>
+      <c r="AA1" s="372"/>
+      <c r="AB1" s="372"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="200"/>
       <c r="B2" s="203" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="919" t="s">
+      <c r="C2" s="926" t="s">
         <v>240</v>
       </c>
-      <c r="D2" s="919"/>
+      <c r="D2" s="926"/>
       <c r="E2" s="201"/>
       <c r="F2" s="201"/>
       <c r="G2" s="201"/>
@@ -61247,8 +61255,15 @@
       <c r="S2" s="201"/>
       <c r="T2" s="201"/>
       <c r="U2" s="201"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V2" s="372"/>
+      <c r="W2" s="372"/>
+      <c r="X2" s="372"/>
+      <c r="Y2" s="372"/>
+      <c r="Z2" s="372"/>
+      <c r="AA2" s="372"/>
+      <c r="AB2" s="372"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="202"/>
       <c r="B3" s="201"/>
       <c r="C3" s="205"/>
@@ -61270,8 +61285,15 @@
       <c r="S3" s="201"/>
       <c r="T3" s="201"/>
       <c r="U3" s="201"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3" s="372"/>
+      <c r="W3" s="372"/>
+      <c r="X3" s="372"/>
+      <c r="Y3" s="372"/>
+      <c r="Z3" s="372"/>
+      <c r="AA3" s="372"/>
+      <c r="AB3" s="372"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="202"/>
       <c r="B4" s="206"/>
       <c r="C4" s="207"/>
@@ -61293,8 +61315,15 @@
       <c r="S4" s="201"/>
       <c r="T4" s="201"/>
       <c r="U4" s="201"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V4" s="372"/>
+      <c r="W4" s="372"/>
+      <c r="X4" s="210"/>
+      <c r="Y4" s="372"/>
+      <c r="Z4" s="372"/>
+      <c r="AA4" s="372"/>
+      <c r="AB4" s="372"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="202"/>
       <c r="B5" s="201"/>
       <c r="C5" s="201"/>
@@ -61316,8 +61345,15 @@
       <c r="S5" s="201"/>
       <c r="T5" s="201"/>
       <c r="U5" s="201"/>
-    </row>
-    <row r="6" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="V5" s="372"/>
+      <c r="W5" s="372"/>
+      <c r="X5" s="372"/>
+      <c r="Y5" s="372"/>
+      <c r="Z5" s="372"/>
+      <c r="AA5" s="372"/>
+      <c r="AB5" s="372"/>
+    </row>
+    <row r="6" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="200"/>
       <c r="B6" s="213" t="s">
         <v>222</v>
@@ -61349,35 +61385,55 @@
       <c r="S6" s="201"/>
       <c r="T6" s="201"/>
       <c r="U6" s="214" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+      <c r="V6" s="372"/>
+      <c r="W6" s="372"/>
+      <c r="X6" s="376" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y6" s="372"/>
+      <c r="Z6" s="372"/>
+      <c r="AA6" s="372"/>
+      <c r="AB6" s="377" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="200"/>
-      <c r="B7" s="920"/>
-      <c r="C7" s="920"/>
-      <c r="D7" s="920"/>
+      <c r="B7" s="927"/>
+      <c r="C7" s="927"/>
+      <c r="D7" s="927"/>
       <c r="E7" s="201"/>
       <c r="F7" s="201"/>
       <c r="G7" s="201"/>
       <c r="H7" s="201"/>
       <c r="I7" s="201"/>
-      <c r="J7" s="920"/>
-      <c r="K7" s="920"/>
-      <c r="L7" s="920"/>
+      <c r="J7" s="927"/>
+      <c r="K7" s="927"/>
+      <c r="L7" s="927"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="201"/>
       <c r="P7" s="202" t="s">
         <v>243</v>
       </c>
-      <c r="Q7" s="920"/>
-      <c r="R7" s="920"/>
-      <c r="S7" s="920"/>
+      <c r="Q7" s="927"/>
+      <c r="R7" s="927"/>
+      <c r="S7" s="927"/>
       <c r="T7" s="201"/>
       <c r="U7" s="215"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V7" s="372"/>
+      <c r="W7" s="372" t="s">
+        <v>243</v>
+      </c>
+      <c r="X7" s="927"/>
+      <c r="Y7" s="927"/>
+      <c r="Z7" s="927"/>
+      <c r="AA7" s="372"/>
+      <c r="AB7" s="215"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="200"/>
       <c r="B8" s="201"/>
       <c r="C8" s="201"/>
@@ -61399,49 +61455,69 @@
       <c r="S8" s="201"/>
       <c r="T8" s="201"/>
       <c r="U8" s="201"/>
-    </row>
-    <row r="9" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V8" s="372"/>
+      <c r="W8" s="372"/>
+      <c r="X8" s="372"/>
+      <c r="Y8" s="372"/>
+      <c r="Z8" s="372"/>
+      <c r="AA8" s="372"/>
+      <c r="AB8" s="372"/>
+    </row>
+    <row r="9" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="200"/>
       <c r="B9" s="216" t="s">
         <v>450</v>
       </c>
-      <c r="C9" s="921" t="s">
+      <c r="C9" s="922" t="s">
         <v>244</v>
       </c>
-      <c r="D9" s="922"/>
-      <c r="E9" s="921" t="s">
+      <c r="D9" s="923"/>
+      <c r="E9" s="922" t="s">
         <v>245</v>
       </c>
-      <c r="F9" s="922"/>
+      <c r="F9" s="923"/>
       <c r="G9" s="201"/>
       <c r="H9" s="201"/>
       <c r="I9" s="201"/>
       <c r="J9" s="216" t="s">
         <v>450</v>
       </c>
-      <c r="K9" s="921" t="s">
+      <c r="K9" s="922" t="s">
         <v>244</v>
       </c>
-      <c r="L9" s="922"/>
-      <c r="M9" s="921" t="s">
+      <c r="L9" s="923"/>
+      <c r="M9" s="922" t="s">
         <v>245</v>
       </c>
-      <c r="N9" s="922"/>
+      <c r="N9" s="923"/>
       <c r="O9" s="201"/>
       <c r="P9" s="201"/>
       <c r="Q9" s="216" t="s">
         <v>450</v>
       </c>
-      <c r="R9" s="921" t="s">
+      <c r="R9" s="922" t="s">
         <v>244</v>
       </c>
-      <c r="S9" s="922"/>
-      <c r="T9" s="921" t="s">
+      <c r="S9" s="923"/>
+      <c r="T9" s="922" t="s">
         <v>245</v>
       </c>
-      <c r="U9" s="922"/>
-    </row>
-    <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U9" s="923"/>
+      <c r="V9" s="372"/>
+      <c r="W9" s="372"/>
+      <c r="X9" s="216" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y9" s="922" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z9" s="923"/>
+      <c r="AA9" s="922" t="s">
+        <v>245</v>
+      </c>
+      <c r="AB9" s="923"/>
+    </row>
+    <row r="10" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="200"/>
       <c r="B10" s="217" t="s">
         <v>241</v>
@@ -61479,7 +61555,7 @@
       <c r="O10" s="201"/>
       <c r="P10" s="201"/>
       <c r="Q10" s="217" t="s">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="R10" s="218" t="s">
         <v>69</v>
@@ -61493,18 +61569,35 @@
       <c r="U10" s="219" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V10" s="372"/>
+      <c r="W10" s="372"/>
+      <c r="X10" s="217" t="s">
+        <v>599</v>
+      </c>
+      <c r="Y10" s="218" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z10" s="219" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA10" s="218" t="s">
+        <v>155</v>
+      </c>
+      <c r="AB10" s="219" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="200"/>
       <c r="B11" s="220" t="s">
         <v>248</v>
       </c>
       <c r="C11" s="221"/>
       <c r="D11" s="221"/>
-      <c r="E11" s="923" t="s">
+      <c r="E11" s="919" t="s">
         <v>249</v>
       </c>
-      <c r="F11" s="924"/>
+      <c r="F11" s="920"/>
       <c r="G11" s="222"/>
       <c r="H11" s="222"/>
       <c r="I11" s="222"/>
@@ -61513,10 +61606,10 @@
       </c>
       <c r="K11" s="201"/>
       <c r="L11" s="201"/>
-      <c r="M11" s="926" t="s">
+      <c r="M11" s="924" t="s">
         <v>249</v>
       </c>
-      <c r="N11" s="927"/>
+      <c r="N11" s="925"/>
       <c r="O11" s="222"/>
       <c r="P11" s="222"/>
       <c r="Q11" s="220" t="s">
@@ -61524,12 +61617,23 @@
       </c>
       <c r="R11" s="221"/>
       <c r="S11" s="221"/>
-      <c r="T11" s="923" t="s">
+      <c r="T11" s="919" t="s">
         <v>249</v>
       </c>
-      <c r="U11" s="924"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U11" s="920"/>
+      <c r="V11" s="372"/>
+      <c r="W11" s="372"/>
+      <c r="X11" s="220" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y11" s="221"/>
+      <c r="Z11" s="221"/>
+      <c r="AA11" s="919" t="s">
+        <v>249</v>
+      </c>
+      <c r="AB11" s="920"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="200"/>
       <c r="B12" s="224" t="s">
         <v>484</v>
@@ -61557,8 +61661,17 @@
       <c r="S12" s="282"/>
       <c r="T12" s="287"/>
       <c r="U12" s="285"/>
-    </row>
-    <row r="13" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V12" s="372"/>
+      <c r="W12" s="372"/>
+      <c r="X12" s="224" t="s">
+        <v>484</v>
+      </c>
+      <c r="Y12" s="300"/>
+      <c r="Z12" s="282"/>
+      <c r="AA12" s="287"/>
+      <c r="AB12" s="285"/>
+    </row>
+    <row r="13" spans="1:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="200"/>
       <c r="B13" s="321" t="s">
         <v>250</v>
@@ -61586,8 +61699,17 @@
       <c r="S13" s="283"/>
       <c r="T13" s="288"/>
       <c r="U13" s="286"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V13" s="372"/>
+      <c r="W13" s="372"/>
+      <c r="X13" s="321" t="s">
+        <v>250</v>
+      </c>
+      <c r="Y13" s="301"/>
+      <c r="Z13" s="283"/>
+      <c r="AA13" s="288"/>
+      <c r="AB13" s="286"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="200"/>
       <c r="B14" s="225" t="s">
         <v>251</v>
@@ -61615,8 +61737,17 @@
       <c r="S14" s="284"/>
       <c r="T14" s="288"/>
       <c r="U14" s="286"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V14" s="372"/>
+      <c r="W14" s="372"/>
+      <c r="X14" s="225" t="s">
+        <v>466</v>
+      </c>
+      <c r="Y14" s="301"/>
+      <c r="Z14" s="284"/>
+      <c r="AA14" s="288"/>
+      <c r="AB14" s="286"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="200"/>
       <c r="B15" s="226" t="s">
         <v>252</v>
@@ -61644,8 +61775,17 @@
       <c r="S15" s="228"/>
       <c r="T15" s="289"/>
       <c r="U15" s="229"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V15" s="372"/>
+      <c r="W15" s="372"/>
+      <c r="X15" s="226" t="s">
+        <v>253</v>
+      </c>
+      <c r="Y15" s="269"/>
+      <c r="Z15" s="270"/>
+      <c r="AA15" s="299"/>
+      <c r="AB15" s="271"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="231"/>
       <c r="B16" s="232" t="s">
         <v>254</v>
@@ -61673,8 +61813,17 @@
       <c r="S16" s="234"/>
       <c r="T16" s="296"/>
       <c r="U16" s="235"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V16" s="372"/>
+      <c r="W16" s="372"/>
+      <c r="X16" s="378" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y16" s="273"/>
+      <c r="Z16" s="278"/>
+      <c r="AA16" s="296"/>
+      <c r="AB16" s="275"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="200"/>
       <c r="B17" s="236" t="s">
         <v>233</v>
@@ -61702,8 +61851,17 @@
       <c r="S17" s="238"/>
       <c r="T17" s="293"/>
       <c r="U17" s="239"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V17" s="277"/>
+      <c r="W17" s="277"/>
+      <c r="X17" s="236" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y17" s="237"/>
+      <c r="Z17" s="238"/>
+      <c r="AA17" s="293"/>
+      <c r="AB17" s="239"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="200"/>
       <c r="B18" s="241" t="s">
         <v>449</v>
@@ -61731,8 +61889,17 @@
       <c r="S18" s="243"/>
       <c r="T18" s="291"/>
       <c r="U18" s="244"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V18" s="372"/>
+      <c r="W18" s="372"/>
+      <c r="X18" s="241" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y18" s="242"/>
+      <c r="Z18" s="243"/>
+      <c r="AA18" s="291"/>
+      <c r="AB18" s="244"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="202"/>
       <c r="B19" s="236"/>
       <c r="C19" s="245"/>
@@ -61754,18 +61921,25 @@
       <c r="S19" s="246"/>
       <c r="T19" s="201"/>
       <c r="U19" s="248"/>
-    </row>
-    <row r="20" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V19" s="372"/>
+      <c r="W19" s="372"/>
+      <c r="X19" s="236"/>
+      <c r="Y19" s="245"/>
+      <c r="Z19" s="246"/>
+      <c r="AA19" s="372"/>
+      <c r="AB19" s="248"/>
+    </row>
+    <row r="20" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="200"/>
       <c r="B20" s="220" t="s">
         <v>255</v>
       </c>
       <c r="C20" s="302"/>
       <c r="D20" s="249"/>
-      <c r="E20" s="923" t="s">
+      <c r="E20" s="919" t="s">
         <v>256</v>
       </c>
-      <c r="F20" s="924"/>
+      <c r="F20" s="920"/>
       <c r="G20" s="230"/>
       <c r="H20" s="230"/>
       <c r="I20" s="201"/>
@@ -61774,10 +61948,10 @@
       </c>
       <c r="K20" s="302"/>
       <c r="L20" s="249"/>
-      <c r="M20" s="923" t="s">
+      <c r="M20" s="919" t="s">
         <v>256</v>
       </c>
-      <c r="N20" s="924"/>
+      <c r="N20" s="920"/>
       <c r="O20" s="240"/>
       <c r="P20" s="240"/>
       <c r="Q20" s="220" t="s">
@@ -61785,12 +61959,23 @@
       </c>
       <c r="R20" s="302"/>
       <c r="S20" s="249"/>
-      <c r="T20" s="923" t="s">
+      <c r="T20" s="919" t="s">
         <v>256</v>
       </c>
-      <c r="U20" s="924"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U20" s="920"/>
+      <c r="V20" s="277"/>
+      <c r="W20" s="277"/>
+      <c r="X20" s="220" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y20" s="302"/>
+      <c r="Z20" s="249"/>
+      <c r="AA20" s="919" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB20" s="920"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="200"/>
       <c r="B21" s="250" t="s">
         <v>253</v>
@@ -61818,8 +62003,17 @@
       <c r="S21" s="228"/>
       <c r="T21" s="289"/>
       <c r="U21" s="229"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V21" s="277"/>
+      <c r="W21" s="277"/>
+      <c r="X21" s="226" t="s">
+        <v>253</v>
+      </c>
+      <c r="Y21" s="269"/>
+      <c r="Z21" s="270"/>
+      <c r="AA21" s="299"/>
+      <c r="AB21" s="271"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="231"/>
       <c r="B22" s="232" t="s">
         <v>254</v>
@@ -61847,8 +62041,17 @@
       <c r="S22" s="234"/>
       <c r="T22" s="296"/>
       <c r="U22" s="235"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V22" s="277"/>
+      <c r="W22" s="277"/>
+      <c r="X22" s="378" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y22" s="273"/>
+      <c r="Z22" s="278"/>
+      <c r="AA22" s="296"/>
+      <c r="AB22" s="275"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="200"/>
       <c r="B23" s="236" t="s">
         <v>257</v>
@@ -61876,8 +62079,17 @@
       <c r="S23" s="238"/>
       <c r="T23" s="293"/>
       <c r="U23" s="239"/>
-    </row>
-    <row r="24" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V23" s="277"/>
+      <c r="W23" s="277"/>
+      <c r="X23" s="236" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y23" s="237"/>
+      <c r="Z23" s="238"/>
+      <c r="AA23" s="293"/>
+      <c r="AB23" s="239"/>
+    </row>
+    <row r="24" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="200"/>
       <c r="B24" s="254" t="s">
         <v>258</v>
@@ -61905,8 +62117,17 @@
       <c r="S24" s="238"/>
       <c r="T24" s="297"/>
       <c r="U24" s="239"/>
-    </row>
-    <row r="25" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V24" s="277"/>
+      <c r="W24" s="277"/>
+      <c r="X24" s="254" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y24" s="255"/>
+      <c r="Z24" s="238"/>
+      <c r="AA24" s="297"/>
+      <c r="AB24" s="239"/>
+    </row>
+    <row r="25" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="200"/>
       <c r="B25" s="254" t="s">
         <v>259</v>
@@ -61934,8 +62155,17 @@
       <c r="S25" s="238"/>
       <c r="T25" s="297"/>
       <c r="U25" s="239"/>
-    </row>
-    <row r="26" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V25" s="277"/>
+      <c r="W25" s="277"/>
+      <c r="X25" s="254" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y25" s="255"/>
+      <c r="Z25" s="238"/>
+      <c r="AA25" s="297"/>
+      <c r="AB25" s="239"/>
+    </row>
+    <row r="26" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="200"/>
       <c r="B26" s="254" t="s">
         <v>260</v>
@@ -61963,8 +62193,17 @@
       <c r="S26" s="238"/>
       <c r="T26" s="297"/>
       <c r="U26" s="239"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V26" s="277"/>
+      <c r="W26" s="277"/>
+      <c r="X26" s="254" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y26" s="255"/>
+      <c r="Z26" s="238"/>
+      <c r="AA26" s="297"/>
+      <c r="AB26" s="239"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" s="200"/>
       <c r="B27" s="256" t="s">
         <v>261</v>
@@ -61992,8 +62231,17 @@
       <c r="S27" s="238"/>
       <c r="T27" s="297"/>
       <c r="U27" s="239"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V27" s="277"/>
+      <c r="W27" s="277"/>
+      <c r="X27" s="254" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y27" s="255"/>
+      <c r="Z27" s="238"/>
+      <c r="AA27" s="297"/>
+      <c r="AB27" s="239"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" s="200"/>
       <c r="B28" s="303" t="s">
         <v>449</v>
@@ -62021,8 +62269,17 @@
       <c r="S28" s="243"/>
       <c r="T28" s="242"/>
       <c r="U28" s="244"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V28" s="277"/>
+      <c r="W28" s="277"/>
+      <c r="X28" s="241" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y28" s="242"/>
+      <c r="Z28" s="243"/>
+      <c r="AA28" s="242"/>
+      <c r="AB28" s="244"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="200"/>
       <c r="B29" s="257"/>
       <c r="C29" s="258"/>
@@ -62044,18 +62301,25 @@
       <c r="S29" s="259"/>
       <c r="T29" s="240"/>
       <c r="U29" s="261"/>
-    </row>
-    <row r="30" spans="1:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V29" s="277"/>
+      <c r="W29" s="277"/>
+      <c r="X29" s="257"/>
+      <c r="Y29" s="258"/>
+      <c r="Z29" s="259"/>
+      <c r="AA29" s="277"/>
+      <c r="AB29" s="261"/>
+    </row>
+    <row r="30" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="200"/>
       <c r="B30" s="220" t="s">
         <v>262</v>
       </c>
       <c r="C30" s="302"/>
       <c r="D30" s="249"/>
-      <c r="E30" s="923" t="s">
+      <c r="E30" s="919" t="s">
         <v>256</v>
       </c>
-      <c r="F30" s="924"/>
+      <c r="F30" s="920"/>
       <c r="G30" s="230"/>
       <c r="H30" s="230"/>
       <c r="I30" s="201"/>
@@ -62064,10 +62328,10 @@
       </c>
       <c r="K30" s="302"/>
       <c r="L30" s="249"/>
-      <c r="M30" s="923" t="s">
-        <v>593</v>
-      </c>
-      <c r="N30" s="924"/>
+      <c r="M30" s="919" t="s">
+        <v>592</v>
+      </c>
+      <c r="N30" s="920"/>
       <c r="O30" s="240"/>
       <c r="P30" s="240"/>
       <c r="Q30" s="220" t="s">
@@ -62075,12 +62339,23 @@
       </c>
       <c r="R30" s="302"/>
       <c r="S30" s="249"/>
-      <c r="T30" s="923" t="s">
+      <c r="T30" s="919" t="s">
         <v>256</v>
       </c>
-      <c r="U30" s="924"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U30" s="920"/>
+      <c r="V30" s="277"/>
+      <c r="W30" s="277"/>
+      <c r="X30" s="220" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y30" s="302"/>
+      <c r="Z30" s="249"/>
+      <c r="AA30" s="919" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB30" s="920"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="262"/>
       <c r="B31" s="250" t="s">
         <v>253</v>
@@ -62116,8 +62391,17 @@
       <c r="S31" s="270"/>
       <c r="T31" s="299"/>
       <c r="U31" s="271"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V31" s="379"/>
+      <c r="W31" s="379"/>
+      <c r="X31" s="226" t="s">
+        <v>253</v>
+      </c>
+      <c r="Y31" s="269"/>
+      <c r="Z31" s="270"/>
+      <c r="AA31" s="299"/>
+      <c r="AB31" s="271"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="272"/>
       <c r="B32" s="232" t="s">
         <v>254</v>
@@ -62153,8 +62437,17 @@
       <c r="S32" s="278"/>
       <c r="T32" s="295"/>
       <c r="U32" s="275"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V32" s="277"/>
+      <c r="W32" s="277"/>
+      <c r="X32" s="378" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y32" s="273"/>
+      <c r="Z32" s="278"/>
+      <c r="AA32" s="296"/>
+      <c r="AB32" s="275"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" s="200"/>
       <c r="B33" s="236" t="s">
         <v>257</v>
@@ -62182,8 +62475,17 @@
       <c r="S33" s="238"/>
       <c r="T33" s="293"/>
       <c r="U33" s="239"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V33" s="277"/>
+      <c r="W33" s="277"/>
+      <c r="X33" s="236" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y33" s="237"/>
+      <c r="Z33" s="238"/>
+      <c r="AA33" s="293"/>
+      <c r="AB33" s="239"/>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" s="279"/>
       <c r="B34" s="254" t="s">
         <v>263</v>
@@ -62211,8 +62513,17 @@
       <c r="S34" s="238"/>
       <c r="T34" s="255"/>
       <c r="U34" s="239"/>
-    </row>
-    <row r="35" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V34" s="280"/>
+      <c r="W34" s="280"/>
+      <c r="X34" s="254" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y34" s="255"/>
+      <c r="Z34" s="238"/>
+      <c r="AA34" s="255"/>
+      <c r="AB34" s="239"/>
+    </row>
+    <row r="35" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="279"/>
       <c r="B35" s="254" t="s">
         <v>264</v>
@@ -62240,8 +62551,17 @@
       <c r="S35" s="238"/>
       <c r="T35" s="255"/>
       <c r="U35" s="239"/>
-    </row>
-    <row r="36" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V35" s="280"/>
+      <c r="W35" s="280"/>
+      <c r="X35" s="254" t="s">
+        <v>264</v>
+      </c>
+      <c r="Y35" s="255"/>
+      <c r="Z35" s="238"/>
+      <c r="AA35" s="255"/>
+      <c r="AB35" s="239"/>
+    </row>
+    <row r="36" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="279"/>
       <c r="B36" s="254" t="s">
         <v>265</v>
@@ -62269,8 +62589,17 @@
       <c r="S36" s="238"/>
       <c r="T36" s="255"/>
       <c r="U36" s="239"/>
-    </row>
-    <row r="37" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V36" s="280"/>
+      <c r="W36" s="280"/>
+      <c r="X36" s="254" t="s">
+        <v>266</v>
+      </c>
+      <c r="Y36" s="255"/>
+      <c r="Z36" s="238"/>
+      <c r="AA36" s="255"/>
+      <c r="AB36" s="239"/>
+    </row>
+    <row r="37" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="279"/>
       <c r="B37" s="254" t="s">
         <v>267</v>
@@ -62298,8 +62627,17 @@
       <c r="S37" s="238"/>
       <c r="T37" s="255"/>
       <c r="U37" s="239"/>
-    </row>
-    <row r="38" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V37" s="280"/>
+      <c r="W37" s="280"/>
+      <c r="X37" s="254" t="s">
+        <v>267</v>
+      </c>
+      <c r="Y37" s="255"/>
+      <c r="Z37" s="238"/>
+      <c r="AA37" s="255"/>
+      <c r="AB37" s="239"/>
+    </row>
+    <row r="38" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="279"/>
       <c r="B38" s="254" t="s">
         <v>259</v>
@@ -62327,8 +62665,17 @@
       <c r="S38" s="238"/>
       <c r="T38" s="255"/>
       <c r="U38" s="239"/>
-    </row>
-    <row r="39" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V38" s="280"/>
+      <c r="W38" s="280"/>
+      <c r="X38" s="254" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y38" s="255"/>
+      <c r="Z38" s="238"/>
+      <c r="AA38" s="255"/>
+      <c r="AB38" s="239"/>
+    </row>
+    <row r="39" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="279"/>
       <c r="B39" s="254" t="s">
         <v>268</v>
@@ -62356,8 +62703,17 @@
       <c r="S39" s="238"/>
       <c r="T39" s="255"/>
       <c r="U39" s="239"/>
-    </row>
-    <row r="40" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V39" s="280"/>
+      <c r="W39" s="280"/>
+      <c r="X39" s="254" t="s">
+        <v>269</v>
+      </c>
+      <c r="Y39" s="255"/>
+      <c r="Z39" s="238"/>
+      <c r="AA39" s="255"/>
+      <c r="AB39" s="239"/>
+    </row>
+    <row r="40" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="279"/>
       <c r="B40" s="254" t="s">
         <v>270</v>
@@ -62385,8 +62741,17 @@
       <c r="S40" s="238"/>
       <c r="T40" s="255"/>
       <c r="U40" s="239"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V40" s="280"/>
+      <c r="W40" s="280"/>
+      <c r="X40" s="254" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y40" s="255"/>
+      <c r="Z40" s="238"/>
+      <c r="AA40" s="255"/>
+      <c r="AB40" s="239"/>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" s="200"/>
       <c r="B41" s="241" t="s">
         <v>449</v>
@@ -62414,14 +62779,23 @@
       <c r="S41" s="243"/>
       <c r="T41" s="242"/>
       <c r="U41" s="244"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V41" s="277"/>
+      <c r="W41" s="277"/>
+      <c r="X41" s="241" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y41" s="242"/>
+      <c r="Z41" s="243"/>
+      <c r="AA41" s="242"/>
+      <c r="AB41" s="244"/>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="200"/>
-      <c r="B42" s="925"/>
-      <c r="C42" s="925"/>
-      <c r="D42" s="925"/>
-      <c r="E42" s="925"/>
-      <c r="F42" s="925"/>
+      <c r="B42" s="921"/>
+      <c r="C42" s="921"/>
+      <c r="D42" s="921"/>
+      <c r="E42" s="921"/>
+      <c r="F42" s="921"/>
       <c r="G42" s="240"/>
       <c r="H42" s="201"/>
       <c r="I42" s="240"/>
@@ -62437,8 +62811,15 @@
       <c r="S42" s="240"/>
       <c r="T42" s="240"/>
       <c r="U42" s="240"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V42" s="277"/>
+      <c r="W42" s="277"/>
+      <c r="X42" s="277"/>
+      <c r="Y42" s="277"/>
+      <c r="Z42" s="277"/>
+      <c r="AA42" s="277"/>
+      <c r="AB42" s="277"/>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" s="200"/>
       <c r="B43" s="281" t="s">
         <v>273</v>
@@ -62462,8 +62843,15 @@
       <c r="S43" s="230"/>
       <c r="T43" s="230"/>
       <c r="U43" s="230"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V43" s="276"/>
+      <c r="W43" s="276"/>
+      <c r="X43" s="276"/>
+      <c r="Y43" s="276"/>
+      <c r="Z43" s="276"/>
+      <c r="AA43" s="276"/>
+      <c r="AB43" s="276"/>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" s="200"/>
       <c r="B44" s="202" t="s">
         <v>274</v>
@@ -62487,8 +62875,15 @@
       <c r="S44" s="230"/>
       <c r="T44" s="230"/>
       <c r="U44" s="230"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V44" s="276"/>
+      <c r="W44" s="276"/>
+      <c r="X44" s="276"/>
+      <c r="Y44" s="276"/>
+      <c r="Z44" s="276"/>
+      <c r="AA44" s="276"/>
+      <c r="AB44" s="276"/>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" s="200"/>
       <c r="B45" s="202" t="s">
         <v>275</v>
@@ -62512,8 +62907,15 @@
       <c r="S45" s="201"/>
       <c r="T45" s="201"/>
       <c r="U45" s="201"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V45" s="372"/>
+      <c r="W45" s="372"/>
+      <c r="X45" s="372"/>
+      <c r="Y45" s="372"/>
+      <c r="Z45" s="372"/>
+      <c r="AA45" s="372"/>
+      <c r="AB45" s="372"/>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" s="200"/>
       <c r="B46" s="202" t="s">
         <v>276</v>
@@ -62537,8 +62939,15 @@
       <c r="S46" s="201"/>
       <c r="T46" s="201"/>
       <c r="U46" s="201"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V46" s="372"/>
+      <c r="W46" s="372"/>
+      <c r="X46" s="372"/>
+      <c r="Y46" s="372"/>
+      <c r="Z46" s="372"/>
+      <c r="AA46" s="372"/>
+      <c r="AB46" s="372"/>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" s="200"/>
       <c r="B47" s="202" t="s">
         <v>277</v>
@@ -62562,10 +62971,32 @@
       <c r="S47" s="201"/>
       <c r="T47" s="201"/>
       <c r="U47" s="201"/>
+      <c r="V47" s="372"/>
+      <c r="W47" s="372"/>
+      <c r="X47" s="372"/>
+      <c r="Y47" s="372"/>
+      <c r="Z47" s="372"/>
+      <c r="AA47" s="372"/>
+      <c r="AB47" s="372"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="20">
+  <mergeCells count="26">
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -62577,15 +63008,6 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
change on sheet 54-area
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
@@ -2041,12 +2041,6 @@
 Number of agglomerations</t>
   </si>
   <si>
-    <t>First date of application of criterion N [Art. 5(2,3)] for this SA</t>
-  </si>
-  <si>
-    <t>First date of application of criterion P [Art. 5(2,3)] for this SA</t>
-  </si>
-  <si>
     <t>First date of application of Art. 5(4)</t>
   </si>
   <si>
@@ -2293,7 +2287,13 @@
     <t>SA/CSA applying Art. 5.4</t>
   </si>
   <si>
-    <t>Date of begin life</t>
+    <t>Date of designation</t>
+  </si>
+  <si>
+    <t>First date of application of criterion N for this SA</t>
+  </si>
+  <si>
+    <t>First date of application of criterion P for this SA</t>
   </si>
 </sst>
 </file>
@@ -5737,45 +5737,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -5810,6 +5771,9 @@
     <xf numFmtId="3" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5858,6 +5822,111 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5870,21 +5939,9 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5900,62 +5957,11 @@
     <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5966,12 +5972,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5990,26 +5990,26 @@
     <xf numFmtId="0" fontId="25" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6039,6 +6039,33 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6071,33 +6098,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6127,6 +6127,58 @@
     <xf numFmtId="3" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6139,18 +6191,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6162,46 +6202,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6541,7 +6541,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="770" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B3" s="773" t="s">
         <v>476</v>
@@ -6549,7 +6549,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="770" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B4" s="773" t="s">
         <v>477</v>
@@ -6557,7 +6557,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="770" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B5" s="771" t="s">
         <v>6</v>
@@ -6565,7 +6565,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="770" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B6" s="771" t="s">
         <v>3</v>
@@ -6573,7 +6573,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="770" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B7" s="771" t="s">
         <v>15</v>
@@ -6581,7 +6581,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="770" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B8" s="771" t="s">
         <v>2</v>
@@ -6589,7 +6589,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="770" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B9" s="771" t="s">
         <v>21</v>
@@ -6597,15 +6597,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="770" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B10" s="771" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="770" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B11" s="771" t="s">
         <v>4</v>
@@ -6613,15 +6613,15 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="770" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B12" s="771" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="770" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B13" s="771" t="s">
         <v>7</v>
@@ -6629,10 +6629,10 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="770" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B14" s="771" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -6640,7 +6640,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="771" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -6648,20 +6648,20 @@
         <v>23</v>
       </c>
       <c r="B16" s="771" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="770" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B17" s="771" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="770" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B18" s="771" t="s">
         <v>13</v>
@@ -6669,7 +6669,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="770" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B19" s="771" t="s">
         <v>10</v>
@@ -6677,7 +6677,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="770" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B20" s="771" t="s">
         <v>12</v>
@@ -6688,7 +6688,7 @@
         <v>509</v>
       </c>
       <c r="B21" s="773" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -6717,7 +6717,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="770" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B25" s="771" t="s">
         <v>9</v>
@@ -6725,7 +6725,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="770" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B26" s="771" t="s">
         <v>17</v>
@@ -6733,15 +6733,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="770" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B27" s="771" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="770" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B28" s="771" t="s">
         <v>14</v>
@@ -6757,7 +6757,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="770" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B30" s="771" t="s">
         <v>16</v>
@@ -6773,7 +6773,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="770" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B32" s="771" t="s">
         <v>5</v>
@@ -6781,42 +6781,42 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="770" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B33" s="771" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="774" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B34" s="775" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="770" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B35" s="775" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="770" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B36" s="771" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="774" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B37" s="771" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -6824,31 +6824,31 @@
         <v>102</v>
       </c>
       <c r="B38" s="771" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="774" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B39" s="775" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="774" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B40" s="775" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="774" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B41" s="775" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -6856,39 +6856,39 @@
         <v>124</v>
       </c>
       <c r="B42" s="775" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="774" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B43" s="775" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="774" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B44" s="775" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="774" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B45" s="775" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="774" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B46" s="775" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
   </sheetData>
@@ -6937,7 +6937,7 @@
     </row>
     <row r="7" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="327" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
@@ -6961,7 +6961,7 @@
         <v>278</v>
       </c>
       <c r="E10" s="929" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F10" s="930"/>
     </row>
@@ -7020,7 +7020,7 @@
     </row>
     <row r="16" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="340" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C16" s="347"/>
       <c r="D16" s="353"/>
@@ -7029,7 +7029,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="338" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C17" s="821"/>
       <c r="D17" s="807"/>
@@ -7047,7 +7047,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="819" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C19" s="820"/>
       <c r="D19" s="822"/>
@@ -7056,7 +7056,7 @@
     </row>
     <row r="20" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="341" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C20" s="347"/>
       <c r="D20" s="354"/>
@@ -7065,7 +7065,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="338" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C21" s="345"/>
       <c r="D21" s="350"/>
@@ -7083,7 +7083,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="803" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C23" s="363"/>
       <c r="D23" s="362"/>
@@ -7095,7 +7095,7 @@
     </row>
     <row r="27" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="327" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
@@ -7119,7 +7119,7 @@
         <v>278</v>
       </c>
       <c r="E30" s="929" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F30" s="930"/>
     </row>
@@ -7178,7 +7178,7 @@
     </row>
     <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="340" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C36" s="347"/>
       <c r="D36" s="353"/>
@@ -7187,7 +7187,7 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="338" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C37" s="345"/>
       <c r="D37" s="350"/>
@@ -7205,7 +7205,7 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="815" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C39" s="816"/>
       <c r="D39" s="822"/>
@@ -7214,7 +7214,7 @@
     </row>
     <row r="40" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="341" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C40" s="347"/>
       <c r="D40" s="354"/>
@@ -7223,7 +7223,7 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="338" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C41" s="345"/>
       <c r="D41" s="350"/>
@@ -7241,7 +7241,7 @@
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="815" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C43" s="360"/>
       <c r="D43" s="355"/>
@@ -7250,7 +7250,7 @@
     </row>
     <row r="46" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B46" s="327" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="47" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
@@ -7274,7 +7274,7 @@
         <v>278</v>
       </c>
       <c r="E49" s="929" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F49" s="930"/>
     </row>
@@ -7333,7 +7333,7 @@
     </row>
     <row r="55" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="340" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C55" s="347"/>
       <c r="D55" s="353"/>
@@ -7342,7 +7342,7 @@
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="338" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C56" s="345"/>
       <c r="D56" s="800"/>
@@ -7360,7 +7360,7 @@
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="814" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C58" s="816"/>
       <c r="D58" s="822"/>
@@ -7369,7 +7369,7 @@
     </row>
     <row r="59" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="340" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C59" s="347"/>
       <c r="D59" s="354"/>
@@ -7378,7 +7378,7 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="338" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C60" s="345"/>
       <c r="D60" s="350"/>
@@ -7396,7 +7396,7 @@
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="803" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C62" s="360"/>
       <c r="D62" s="364"/>
@@ -7405,7 +7405,7 @@
     </row>
     <row r="65" spans="2:6" ht="21" x14ac:dyDescent="0.4">
       <c r="B65" s="327" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="66" spans="2:6" ht="21" x14ac:dyDescent="0.4">
@@ -7429,7 +7429,7 @@
         <v>278</v>
       </c>
       <c r="E68" s="929" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F68" s="930"/>
     </row>
@@ -7488,7 +7488,7 @@
     </row>
     <row r="74" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B74" s="340" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C74" s="347"/>
       <c r="D74" s="353"/>
@@ -7497,7 +7497,7 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="817" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C75" s="813"/>
       <c r="D75" s="350"/>
@@ -7515,7 +7515,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="814" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C77" s="816"/>
       <c r="D77" s="822"/>
@@ -7524,7 +7524,7 @@
     </row>
     <row r="78" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B78" s="340" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C78" s="347"/>
       <c r="D78" s="354"/>
@@ -7533,7 +7533,7 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="338" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C79" s="345"/>
       <c r="D79" s="350"/>
@@ -7551,7 +7551,7 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" s="803" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C81" s="360"/>
       <c r="D81" s="364"/>
@@ -7605,8 +7605,8 @@
       </c>
       <c r="C2" s="373"/>
       <c r="D2" s="373"/>
-      <c r="E2" s="924"/>
-      <c r="F2" s="924"/>
+      <c r="E2" s="926"/>
+      <c r="F2" s="926"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="372"/>
@@ -7627,7 +7627,7 @@
     <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="370"/>
       <c r="B5" s="376" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C5" s="376"/>
       <c r="D5" s="376"/>
@@ -7638,13 +7638,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="370"/>
-      <c r="B6" s="921" t="s">
+      <c r="B6" s="927" t="s">
         <v>452</v>
       </c>
-      <c r="C6" s="921"/>
-      <c r="D6" s="921"/>
-      <c r="E6" s="921"/>
-      <c r="F6" s="921"/>
+      <c r="C6" s="927"/>
+      <c r="D6" s="927"/>
+      <c r="E6" s="927"/>
+      <c r="F6" s="927"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="370"/>
@@ -7737,7 +7737,7 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="385"/>
       <c r="B15" s="402" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C15" s="384"/>
       <c r="D15" s="386"/>
@@ -7775,7 +7775,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="385"/>
       <c r="B19" s="402" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C19" s="384"/>
       <c r="D19" s="386"/>
@@ -7802,11 +7802,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="370"/>
-      <c r="B22" s="925"/>
-      <c r="C22" s="925"/>
-      <c r="D22" s="925"/>
-      <c r="E22" s="925"/>
-      <c r="F22" s="925"/>
+      <c r="B22" s="921"/>
+      <c r="C22" s="921"/>
+      <c r="D22" s="921"/>
+      <c r="E22" s="921"/>
+      <c r="F22" s="921"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="370"/>
@@ -7829,7 +7829,7 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="370"/>
       <c r="B25" s="769" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C25" s="371"/>
       <c r="D25" s="371"/>
@@ -7839,7 +7839,7 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="370"/>
       <c r="B26" s="769" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C26" s="371"/>
       <c r="D26" s="371"/>
@@ -7957,7 +7957,7 @@
         <v>299</v>
       </c>
       <c r="C4" s="425" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D4" s="425"/>
       <c r="E4" s="426"/>
@@ -8103,43 +8103,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="941" t="s">
+      <c r="A1" s="950" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="942"/>
+      <c r="B1" s="951"/>
       <c r="C1" s="455"/>
-      <c r="D1" s="952" t="s">
+      <c r="D1" s="941" t="s">
         <v>300</v>
       </c>
-      <c r="E1" s="953"/>
-      <c r="F1" s="953"/>
-      <c r="G1" s="953"/>
-      <c r="H1" s="953"/>
-      <c r="I1" s="954"/>
-      <c r="J1" s="943" t="s">
+      <c r="E1" s="942"/>
+      <c r="F1" s="942"/>
+      <c r="G1" s="942"/>
+      <c r="H1" s="942"/>
+      <c r="I1" s="943"/>
+      <c r="J1" s="952" t="s">
         <v>301</v>
       </c>
-      <c r="K1" s="944"/>
-      <c r="L1" s="944"/>
-      <c r="M1" s="944"/>
-      <c r="N1" s="945"/>
-      <c r="O1" s="946" t="s">
+      <c r="K1" s="953"/>
+      <c r="L1" s="953"/>
+      <c r="M1" s="953"/>
+      <c r="N1" s="954"/>
+      <c r="O1" s="955" t="s">
         <v>302</v>
       </c>
-      <c r="P1" s="947"/>
-      <c r="Q1" s="948"/>
+      <c r="P1" s="956"/>
+      <c r="Q1" s="957"/>
       <c r="R1" s="442" t="s">
         <v>81</v>
       </c>
       <c r="S1" s="443"/>
-      <c r="T1" s="940" t="s">
+      <c r="T1" s="949" t="s">
         <v>495</v>
       </c>
-      <c r="U1" s="940"/>
-      <c r="V1" s="940"/>
-      <c r="W1" s="940"/>
-      <c r="X1" s="940"/>
-      <c r="Y1" s="940"/>
+      <c r="U1" s="949"/>
+      <c r="V1" s="949"/>
+      <c r="W1" s="949"/>
+      <c r="X1" s="949"/>
+      <c r="Y1" s="949"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="445" t="s">
@@ -8151,18 +8151,18 @@
       <c r="C2" s="446" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="957" t="s">
+      <c r="D2" s="946" t="s">
         <v>304</v>
       </c>
-      <c r="E2" s="956"/>
-      <c r="F2" s="956" t="s">
+      <c r="E2" s="945"/>
+      <c r="F2" s="945" t="s">
         <v>305</v>
       </c>
-      <c r="G2" s="956"/>
-      <c r="H2" s="955" t="s">
+      <c r="G2" s="945"/>
+      <c r="H2" s="944" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="955"/>
+      <c r="I2" s="944"/>
       <c r="J2" s="447">
         <v>0</v>
       </c>
@@ -8193,18 +8193,18 @@
       <c r="S2" s="681" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="938" t="s">
+      <c r="T2" s="947" t="s">
         <v>464</v>
       </c>
-      <c r="U2" s="938"/>
-      <c r="V2" s="939" t="s">
+      <c r="U2" s="947"/>
+      <c r="V2" s="948" t="s">
         <v>481</v>
       </c>
-      <c r="W2" s="939"/>
-      <c r="X2" s="939" t="s">
+      <c r="W2" s="948"/>
+      <c r="X2" s="948" t="s">
         <v>482</v>
       </c>
-      <c r="Y2" s="939"/>
+      <c r="Y2" s="948"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="450"/>
@@ -8230,13 +8230,13 @@
       <c r="I3" s="665" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="949" t="s">
+      <c r="J3" s="938" t="s">
         <v>311</v>
       </c>
-      <c r="K3" s="950"/>
-      <c r="L3" s="950"/>
-      <c r="M3" s="950"/>
-      <c r="N3" s="951"/>
+      <c r="K3" s="939"/>
+      <c r="L3" s="939"/>
+      <c r="M3" s="939"/>
+      <c r="N3" s="940"/>
       <c r="O3" s="458"/>
       <c r="P3" s="458"/>
       <c r="Q3" s="458"/>
@@ -9465,11 +9465,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:X4"/>
   <mergeCells count="12">
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -9477,6 +9472,11 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9516,14 +9516,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="836" t="s">
+      <c r="A1" s="865" t="s">
         <v>312</v>
       </c>
-      <c r="B1" s="837"/>
-      <c r="C1" s="837"/>
-      <c r="D1" s="837"/>
-      <c r="E1" s="837"/>
-      <c r="F1" s="837"/>
+      <c r="B1" s="866"/>
+      <c r="C1" s="866"/>
+      <c r="D1" s="866"/>
+      <c r="E1" s="866"/>
+      <c r="F1" s="866"/>
       <c r="G1" s="472"/>
       <c r="H1" s="964" t="s">
         <v>169</v>
@@ -9564,8 +9564,8 @@
       <c r="AF1" s="961" t="s">
         <v>480</v>
       </c>
-      <c r="AG1" s="940"/>
-      <c r="AH1" s="940"/>
+      <c r="AG1" s="949"/>
+      <c r="AH1" s="949"/>
       <c r="AI1" s="688"/>
       <c r="AJ1" s="688"/>
       <c r="AK1" s="688"/>
@@ -10559,11 +10559,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:AH4"/>
   <mergeCells count="18">
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AE1:AE2"/>
@@ -10577,6 +10572,11 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10791,9 +10791,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="968"/>
-      <c r="B1" s="867"/>
-      <c r="C1" s="867"/>
+      <c r="A1" s="986"/>
+      <c r="B1" s="855"/>
+      <c r="C1" s="855"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="741"/>
@@ -10808,21 +10808,21 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="976" t="s">
+      <c r="A3" s="990" t="s">
         <v>345</v>
       </c>
-      <c r="B3" s="978" t="s">
+      <c r="B3" s="992" t="s">
         <v>453</v>
       </c>
-      <c r="C3" s="979"/>
-      <c r="D3" s="974" t="s">
+      <c r="C3" s="993"/>
+      <c r="D3" s="978" t="s">
         <v>454</v>
       </c>
-      <c r="E3" s="975"/>
-      <c r="F3" s="974" t="s">
+      <c r="E3" s="979"/>
+      <c r="F3" s="978" t="s">
         <v>488</v>
       </c>
-      <c r="G3" s="975"/>
+      <c r="G3" s="979"/>
       <c r="I3" s="739" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
@@ -10833,14 +10833,14 @@
       <c r="K3" s="721"/>
       <c r="L3" s="721"/>
       <c r="N3" s="706"/>
-      <c r="O3" s="990" t="s">
+      <c r="O3" s="975" t="s">
         <v>346</v>
       </c>
-      <c r="P3" s="990"/>
-      <c r="Q3" s="990" t="s">
+      <c r="P3" s="975"/>
+      <c r="Q3" s="975" t="s">
         <v>347</v>
       </c>
-      <c r="R3" s="990"/>
+      <c r="R3" s="975"/>
       <c r="S3" s="706"/>
       <c r="T3" s="714" t="s">
         <v>348</v>
@@ -10848,7 +10848,7 @@
       <c r="U3" s="706"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="977"/>
+      <c r="A4" s="991"/>
       <c r="B4" s="512" t="s">
         <v>349</v>
       </c>
@@ -11107,14 +11107,14 @@
       <c r="K10" s="721"/>
       <c r="L10" s="721"/>
       <c r="N10" s="714"/>
-      <c r="O10" s="990" t="s">
+      <c r="O10" s="975" t="s">
         <v>349</v>
       </c>
-      <c r="P10" s="990"/>
-      <c r="Q10" s="990" t="s">
+      <c r="P10" s="975"/>
+      <c r="Q10" s="975" t="s">
         <v>356</v>
       </c>
-      <c r="R10" s="990"/>
+      <c r="R10" s="975"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I11" s="739" t="str">
@@ -11178,7 +11178,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="976" t="s">
+      <c r="A13" s="990" t="s">
         <v>357</v>
       </c>
       <c r="B13" s="511" t="str">
@@ -11224,7 +11224,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="977"/>
+      <c r="A14" s="991"/>
       <c r="B14" s="514" t="s">
         <v>350</v>
       </c>
@@ -11354,34 +11354,34 @@
       <c r="A21" s="502" t="s">
         <v>362</v>
       </c>
-      <c r="B21" s="991" t="s">
+      <c r="B21" s="980" t="s">
         <v>507</v>
       </c>
-      <c r="C21" s="992"/>
-      <c r="D21" s="992"/>
-      <c r="E21" s="992"/>
-      <c r="F21" s="992"/>
-      <c r="G21" s="992"/>
+      <c r="C21" s="981"/>
+      <c r="D21" s="981"/>
+      <c r="E21" s="981"/>
+      <c r="F21" s="981"/>
+      <c r="G21" s="981"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="516" t="s">
         <v>326</v>
       </c>
-      <c r="B22" s="980" t="str">
+      <c r="B22" s="982" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="981"/>
-      <c r="D22" s="980" t="str">
+      <c r="C22" s="983"/>
+      <c r="D22" s="982" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="981"/>
-      <c r="F22" s="980" t="str">
+      <c r="E22" s="983"/>
+      <c r="F22" s="982" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="981"/>
+      <c r="G22" s="983"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="517"/>
@@ -11808,21 +11808,21 @@
       <c r="A41" s="519" t="s">
         <v>372</v>
       </c>
-      <c r="B41" s="970" t="str">
+      <c r="B41" s="988" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="971"/>
-      <c r="D41" s="972" t="str">
+      <c r="C41" s="989"/>
+      <c r="D41" s="976" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="973"/>
-      <c r="F41" s="972" t="str">
+      <c r="E41" s="977"/>
+      <c r="F41" s="976" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G41" s="973"/>
+      <c r="G41" s="977"/>
       <c r="N41" s="706"/>
       <c r="O41" s="733" t="s">
         <v>458</v>
@@ -12036,11 +12036,11 @@
       <c r="F53" s="711" t="s">
         <v>513</v>
       </c>
-      <c r="H53" s="993" t="s">
+      <c r="H53" s="968" t="s">
         <v>500</v>
       </c>
-      <c r="I53" s="993"/>
-      <c r="J53" s="993"/>
+      <c r="I53" s="968"/>
+      <c r="J53" s="968"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="702" t="s">
@@ -12210,11 +12210,11 @@
       <c r="F63" s="711" t="s">
         <v>513</v>
       </c>
-      <c r="H63" s="993" t="s">
+      <c r="H63" s="968" t="s">
         <v>514</v>
       </c>
-      <c r="I63" s="993"/>
-      <c r="J63" s="993"/>
+      <c r="I63" s="968"/>
+      <c r="J63" s="968"/>
       <c r="L63" s="709"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -12401,12 +12401,12 @@
       <c r="A74" s="623" t="s">
         <v>371</v>
       </c>
-      <c r="B74" s="969" t="s">
+      <c r="B74" s="987" t="s">
         <v>455</v>
       </c>
-      <c r="C74" s="969"/>
-      <c r="D74" s="969"/>
-      <c r="E74" s="969"/>
+      <c r="C74" s="987"/>
+      <c r="D74" s="987"/>
+      <c r="E74" s="987"/>
       <c r="I74" s="710"/>
       <c r="J74" s="710"/>
       <c r="K74" s="710"/>
@@ -12722,21 +12722,21 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="984" t="str">
+      <c r="B85" s="973" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="985"/>
-      <c r="D85" s="984" t="str">
+      <c r="C85" s="974"/>
+      <c r="D85" s="973" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="985"/>
-      <c r="F85" s="984" t="str">
+      <c r="E85" s="974"/>
+      <c r="F85" s="973" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="985"/>
+      <c r="G85" s="974"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="503"/>
@@ -13032,21 +13032,21 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="984" t="str">
+      <c r="B101" s="973" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="985"/>
-      <c r="D101" s="984" t="str">
+      <c r="C101" s="974"/>
+      <c r="D101" s="973" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="985"/>
-      <c r="F101" s="984" t="str">
+      <c r="E101" s="974"/>
+      <c r="F101" s="973" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="985"/>
+      <c r="G101" s="974"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="503"/>
@@ -13342,36 +13342,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="986" t="str">
+      <c r="B116" s="969" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="987"/>
-      <c r="D116" s="986" t="str">
+      <c r="C116" s="970"/>
+      <c r="D116" s="969" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="987"/>
-      <c r="F116" s="986" t="str">
+      <c r="E116" s="970"/>
+      <c r="F116" s="969" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="987"/>
+      <c r="G116" s="970"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="542"/>
-      <c r="B117" s="988" t="s">
+      <c r="B117" s="971" t="s">
         <v>279</v>
       </c>
-      <c r="C117" s="989"/>
-      <c r="D117" s="988" t="s">
+      <c r="C117" s="972"/>
+      <c r="D117" s="971" t="s">
         <v>279</v>
       </c>
-      <c r="E117" s="989"/>
-      <c r="F117" s="988" t="s">
+      <c r="E117" s="972"/>
+      <c r="F117" s="971" t="s">
         <v>279</v>
       </c>
-      <c r="G117" s="989"/>
+      <c r="G117" s="972"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="543" t="s">
@@ -13674,12 +13674,12 @@
       <c r="A129" s="546" t="s">
         <v>357</v>
       </c>
-      <c r="B129" s="982" t="str">
+      <c r="B129" s="984" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="983"/>
-      <c r="D129" s="983"/>
+      <c r="C129" s="985"/>
+      <c r="D129" s="985"/>
       <c r="N129" s="714" t="s">
         <v>398</v>
       </c>
@@ -13901,7 +13901,7 @@
     </row>
     <row r="150" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="556" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B150" s="556" t="s">
         <v>73</v>
@@ -13920,7 +13920,7 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" s="556" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B151" s="556" t="s">
         <v>73</v>
@@ -14455,22 +14455,16 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="39">
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -14484,16 +14478,22 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17943,7 +17943,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="796" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D5" s="828" t="s">
         <v>27</v>
@@ -58414,7 +58414,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:A2"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58436,16 +58436,16 @@
         <v>26</v>
       </c>
       <c r="C1" s="824" t="s">
+        <v>597</v>
+      </c>
+      <c r="D1" s="767" t="s">
+        <v>598</v>
+      </c>
+      <c r="E1" s="767" t="s">
         <v>599</v>
       </c>
-      <c r="D1" s="767" t="s">
+      <c r="F1" s="661" t="s">
         <v>515</v>
-      </c>
-      <c r="E1" s="767" t="s">
-        <v>516</v>
-      </c>
-      <c r="F1" s="661" t="s">
-        <v>517</v>
       </c>
       <c r="G1" s="661" t="s">
         <v>50</v>
@@ -58647,123 +58647,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="658" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="836" t="s">
+      <c r="A1" s="865" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="837"/>
-      <c r="C1" s="837"/>
-      <c r="D1" s="837"/>
-      <c r="E1" s="837"/>
-      <c r="F1" s="837"/>
-      <c r="G1" s="837"/>
-      <c r="H1" s="838" t="s">
+      <c r="B1" s="866"/>
+      <c r="C1" s="866"/>
+      <c r="D1" s="866"/>
+      <c r="E1" s="866"/>
+      <c r="F1" s="866"/>
+      <c r="G1" s="866"/>
+      <c r="H1" s="867" t="s">
         <v>464</v>
       </c>
-      <c r="I1" s="839"/>
-      <c r="J1" s="839"/>
-      <c r="K1" s="839"/>
-      <c r="L1" s="839"/>
-      <c r="M1" s="840"/>
-      <c r="N1" s="841" t="s">
+      <c r="I1" s="868"/>
+      <c r="J1" s="868"/>
+      <c r="K1" s="868"/>
+      <c r="L1" s="868"/>
+      <c r="M1" s="869"/>
+      <c r="N1" s="870" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="842"/>
-      <c r="P1" s="842"/>
-      <c r="Q1" s="842"/>
-      <c r="R1" s="842"/>
-      <c r="S1" s="842"/>
-      <c r="T1" s="842"/>
-      <c r="U1" s="842"/>
-      <c r="V1" s="843" t="s">
+      <c r="O1" s="848"/>
+      <c r="P1" s="848"/>
+      <c r="Q1" s="848"/>
+      <c r="R1" s="848"/>
+      <c r="S1" s="848"/>
+      <c r="T1" s="848"/>
+      <c r="U1" s="848"/>
+      <c r="V1" s="871" t="s">
         <v>83</v>
       </c>
-      <c r="W1" s="844"/>
-      <c r="X1" s="845"/>
-      <c r="Y1" s="845"/>
-      <c r="Z1" s="846"/>
-      <c r="AA1" s="847" t="s">
+      <c r="W1" s="872"/>
+      <c r="X1" s="873"/>
+      <c r="Y1" s="873"/>
+      <c r="Z1" s="874"/>
+      <c r="AA1" s="875" t="s">
         <v>84</v>
       </c>
-      <c r="AB1" s="848"/>
-      <c r="AC1" s="848"/>
-      <c r="AD1" s="848"/>
-      <c r="AE1" s="848"/>
-      <c r="AF1" s="848"/>
-      <c r="AG1" s="848"/>
-      <c r="AH1" s="848"/>
-      <c r="AI1" s="848"/>
-      <c r="AJ1" s="848"/>
-      <c r="AK1" s="848"/>
-      <c r="AL1" s="848"/>
-      <c r="AM1" s="848"/>
+      <c r="AB1" s="876"/>
+      <c r="AC1" s="876"/>
+      <c r="AD1" s="876"/>
+      <c r="AE1" s="876"/>
+      <c r="AF1" s="876"/>
+      <c r="AG1" s="876"/>
+      <c r="AH1" s="876"/>
+      <c r="AI1" s="876"/>
+      <c r="AJ1" s="876"/>
+      <c r="AK1" s="876"/>
+      <c r="AL1" s="876"/>
+      <c r="AM1" s="876"/>
       <c r="AN1" s="52"/>
       <c r="AO1" s="53"/>
-      <c r="AP1" s="860" t="s">
+      <c r="AP1" s="847" t="s">
         <v>85</v>
       </c>
-      <c r="AQ1" s="842"/>
-      <c r="AR1" s="842"/>
-      <c r="AS1" s="842"/>
-      <c r="AT1" s="842"/>
-      <c r="AU1" s="842"/>
-      <c r="AV1" s="842"/>
-      <c r="AW1" s="861"/>
-      <c r="AX1" s="868" t="s">
-        <v>596</v>
-      </c>
-      <c r="AY1" s="869"/>
-      <c r="AZ1" s="869"/>
-      <c r="BA1" s="869"/>
-      <c r="BB1" s="869"/>
-      <c r="BC1" s="870"/>
-      <c r="BD1" s="871" t="s">
+      <c r="AQ1" s="848"/>
+      <c r="AR1" s="848"/>
+      <c r="AS1" s="848"/>
+      <c r="AT1" s="848"/>
+      <c r="AU1" s="848"/>
+      <c r="AV1" s="848"/>
+      <c r="AW1" s="849"/>
+      <c r="AX1" s="856" t="s">
+        <v>594</v>
+      </c>
+      <c r="AY1" s="857"/>
+      <c r="AZ1" s="857"/>
+      <c r="BA1" s="857"/>
+      <c r="BB1" s="857"/>
+      <c r="BC1" s="858"/>
+      <c r="BD1" s="859" t="s">
         <v>86</v>
       </c>
-      <c r="BE1" s="872"/>
-      <c r="BF1" s="872"/>
-      <c r="BG1" s="872"/>
-      <c r="BH1" s="872"/>
-      <c r="BI1" s="873"/>
-      <c r="BJ1" s="874" t="s">
+      <c r="BE1" s="860"/>
+      <c r="BF1" s="860"/>
+      <c r="BG1" s="860"/>
+      <c r="BH1" s="860"/>
+      <c r="BI1" s="861"/>
+      <c r="BJ1" s="862" t="s">
         <v>87</v>
       </c>
-      <c r="BK1" s="875"/>
-      <c r="BL1" s="875"/>
-      <c r="BM1" s="875"/>
-      <c r="BN1" s="875"/>
-      <c r="BO1" s="875"/>
-      <c r="BP1" s="876"/>
-      <c r="BQ1" s="849" t="s">
+      <c r="BK1" s="863"/>
+      <c r="BL1" s="863"/>
+      <c r="BM1" s="863"/>
+      <c r="BN1" s="863"/>
+      <c r="BO1" s="863"/>
+      <c r="BP1" s="864"/>
+      <c r="BQ1" s="836" t="s">
         <v>88</v>
       </c>
-      <c r="BR1" s="850"/>
-      <c r="BS1" s="850"/>
-      <c r="BT1" s="850"/>
-      <c r="BU1" s="850"/>
-      <c r="BV1" s="850"/>
+      <c r="BR1" s="837"/>
+      <c r="BS1" s="837"/>
+      <c r="BT1" s="837"/>
+      <c r="BU1" s="837"/>
+      <c r="BV1" s="837"/>
       <c r="BW1" s="53"/>
       <c r="BX1" s="54"/>
-      <c r="BY1" s="851" t="s">
+      <c r="BY1" s="838" t="s">
         <v>89</v>
       </c>
-      <c r="BZ1" s="852"/>
-      <c r="CA1" s="852"/>
-      <c r="CB1" s="852"/>
-      <c r="CC1" s="852"/>
-      <c r="CD1" s="852"/>
-      <c r="CE1" s="852"/>
-      <c r="CF1" s="853"/>
-      <c r="CG1" s="853"/>
-      <c r="CH1" s="853"/>
-      <c r="CI1" s="853"/>
-      <c r="CJ1" s="853"/>
-      <c r="CK1" s="853"/>
-      <c r="CL1" s="853"/>
-      <c r="CM1" s="853"/>
-      <c r="CN1" s="853"/>
-      <c r="CO1" s="853"/>
-      <c r="CP1" s="853"/>
-      <c r="CQ1" s="853"/>
+      <c r="BZ1" s="839"/>
+      <c r="CA1" s="839"/>
+      <c r="CB1" s="839"/>
+      <c r="CC1" s="839"/>
+      <c r="CD1" s="839"/>
+      <c r="CE1" s="839"/>
+      <c r="CF1" s="840"/>
+      <c r="CG1" s="840"/>
+      <c r="CH1" s="840"/>
+      <c r="CI1" s="840"/>
+      <c r="CJ1" s="840"/>
+      <c r="CK1" s="840"/>
+      <c r="CL1" s="840"/>
+      <c r="CM1" s="840"/>
+      <c r="CN1" s="840"/>
+      <c r="CO1" s="840"/>
+      <c r="CP1" s="840"/>
+      <c r="CQ1" s="840"/>
     </row>
     <row r="2" spans="1:95" s="658" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -58787,18 +58787,18 @@
       <c r="G2" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="854" t="s">
+      <c r="H2" s="841" t="s">
         <v>465</v>
       </c>
-      <c r="I2" s="855"/>
-      <c r="J2" s="855" t="s">
+      <c r="I2" s="842"/>
+      <c r="J2" s="842" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="855"/>
-      <c r="L2" s="855" t="s">
+      <c r="K2" s="842"/>
+      <c r="L2" s="842" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="856"/>
+      <c r="M2" s="843"/>
       <c r="N2" s="57" t="s">
         <v>90</v>
       </c>
@@ -58833,10 +58833,10 @@
         <v>103</v>
       </c>
       <c r="Y2" s="61" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="Z2" s="63" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="AA2" s="64" t="s">
         <v>106</v>
@@ -58869,10 +58869,10 @@
         <v>114</v>
       </c>
       <c r="AK2" s="67" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AL2" s="67" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="AM2" s="67" t="s">
         <v>115</v>
@@ -58907,36 +58907,36 @@
       <c r="AW2" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="AX2" s="857" t="s">
+      <c r="AX2" s="844" t="s">
         <v>125</v>
       </c>
-      <c r="AY2" s="858"/>
-      <c r="AZ2" s="858"/>
-      <c r="BA2" s="858" t="s">
+      <c r="AY2" s="845"/>
+      <c r="AZ2" s="845"/>
+      <c r="BA2" s="845" t="s">
         <v>126</v>
       </c>
-      <c r="BB2" s="858"/>
-      <c r="BC2" s="859"/>
-      <c r="BD2" s="862" t="s">
+      <c r="BB2" s="845"/>
+      <c r="BC2" s="846"/>
+      <c r="BD2" s="850" t="s">
         <v>125</v>
       </c>
-      <c r="BE2" s="863"/>
-      <c r="BF2" s="863"/>
-      <c r="BG2" s="863" t="s">
+      <c r="BE2" s="851"/>
+      <c r="BF2" s="851"/>
+      <c r="BG2" s="851" t="s">
         <v>126</v>
       </c>
-      <c r="BH2" s="863"/>
-      <c r="BI2" s="864"/>
-      <c r="BJ2" s="865" t="s">
+      <c r="BH2" s="851"/>
+      <c r="BI2" s="852"/>
+      <c r="BJ2" s="853" t="s">
         <v>125</v>
       </c>
-      <c r="BK2" s="866"/>
-      <c r="BL2" s="866"/>
-      <c r="BM2" s="866" t="s">
+      <c r="BK2" s="854"/>
+      <c r="BL2" s="854"/>
+      <c r="BM2" s="854" t="s">
         <v>126</v>
       </c>
-      <c r="BN2" s="867"/>
-      <c r="BO2" s="867"/>
+      <c r="BN2" s="855"/>
+      <c r="BO2" s="855"/>
       <c r="BP2" s="69" t="s">
         <v>127</v>
       </c>
@@ -59569,6 +59569,11 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -59584,11 +59589,6 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -59671,100 +59671,100 @@
         <v>167</v>
       </c>
       <c r="L1" s="145"/>
-      <c r="M1" s="877" t="s">
+      <c r="M1" s="900" t="s">
         <v>168</v>
       </c>
-      <c r="N1" s="878" t="s">
-        <v>522</v>
-      </c>
-      <c r="O1" s="879"/>
-      <c r="P1" s="879"/>
-      <c r="Q1" s="879"/>
-      <c r="R1" s="880" t="s">
+      <c r="N1" s="901" t="s">
+        <v>520</v>
+      </c>
+      <c r="O1" s="902"/>
+      <c r="P1" s="902"/>
+      <c r="Q1" s="902"/>
+      <c r="R1" s="903" t="s">
         <v>464</v>
       </c>
-      <c r="S1" s="881"/>
-      <c r="T1" s="881"/>
-      <c r="U1" s="881"/>
-      <c r="V1" s="881"/>
-      <c r="W1" s="881"/>
-      <c r="X1" s="882"/>
-      <c r="Y1" s="883" t="s">
+      <c r="S1" s="896"/>
+      <c r="T1" s="896"/>
+      <c r="U1" s="896"/>
+      <c r="V1" s="896"/>
+      <c r="W1" s="896"/>
+      <c r="X1" s="904"/>
+      <c r="Y1" s="890" t="s">
         <v>472</v>
       </c>
-      <c r="Z1" s="872"/>
-      <c r="AA1" s="886" t="s">
+      <c r="Z1" s="860"/>
+      <c r="AA1" s="905" t="s">
         <v>169</v>
       </c>
-      <c r="AB1" s="897" t="s">
+      <c r="AB1" s="878" t="s">
         <v>170</v>
       </c>
-      <c r="AC1" s="893" t="s">
+      <c r="AC1" s="892" t="s">
         <v>171</v>
       </c>
-      <c r="AD1" s="894"/>
-      <c r="AE1" s="894"/>
-      <c r="AF1" s="895"/>
-      <c r="AG1" s="896" t="s">
+      <c r="AD1" s="893"/>
+      <c r="AE1" s="893"/>
+      <c r="AF1" s="894"/>
+      <c r="AG1" s="895" t="s">
         <v>172</v>
       </c>
-      <c r="AH1" s="881"/>
-      <c r="AI1" s="881"/>
-      <c r="AJ1" s="881"/>
-      <c r="AK1" s="881"/>
-      <c r="AL1" s="881"/>
-      <c r="AM1" s="881"/>
-      <c r="AN1" s="881"/>
-      <c r="AO1" s="897" t="s">
+      <c r="AH1" s="896"/>
+      <c r="AI1" s="896"/>
+      <c r="AJ1" s="896"/>
+      <c r="AK1" s="896"/>
+      <c r="AL1" s="896"/>
+      <c r="AM1" s="896"/>
+      <c r="AN1" s="896"/>
+      <c r="AO1" s="878" t="s">
         <v>173</v>
       </c>
-      <c r="AP1" s="883" t="s">
+      <c r="AP1" s="890" t="s">
         <v>471</v>
       </c>
-      <c r="AQ1" s="872"/>
-      <c r="AR1" s="872"/>
-      <c r="AS1" s="873"/>
-      <c r="AT1" s="900" t="s">
+      <c r="AQ1" s="860"/>
+      <c r="AR1" s="860"/>
+      <c r="AS1" s="861"/>
+      <c r="AT1" s="898" t="s">
         <v>174</v>
       </c>
-      <c r="AU1" s="901"/>
-      <c r="AV1" s="901"/>
-      <c r="AW1" s="901"/>
-      <c r="AX1" s="901"/>
-      <c r="AY1" s="901"/>
-      <c r="AZ1" s="901"/>
-      <c r="BA1" s="901"/>
-      <c r="BB1" s="901"/>
-      <c r="BC1" s="901"/>
-      <c r="BD1" s="901"/>
-      <c r="BE1" s="901"/>
-      <c r="BF1" s="901"/>
-      <c r="BG1" s="901"/>
-      <c r="BH1" s="901"/>
-      <c r="BI1" s="901"/>
-      <c r="BJ1" s="901"/>
-      <c r="BK1" s="901"/>
-      <c r="BL1" s="901"/>
-      <c r="BM1" s="901"/>
-      <c r="BN1" s="901"/>
-      <c r="BO1" s="901"/>
-      <c r="BP1" s="901"/>
-      <c r="BQ1" s="901"/>
-      <c r="BR1" s="901"/>
-      <c r="BS1" s="901"/>
-      <c r="BT1" s="901"/>
-      <c r="BU1" s="901"/>
-      <c r="BV1" s="901"/>
-      <c r="BW1" s="897" t="s">
+      <c r="AU1" s="899"/>
+      <c r="AV1" s="899"/>
+      <c r="AW1" s="899"/>
+      <c r="AX1" s="899"/>
+      <c r="AY1" s="899"/>
+      <c r="AZ1" s="899"/>
+      <c r="BA1" s="899"/>
+      <c r="BB1" s="899"/>
+      <c r="BC1" s="899"/>
+      <c r="BD1" s="899"/>
+      <c r="BE1" s="899"/>
+      <c r="BF1" s="899"/>
+      <c r="BG1" s="899"/>
+      <c r="BH1" s="899"/>
+      <c r="BI1" s="899"/>
+      <c r="BJ1" s="899"/>
+      <c r="BK1" s="899"/>
+      <c r="BL1" s="899"/>
+      <c r="BM1" s="899"/>
+      <c r="BN1" s="899"/>
+      <c r="BO1" s="899"/>
+      <c r="BP1" s="899"/>
+      <c r="BQ1" s="899"/>
+      <c r="BR1" s="899"/>
+      <c r="BS1" s="899"/>
+      <c r="BT1" s="899"/>
+      <c r="BU1" s="899"/>
+      <c r="BV1" s="899"/>
+      <c r="BW1" s="878" t="s">
         <v>175</v>
       </c>
-      <c r="BX1" s="883" t="s">
+      <c r="BX1" s="890" t="s">
         <v>470</v>
       </c>
-      <c r="BY1" s="872"/>
-      <c r="BZ1" s="872"/>
-      <c r="CA1" s="873"/>
-      <c r="CB1" s="909" t="s">
+      <c r="BY1" s="860"/>
+      <c r="BZ1" s="860"/>
+      <c r="CA1" s="861"/>
+      <c r="CB1" s="889" t="s">
         <v>487</v>
       </c>
       <c r="CC1" s="891" t="s">
@@ -59782,16 +59782,16 @@
       <c r="CM1" s="891"/>
       <c r="CN1" s="891"/>
       <c r="CO1" s="146"/>
-      <c r="CP1" s="905" t="s">
+      <c r="CP1" s="877" t="s">
         <v>88</v>
       </c>
-      <c r="CQ1" s="842"/>
-      <c r="CR1" s="842"/>
-      <c r="CS1" s="842"/>
-      <c r="CT1" s="842"/>
-      <c r="CU1" s="842"/>
-      <c r="CV1" s="842"/>
-      <c r="CW1" s="861"/>
+      <c r="CQ1" s="848"/>
+      <c r="CR1" s="848"/>
+      <c r="CS1" s="848"/>
+      <c r="CT1" s="848"/>
+      <c r="CU1" s="848"/>
+      <c r="CV1" s="848"/>
+      <c r="CW1" s="849"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="147" t="s">
@@ -59830,7 +59830,7 @@
       <c r="L2" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="M2" s="877"/>
+      <c r="M2" s="900"/>
       <c r="N2" s="152" t="s">
         <v>180</v>
       </c>
@@ -59846,22 +59846,22 @@
       <c r="R2" s="157" t="s">
         <v>183</v>
       </c>
-      <c r="S2" s="888" t="s">
+      <c r="S2" s="907" t="s">
         <v>465</v>
       </c>
-      <c r="T2" s="867"/>
-      <c r="U2" s="889" t="s">
+      <c r="T2" s="855"/>
+      <c r="U2" s="908" t="s">
         <v>97</v>
       </c>
-      <c r="V2" s="889"/>
-      <c r="W2" s="889" t="s">
+      <c r="V2" s="908"/>
+      <c r="W2" s="908" t="s">
         <v>98</v>
       </c>
-      <c r="X2" s="890"/>
+      <c r="X2" s="909"/>
       <c r="Y2" s="884"/>
       <c r="Z2" s="885"/>
-      <c r="AA2" s="887"/>
-      <c r="AB2" s="898"/>
+      <c r="AA2" s="906"/>
+      <c r="AB2" s="879"/>
       <c r="AC2" s="153" t="s">
         <v>184</v>
       </c>
@@ -59874,81 +59874,81 @@
       <c r="AF2" s="153" t="s">
         <v>187</v>
       </c>
-      <c r="AG2" s="899" t="s">
+      <c r="AG2" s="897" t="s">
         <v>188</v>
       </c>
-      <c r="AH2" s="892"/>
-      <c r="AI2" s="892" t="s">
+      <c r="AH2" s="882"/>
+      <c r="AI2" s="882" t="s">
         <v>189</v>
       </c>
-      <c r="AJ2" s="892"/>
-      <c r="AK2" s="892" t="s">
+      <c r="AJ2" s="882"/>
+      <c r="AK2" s="882" t="s">
         <v>190</v>
       </c>
-      <c r="AL2" s="892"/>
+      <c r="AL2" s="882"/>
       <c r="AM2" s="154" t="s">
         <v>191</v>
       </c>
       <c r="AN2" s="154" t="s">
         <v>192</v>
       </c>
-      <c r="AO2" s="898"/>
+      <c r="AO2" s="879"/>
       <c r="AP2" s="884" t="s">
         <v>193</v>
       </c>
       <c r="AQ2" s="885"/>
-      <c r="AR2" s="902" t="s">
+      <c r="AR2" s="886" t="s">
         <v>194</v>
       </c>
-      <c r="AS2" s="903"/>
-      <c r="AT2" s="892" t="s">
+      <c r="AS2" s="887"/>
+      <c r="AT2" s="882" t="s">
         <v>195</v>
       </c>
-      <c r="AU2" s="892"/>
-      <c r="AV2" s="904" t="s">
+      <c r="AU2" s="882"/>
+      <c r="AV2" s="883" t="s">
         <v>196</v>
       </c>
-      <c r="AW2" s="904"/>
-      <c r="AX2" s="904" t="s">
+      <c r="AW2" s="883"/>
+      <c r="AX2" s="883" t="s">
         <v>197</v>
       </c>
-      <c r="AY2" s="904"/>
+      <c r="AY2" s="883"/>
       <c r="AZ2" s="154" t="s">
         <v>198</v>
       </c>
       <c r="BA2" s="154" t="s">
         <v>199</v>
       </c>
-      <c r="BB2" s="892" t="s">
+      <c r="BB2" s="882" t="s">
         <v>200</v>
       </c>
-      <c r="BC2" s="892"/>
-      <c r="BD2" s="904" t="s">
+      <c r="BC2" s="882"/>
+      <c r="BD2" s="883" t="s">
         <v>201</v>
       </c>
-      <c r="BE2" s="904"/>
-      <c r="BF2" s="904" t="s">
+      <c r="BE2" s="883"/>
+      <c r="BF2" s="883" t="s">
         <v>202</v>
       </c>
-      <c r="BG2" s="904"/>
+      <c r="BG2" s="883"/>
       <c r="BH2" s="154" t="s">
         <v>203</v>
       </c>
       <c r="BI2" s="154" t="s">
         <v>204</v>
       </c>
-      <c r="BJ2" s="892" t="s">
+      <c r="BJ2" s="882" t="s">
         <v>205</v>
       </c>
-      <c r="BK2" s="892"/>
-      <c r="BL2" s="904" t="s">
+      <c r="BK2" s="882"/>
+      <c r="BL2" s="883" t="s">
         <v>206</v>
       </c>
-      <c r="BM2" s="904"/>
-      <c r="BN2" s="904" t="s">
+      <c r="BM2" s="883"/>
+      <c r="BN2" s="883" t="s">
         <v>207</v>
       </c>
-      <c r="BO2" s="904"/>
+      <c r="BO2" s="883"/>
       <c r="BP2" s="154" t="s">
         <v>208</v>
       </c>
@@ -59970,16 +59970,16 @@
       <c r="BV2" s="154" t="s">
         <v>214</v>
       </c>
-      <c r="BW2" s="898"/>
+      <c r="BW2" s="879"/>
       <c r="BX2" s="884" t="s">
         <v>193</v>
       </c>
       <c r="BY2" s="885"/>
-      <c r="BZ2" s="902" t="s">
+      <c r="BZ2" s="886" t="s">
         <v>194</v>
       </c>
-      <c r="CA2" s="903"/>
-      <c r="CB2" s="909"/>
+      <c r="CA2" s="887"/>
+      <c r="CB2" s="889"/>
       <c r="CC2" s="138" t="s">
         <v>106</v>
       </c>
@@ -60008,10 +60008,10 @@
         <v>35</v>
       </c>
       <c r="CL2" s="140" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="CM2" s="140" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="CN2" s="140" t="s">
         <v>44</v>
@@ -60019,22 +60019,22 @@
       <c r="CO2" s="140" t="s">
         <v>473</v>
       </c>
-      <c r="CP2" s="908" t="s">
+      <c r="CP2" s="888" t="s">
         <v>216</v>
       </c>
-      <c r="CQ2" s="906"/>
-      <c r="CR2" s="906" t="s">
+      <c r="CQ2" s="880"/>
+      <c r="CR2" s="880" t="s">
         <v>217</v>
       </c>
-      <c r="CS2" s="906"/>
-      <c r="CT2" s="906" t="s">
+      <c r="CS2" s="880"/>
+      <c r="CT2" s="880" t="s">
         <v>218</v>
       </c>
-      <c r="CU2" s="906"/>
-      <c r="CV2" s="906" t="s">
+      <c r="CU2" s="880"/>
+      <c r="CV2" s="880" t="s">
         <v>219</v>
       </c>
-      <c r="CW2" s="907"/>
+      <c r="CW2" s="881"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="168"/>
@@ -60899,6 +60899,29 @@
     </sortState>
   </autoFilter>
   <mergeCells count="39">
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="CC1:CN1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AN1"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
     <mergeCell ref="CP1:CW1"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="CV2:CW2"/>
@@ -60915,29 +60938,6 @@
     <mergeCell ref="CT2:CU2"/>
     <mergeCell ref="CB1:CB2"/>
     <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CC1:CN1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AN1"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -60980,72 +60980,72 @@
       <c r="K1" s="144"/>
       <c r="L1" s="145"/>
       <c r="M1" s="695"/>
-      <c r="N1" s="913"/>
-      <c r="O1" s="914"/>
-      <c r="P1" s="914"/>
-      <c r="Q1" s="914"/>
-      <c r="R1" s="880"/>
-      <c r="S1" s="881"/>
-      <c r="T1" s="881"/>
-      <c r="U1" s="881"/>
-      <c r="V1" s="881"/>
-      <c r="W1" s="881"/>
-      <c r="X1" s="882"/>
-      <c r="Y1" s="883"/>
-      <c r="Z1" s="872"/>
+      <c r="N1" s="910"/>
+      <c r="O1" s="911"/>
+      <c r="P1" s="911"/>
+      <c r="Q1" s="911"/>
+      <c r="R1" s="903"/>
+      <c r="S1" s="896"/>
+      <c r="T1" s="896"/>
+      <c r="U1" s="896"/>
+      <c r="V1" s="896"/>
+      <c r="W1" s="896"/>
+      <c r="X1" s="904"/>
+      <c r="Y1" s="890"/>
+      <c r="Z1" s="860"/>
       <c r="AA1" s="696"/>
       <c r="AB1" s="694"/>
-      <c r="AC1" s="893"/>
-      <c r="AD1" s="894"/>
-      <c r="AE1" s="894"/>
-      <c r="AF1" s="895"/>
-      <c r="AG1" s="896"/>
-      <c r="AH1" s="881"/>
-      <c r="AI1" s="881"/>
-      <c r="AJ1" s="881"/>
-      <c r="AK1" s="881"/>
-      <c r="AL1" s="881"/>
-      <c r="AM1" s="881"/>
-      <c r="AN1" s="881"/>
+      <c r="AC1" s="892"/>
+      <c r="AD1" s="893"/>
+      <c r="AE1" s="893"/>
+      <c r="AF1" s="894"/>
+      <c r="AG1" s="895"/>
+      <c r="AH1" s="896"/>
+      <c r="AI1" s="896"/>
+      <c r="AJ1" s="896"/>
+      <c r="AK1" s="896"/>
+      <c r="AL1" s="896"/>
+      <c r="AM1" s="896"/>
+      <c r="AN1" s="896"/>
       <c r="AO1" s="694"/>
-      <c r="AP1" s="883"/>
-      <c r="AQ1" s="872"/>
-      <c r="AR1" s="872"/>
-      <c r="AS1" s="873"/>
-      <c r="AT1" s="900"/>
-      <c r="AU1" s="901"/>
-      <c r="AV1" s="901"/>
-      <c r="AW1" s="901"/>
-      <c r="AX1" s="901"/>
-      <c r="AY1" s="901"/>
-      <c r="AZ1" s="901"/>
-      <c r="BA1" s="901"/>
-      <c r="BB1" s="901"/>
-      <c r="BC1" s="901"/>
-      <c r="BD1" s="901"/>
-      <c r="BE1" s="901"/>
-      <c r="BF1" s="901"/>
-      <c r="BG1" s="901"/>
-      <c r="BH1" s="901"/>
-      <c r="BI1" s="901"/>
-      <c r="BJ1" s="901"/>
-      <c r="BK1" s="901"/>
-      <c r="BL1" s="901"/>
-      <c r="BM1" s="901"/>
-      <c r="BN1" s="901"/>
-      <c r="BO1" s="901"/>
-      <c r="BP1" s="901"/>
-      <c r="BQ1" s="901"/>
-      <c r="BR1" s="901"/>
-      <c r="BS1" s="901"/>
-      <c r="BT1" s="901"/>
-      <c r="BU1" s="901"/>
-      <c r="BV1" s="901"/>
+      <c r="AP1" s="890"/>
+      <c r="AQ1" s="860"/>
+      <c r="AR1" s="860"/>
+      <c r="AS1" s="861"/>
+      <c r="AT1" s="898"/>
+      <c r="AU1" s="899"/>
+      <c r="AV1" s="899"/>
+      <c r="AW1" s="899"/>
+      <c r="AX1" s="899"/>
+      <c r="AY1" s="899"/>
+      <c r="AZ1" s="899"/>
+      <c r="BA1" s="899"/>
+      <c r="BB1" s="899"/>
+      <c r="BC1" s="899"/>
+      <c r="BD1" s="899"/>
+      <c r="BE1" s="899"/>
+      <c r="BF1" s="899"/>
+      <c r="BG1" s="899"/>
+      <c r="BH1" s="899"/>
+      <c r="BI1" s="899"/>
+      <c r="BJ1" s="899"/>
+      <c r="BK1" s="899"/>
+      <c r="BL1" s="899"/>
+      <c r="BM1" s="899"/>
+      <c r="BN1" s="899"/>
+      <c r="BO1" s="899"/>
+      <c r="BP1" s="899"/>
+      <c r="BQ1" s="899"/>
+      <c r="BR1" s="899"/>
+      <c r="BS1" s="899"/>
+      <c r="BT1" s="899"/>
+      <c r="BU1" s="899"/>
+      <c r="BV1" s="899"/>
       <c r="BW1" s="694"/>
-      <c r="BX1" s="883"/>
-      <c r="BY1" s="872"/>
-      <c r="BZ1" s="872"/>
-      <c r="CA1" s="873"/>
+      <c r="BX1" s="890"/>
+      <c r="BY1" s="860"/>
+      <c r="BZ1" s="860"/>
+      <c r="CA1" s="861"/>
       <c r="CB1" s="891"/>
       <c r="CC1" s="891"/>
       <c r="CD1" s="891"/>
@@ -61059,31 +61059,26 @@
       <c r="CL1" s="891"/>
       <c r="CM1" s="891"/>
       <c r="CN1" s="693"/>
-      <c r="CO1" s="905"/>
-      <c r="CP1" s="842"/>
-      <c r="CQ1" s="842"/>
-      <c r="CR1" s="842"/>
-      <c r="CS1" s="842"/>
-      <c r="CT1" s="842"/>
-      <c r="CU1" s="842"/>
-      <c r="CV1" s="861"/>
-      <c r="CW1" s="910"/>
-      <c r="CX1" s="911"/>
-      <c r="CY1" s="911"/>
-      <c r="CZ1" s="912"/>
-      <c r="DA1" s="911"/>
-      <c r="DB1" s="911"/>
-      <c r="DC1" s="912"/>
-      <c r="DD1" s="911"/>
-      <c r="DE1" s="911"/>
+      <c r="CO1" s="877"/>
+      <c r="CP1" s="848"/>
+      <c r="CQ1" s="848"/>
+      <c r="CR1" s="848"/>
+      <c r="CS1" s="848"/>
+      <c r="CT1" s="848"/>
+      <c r="CU1" s="848"/>
+      <c r="CV1" s="849"/>
+      <c r="CW1" s="912"/>
+      <c r="CX1" s="913"/>
+      <c r="CY1" s="913"/>
+      <c r="CZ1" s="914"/>
+      <c r="DA1" s="913"/>
+      <c r="DB1" s="913"/>
+      <c r="DC1" s="914"/>
+      <c r="DD1" s="913"/>
+      <c r="DE1" s="913"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="CZ1:DB1"/>
     <mergeCell ref="DC1:DE1"/>
@@ -61092,6 +61087,11 @@
     <mergeCell ref="AG1:AN1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CB1:CM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -61228,10 +61228,10 @@
       <c r="B2" s="203" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="924" t="s">
+      <c r="C2" s="926" t="s">
         <v>240</v>
       </c>
-      <c r="D2" s="924"/>
+      <c r="D2" s="926"/>
       <c r="E2" s="201"/>
       <c r="F2" s="201"/>
       <c r="G2" s="201"/>
@@ -61379,7 +61379,7 @@
       <c r="S6" s="201"/>
       <c r="T6" s="201"/>
       <c r="U6" s="214" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="V6" s="372"/>
       <c r="W6" s="372"/>
@@ -61390,40 +61390,40 @@
       <c r="Z6" s="372"/>
       <c r="AA6" s="372"/>
       <c r="AB6" s="377" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="200"/>
-      <c r="B7" s="921"/>
-      <c r="C7" s="921"/>
-      <c r="D7" s="921"/>
+      <c r="B7" s="927"/>
+      <c r="C7" s="927"/>
+      <c r="D7" s="927"/>
       <c r="E7" s="201"/>
       <c r="F7" s="201"/>
       <c r="G7" s="201"/>
       <c r="H7" s="201"/>
       <c r="I7" s="201"/>
-      <c r="J7" s="921"/>
-      <c r="K7" s="921"/>
-      <c r="L7" s="921"/>
+      <c r="J7" s="927"/>
+      <c r="K7" s="927"/>
+      <c r="L7" s="927"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="201"/>
       <c r="P7" s="202" t="s">
         <v>243</v>
       </c>
-      <c r="Q7" s="921"/>
-      <c r="R7" s="921"/>
-      <c r="S7" s="921"/>
+      <c r="Q7" s="927"/>
+      <c r="R7" s="927"/>
+      <c r="S7" s="927"/>
       <c r="T7" s="201"/>
       <c r="U7" s="215"/>
       <c r="V7" s="372"/>
       <c r="W7" s="372" t="s">
         <v>243</v>
       </c>
-      <c r="X7" s="921"/>
-      <c r="Y7" s="921"/>
-      <c r="Z7" s="921"/>
+      <c r="X7" s="927"/>
+      <c r="Y7" s="927"/>
+      <c r="Z7" s="927"/>
       <c r="AA7" s="372"/>
       <c r="AB7" s="215"/>
     </row>
@@ -61549,7 +61549,7 @@
       <c r="O10" s="201"/>
       <c r="P10" s="201"/>
       <c r="Q10" s="217" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="R10" s="218" t="s">
         <v>69</v>
@@ -61566,7 +61566,7 @@
       <c r="V10" s="372"/>
       <c r="W10" s="372"/>
       <c r="X10" s="217" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="Y10" s="218" t="s">
         <v>69</v>
@@ -61600,10 +61600,10 @@
       </c>
       <c r="K11" s="201"/>
       <c r="L11" s="201"/>
-      <c r="M11" s="926" t="s">
+      <c r="M11" s="924" t="s">
         <v>249</v>
       </c>
-      <c r="N11" s="927"/>
+      <c r="N11" s="925"/>
       <c r="O11" s="222"/>
       <c r="P11" s="222"/>
       <c r="Q11" s="220" t="s">
@@ -62323,7 +62323,7 @@
       <c r="K30" s="302"/>
       <c r="L30" s="249"/>
       <c r="M30" s="919" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="N30" s="920"/>
       <c r="O30" s="240"/>
@@ -62785,11 +62785,11 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="200"/>
-      <c r="B42" s="925"/>
-      <c r="C42" s="925"/>
-      <c r="D42" s="925"/>
-      <c r="E42" s="925"/>
-      <c r="F42" s="925"/>
+      <c r="B42" s="921"/>
+      <c r="C42" s="921"/>
+      <c r="D42" s="921"/>
+      <c r="E42" s="921"/>
+      <c r="F42" s="921"/>
       <c r="G42" s="240"/>
       <c r="H42" s="201"/>
       <c r="I42" s="240"/>
@@ -62976,6 +62976,21 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="26">
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -62987,21 +63002,6 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA20:AB20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
fix on agglo compliance sheet
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
@@ -35,7 +35,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'5(4)-areas'!$A$3:$Q$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Agglo Compliance'!$A$4:$L$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Agglo Compliance'!$A$4:$O$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'agglomeration debug level'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'agglomeration level'!$A$4:$CW$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">Agglomerationout!$A$5:$D$5</definedName>
@@ -2322,7 +2322,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\/mm\/dd"/>
     <numFmt numFmtId="168" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2616,6 +2616,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -5718,9 +5725,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5752,6 +5756,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5788,9 +5831,6 @@
     <xf numFmtId="3" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5839,140 +5879,113 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5980,15 +5993,6 @@
     <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6001,26 +6005,26 @@
     <xf numFmtId="0" fontId="25" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6050,6 +6054,39 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -6077,40 +6114,10 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6135,84 +6142,84 @@
     <xf numFmtId="3" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="45" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6524,6 +6531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -6912,6 +6920,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil10"/>
   <dimension ref="B2:F81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6937,8 +6946,8 @@
       <c r="B3" s="324" t="s">
         <v>239</v>
       </c>
-      <c r="C3" s="926"/>
-      <c r="D3" s="926"/>
+      <c r="C3" s="925"/>
+      <c r="D3" s="925"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C4" s="325"/>
@@ -6971,10 +6980,10 @@
       <c r="D10" s="332" t="s">
         <v>278</v>
       </c>
-      <c r="E10" s="927" t="s">
+      <c r="E10" s="926" t="s">
         <v>530</v>
       </c>
-      <c r="F10" s="928"/>
+      <c r="F10" s="927"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="333" t="s">
@@ -7129,10 +7138,10 @@
       <c r="D30" s="342" t="s">
         <v>278</v>
       </c>
-      <c r="E30" s="927" t="s">
+      <c r="E30" s="926" t="s">
         <v>530</v>
       </c>
-      <c r="F30" s="928"/>
+      <c r="F30" s="927"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="333" t="s">
@@ -7284,10 +7293,10 @@
       <c r="D49" s="342" t="s">
         <v>278</v>
       </c>
-      <c r="E49" s="927" t="s">
+      <c r="E49" s="926" t="s">
         <v>530</v>
       </c>
-      <c r="F49" s="928"/>
+      <c r="F49" s="927"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="333" t="s">
@@ -7439,10 +7448,10 @@
       <c r="D68" s="342" t="s">
         <v>278</v>
       </c>
-      <c r="E68" s="927" t="s">
+      <c r="E68" s="926" t="s">
         <v>530</v>
       </c>
-      <c r="F68" s="928"/>
+      <c r="F68" s="927"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="504" t="s">
@@ -7584,6 +7593,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil11"/>
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7616,8 +7626,8 @@
       </c>
       <c r="C2" s="373"/>
       <c r="D2" s="373"/>
-      <c r="E2" s="924"/>
-      <c r="F2" s="924"/>
+      <c r="E2" s="921"/>
+      <c r="F2" s="921"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="372"/>
@@ -7649,13 +7659,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="370"/>
-      <c r="B6" s="925" t="s">
+      <c r="B6" s="918" t="s">
         <v>452</v>
       </c>
-      <c r="C6" s="925"/>
-      <c r="D6" s="925"/>
-      <c r="E6" s="925"/>
-      <c r="F6" s="925"/>
+      <c r="C6" s="918"/>
+      <c r="D6" s="918"/>
+      <c r="E6" s="918"/>
+      <c r="F6" s="918"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="370"/>
@@ -7670,14 +7680,14 @@
       <c r="B8" s="399" t="s">
         <v>484</v>
       </c>
-      <c r="C8" s="929" t="s">
+      <c r="C8" s="928" t="s">
         <v>244</v>
       </c>
-      <c r="D8" s="930"/>
-      <c r="E8" s="929" t="s">
+      <c r="D8" s="929"/>
+      <c r="E8" s="928" t="s">
         <v>245</v>
       </c>
-      <c r="F8" s="930"/>
+      <c r="F8" s="929"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="370"/>
@@ -7813,11 +7823,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="370"/>
-      <c r="B22" s="919"/>
-      <c r="C22" s="919"/>
-      <c r="D22" s="919"/>
-      <c r="E22" s="919"/>
-      <c r="F22" s="919"/>
+      <c r="B22" s="922"/>
+      <c r="C22" s="922"/>
+      <c r="D22" s="922"/>
+      <c r="E22" s="922"/>
+      <c r="F22" s="922"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="370"/>
@@ -7872,6 +7882,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil12"/>
   <dimension ref="A2:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7888,13 +7899,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="931" t="s">
+      <c r="B2" s="930" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="932" t="s">
+      <c r="C2" s="931" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="932" t="s">
+      <c r="D2" s="931" t="s">
         <v>178</v>
       </c>
       <c r="E2" s="424" t="s">
@@ -7929,9 +7940,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="931"/>
-      <c r="C3" s="933"/>
-      <c r="D3" s="933"/>
+      <c r="B3" s="930"/>
+      <c r="C3" s="932"/>
+      <c r="D3" s="932"/>
       <c r="E3" s="439" t="s">
         <v>296</v>
       </c>
@@ -7964,7 +7975,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="934" t="s">
+      <c r="B4" s="933" t="s">
         <v>299</v>
       </c>
       <c r="C4" s="425" t="s">
@@ -7983,7 +7994,7 @@
       <c r="N4" s="427"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="934"/>
+      <c r="B5" s="933"/>
       <c r="C5" s="425" t="s">
         <v>93</v>
       </c>
@@ -8000,7 +8011,7 @@
       <c r="N5" s="427"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="935"/>
+      <c r="B6" s="934"/>
       <c r="C6" s="435" t="s">
         <v>289</v>
       </c>
@@ -8092,6 +8103,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil13"/>
   <dimension ref="A1:Y55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8114,43 +8126,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="948" t="s">
+      <c r="A1" s="938" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="949"/>
+      <c r="B1" s="939"/>
       <c r="C1" s="455"/>
-      <c r="D1" s="939" t="s">
+      <c r="D1" s="949" t="s">
         <v>300</v>
       </c>
-      <c r="E1" s="940"/>
-      <c r="F1" s="940"/>
-      <c r="G1" s="940"/>
-      <c r="H1" s="940"/>
-      <c r="I1" s="941"/>
-      <c r="J1" s="950" t="s">
+      <c r="E1" s="950"/>
+      <c r="F1" s="950"/>
+      <c r="G1" s="950"/>
+      <c r="H1" s="950"/>
+      <c r="I1" s="951"/>
+      <c r="J1" s="940" t="s">
         <v>301</v>
       </c>
-      <c r="K1" s="951"/>
-      <c r="L1" s="951"/>
-      <c r="M1" s="951"/>
-      <c r="N1" s="952"/>
-      <c r="O1" s="953" t="s">
+      <c r="K1" s="941"/>
+      <c r="L1" s="941"/>
+      <c r="M1" s="941"/>
+      <c r="N1" s="942"/>
+      <c r="O1" s="943" t="s">
         <v>302</v>
       </c>
-      <c r="P1" s="954"/>
-      <c r="Q1" s="955"/>
+      <c r="P1" s="944"/>
+      <c r="Q1" s="945"/>
       <c r="R1" s="442" t="s">
         <v>81</v>
       </c>
       <c r="S1" s="443"/>
-      <c r="T1" s="947" t="s">
+      <c r="T1" s="937" t="s">
         <v>495</v>
       </c>
-      <c r="U1" s="947"/>
-      <c r="V1" s="947"/>
-      <c r="W1" s="947"/>
-      <c r="X1" s="947"/>
-      <c r="Y1" s="947"/>
+      <c r="U1" s="937"/>
+      <c r="V1" s="937"/>
+      <c r="W1" s="937"/>
+      <c r="X1" s="937"/>
+      <c r="Y1" s="937"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="445" t="s">
@@ -8162,18 +8174,18 @@
       <c r="C2" s="446" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="944" t="s">
+      <c r="D2" s="954" t="s">
         <v>304</v>
       </c>
-      <c r="E2" s="943"/>
-      <c r="F2" s="943" t="s">
+      <c r="E2" s="953"/>
+      <c r="F2" s="953" t="s">
         <v>305</v>
       </c>
-      <c r="G2" s="943"/>
-      <c r="H2" s="942" t="s">
+      <c r="G2" s="953"/>
+      <c r="H2" s="952" t="s">
         <v>306</v>
       </c>
-      <c r="I2" s="942"/>
+      <c r="I2" s="952"/>
       <c r="J2" s="447">
         <v>0</v>
       </c>
@@ -8204,18 +8216,18 @@
       <c r="S2" s="681" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="945" t="s">
+      <c r="T2" s="935" t="s">
         <v>464</v>
       </c>
-      <c r="U2" s="945"/>
-      <c r="V2" s="946" t="s">
+      <c r="U2" s="935"/>
+      <c r="V2" s="936" t="s">
         <v>481</v>
       </c>
-      <c r="W2" s="946"/>
-      <c r="X2" s="946" t="s">
+      <c r="W2" s="936"/>
+      <c r="X2" s="936" t="s">
         <v>482</v>
       </c>
-      <c r="Y2" s="946"/>
+      <c r="Y2" s="936"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="450"/>
@@ -8241,13 +8253,13 @@
       <c r="I3" s="665" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="936" t="s">
+      <c r="J3" s="946" t="s">
         <v>311</v>
       </c>
-      <c r="K3" s="937"/>
-      <c r="L3" s="937"/>
-      <c r="M3" s="937"/>
-      <c r="N3" s="938"/>
+      <c r="K3" s="947"/>
+      <c r="L3" s="947"/>
+      <c r="M3" s="947"/>
+      <c r="N3" s="948"/>
       <c r="O3" s="458"/>
       <c r="P3" s="458"/>
       <c r="Q3" s="458"/>
@@ -9476,6 +9488,11 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:X4"/>
   <mergeCells count="12">
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -9483,11 +9500,6 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9496,6 +9508,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil14"/>
   <dimension ref="A1:CC22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9527,14 +9540,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="865" t="s">
+      <c r="A1" s="835" t="s">
         <v>312</v>
       </c>
-      <c r="B1" s="866"/>
-      <c r="C1" s="866"/>
-      <c r="D1" s="866"/>
-      <c r="E1" s="866"/>
-      <c r="F1" s="866"/>
+      <c r="B1" s="836"/>
+      <c r="C1" s="836"/>
+      <c r="D1" s="836"/>
+      <c r="E1" s="836"/>
+      <c r="F1" s="836"/>
       <c r="G1" s="472"/>
       <c r="H1" s="961" t="s">
         <v>169</v>
@@ -9575,8 +9588,8 @@
       <c r="AF1" s="958" t="s">
         <v>480</v>
       </c>
-      <c r="AG1" s="947"/>
-      <c r="AH1" s="947"/>
+      <c r="AG1" s="937"/>
+      <c r="AH1" s="937"/>
       <c r="AI1" s="688"/>
       <c r="AJ1" s="688"/>
       <c r="AK1" s="688"/>
@@ -9644,46 +9657,46 @@
       </c>
       <c r="G2" s="957"/>
       <c r="H2" s="468"/>
-      <c r="I2" s="956" t="s">
+      <c r="I2" s="955" t="s">
         <v>188</v>
       </c>
-      <c r="J2" s="956"/>
-      <c r="K2" s="956" t="s">
+      <c r="J2" s="955"/>
+      <c r="K2" s="955" t="s">
         <v>189</v>
       </c>
-      <c r="L2" s="956"/>
-      <c r="M2" s="956" t="s">
+      <c r="L2" s="955"/>
+      <c r="M2" s="955" t="s">
         <v>190</v>
       </c>
-      <c r="N2" s="965"/>
+      <c r="N2" s="956"/>
       <c r="O2" s="960"/>
       <c r="P2" s="469"/>
-      <c r="Q2" s="956" t="s">
+      <c r="Q2" s="955" t="s">
         <v>188</v>
       </c>
-      <c r="R2" s="956"/>
-      <c r="S2" s="956" t="s">
+      <c r="R2" s="955"/>
+      <c r="S2" s="955" t="s">
         <v>189</v>
       </c>
-      <c r="T2" s="956"/>
-      <c r="U2" s="956" t="s">
+      <c r="T2" s="955"/>
+      <c r="U2" s="955" t="s">
         <v>190</v>
       </c>
-      <c r="V2" s="965"/>
+      <c r="V2" s="956"/>
       <c r="W2" s="960"/>
       <c r="X2" s="469"/>
-      <c r="Y2" s="956" t="s">
+      <c r="Y2" s="955" t="s">
         <v>188</v>
       </c>
-      <c r="Z2" s="956"/>
-      <c r="AA2" s="956" t="s">
+      <c r="Z2" s="955"/>
+      <c r="AA2" s="955" t="s">
         <v>189</v>
       </c>
-      <c r="AB2" s="956"/>
-      <c r="AC2" s="956" t="s">
+      <c r="AB2" s="955"/>
+      <c r="AC2" s="955" t="s">
         <v>190</v>
       </c>
-      <c r="AD2" s="965"/>
+      <c r="AD2" s="956"/>
       <c r="AE2" s="960"/>
       <c r="AF2" s="682" t="s">
         <v>464</v>
@@ -10570,11 +10583,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:AH4"/>
   <mergeCells count="18">
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="A1:F1"/>
@@ -10588,6 +10596,11 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10595,6 +10608,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil15"/>
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
@@ -10775,6 +10789,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil16"/>
   <dimension ref="A1:U179"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -10802,9 +10817,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="984"/>
-      <c r="B1" s="855"/>
-      <c r="C1" s="855"/>
+      <c r="A1" s="965"/>
+      <c r="B1" s="866"/>
+      <c r="C1" s="866"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="740"/>
@@ -10819,21 +10834,21 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="988" t="s">
+      <c r="A3" s="973" t="s">
         <v>345</v>
       </c>
-      <c r="B3" s="990" t="s">
+      <c r="B3" s="975" t="s">
         <v>453</v>
       </c>
-      <c r="C3" s="991"/>
-      <c r="D3" s="976" t="s">
+      <c r="C3" s="976"/>
+      <c r="D3" s="971" t="s">
         <v>454</v>
       </c>
-      <c r="E3" s="977"/>
-      <c r="F3" s="976" t="s">
+      <c r="E3" s="972"/>
+      <c r="F3" s="971" t="s">
         <v>488</v>
       </c>
-      <c r="G3" s="977"/>
+      <c r="G3" s="972"/>
       <c r="I3" s="738" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
@@ -10844,14 +10859,14 @@
       <c r="K3" s="720"/>
       <c r="L3" s="720"/>
       <c r="N3" s="705"/>
-      <c r="O3" s="973" t="s">
+      <c r="O3" s="987" t="s">
         <v>346</v>
       </c>
-      <c r="P3" s="973"/>
-      <c r="Q3" s="973" t="s">
+      <c r="P3" s="987"/>
+      <c r="Q3" s="987" t="s">
         <v>347</v>
       </c>
-      <c r="R3" s="973"/>
+      <c r="R3" s="987"/>
       <c r="S3" s="705"/>
       <c r="T3" s="713" t="s">
         <v>348</v>
@@ -10859,7 +10874,7 @@
       <c r="U3" s="705"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="989"/>
+      <c r="A4" s="974"/>
       <c r="B4" s="512" t="s">
         <v>349</v>
       </c>
@@ -11118,14 +11133,14 @@
       <c r="K10" s="720"/>
       <c r="L10" s="720"/>
       <c r="N10" s="713"/>
-      <c r="O10" s="973" t="s">
+      <c r="O10" s="987" t="s">
         <v>349</v>
       </c>
-      <c r="P10" s="973"/>
-      <c r="Q10" s="973" t="s">
+      <c r="P10" s="987"/>
+      <c r="Q10" s="987" t="s">
         <v>356</v>
       </c>
-      <c r="R10" s="973"/>
+      <c r="R10" s="987"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I11" s="738" t="str">
@@ -11189,7 +11204,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="988" t="s">
+      <c r="A13" s="973" t="s">
         <v>357</v>
       </c>
       <c r="B13" s="511" t="str">
@@ -11235,7 +11250,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="989"/>
+      <c r="A14" s="974"/>
       <c r="B14" s="514" t="s">
         <v>350</v>
       </c>
@@ -11365,34 +11380,34 @@
       <c r="A21" s="502" t="s">
         <v>362</v>
       </c>
-      <c r="B21" s="978" t="s">
+      <c r="B21" s="988" t="s">
         <v>507</v>
       </c>
-      <c r="C21" s="979"/>
-      <c r="D21" s="979"/>
-      <c r="E21" s="979"/>
-      <c r="F21" s="979"/>
-      <c r="G21" s="979"/>
+      <c r="C21" s="989"/>
+      <c r="D21" s="989"/>
+      <c r="E21" s="989"/>
+      <c r="F21" s="989"/>
+      <c r="G21" s="989"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="516" t="s">
         <v>326</v>
       </c>
-      <c r="B22" s="980" t="str">
+      <c r="B22" s="977" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="981"/>
-      <c r="D22" s="980" t="str">
+      <c r="C22" s="978"/>
+      <c r="D22" s="977" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="981"/>
-      <c r="F22" s="980" t="str">
+      <c r="E22" s="978"/>
+      <c r="F22" s="977" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="981"/>
+      <c r="G22" s="978"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="517"/>
@@ -11819,21 +11834,21 @@
       <c r="A41" s="519" t="s">
         <v>372</v>
       </c>
-      <c r="B41" s="986" t="str">
+      <c r="B41" s="967" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="987"/>
-      <c r="D41" s="974" t="str">
+      <c r="C41" s="968"/>
+      <c r="D41" s="969" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="975"/>
-      <c r="F41" s="974" t="str">
+      <c r="E41" s="970"/>
+      <c r="F41" s="969" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G41" s="975"/>
+      <c r="G41" s="970"/>
       <c r="N41" s="705"/>
       <c r="O41" s="732" t="s">
         <v>458</v>
@@ -12047,11 +12062,11 @@
       <c r="F53" s="710" t="s">
         <v>513</v>
       </c>
-      <c r="H53" s="966" t="s">
+      <c r="H53" s="990" t="s">
         <v>500</v>
       </c>
-      <c r="I53" s="966"/>
-      <c r="J53" s="966"/>
+      <c r="I53" s="990"/>
+      <c r="J53" s="990"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="701" t="s">
@@ -12221,11 +12236,11 @@
       <c r="F63" s="710" t="s">
         <v>513</v>
       </c>
-      <c r="H63" s="966" t="s">
+      <c r="H63" s="990" t="s">
         <v>514</v>
       </c>
-      <c r="I63" s="966"/>
-      <c r="J63" s="966"/>
+      <c r="I63" s="990"/>
+      <c r="J63" s="990"/>
       <c r="L63" s="708"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -12412,12 +12427,12 @@
       <c r="A74" s="623" t="s">
         <v>371</v>
       </c>
-      <c r="B74" s="985" t="s">
+      <c r="B74" s="966" t="s">
         <v>455</v>
       </c>
-      <c r="C74" s="985"/>
-      <c r="D74" s="985"/>
-      <c r="E74" s="985"/>
+      <c r="C74" s="966"/>
+      <c r="D74" s="966"/>
+      <c r="E74" s="966"/>
       <c r="I74" s="709"/>
       <c r="J74" s="709"/>
       <c r="K74" s="709"/>
@@ -12733,36 +12748,36 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="971" t="str">
+      <c r="B85" s="981" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="972"/>
-      <c r="D85" s="971" t="str">
+      <c r="C85" s="982"/>
+      <c r="D85" s="981" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="972"/>
-      <c r="F85" s="971" t="str">
+      <c r="E85" s="982"/>
+      <c r="F85" s="981" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="972"/>
+      <c r="G85" s="982"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="503"/>
-      <c r="B86" s="927" t="s">
+      <c r="B86" s="926" t="s">
         <v>279</v>
       </c>
-      <c r="C86" s="928"/>
-      <c r="D86" s="927" t="s">
+      <c r="C86" s="927"/>
+      <c r="D86" s="926" t="s">
         <v>279</v>
       </c>
-      <c r="E86" s="928"/>
-      <c r="F86" s="927" t="s">
+      <c r="E86" s="927"/>
+      <c r="F86" s="926" t="s">
         <v>279</v>
       </c>
-      <c r="G86" s="928"/>
+      <c r="G86" s="927"/>
       <c r="N86" s="713" t="s">
         <v>398</v>
       </c>
@@ -13043,36 +13058,36 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="971" t="str">
+      <c r="B101" s="981" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="972"/>
-      <c r="D101" s="971" t="str">
+      <c r="C101" s="982"/>
+      <c r="D101" s="981" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="972"/>
-      <c r="F101" s="971" t="str">
+      <c r="E101" s="982"/>
+      <c r="F101" s="981" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="972"/>
+      <c r="G101" s="982"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="503"/>
-      <c r="B102" s="927" t="s">
+      <c r="B102" s="926" t="s">
         <v>279</v>
       </c>
-      <c r="C102" s="928"/>
-      <c r="D102" s="927" t="s">
+      <c r="C102" s="927"/>
+      <c r="D102" s="926" t="s">
         <v>279</v>
       </c>
-      <c r="E102" s="928"/>
-      <c r="F102" s="927" t="s">
+      <c r="E102" s="927"/>
+      <c r="F102" s="926" t="s">
         <v>279</v>
       </c>
-      <c r="G102" s="928"/>
+      <c r="G102" s="927"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="504" t="s">
@@ -13353,36 +13368,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="967" t="str">
+      <c r="B116" s="983" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="968"/>
-      <c r="D116" s="967" t="str">
+      <c r="C116" s="984"/>
+      <c r="D116" s="983" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="968"/>
-      <c r="F116" s="967" t="str">
+      <c r="E116" s="984"/>
+      <c r="F116" s="983" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="968"/>
+      <c r="G116" s="984"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="542"/>
-      <c r="B117" s="969" t="s">
+      <c r="B117" s="985" t="s">
         <v>279</v>
       </c>
-      <c r="C117" s="970"/>
-      <c r="D117" s="969" t="s">
+      <c r="C117" s="986"/>
+      <c r="D117" s="985" t="s">
         <v>279</v>
       </c>
-      <c r="E117" s="970"/>
-      <c r="F117" s="969" t="s">
+      <c r="E117" s="986"/>
+      <c r="F117" s="985" t="s">
         <v>279</v>
       </c>
-      <c r="G117" s="970"/>
+      <c r="G117" s="986"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="543" t="s">
@@ -13685,12 +13700,12 @@
       <c r="A129" s="546" t="s">
         <v>357</v>
       </c>
-      <c r="B129" s="982" t="str">
+      <c r="B129" s="979" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="983"/>
-      <c r="D129" s="983"/>
+      <c r="C129" s="980"/>
+      <c r="D129" s="980"/>
       <c r="N129" s="713" t="s">
         <v>398</v>
       </c>
@@ -14466,16 +14481,22 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="39">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -14489,22 +14510,16 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14513,6 +14528,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil17"/>
   <dimension ref="A2:D132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15320,6 +15336,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil18"/>
   <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15375,6 +15392,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil19"/>
   <dimension ref="A2:F300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17789,6 +17807,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:AQ10000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17900,66 +17919,66 @@
       <c r="AQ3" s="6"/>
     </row>
     <row r="4" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="825" t="s">
+      <c r="A4" s="824" t="s">
         <v>510</v>
       </c>
-      <c r="B4" s="826"/>
-      <c r="C4" s="826"/>
-      <c r="D4" s="826"/>
-      <c r="E4" s="826"/>
-      <c r="F4" s="827"/>
-      <c r="G4" s="827"/>
-      <c r="H4" s="827"/>
-      <c r="I4" s="827"/>
-      <c r="J4" s="827"/>
-      <c r="K4" s="827"/>
-      <c r="L4" s="827"/>
-      <c r="M4" s="827"/>
-      <c r="N4" s="827"/>
-      <c r="O4" s="827"/>
-      <c r="P4" s="827"/>
-      <c r="Q4" s="827"/>
-      <c r="R4" s="827"/>
-      <c r="S4" s="827"/>
-      <c r="T4" s="827"/>
-      <c r="U4" s="827"/>
-      <c r="V4" s="827"/>
-      <c r="W4" s="827"/>
-      <c r="X4" s="827"/>
-      <c r="Y4" s="827"/>
-      <c r="Z4" s="827"/>
-      <c r="AA4" s="827"/>
-      <c r="AB4" s="827"/>
-      <c r="AC4" s="827"/>
-      <c r="AD4" s="827"/>
-      <c r="AE4" s="827"/>
-      <c r="AF4" s="827"/>
-      <c r="AG4" s="827"/>
-      <c r="AH4" s="827"/>
-      <c r="AI4" s="827"/>
-      <c r="AJ4" s="827"/>
-      <c r="AK4" s="827"/>
-      <c r="AL4" s="827"/>
-      <c r="AM4" s="827"/>
-      <c r="AN4" s="827"/>
-      <c r="AO4" s="827"/>
-      <c r="AP4" s="827"/>
-      <c r="AQ4" s="827"/>
+      <c r="B4" s="825"/>
+      <c r="C4" s="825"/>
+      <c r="D4" s="825"/>
+      <c r="E4" s="825"/>
+      <c r="F4" s="826"/>
+      <c r="G4" s="826"/>
+      <c r="H4" s="826"/>
+      <c r="I4" s="826"/>
+      <c r="J4" s="826"/>
+      <c r="K4" s="826"/>
+      <c r="L4" s="826"/>
+      <c r="M4" s="826"/>
+      <c r="N4" s="826"/>
+      <c r="O4" s="826"/>
+      <c r="P4" s="826"/>
+      <c r="Q4" s="826"/>
+      <c r="R4" s="826"/>
+      <c r="S4" s="826"/>
+      <c r="T4" s="826"/>
+      <c r="U4" s="826"/>
+      <c r="V4" s="826"/>
+      <c r="W4" s="826"/>
+      <c r="X4" s="826"/>
+      <c r="Y4" s="826"/>
+      <c r="Z4" s="826"/>
+      <c r="AA4" s="826"/>
+      <c r="AB4" s="826"/>
+      <c r="AC4" s="826"/>
+      <c r="AD4" s="826"/>
+      <c r="AE4" s="826"/>
+      <c r="AF4" s="826"/>
+      <c r="AG4" s="826"/>
+      <c r="AH4" s="826"/>
+      <c r="AI4" s="826"/>
+      <c r="AJ4" s="826"/>
+      <c r="AK4" s="826"/>
+      <c r="AL4" s="826"/>
+      <c r="AM4" s="826"/>
+      <c r="AN4" s="826"/>
+      <c r="AO4" s="826"/>
+      <c r="AP4" s="826"/>
+      <c r="AQ4" s="826"/>
     </row>
     <row r="5" spans="1:43" s="7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="828" t="s">
+      <c r="A5" s="827" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="828" t="s">
+      <c r="B5" s="827" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="795" t="s">
         <v>593</v>
       </c>
-      <c r="D5" s="828" t="s">
+      <c r="D5" s="827" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="828" t="s">
+      <c r="E5" s="827" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="12" t="s">
@@ -18019,10 +18038,10 @@
       <c r="X5" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="Y5" s="830" t="s">
+      <c r="Y5" s="829" t="s">
         <v>48</v>
       </c>
-      <c r="Z5" s="830" t="s">
+      <c r="Z5" s="829" t="s">
         <v>49</v>
       </c>
       <c r="AA5" s="16" t="s">
@@ -18052,7 +18071,7 @@
       <c r="AI5" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AJ5" s="830" t="s">
+      <c r="AJ5" s="829" t="s">
         <v>58</v>
       </c>
       <c r="AK5" s="16" t="s">
@@ -18061,28 +18080,28 @@
       <c r="AL5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="AM5" s="828" t="s">
+      <c r="AM5" s="827" t="s">
         <v>61</v>
       </c>
-      <c r="AN5" s="828" t="s">
+      <c r="AN5" s="827" t="s">
         <v>62</v>
       </c>
-      <c r="AO5" s="828" t="s">
+      <c r="AO5" s="827" t="s">
         <v>63</v>
       </c>
-      <c r="AP5" s="828" t="s">
+      <c r="AP5" s="827" t="s">
         <v>64</v>
       </c>
-      <c r="AQ5" s="828" t="s">
+      <c r="AQ5" s="827" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:43" s="9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="829"/>
-      <c r="B6" s="829"/>
+      <c r="A6" s="828"/>
+      <c r="B6" s="828"/>
       <c r="C6" s="796"/>
-      <c r="D6" s="829"/>
-      <c r="E6" s="829"/>
+      <c r="D6" s="828"/>
+      <c r="E6" s="828"/>
       <c r="F6" s="14" t="s">
         <v>66</v>
       </c>
@@ -18140,8 +18159,8 @@
       <c r="X6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="Y6" s="831"/>
-      <c r="Z6" s="831"/>
+      <c r="Y6" s="830"/>
+      <c r="Z6" s="830"/>
       <c r="AA6" s="9" t="s">
         <v>67</v>
       </c>
@@ -18169,18 +18188,18 @@
       <c r="AI6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="AJ6" s="831"/>
+      <c r="AJ6" s="830"/>
       <c r="AK6" s="9" t="s">
         <v>67</v>
       </c>
       <c r="AL6" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AM6" s="829"/>
-      <c r="AN6" s="829"/>
-      <c r="AO6" s="829"/>
-      <c r="AP6" s="829"/>
-      <c r="AQ6" s="829"/>
+      <c r="AM6" s="828"/>
+      <c r="AN6" s="828"/>
+      <c r="AO6" s="828"/>
+      <c r="AP6" s="828"/>
+      <c r="AQ6" s="828"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="AE7" s="8"/>
@@ -58235,6 +58254,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil20"/>
   <dimension ref="A2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -58308,6 +58328,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -58419,6 +58440,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -58440,10 +58462,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="58.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="832" t="s">
+      <c r="A1" s="831" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="834" t="s">
+      <c r="B1" s="833" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="823" t="s">
@@ -58493,8 +58515,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="833"/>
-      <c r="B2" s="835"/>
+      <c r="A2" s="832"/>
+      <c r="B2" s="834"/>
       <c r="C2" s="9" t="s">
         <v>67</v>
       </c>
@@ -58628,6 +58650,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:CQ13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -58658,123 +58681,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="658" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="865" t="s">
+      <c r="A1" s="835" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="866"/>
-      <c r="C1" s="866"/>
-      <c r="D1" s="866"/>
-      <c r="E1" s="866"/>
-      <c r="F1" s="866"/>
-      <c r="G1" s="866"/>
-      <c r="H1" s="867" t="s">
+      <c r="B1" s="836"/>
+      <c r="C1" s="836"/>
+      <c r="D1" s="836"/>
+      <c r="E1" s="836"/>
+      <c r="F1" s="836"/>
+      <c r="G1" s="836"/>
+      <c r="H1" s="837" t="s">
         <v>464</v>
       </c>
-      <c r="I1" s="868"/>
-      <c r="J1" s="868"/>
-      <c r="K1" s="868"/>
-      <c r="L1" s="868"/>
-      <c r="M1" s="869"/>
-      <c r="N1" s="870" t="s">
+      <c r="I1" s="838"/>
+      <c r="J1" s="838"/>
+      <c r="K1" s="838"/>
+      <c r="L1" s="838"/>
+      <c r="M1" s="839"/>
+      <c r="N1" s="840" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="848"/>
-      <c r="P1" s="848"/>
-      <c r="Q1" s="848"/>
-      <c r="R1" s="848"/>
-      <c r="S1" s="848"/>
-      <c r="T1" s="848"/>
-      <c r="U1" s="848"/>
-      <c r="V1" s="871" t="s">
+      <c r="O1" s="841"/>
+      <c r="P1" s="841"/>
+      <c r="Q1" s="841"/>
+      <c r="R1" s="841"/>
+      <c r="S1" s="841"/>
+      <c r="T1" s="841"/>
+      <c r="U1" s="841"/>
+      <c r="V1" s="842" t="s">
         <v>83</v>
       </c>
-      <c r="W1" s="872"/>
-      <c r="X1" s="873"/>
-      <c r="Y1" s="873"/>
-      <c r="Z1" s="874"/>
-      <c r="AA1" s="875" t="s">
+      <c r="W1" s="843"/>
+      <c r="X1" s="844"/>
+      <c r="Y1" s="844"/>
+      <c r="Z1" s="845"/>
+      <c r="AA1" s="846" t="s">
         <v>84</v>
       </c>
-      <c r="AB1" s="876"/>
-      <c r="AC1" s="876"/>
-      <c r="AD1" s="876"/>
-      <c r="AE1" s="876"/>
-      <c r="AF1" s="876"/>
-      <c r="AG1" s="876"/>
-      <c r="AH1" s="876"/>
-      <c r="AI1" s="876"/>
-      <c r="AJ1" s="876"/>
-      <c r="AK1" s="876"/>
-      <c r="AL1" s="876"/>
-      <c r="AM1" s="876"/>
+      <c r="AB1" s="847"/>
+      <c r="AC1" s="847"/>
+      <c r="AD1" s="847"/>
+      <c r="AE1" s="847"/>
+      <c r="AF1" s="847"/>
+      <c r="AG1" s="847"/>
+      <c r="AH1" s="847"/>
+      <c r="AI1" s="847"/>
+      <c r="AJ1" s="847"/>
+      <c r="AK1" s="847"/>
+      <c r="AL1" s="847"/>
+      <c r="AM1" s="847"/>
       <c r="AN1" s="52"/>
       <c r="AO1" s="53"/>
-      <c r="AP1" s="847" t="s">
+      <c r="AP1" s="859" t="s">
         <v>85</v>
       </c>
-      <c r="AQ1" s="848"/>
-      <c r="AR1" s="848"/>
-      <c r="AS1" s="848"/>
-      <c r="AT1" s="848"/>
-      <c r="AU1" s="848"/>
-      <c r="AV1" s="848"/>
-      <c r="AW1" s="849"/>
-      <c r="AX1" s="856" t="s">
+      <c r="AQ1" s="841"/>
+      <c r="AR1" s="841"/>
+      <c r="AS1" s="841"/>
+      <c r="AT1" s="841"/>
+      <c r="AU1" s="841"/>
+      <c r="AV1" s="841"/>
+      <c r="AW1" s="860"/>
+      <c r="AX1" s="867" t="s">
         <v>594</v>
       </c>
-      <c r="AY1" s="857"/>
-      <c r="AZ1" s="857"/>
-      <c r="BA1" s="857"/>
-      <c r="BB1" s="857"/>
-      <c r="BC1" s="858"/>
-      <c r="BD1" s="859" t="s">
+      <c r="AY1" s="868"/>
+      <c r="AZ1" s="868"/>
+      <c r="BA1" s="868"/>
+      <c r="BB1" s="868"/>
+      <c r="BC1" s="869"/>
+      <c r="BD1" s="870" t="s">
         <v>86</v>
       </c>
-      <c r="BE1" s="860"/>
-      <c r="BF1" s="860"/>
-      <c r="BG1" s="860"/>
-      <c r="BH1" s="860"/>
-      <c r="BI1" s="861"/>
-      <c r="BJ1" s="862" t="s">
+      <c r="BE1" s="871"/>
+      <c r="BF1" s="871"/>
+      <c r="BG1" s="871"/>
+      <c r="BH1" s="871"/>
+      <c r="BI1" s="872"/>
+      <c r="BJ1" s="873" t="s">
         <v>87</v>
       </c>
-      <c r="BK1" s="863"/>
-      <c r="BL1" s="863"/>
-      <c r="BM1" s="863"/>
-      <c r="BN1" s="863"/>
-      <c r="BO1" s="863"/>
-      <c r="BP1" s="864"/>
-      <c r="BQ1" s="836" t="s">
+      <c r="BK1" s="874"/>
+      <c r="BL1" s="874"/>
+      <c r="BM1" s="874"/>
+      <c r="BN1" s="874"/>
+      <c r="BO1" s="874"/>
+      <c r="BP1" s="875"/>
+      <c r="BQ1" s="848" t="s">
         <v>88</v>
       </c>
-      <c r="BR1" s="837"/>
-      <c r="BS1" s="837"/>
-      <c r="BT1" s="837"/>
-      <c r="BU1" s="837"/>
-      <c r="BV1" s="837"/>
+      <c r="BR1" s="849"/>
+      <c r="BS1" s="849"/>
+      <c r="BT1" s="849"/>
+      <c r="BU1" s="849"/>
+      <c r="BV1" s="849"/>
       <c r="BW1" s="53"/>
       <c r="BX1" s="54"/>
-      <c r="BY1" s="838" t="s">
+      <c r="BY1" s="850" t="s">
         <v>89</v>
       </c>
-      <c r="BZ1" s="839"/>
-      <c r="CA1" s="839"/>
-      <c r="CB1" s="839"/>
-      <c r="CC1" s="839"/>
-      <c r="CD1" s="839"/>
-      <c r="CE1" s="839"/>
-      <c r="CF1" s="840"/>
-      <c r="CG1" s="840"/>
-      <c r="CH1" s="840"/>
-      <c r="CI1" s="840"/>
-      <c r="CJ1" s="840"/>
-      <c r="CK1" s="840"/>
-      <c r="CL1" s="840"/>
-      <c r="CM1" s="840"/>
-      <c r="CN1" s="840"/>
-      <c r="CO1" s="840"/>
-      <c r="CP1" s="840"/>
-      <c r="CQ1" s="840"/>
+      <c r="BZ1" s="851"/>
+      <c r="CA1" s="851"/>
+      <c r="CB1" s="851"/>
+      <c r="CC1" s="851"/>
+      <c r="CD1" s="851"/>
+      <c r="CE1" s="851"/>
+      <c r="CF1" s="852"/>
+      <c r="CG1" s="852"/>
+      <c r="CH1" s="852"/>
+      <c r="CI1" s="852"/>
+      <c r="CJ1" s="852"/>
+      <c r="CK1" s="852"/>
+      <c r="CL1" s="852"/>
+      <c r="CM1" s="852"/>
+      <c r="CN1" s="852"/>
+      <c r="CO1" s="852"/>
+      <c r="CP1" s="852"/>
+      <c r="CQ1" s="852"/>
     </row>
     <row r="2" spans="1:95" s="658" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -58798,18 +58821,18 @@
       <c r="G2" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="841" t="s">
+      <c r="H2" s="853" t="s">
         <v>465</v>
       </c>
-      <c r="I2" s="842"/>
-      <c r="J2" s="842" t="s">
+      <c r="I2" s="854"/>
+      <c r="J2" s="854" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="842"/>
-      <c r="L2" s="842" t="s">
+      <c r="K2" s="854"/>
+      <c r="L2" s="854" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="843"/>
+      <c r="M2" s="855"/>
       <c r="N2" s="57" t="s">
         <v>90</v>
       </c>
@@ -58918,36 +58941,36 @@
       <c r="AW2" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="AX2" s="844" t="s">
+      <c r="AX2" s="856" t="s">
         <v>125</v>
       </c>
-      <c r="AY2" s="845"/>
-      <c r="AZ2" s="845"/>
-      <c r="BA2" s="845" t="s">
+      <c r="AY2" s="857"/>
+      <c r="AZ2" s="857"/>
+      <c r="BA2" s="857" t="s">
         <v>126</v>
       </c>
-      <c r="BB2" s="845"/>
-      <c r="BC2" s="846"/>
-      <c r="BD2" s="850" t="s">
+      <c r="BB2" s="857"/>
+      <c r="BC2" s="858"/>
+      <c r="BD2" s="861" t="s">
         <v>125</v>
       </c>
-      <c r="BE2" s="851"/>
-      <c r="BF2" s="851"/>
-      <c r="BG2" s="851" t="s">
+      <c r="BE2" s="862"/>
+      <c r="BF2" s="862"/>
+      <c r="BG2" s="862" t="s">
         <v>126</v>
       </c>
-      <c r="BH2" s="851"/>
-      <c r="BI2" s="852"/>
-      <c r="BJ2" s="853" t="s">
+      <c r="BH2" s="862"/>
+      <c r="BI2" s="863"/>
+      <c r="BJ2" s="864" t="s">
         <v>125</v>
       </c>
-      <c r="BK2" s="854"/>
-      <c r="BL2" s="854"/>
-      <c r="BM2" s="854" t="s">
+      <c r="BK2" s="865"/>
+      <c r="BL2" s="865"/>
+      <c r="BM2" s="865" t="s">
         <v>126</v>
       </c>
-      <c r="BN2" s="855"/>
-      <c r="BO2" s="855"/>
+      <c r="BN2" s="866"/>
+      <c r="BO2" s="866"/>
       <c r="BP2" s="69" t="s">
         <v>127</v>
       </c>
@@ -59580,11 +59603,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -59600,6 +59618,11 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -59608,6 +59631,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil6"/>
   <dimension ref="A1:CZ47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -59682,32 +59706,32 @@
         <v>167</v>
       </c>
       <c r="L1" s="145"/>
-      <c r="M1" s="900" t="s">
+      <c r="M1" s="876" t="s">
         <v>168</v>
       </c>
-      <c r="N1" s="901" t="s">
+      <c r="N1" s="877" t="s">
         <v>520</v>
       </c>
-      <c r="O1" s="902"/>
-      <c r="P1" s="902"/>
-      <c r="Q1" s="902"/>
-      <c r="R1" s="903" t="s">
+      <c r="O1" s="878"/>
+      <c r="P1" s="878"/>
+      <c r="Q1" s="878"/>
+      <c r="R1" s="879" t="s">
         <v>464</v>
       </c>
-      <c r="S1" s="896"/>
-      <c r="T1" s="896"/>
-      <c r="U1" s="896"/>
-      <c r="V1" s="896"/>
-      <c r="W1" s="896"/>
-      <c r="X1" s="904"/>
-      <c r="Y1" s="890" t="s">
+      <c r="S1" s="880"/>
+      <c r="T1" s="880"/>
+      <c r="U1" s="880"/>
+      <c r="V1" s="880"/>
+      <c r="W1" s="880"/>
+      <c r="X1" s="881"/>
+      <c r="Y1" s="882" t="s">
         <v>472</v>
       </c>
-      <c r="Z1" s="860"/>
-      <c r="AA1" s="905" t="s">
+      <c r="Z1" s="871"/>
+      <c r="AA1" s="885" t="s">
         <v>169</v>
       </c>
-      <c r="AB1" s="878" t="s">
+      <c r="AB1" s="896" t="s">
         <v>170</v>
       </c>
       <c r="AC1" s="892" t="s">
@@ -59719,90 +59743,90 @@
       <c r="AG1" s="895" t="s">
         <v>172</v>
       </c>
-      <c r="AH1" s="896"/>
-      <c r="AI1" s="896"/>
-      <c r="AJ1" s="896"/>
-      <c r="AK1" s="896"/>
-      <c r="AL1" s="896"/>
-      <c r="AM1" s="896"/>
-      <c r="AN1" s="896"/>
-      <c r="AO1" s="878" t="s">
+      <c r="AH1" s="880"/>
+      <c r="AI1" s="880"/>
+      <c r="AJ1" s="880"/>
+      <c r="AK1" s="880"/>
+      <c r="AL1" s="880"/>
+      <c r="AM1" s="880"/>
+      <c r="AN1" s="880"/>
+      <c r="AO1" s="896" t="s">
         <v>173</v>
       </c>
-      <c r="AP1" s="890" t="s">
+      <c r="AP1" s="882" t="s">
         <v>471</v>
       </c>
-      <c r="AQ1" s="860"/>
-      <c r="AR1" s="860"/>
-      <c r="AS1" s="861"/>
-      <c r="AT1" s="898" t="s">
+      <c r="AQ1" s="871"/>
+      <c r="AR1" s="871"/>
+      <c r="AS1" s="872"/>
+      <c r="AT1" s="899" t="s">
         <v>174</v>
       </c>
-      <c r="AU1" s="899"/>
-      <c r="AV1" s="899"/>
-      <c r="AW1" s="899"/>
-      <c r="AX1" s="899"/>
-      <c r="AY1" s="899"/>
-      <c r="AZ1" s="899"/>
-      <c r="BA1" s="899"/>
-      <c r="BB1" s="899"/>
-      <c r="BC1" s="899"/>
-      <c r="BD1" s="899"/>
-      <c r="BE1" s="899"/>
-      <c r="BF1" s="899"/>
-      <c r="BG1" s="899"/>
-      <c r="BH1" s="899"/>
-      <c r="BI1" s="899"/>
-      <c r="BJ1" s="899"/>
-      <c r="BK1" s="899"/>
-      <c r="BL1" s="899"/>
-      <c r="BM1" s="899"/>
-      <c r="BN1" s="899"/>
-      <c r="BO1" s="899"/>
-      <c r="BP1" s="899"/>
-      <c r="BQ1" s="899"/>
-      <c r="BR1" s="899"/>
-      <c r="BS1" s="899"/>
-      <c r="BT1" s="899"/>
-      <c r="BU1" s="899"/>
-      <c r="BV1" s="899"/>
-      <c r="BW1" s="878" t="s">
+      <c r="AU1" s="900"/>
+      <c r="AV1" s="900"/>
+      <c r="AW1" s="900"/>
+      <c r="AX1" s="900"/>
+      <c r="AY1" s="900"/>
+      <c r="AZ1" s="900"/>
+      <c r="BA1" s="900"/>
+      <c r="BB1" s="900"/>
+      <c r="BC1" s="900"/>
+      <c r="BD1" s="900"/>
+      <c r="BE1" s="900"/>
+      <c r="BF1" s="900"/>
+      <c r="BG1" s="900"/>
+      <c r="BH1" s="900"/>
+      <c r="BI1" s="900"/>
+      <c r="BJ1" s="900"/>
+      <c r="BK1" s="900"/>
+      <c r="BL1" s="900"/>
+      <c r="BM1" s="900"/>
+      <c r="BN1" s="900"/>
+      <c r="BO1" s="900"/>
+      <c r="BP1" s="900"/>
+      <c r="BQ1" s="900"/>
+      <c r="BR1" s="900"/>
+      <c r="BS1" s="900"/>
+      <c r="BT1" s="900"/>
+      <c r="BU1" s="900"/>
+      <c r="BV1" s="900"/>
+      <c r="BW1" s="896" t="s">
         <v>175</v>
       </c>
-      <c r="BX1" s="890" t="s">
+      <c r="BX1" s="882" t="s">
         <v>470</v>
       </c>
-      <c r="BY1" s="860"/>
-      <c r="BZ1" s="860"/>
-      <c r="CA1" s="861"/>
-      <c r="CB1" s="889" t="s">
+      <c r="BY1" s="871"/>
+      <c r="BZ1" s="871"/>
+      <c r="CA1" s="872"/>
+      <c r="CB1" s="908" t="s">
         <v>487</v>
       </c>
-      <c r="CC1" s="891" t="s">
+      <c r="CC1" s="890" t="s">
         <v>84</v>
       </c>
-      <c r="CD1" s="891"/>
-      <c r="CE1" s="891"/>
-      <c r="CF1" s="891"/>
-      <c r="CG1" s="891"/>
-      <c r="CH1" s="891"/>
-      <c r="CI1" s="891"/>
-      <c r="CJ1" s="891"/>
-      <c r="CK1" s="891"/>
-      <c r="CL1" s="891"/>
-      <c r="CM1" s="891"/>
-      <c r="CN1" s="891"/>
+      <c r="CD1" s="890"/>
+      <c r="CE1" s="890"/>
+      <c r="CF1" s="890"/>
+      <c r="CG1" s="890"/>
+      <c r="CH1" s="890"/>
+      <c r="CI1" s="890"/>
+      <c r="CJ1" s="890"/>
+      <c r="CK1" s="890"/>
+      <c r="CL1" s="890"/>
+      <c r="CM1" s="890"/>
+      <c r="CN1" s="890"/>
       <c r="CO1" s="146"/>
-      <c r="CP1" s="877" t="s">
+      <c r="CP1" s="904" t="s">
         <v>88</v>
       </c>
-      <c r="CQ1" s="848"/>
-      <c r="CR1" s="848"/>
-      <c r="CS1" s="848"/>
-      <c r="CT1" s="848"/>
-      <c r="CU1" s="848"/>
-      <c r="CV1" s="848"/>
-      <c r="CW1" s="849"/>
+      <c r="CQ1" s="841"/>
+      <c r="CR1" s="841"/>
+      <c r="CS1" s="841"/>
+      <c r="CT1" s="841"/>
+      <c r="CU1" s="841"/>
+      <c r="CV1" s="841"/>
+      <c r="CW1" s="860"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="147" t="s">
@@ -59841,7 +59865,7 @@
       <c r="L2" s="151" t="s">
         <v>91</v>
       </c>
-      <c r="M2" s="900"/>
+      <c r="M2" s="876"/>
       <c r="N2" s="152" t="s">
         <v>180</v>
       </c>
@@ -59857,22 +59881,22 @@
       <c r="R2" s="157" t="s">
         <v>183</v>
       </c>
-      <c r="S2" s="907" t="s">
+      <c r="S2" s="887" t="s">
         <v>465</v>
       </c>
-      <c r="T2" s="855"/>
-      <c r="U2" s="908" t="s">
+      <c r="T2" s="866"/>
+      <c r="U2" s="888" t="s">
         <v>97</v>
       </c>
-      <c r="V2" s="908"/>
-      <c r="W2" s="908" t="s">
+      <c r="V2" s="888"/>
+      <c r="W2" s="888" t="s">
         <v>98</v>
       </c>
-      <c r="X2" s="909"/>
-      <c r="Y2" s="884"/>
-      <c r="Z2" s="885"/>
-      <c r="AA2" s="906"/>
-      <c r="AB2" s="879"/>
+      <c r="X2" s="889"/>
+      <c r="Y2" s="883"/>
+      <c r="Z2" s="884"/>
+      <c r="AA2" s="886"/>
+      <c r="AB2" s="897"/>
       <c r="AC2" s="153" t="s">
         <v>184</v>
       </c>
@@ -59885,81 +59909,81 @@
       <c r="AF2" s="153" t="s">
         <v>187</v>
       </c>
-      <c r="AG2" s="897" t="s">
+      <c r="AG2" s="898" t="s">
         <v>188</v>
       </c>
-      <c r="AH2" s="882"/>
-      <c r="AI2" s="882" t="s">
+      <c r="AH2" s="891"/>
+      <c r="AI2" s="891" t="s">
         <v>189</v>
       </c>
-      <c r="AJ2" s="882"/>
-      <c r="AK2" s="882" t="s">
+      <c r="AJ2" s="891"/>
+      <c r="AK2" s="891" t="s">
         <v>190</v>
       </c>
-      <c r="AL2" s="882"/>
+      <c r="AL2" s="891"/>
       <c r="AM2" s="154" t="s">
         <v>191</v>
       </c>
       <c r="AN2" s="154" t="s">
         <v>192</v>
       </c>
-      <c r="AO2" s="879"/>
-      <c r="AP2" s="884" t="s">
+      <c r="AO2" s="897"/>
+      <c r="AP2" s="883" t="s">
         <v>193</v>
       </c>
-      <c r="AQ2" s="885"/>
-      <c r="AR2" s="886" t="s">
+      <c r="AQ2" s="884"/>
+      <c r="AR2" s="901" t="s">
         <v>194</v>
       </c>
-      <c r="AS2" s="887"/>
-      <c r="AT2" s="882" t="s">
+      <c r="AS2" s="902"/>
+      <c r="AT2" s="891" t="s">
         <v>195</v>
       </c>
-      <c r="AU2" s="882"/>
-      <c r="AV2" s="883" t="s">
+      <c r="AU2" s="891"/>
+      <c r="AV2" s="903" t="s">
         <v>196</v>
       </c>
-      <c r="AW2" s="883"/>
-      <c r="AX2" s="883" t="s">
+      <c r="AW2" s="903"/>
+      <c r="AX2" s="903" t="s">
         <v>197</v>
       </c>
-      <c r="AY2" s="883"/>
+      <c r="AY2" s="903"/>
       <c r="AZ2" s="154" t="s">
         <v>198</v>
       </c>
       <c r="BA2" s="154" t="s">
         <v>199</v>
       </c>
-      <c r="BB2" s="882" t="s">
+      <c r="BB2" s="891" t="s">
         <v>200</v>
       </c>
-      <c r="BC2" s="882"/>
-      <c r="BD2" s="883" t="s">
+      <c r="BC2" s="891"/>
+      <c r="BD2" s="903" t="s">
         <v>201</v>
       </c>
-      <c r="BE2" s="883"/>
-      <c r="BF2" s="883" t="s">
+      <c r="BE2" s="903"/>
+      <c r="BF2" s="903" t="s">
         <v>202</v>
       </c>
-      <c r="BG2" s="883"/>
+      <c r="BG2" s="903"/>
       <c r="BH2" s="154" t="s">
         <v>203</v>
       </c>
       <c r="BI2" s="154" t="s">
         <v>204</v>
       </c>
-      <c r="BJ2" s="882" t="s">
+      <c r="BJ2" s="891" t="s">
         <v>205</v>
       </c>
-      <c r="BK2" s="882"/>
-      <c r="BL2" s="883" t="s">
+      <c r="BK2" s="891"/>
+      <c r="BL2" s="903" t="s">
         <v>206</v>
       </c>
-      <c r="BM2" s="883"/>
-      <c r="BN2" s="883" t="s">
+      <c r="BM2" s="903"/>
+      <c r="BN2" s="903" t="s">
         <v>207</v>
       </c>
-      <c r="BO2" s="883"/>
+      <c r="BO2" s="903"/>
       <c r="BP2" s="154" t="s">
         <v>208</v>
       </c>
@@ -59981,16 +60005,16 @@
       <c r="BV2" s="154" t="s">
         <v>214</v>
       </c>
-      <c r="BW2" s="879"/>
-      <c r="BX2" s="884" t="s">
+      <c r="BW2" s="897"/>
+      <c r="BX2" s="883" t="s">
         <v>193</v>
       </c>
-      <c r="BY2" s="885"/>
-      <c r="BZ2" s="886" t="s">
+      <c r="BY2" s="884"/>
+      <c r="BZ2" s="901" t="s">
         <v>194</v>
       </c>
-      <c r="CA2" s="887"/>
-      <c r="CB2" s="889"/>
+      <c r="CA2" s="902"/>
+      <c r="CB2" s="908"/>
       <c r="CC2" s="138" t="s">
         <v>106</v>
       </c>
@@ -60030,22 +60054,22 @@
       <c r="CO2" s="140" t="s">
         <v>473</v>
       </c>
-      <c r="CP2" s="888" t="s">
+      <c r="CP2" s="907" t="s">
         <v>216</v>
       </c>
-      <c r="CQ2" s="880"/>
-      <c r="CR2" s="880" t="s">
+      <c r="CQ2" s="905"/>
+      <c r="CR2" s="905" t="s">
         <v>217</v>
       </c>
-      <c r="CS2" s="880"/>
-      <c r="CT2" s="880" t="s">
+      <c r="CS2" s="905"/>
+      <c r="CT2" s="905" t="s">
         <v>218</v>
       </c>
-      <c r="CU2" s="880"/>
-      <c r="CV2" s="880" t="s">
+      <c r="CU2" s="905"/>
+      <c r="CV2" s="905" t="s">
         <v>219</v>
       </c>
-      <c r="CW2" s="881"/>
+      <c r="CW2" s="906"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="168"/>
@@ -60910,29 +60934,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="39">
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="CC1:CN1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AN1"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
     <mergeCell ref="CP1:CW1"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="CV2:CW2"/>
@@ -60949,6 +60950,29 @@
     <mergeCell ref="CT2:CU2"/>
     <mergeCell ref="CB1:CB2"/>
     <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CC1:CN1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AN1"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -60957,6 +60981,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil7"/>
   <dimension ref="A1:DE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -60991,19 +61016,19 @@
       <c r="K1" s="144"/>
       <c r="L1" s="145"/>
       <c r="M1" s="695"/>
-      <c r="N1" s="910"/>
-      <c r="O1" s="911"/>
-      <c r="P1" s="911"/>
-      <c r="Q1" s="911"/>
-      <c r="R1" s="903"/>
-      <c r="S1" s="896"/>
-      <c r="T1" s="896"/>
-      <c r="U1" s="896"/>
-      <c r="V1" s="896"/>
-      <c r="W1" s="896"/>
-      <c r="X1" s="904"/>
-      <c r="Y1" s="890"/>
-      <c r="Z1" s="860"/>
+      <c r="N1" s="912"/>
+      <c r="O1" s="913"/>
+      <c r="P1" s="913"/>
+      <c r="Q1" s="913"/>
+      <c r="R1" s="879"/>
+      <c r="S1" s="880"/>
+      <c r="T1" s="880"/>
+      <c r="U1" s="880"/>
+      <c r="V1" s="880"/>
+      <c r="W1" s="880"/>
+      <c r="X1" s="881"/>
+      <c r="Y1" s="882"/>
+      <c r="Z1" s="871"/>
       <c r="AA1" s="696"/>
       <c r="AB1" s="694"/>
       <c r="AC1" s="892"/>
@@ -61011,85 +61036,90 @@
       <c r="AE1" s="893"/>
       <c r="AF1" s="894"/>
       <c r="AG1" s="895"/>
-      <c r="AH1" s="896"/>
-      <c r="AI1" s="896"/>
-      <c r="AJ1" s="896"/>
-      <c r="AK1" s="896"/>
-      <c r="AL1" s="896"/>
-      <c r="AM1" s="896"/>
-      <c r="AN1" s="896"/>
+      <c r="AH1" s="880"/>
+      <c r="AI1" s="880"/>
+      <c r="AJ1" s="880"/>
+      <c r="AK1" s="880"/>
+      <c r="AL1" s="880"/>
+      <c r="AM1" s="880"/>
+      <c r="AN1" s="880"/>
       <c r="AO1" s="694"/>
-      <c r="AP1" s="890"/>
-      <c r="AQ1" s="860"/>
-      <c r="AR1" s="860"/>
-      <c r="AS1" s="861"/>
-      <c r="AT1" s="898"/>
-      <c r="AU1" s="899"/>
-      <c r="AV1" s="899"/>
-      <c r="AW1" s="899"/>
-      <c r="AX1" s="899"/>
-      <c r="AY1" s="899"/>
-      <c r="AZ1" s="899"/>
-      <c r="BA1" s="899"/>
-      <c r="BB1" s="899"/>
-      <c r="BC1" s="899"/>
-      <c r="BD1" s="899"/>
-      <c r="BE1" s="899"/>
-      <c r="BF1" s="899"/>
-      <c r="BG1" s="899"/>
-      <c r="BH1" s="899"/>
-      <c r="BI1" s="899"/>
-      <c r="BJ1" s="899"/>
-      <c r="BK1" s="899"/>
-      <c r="BL1" s="899"/>
-      <c r="BM1" s="899"/>
-      <c r="BN1" s="899"/>
-      <c r="BO1" s="899"/>
-      <c r="BP1" s="899"/>
-      <c r="BQ1" s="899"/>
-      <c r="BR1" s="899"/>
-      <c r="BS1" s="899"/>
-      <c r="BT1" s="899"/>
-      <c r="BU1" s="899"/>
-      <c r="BV1" s="899"/>
+      <c r="AP1" s="882"/>
+      <c r="AQ1" s="871"/>
+      <c r="AR1" s="871"/>
+      <c r="AS1" s="872"/>
+      <c r="AT1" s="899"/>
+      <c r="AU1" s="900"/>
+      <c r="AV1" s="900"/>
+      <c r="AW1" s="900"/>
+      <c r="AX1" s="900"/>
+      <c r="AY1" s="900"/>
+      <c r="AZ1" s="900"/>
+      <c r="BA1" s="900"/>
+      <c r="BB1" s="900"/>
+      <c r="BC1" s="900"/>
+      <c r="BD1" s="900"/>
+      <c r="BE1" s="900"/>
+      <c r="BF1" s="900"/>
+      <c r="BG1" s="900"/>
+      <c r="BH1" s="900"/>
+      <c r="BI1" s="900"/>
+      <c r="BJ1" s="900"/>
+      <c r="BK1" s="900"/>
+      <c r="BL1" s="900"/>
+      <c r="BM1" s="900"/>
+      <c r="BN1" s="900"/>
+      <c r="BO1" s="900"/>
+      <c r="BP1" s="900"/>
+      <c r="BQ1" s="900"/>
+      <c r="BR1" s="900"/>
+      <c r="BS1" s="900"/>
+      <c r="BT1" s="900"/>
+      <c r="BU1" s="900"/>
+      <c r="BV1" s="900"/>
       <c r="BW1" s="694"/>
-      <c r="BX1" s="890"/>
-      <c r="BY1" s="860"/>
-      <c r="BZ1" s="860"/>
-      <c r="CA1" s="861"/>
-      <c r="CB1" s="891"/>
-      <c r="CC1" s="891"/>
-      <c r="CD1" s="891"/>
-      <c r="CE1" s="891"/>
-      <c r="CF1" s="891"/>
-      <c r="CG1" s="891"/>
-      <c r="CH1" s="891"/>
-      <c r="CI1" s="891"/>
-      <c r="CJ1" s="891"/>
-      <c r="CK1" s="891"/>
-      <c r="CL1" s="891"/>
-      <c r="CM1" s="891"/>
+      <c r="BX1" s="882"/>
+      <c r="BY1" s="871"/>
+      <c r="BZ1" s="871"/>
+      <c r="CA1" s="872"/>
+      <c r="CB1" s="890"/>
+      <c r="CC1" s="890"/>
+      <c r="CD1" s="890"/>
+      <c r="CE1" s="890"/>
+      <c r="CF1" s="890"/>
+      <c r="CG1" s="890"/>
+      <c r="CH1" s="890"/>
+      <c r="CI1" s="890"/>
+      <c r="CJ1" s="890"/>
+      <c r="CK1" s="890"/>
+      <c r="CL1" s="890"/>
+      <c r="CM1" s="890"/>
       <c r="CN1" s="693"/>
-      <c r="CO1" s="877"/>
-      <c r="CP1" s="848"/>
-      <c r="CQ1" s="848"/>
-      <c r="CR1" s="848"/>
-      <c r="CS1" s="848"/>
-      <c r="CT1" s="848"/>
-      <c r="CU1" s="848"/>
-      <c r="CV1" s="849"/>
-      <c r="CW1" s="912"/>
-      <c r="CX1" s="913"/>
-      <c r="CY1" s="913"/>
-      <c r="CZ1" s="914"/>
-      <c r="DA1" s="913"/>
-      <c r="DB1" s="913"/>
-      <c r="DC1" s="914"/>
-      <c r="DD1" s="913"/>
-      <c r="DE1" s="913"/>
+      <c r="CO1" s="904"/>
+      <c r="CP1" s="841"/>
+      <c r="CQ1" s="841"/>
+      <c r="CR1" s="841"/>
+      <c r="CS1" s="841"/>
+      <c r="CT1" s="841"/>
+      <c r="CU1" s="841"/>
+      <c r="CV1" s="860"/>
+      <c r="CW1" s="909"/>
+      <c r="CX1" s="910"/>
+      <c r="CY1" s="910"/>
+      <c r="CZ1" s="911"/>
+      <c r="DA1" s="910"/>
+      <c r="DB1" s="910"/>
+      <c r="DC1" s="911"/>
+      <c r="DD1" s="910"/>
+      <c r="DE1" s="910"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="CZ1:DB1"/>
     <mergeCell ref="DC1:DE1"/>
@@ -61098,11 +61128,6 @@
     <mergeCell ref="AG1:AN1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CB1:CM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -61111,18 +61136,25 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil8"/>
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="3" width="32.44140625" customWidth="1"/>
-    <col min="8" max="8" width="23.21875" customWidth="1"/>
-    <col min="12" max="12" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.4">
@@ -61135,20 +61167,20 @@
       <c r="E1" s="143"/>
       <c r="F1" s="143"/>
       <c r="G1" s="143"/>
-      <c r="H1" s="916" t="s">
+      <c r="H1" s="915" t="s">
         <v>603</v>
       </c>
-      <c r="I1" s="916"/>
-      <c r="J1" s="916"/>
-      <c r="K1" s="916"/>
-      <c r="L1" s="915" t="s">
+      <c r="I1" s="915"/>
+      <c r="J1" s="915"/>
+      <c r="K1" s="915"/>
+      <c r="L1" s="914" t="s">
         <v>604</v>
       </c>
-      <c r="M1" s="915"/>
-      <c r="N1" s="915"/>
-      <c r="O1" s="915"/>
-    </row>
-    <row r="2" spans="1:15" ht="42" x14ac:dyDescent="0.3">
+      <c r="M1" s="914"/>
+      <c r="N1" s="914"/>
+      <c r="O1" s="914"/>
+    </row>
+    <row r="2" spans="1:15" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="444" t="s">
         <v>90</v>
       </c>
@@ -61182,16 +61214,16 @@
       <c r="K2" s="140" t="s">
         <v>602</v>
       </c>
-      <c r="L2" s="824" t="s">
+      <c r="L2" s="991" t="s">
         <v>600</v>
       </c>
-      <c r="M2" s="824" t="s">
+      <c r="M2" s="991" t="s">
         <v>255</v>
       </c>
-      <c r="N2" s="824" t="s">
+      <c r="N2" s="991" t="s">
         <v>262</v>
       </c>
-      <c r="O2" s="824" t="s">
+      <c r="O2" s="991" t="s">
         <v>601</v>
       </c>
     </row>
@@ -61250,7 +61282,7 @@
       <c r="J6" s="167"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:D4"/>
+  <autoFilter ref="A4:O4"/>
   <mergeCells count="2">
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="H1:K1"/>
@@ -61262,6 +61294,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -61318,10 +61351,10 @@
       <c r="B2" s="203" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="924" t="s">
+      <c r="C2" s="921" t="s">
         <v>240</v>
       </c>
-      <c r="D2" s="924"/>
+      <c r="D2" s="921"/>
       <c r="E2" s="201"/>
       <c r="F2" s="201"/>
       <c r="G2" s="201"/>
@@ -61485,35 +61518,35 @@
     </row>
     <row r="7" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="200"/>
-      <c r="B7" s="925"/>
-      <c r="C7" s="925"/>
-      <c r="D7" s="925"/>
+      <c r="B7" s="918"/>
+      <c r="C7" s="918"/>
+      <c r="D7" s="918"/>
       <c r="E7" s="201"/>
       <c r="F7" s="201"/>
       <c r="G7" s="201"/>
       <c r="H7" s="201"/>
       <c r="I7" s="201"/>
-      <c r="J7" s="925"/>
-      <c r="K7" s="925"/>
-      <c r="L7" s="925"/>
+      <c r="J7" s="918"/>
+      <c r="K7" s="918"/>
+      <c r="L7" s="918"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="201"/>
       <c r="P7" s="202" t="s">
         <v>243</v>
       </c>
-      <c r="Q7" s="925"/>
-      <c r="R7" s="925"/>
-      <c r="S7" s="925"/>
+      <c r="Q7" s="918"/>
+      <c r="R7" s="918"/>
+      <c r="S7" s="918"/>
       <c r="T7" s="201"/>
       <c r="U7" s="215"/>
       <c r="V7" s="372"/>
       <c r="W7" s="372" t="s">
         <v>243</v>
       </c>
-      <c r="X7" s="925"/>
-      <c r="Y7" s="925"/>
-      <c r="Z7" s="925"/>
+      <c r="X7" s="918"/>
+      <c r="Y7" s="918"/>
+      <c r="Z7" s="918"/>
       <c r="AA7" s="372"/>
       <c r="AB7" s="215"/>
     </row>
@@ -61552,54 +61585,54 @@
       <c r="B9" s="216" t="s">
         <v>450</v>
       </c>
-      <c r="C9" s="920" t="s">
+      <c r="C9" s="919" t="s">
         <v>244</v>
       </c>
-      <c r="D9" s="921"/>
-      <c r="E9" s="920" t="s">
+      <c r="D9" s="920"/>
+      <c r="E9" s="919" t="s">
         <v>245</v>
       </c>
-      <c r="F9" s="921"/>
+      <c r="F9" s="920"/>
       <c r="G9" s="201"/>
       <c r="H9" s="201"/>
       <c r="I9" s="201"/>
       <c r="J9" s="216" t="s">
         <v>450</v>
       </c>
-      <c r="K9" s="920" t="s">
+      <c r="K9" s="919" t="s">
         <v>244</v>
       </c>
-      <c r="L9" s="921"/>
-      <c r="M9" s="920" t="s">
+      <c r="L9" s="920"/>
+      <c r="M9" s="919" t="s">
         <v>245</v>
       </c>
-      <c r="N9" s="921"/>
+      <c r="N9" s="920"/>
       <c r="O9" s="201"/>
       <c r="P9" s="201"/>
       <c r="Q9" s="216" t="s">
         <v>450</v>
       </c>
-      <c r="R9" s="920" t="s">
+      <c r="R9" s="919" t="s">
         <v>244</v>
       </c>
-      <c r="S9" s="921"/>
-      <c r="T9" s="920" t="s">
+      <c r="S9" s="920"/>
+      <c r="T9" s="919" t="s">
         <v>245</v>
       </c>
-      <c r="U9" s="921"/>
+      <c r="U9" s="920"/>
       <c r="V9" s="372"/>
       <c r="W9" s="372"/>
       <c r="X9" s="216" t="s">
         <v>450</v>
       </c>
-      <c r="Y9" s="920" t="s">
+      <c r="Y9" s="919" t="s">
         <v>244</v>
       </c>
-      <c r="Z9" s="921"/>
-      <c r="AA9" s="920" t="s">
+      <c r="Z9" s="920"/>
+      <c r="AA9" s="919" t="s">
         <v>245</v>
       </c>
-      <c r="AB9" s="921"/>
+      <c r="AB9" s="920"/>
     </row>
     <row r="10" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="200"/>
@@ -61678,10 +61711,10 @@
       </c>
       <c r="C11" s="221"/>
       <c r="D11" s="221"/>
-      <c r="E11" s="917" t="s">
+      <c r="E11" s="916" t="s">
         <v>249</v>
       </c>
-      <c r="F11" s="918"/>
+      <c r="F11" s="917"/>
       <c r="G11" s="222"/>
       <c r="H11" s="222"/>
       <c r="I11" s="222"/>
@@ -61690,10 +61723,10 @@
       </c>
       <c r="K11" s="201"/>
       <c r="L11" s="201"/>
-      <c r="M11" s="922" t="s">
+      <c r="M11" s="923" t="s">
         <v>249</v>
       </c>
-      <c r="N11" s="923"/>
+      <c r="N11" s="924"/>
       <c r="O11" s="222"/>
       <c r="P11" s="222"/>
       <c r="Q11" s="220" t="s">
@@ -61701,10 +61734,10 @@
       </c>
       <c r="R11" s="221"/>
       <c r="S11" s="221"/>
-      <c r="T11" s="917" t="s">
+      <c r="T11" s="916" t="s">
         <v>249</v>
       </c>
-      <c r="U11" s="918"/>
+      <c r="U11" s="917"/>
       <c r="V11" s="372"/>
       <c r="W11" s="372"/>
       <c r="X11" s="220" t="s">
@@ -61712,10 +61745,10 @@
       </c>
       <c r="Y11" s="221"/>
       <c r="Z11" s="221"/>
-      <c r="AA11" s="917" t="s">
+      <c r="AA11" s="916" t="s">
         <v>249</v>
       </c>
-      <c r="AB11" s="918"/>
+      <c r="AB11" s="917"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="200"/>
@@ -62020,10 +62053,10 @@
       </c>
       <c r="C20" s="302"/>
       <c r="D20" s="249"/>
-      <c r="E20" s="917" t="s">
+      <c r="E20" s="916" t="s">
         <v>256</v>
       </c>
-      <c r="F20" s="918"/>
+      <c r="F20" s="917"/>
       <c r="G20" s="230"/>
       <c r="H20" s="230"/>
       <c r="I20" s="201"/>
@@ -62032,10 +62065,10 @@
       </c>
       <c r="K20" s="302"/>
       <c r="L20" s="249"/>
-      <c r="M20" s="917" t="s">
+      <c r="M20" s="916" t="s">
         <v>256</v>
       </c>
-      <c r="N20" s="918"/>
+      <c r="N20" s="917"/>
       <c r="O20" s="240"/>
       <c r="P20" s="240"/>
       <c r="Q20" s="220" t="s">
@@ -62043,10 +62076,10 @@
       </c>
       <c r="R20" s="302"/>
       <c r="S20" s="249"/>
-      <c r="T20" s="917" t="s">
+      <c r="T20" s="916" t="s">
         <v>256</v>
       </c>
-      <c r="U20" s="918"/>
+      <c r="U20" s="917"/>
       <c r="V20" s="277"/>
       <c r="W20" s="277"/>
       <c r="X20" s="220" t="s">
@@ -62054,10 +62087,10 @@
       </c>
       <c r="Y20" s="302"/>
       <c r="Z20" s="249"/>
-      <c r="AA20" s="917" t="s">
+      <c r="AA20" s="916" t="s">
         <v>256</v>
       </c>
-      <c r="AB20" s="918"/>
+      <c r="AB20" s="917"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="200"/>
@@ -62400,10 +62433,10 @@
       </c>
       <c r="C30" s="302"/>
       <c r="D30" s="249"/>
-      <c r="E30" s="917" t="s">
+      <c r="E30" s="916" t="s">
         <v>256</v>
       </c>
-      <c r="F30" s="918"/>
+      <c r="F30" s="917"/>
       <c r="G30" s="230"/>
       <c r="H30" s="230"/>
       <c r="I30" s="201"/>
@@ -62412,10 +62445,10 @@
       </c>
       <c r="K30" s="302"/>
       <c r="L30" s="249"/>
-      <c r="M30" s="917" t="s">
+      <c r="M30" s="916" t="s">
         <v>589</v>
       </c>
-      <c r="N30" s="918"/>
+      <c r="N30" s="917"/>
       <c r="O30" s="240"/>
       <c r="P30" s="240"/>
       <c r="Q30" s="220" t="s">
@@ -62423,10 +62456,10 @@
       </c>
       <c r="R30" s="302"/>
       <c r="S30" s="249"/>
-      <c r="T30" s="917" t="s">
+      <c r="T30" s="916" t="s">
         <v>256</v>
       </c>
-      <c r="U30" s="918"/>
+      <c r="U30" s="917"/>
       <c r="V30" s="277"/>
       <c r="W30" s="277"/>
       <c r="X30" s="220" t="s">
@@ -62434,10 +62467,10 @@
       </c>
       <c r="Y30" s="302"/>
       <c r="Z30" s="249"/>
-      <c r="AA30" s="917" t="s">
+      <c r="AA30" s="916" t="s">
         <v>256</v>
       </c>
-      <c r="AB30" s="918"/>
+      <c r="AB30" s="917"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="262"/>
@@ -62875,11 +62908,11 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="200"/>
-      <c r="B42" s="919"/>
-      <c r="C42" s="919"/>
-      <c r="D42" s="919"/>
-      <c r="E42" s="919"/>
-      <c r="F42" s="919"/>
+      <c r="B42" s="922"/>
+      <c r="C42" s="922"/>
+      <c r="D42" s="922"/>
+      <c r="E42" s="922"/>
+      <c r="F42" s="922"/>
       <c r="G42" s="240"/>
       <c r="H42" s="201"/>
       <c r="I42" s="240"/>
@@ -63066,21 +63099,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="26">
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -63092,6 +63110,21 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA20:AB20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add discalimer for art 5.4
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368" activeTab="5"/>
+    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'agglomeration level'!$A$4:$CW$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">Agglomerationout!$A$5:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">breach_list!$B$7:$N$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Glossary!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Glossary!$A$8:$B$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Information on sensitive area'!$A$7:$AQ$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'New agglomerations'!$A$5:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'New treatment plants'!$A$4:$F$4</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="615">
   <si>
     <t>Acronym</t>
   </si>
@@ -2085,9 +2085,6 @@
     <t>EXP-PD</t>
   </si>
   <si>
-    <t>EXPired deadline - Pending Deadline (used when deadline date different for the articles 3, 4 and 5)</t>
-  </si>
-  <si>
     <t>FW</t>
   </si>
   <si>
@@ -2125,9 +2122,6 @@
   </si>
   <si>
     <t xml:space="preserve">NPO   </t>
-  </si>
-  <si>
-    <t>No Information provided (and required/needed)</t>
   </si>
   <si>
     <t xml:space="preserve">O </t>
@@ -2172,22 +2166,10 @@
     <t>SA history</t>
   </si>
   <si>
-    <t>This sheet presents in summary the status of the sensitve areas and their historical change(s) where relevant.</t>
-  </si>
-  <si>
     <t>entering load calculated</t>
   </si>
   <si>
-    <t>(sheet UWWTP Level) The load is calculated from the share (%) of generated load of agglomeration collected in collecting system and entering particular plant which is declared at agglomeration level.</t>
-  </si>
-  <si>
-    <t>(sheet UWWTP Level) The load entering the treatment plant is declared at the plant level. If difference with entering load calculated &gt;30%, warning message.</t>
-  </si>
-  <si>
     <t>In case of discharge on land</t>
-  </si>
-  <si>
-    <t>(sheet UWWTP Level) Refers to situations where discharged waste water is reused at least partly for infiltration, irrigation or other purposes.</t>
   </si>
   <si>
     <t>Starting date of application 5 N</t>
@@ -2202,25 +2184,10 @@
     <t>(sheet UWWTP Level and sheet agglomeration level) Refers to starting date of application of criterion P for the sensitive area. It is relevant for sensitive areas under article 5(4) and under 5(2,3)P</t>
   </si>
   <si>
-    <t>(sheet UWWTP Level) Refers to situations where the country reported equipment to treat nutrients and no monitoring results for N and/or P or monitoring results and no equipment.</t>
-  </si>
-  <si>
-    <t>(sheet agglomeration level) These columns present the agglomeration information in previous reporting. It can be a different agglomeration in some cases.</t>
-  </si>
-  <si>
-    <t>(sheet agglomeration leve &amp; distance to compliance) it represents the remaining effort necessary to meet the required level for the article. For the treatment, it is separated in equipment and performance of the equipment. The DTT on collection is added to the DTT for article 4 and where relevant article 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">monitoring results meet requirements </t>
   </si>
   <si>
-    <t>(sheet distance to compliance) for each level of treatment, it is necessary to reach a fixed performance (reduction of load) on a set of monitored parameters. This performance is summarised by year for each parameter by a simple word: pass or fail. Monitoring results meet requirements only if all parameters for this level of treatment are pass.</t>
-  </si>
-  <si>
     <t>Summary_installation_in_place</t>
-  </si>
-  <si>
-    <t>This sheet presents at country level aggregated values for waste water collection and treatment situation when for each level of treatment respectively equipment is in place and performance = pass. This is different from sheet summary legal compliance which considers all rules of the Directive.</t>
   </si>
   <si>
     <t>NR (reference: wastewater load connected to collecting system)</t>
@@ -2325,6 +2292,150 @@
   <si>
     <t>of which DTT due to insufficient collection</t>
   </si>
+  <si>
+    <t>EXPired deadline - Pending Deadline (used when deadline date different for the articles 3, 4 and 5 and at least one deadline is not expired)</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>discharge on land (catchment of coastal water)</t>
+  </si>
+  <si>
+    <t>No Information provided (while this is required by reporting/needed)</t>
+  </si>
+  <si>
+    <t>(sheet UWWTP Level, columns Q &amp; R) Member States have to report the share (%) of generated load (this is often a theoretical value derived from a specific methodology to include anticipated evolutions of an agglomeration, see definition in terms and definitions) of agglomeration collected in collecting system and entering the different plants which are connected to this agglomeration. This value is shown in column Q and the load is calculated in column R.</t>
+  </si>
+  <si>
+    <t>(sheet UWWTP Level, columns S &amp; T) Member States have to report the load entering the treatment plants. This is often based on monitoring at plant level. The value is presented in column T and the % of generated load of the agglomeration it is connected to is calculated. If difference with entering load calculated is &gt;30%, a feedback to MS is made to check why.</t>
+  </si>
+  <si>
+    <r>
+      <t>(sheet final graphs, agglomeration level, distance to compliance &amp; Summary_big_cities) it represents the remaining effort necessary to meet the required level for complying with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the article (and with UWWTD) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>in the agglomeration in question</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. For the collection, it covers part of generated waste water not currently collected. It is conveyed to DTT for article 4 and 5 because waste water not currently collected needs to be collected but also afterwards be treated. For the treatment, it is separated in "equipment in place" and performance of the equipment i.e. "monitoring results meet requirements". The DTT on collection is added to the DTT for article 4 and where relevant article 5. DTT for "monitoring results meet requirements" generally include also DTT "equipment in place" because it is rarely possible to reach the performance without equipment.  There are however some exceptions because some specific secondary treatment allow good performance on nutrient removal or because under UWWTD it is not required to report monitoring results for more stringent treatment in case of discharge in catchment of sensitive areas. The DTT refered to in part "pending deadline" of the tables refers to situations where the agglomerations have still pending deadline and do not need currently to reach this level of equipment respectively performance. It allow also see separately the remaining effort necessary for those agglomerations.</t>
+    </r>
+  </si>
+  <si>
+    <t>For different reasons, local situation may differ and in particular waste water is treated to an higher degree than what is required as a minimum under UWWTD. This sheet presents, at country level, aggregated values for waste water collection and treatment situation when for each level of treatment respectively equipment is in place and monitoring results = pass. This is different from sheet summary legal compliance which considers solely the minimum requirements of the Directive. column BQ = 1 if secondary treatment in place, column BR if COD and BOD performance = pass, column BS if BQ+BR=2 (equipment + performance) and same for the following. In some cases compliance art4 fail because of issue in collection, but installation and performance are correct. In some cases MS declare a more stringent treatment while the standard directive rule do not require.</t>
+  </si>
+  <si>
+    <t>Information on sensitive area</t>
+  </si>
+  <si>
+    <t>this sheet presents in summary the status of the sensitive areas and details on their specificities: zone type, parameters, dates for designation and application, link to other areas, and for article 5(4) number of plants and loads. Normally a single area applies only one specialised zone type (article 5(8), article 5(4) or article 5(2,3)) but in the case of France, the country applies both article 5(4) and article 5(2,3) and therefore dates can be found in columns K &amp; M, N, P and Q.</t>
+  </si>
+  <si>
+    <t>This sheet presents in summary the status of the sensitive areas and their historical change(s) along the various reportings where relevant. It is used to check coherence of situation and changes introduced if any.</t>
+  </si>
+  <si>
+    <t>(sheet UWWTP Level) Refers to situations where discharged waste water is reused at least partly. This value should be reported if part or all the treated waste water is reused and possible values are " infiltration", "irrigation" or "other purposes". When more than one discharge point, it is possible that different reuse may be reported. In such case they are listed and separated by a ";".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(sheet UWWTP Level column AW) For treatment, in particular of nutrients N and P two information are reported: the equipment in place and the monitoring results of this treatment. In some cases the reporting does not include both information. This column therefore indicate when both information are reported with "no" and when this is not the case with "yes". </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(sheet agglomeration level columns N to Q) These columns present the same information than previous columns of this table, taken from previous reporting, to allow compare current situation with previous reporting. It can be a different agglomeration in some cases. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(sheet distance to compliance &amp; summary installation in place) For waste water treatment, it is necessary to reach a so called </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Minimum percentage of reduction in relation to the load of the influent." (table 1 and 2 of annexe I of UWWTD)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for parameters BOD5 and COD for secondary treatment and in addition for parameters Ntot and/or Ptot and or other parameter for more stringent treatment. Member States have to monitor these paramaters. When the minimum percentage is reached for one of the parameters, it is summarised in the reporting by a simple word: "pass" or "fail". In sheet "distance to compliance" these information are used to calculate if, for a waste water treatm ent plant, the monitoring results meet UWWTD requirements. This is the case only if all parameters for this level of treatment (secondary or more stringent) are = "pass". In sheet "summary installation in place" these information are used to calculate if, for a waste water treatment plant, the monitoring results reported meet the specific level of treatment (secondary respectively more stringent), with no consideration of  UWWTD requirements, i.e. including cases in which it is not required by the UWWTD. For agglomerations without obligations under the Directive, it is not mandatory to report monitoring results, this is why generally there is a significant difference between equipment and monitoring results for article 5 in sheet summary installation in place.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(sheet distance to compliance &amp; summary installation in place) For waste water treatment, it is necessary under article 4 to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"ensure that urban waste water entering collecting systems shall before discharge be subject to secondary treatment"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and respectively under article 5 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"ensure that urban waste water entering collecting systems shall before discharge into sensitive areas be subject to more stringent treatment"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Member States have to report the treatment for each of their treatment plant in categories "primary", "secondary", "Other" (for more stringent treatment) and details for more stringent in categories "Nremoval", "Premoval", "UV", "Chlorination", "ozonation", "sand filtration", "microfiltration"  and "other". In sheet "distance to compliance" these information are used to calculate if, for a waste water treatment plant, the equipment reported (in place) meet UWWTD requirements. This is the case only if all equipment for this level of treatment (secondary or more stringent) are reported. In sheet "summary installation in place" these information are used to calculate if, for a waste water treatment plant, the equipment reported (in place) meet the specific level of treatment (secondary respectively more stringent), with no consideration of  UWWTD requirements, i.e. including cases in which it is not required by the UWWTD.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -2337,7 +2448,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\/mm\/dd"/>
     <numFmt numFmtId="168" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2640,6 +2751,38 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="49">
@@ -3789,7 +3932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="993">
+  <cellXfs count="1001">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -5656,9 +5799,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="45" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -5776,45 +5916,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -5849,6 +5950,9 @@
     <xf numFmtId="3" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5897,6 +6001,111 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5909,21 +6118,12 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5939,59 +6139,11 @@
     <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6002,12 +6154,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6020,26 +6166,26 @@
     <xf numFmtId="0" fontId="25" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6069,6 +6215,33 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6101,39 +6274,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6157,6 +6297,64 @@
     <xf numFmtId="3" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6169,18 +6367,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6193,51 +6379,32 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="46" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="48" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6550,9 +6717,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6561,378 +6730,438 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="769" t="s">
+      <c r="A1" s="1000"/>
+      <c r="B1" s="992"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="771"/>
+      <c r="B2" s="772"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="769"/>
+      <c r="B3" s="772"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="769"/>
+      <c r="B4" s="772"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="769"/>
+      <c r="B5" s="772"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="769"/>
+      <c r="B6" s="772"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="769"/>
+      <c r="B7" s="772"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="994" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="770" t="s">
+      <c r="B8" s="992" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="771" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="995" t="s">
         <v>461</v>
       </c>
-      <c r="B2" s="772" t="s">
+      <c r="B9" s="772" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="769" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="996" t="s">
         <v>522</v>
       </c>
-      <c r="B3" s="772" t="s">
+      <c r="B10" s="772" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="769" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="996" t="s">
         <v>523</v>
       </c>
-      <c r="B4" s="772" t="s">
+      <c r="B11" s="772" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="769" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="996" t="s">
         <v>524</v>
       </c>
-      <c r="B5" s="770" t="s">
+      <c r="B12" s="770" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="769" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="996" t="s">
         <v>525</v>
       </c>
-      <c r="B6" s="770" t="s">
+      <c r="B13" s="770" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="769" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="996" t="s">
         <v>526</v>
       </c>
-      <c r="B7" s="770" t="s">
+      <c r="B14" s="770" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="769" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="996" t="s">
         <v>527</v>
       </c>
-      <c r="B8" s="770" t="s">
+      <c r="B15" s="770" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="769" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="996" t="s">
         <v>528</v>
       </c>
-      <c r="B9" s="770" t="s">
+      <c r="B16" s="770" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="769" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="996" t="s">
         <v>529</v>
       </c>
-      <c r="B10" s="770" t="s">
+      <c r="B17" s="770" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="996" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="769" t="s">
+      <c r="B18" s="770" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="996" t="s">
         <v>531</v>
       </c>
-      <c r="B11" s="770" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="769" t="s">
+      <c r="B19" s="770" t="s">
         <v>532</v>
       </c>
-      <c r="B12" s="770" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="996" t="s">
+        <v>600</v>
+      </c>
+      <c r="B20" s="770" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="996" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="769" t="s">
+      <c r="B21" s="770" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="996" t="s">
         <v>534</v>
       </c>
-      <c r="B13" s="770" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="769" t="s">
+      <c r="B22" s="770" t="s">
         <v>535</v>
       </c>
-      <c r="B14" s="770" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="996" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="770" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="769" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="770" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="996" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="770" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="769" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="770" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="996" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="769" t="s">
+      <c r="B25" s="770" t="s">
         <v>539</v>
       </c>
-      <c r="B17" s="770" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="996" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="769" t="s">
+      <c r="B26" s="770" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="996" t="s">
         <v>541</v>
       </c>
-      <c r="B18" s="770" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="769" t="s">
+      <c r="B27" s="770" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="996" t="s">
         <v>542</v>
       </c>
-      <c r="B19" s="770" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="769" t="s">
+      <c r="B28" s="770" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="996" t="s">
+        <v>496</v>
+      </c>
+      <c r="B29" s="772" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="996" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" s="770" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="996" t="s">
+        <v>490</v>
+      </c>
+      <c r="B31" s="770" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="996" t="s">
+        <v>492</v>
+      </c>
+      <c r="B32" s="770" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="996" t="s">
         <v>543</v>
       </c>
-      <c r="B20" s="770" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="769" t="s">
-        <v>496</v>
-      </c>
-      <c r="B21" s="772" t="s">
+      <c r="B33" s="770" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="996" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="769" t="s">
-        <v>223</v>
-      </c>
-      <c r="B22" s="770" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="769" t="s">
-        <v>490</v>
-      </c>
-      <c r="B23" s="770" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="769" t="s">
-        <v>492</v>
-      </c>
-      <c r="B24" s="770" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="769" t="s">
+      <c r="B34" s="770" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="996" t="s">
         <v>545</v>
       </c>
-      <c r="B25" s="770" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="769" t="s">
+      <c r="B35" s="770" t="s">
         <v>546</v>
       </c>
-      <c r="B26" s="770" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="769" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="996" t="s">
         <v>547</v>
       </c>
-      <c r="B27" s="770" t="s">
+      <c r="B36" s="770" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="996">
+        <v>1</v>
+      </c>
+      <c r="B37" s="770" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="996" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="769" t="s">
+      <c r="B38" s="770" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="996">
+        <v>2</v>
+      </c>
+      <c r="B39" s="770" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="996" t="s">
         <v>549</v>
       </c>
-      <c r="B28" s="770" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="769">
-        <v>1</v>
-      </c>
-      <c r="B29" s="770" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="769" t="s">
+      <c r="B40" s="770" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="996" t="s">
         <v>550</v>
       </c>
-      <c r="B30" s="770" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="769">
-        <v>2</v>
-      </c>
-      <c r="B31" s="770" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="769" t="s">
+      <c r="B41" s="770" t="s">
         <v>551</v>
       </c>
-      <c r="B32" s="770" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="769" t="s">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="997" t="s">
         <v>552</v>
       </c>
-      <c r="B33" s="770" t="s">
+      <c r="B42" s="993" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="773" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="996" t="s">
         <v>554</v>
       </c>
-      <c r="B34" s="774" t="s">
+      <c r="B43" s="993" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="769" t="s">
+    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="996" t="s">
         <v>556</v>
       </c>
-      <c r="B35" s="774" t="s">
+      <c r="B44" s="770" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="997" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="769" t="s">
+      <c r="B45" s="770" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="997" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="770" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="997" t="s">
         <v>558</v>
       </c>
-      <c r="B36" s="770" t="s">
+      <c r="B47" s="993" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="997" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="773" t="s">
+      <c r="B48" s="993" t="s">
         <v>560</v>
       </c>
-      <c r="B37" s="770" t="s">
+    </row>
+    <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="997" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="773" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="770" t="s">
+      <c r="B49" s="993" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="773" t="s">
+    <row r="50" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="998" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="772" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="997" t="s">
+        <v>507</v>
+      </c>
+      <c r="B51" s="772" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="997" t="s">
+        <v>517</v>
+      </c>
+      <c r="B52" s="993" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="997" t="s">
         <v>563</v>
       </c>
-      <c r="B39" s="774" t="s">
+      <c r="B53" s="993" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="997" t="s">
+        <v>511</v>
+      </c>
+      <c r="B54" s="999" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A55" s="997" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="773" t="s">
-        <v>565</v>
-      </c>
-      <c r="B40" s="774" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="773" t="s">
-        <v>567</v>
-      </c>
-      <c r="B41" s="774" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="775" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" s="774" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="773" t="s">
-        <v>507</v>
-      </c>
-      <c r="B43" s="774" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="773" t="s">
-        <v>517</v>
-      </c>
-      <c r="B44" s="774" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="773" t="s">
-        <v>572</v>
-      </c>
-      <c r="B45" s="774" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="773" t="s">
-        <v>574</v>
-      </c>
-      <c r="B46" s="774" t="s">
-        <v>575</v>
-      </c>
+      <c r="B55" s="993" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A56" s="997" t="s">
+        <v>607</v>
+      </c>
+      <c r="B56" s="993" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="997"/>
+      <c r="B57" s="993"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="997"/>
+      <c r="B58" s="993"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A1:B1"/>
+  <autoFilter ref="A8:B8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6965,8 +7194,8 @@
       <c r="B3" s="324" t="s">
         <v>227</v>
       </c>
-      <c r="C3" s="925"/>
-      <c r="D3" s="925"/>
+      <c r="C3" s="926"/>
+      <c r="D3" s="926"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C4" s="325"/>
@@ -6999,10 +7228,10 @@
       <c r="D10" s="332" t="s">
         <v>265</v>
       </c>
-      <c r="E10" s="926" t="s">
+      <c r="E10" s="927" t="s">
         <v>517</v>
       </c>
-      <c r="F10" s="927"/>
+      <c r="F10" s="928"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="333" t="s">
@@ -7055,7 +7284,7 @@
       <c r="C15" s="346"/>
       <c r="D15" s="351"/>
       <c r="E15" s="352"/>
-      <c r="F15" s="800"/>
+      <c r="F15" s="799"/>
     </row>
     <row r="16" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="340" t="s">
@@ -7064,34 +7293,34 @@
       <c r="C16" s="347"/>
       <c r="D16" s="353"/>
       <c r="E16" s="353"/>
-      <c r="F16" s="801"/>
+      <c r="F16" s="800"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="338" t="s">
-        <v>606</v>
-      </c>
-      <c r="C17" s="820"/>
-      <c r="D17" s="806"/>
-      <c r="E17" s="804"/>
-      <c r="F17" s="800"/>
+        <v>595</v>
+      </c>
+      <c r="C17" s="819"/>
+      <c r="D17" s="805"/>
+      <c r="E17" s="803"/>
+      <c r="F17" s="799"/>
     </row>
     <row r="18" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="797" t="s">
+      <c r="B18" s="796" t="s">
         <v>269</v>
       </c>
-      <c r="C18" s="803"/>
-      <c r="D18" s="805"/>
-      <c r="E18" s="805"/>
-      <c r="F18" s="809"/>
+      <c r="C18" s="802"/>
+      <c r="D18" s="804"/>
+      <c r="E18" s="804"/>
+      <c r="F18" s="808"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="818" t="s">
-        <v>579</v>
-      </c>
-      <c r="C19" s="819"/>
-      <c r="D19" s="821"/>
-      <c r="E19" s="821"/>
-      <c r="F19" s="808"/>
+      <c r="B19" s="817" t="s">
+        <v>568</v>
+      </c>
+      <c r="C19" s="818"/>
+      <c r="D19" s="820"/>
+      <c r="E19" s="820"/>
+      <c r="F19" s="807"/>
     </row>
     <row r="20" spans="2:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="341" t="s">
@@ -7100,16 +7329,16 @@
       <c r="C20" s="347"/>
       <c r="D20" s="354"/>
       <c r="E20" s="354"/>
-      <c r="F20" s="801"/>
+      <c r="F20" s="800"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="338" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="C21" s="345"/>
       <c r="D21" s="350"/>
       <c r="E21" s="350"/>
-      <c r="F21" s="800"/>
+      <c r="F21" s="799"/>
     </row>
     <row r="22" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="369" t="s">
@@ -7118,16 +7347,16 @@
       <c r="C22" s="345"/>
       <c r="D22" s="350"/>
       <c r="E22" s="350"/>
-      <c r="F22" s="800"/>
+      <c r="F22" s="799"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="802" t="s">
-        <v>579</v>
+      <c r="B23" s="801" t="s">
+        <v>568</v>
       </c>
       <c r="C23" s="363"/>
       <c r="D23" s="362"/>
       <c r="E23" s="361"/>
-      <c r="F23" s="801"/>
+      <c r="F23" s="800"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D26" s="326"/>
@@ -7157,10 +7386,10 @@
       <c r="D30" s="342" t="s">
         <v>265</v>
       </c>
-      <c r="E30" s="926" t="s">
+      <c r="E30" s="927" t="s">
         <v>517</v>
       </c>
-      <c r="F30" s="927"/>
+      <c r="F30" s="928"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="333" t="s">
@@ -7213,7 +7442,7 @@
       <c r="C35" s="346"/>
       <c r="D35" s="351"/>
       <c r="E35" s="352"/>
-      <c r="F35" s="800"/>
+      <c r="F35" s="799"/>
     </row>
     <row r="36" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="340" t="s">
@@ -7222,34 +7451,34 @@
       <c r="C36" s="347"/>
       <c r="D36" s="353"/>
       <c r="E36" s="353"/>
-      <c r="F36" s="801"/>
+      <c r="F36" s="800"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="338" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="C37" s="345"/>
       <c r="D37" s="350"/>
       <c r="E37" s="350"/>
-      <c r="F37" s="800"/>
+      <c r="F37" s="799"/>
     </row>
     <row r="38" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="811" t="s">
-        <v>608</v>
-      </c>
-      <c r="C38" s="798"/>
-      <c r="D38" s="805"/>
-      <c r="E38" s="805"/>
-      <c r="F38" s="809"/>
+      <c r="B38" s="810" t="s">
+        <v>597</v>
+      </c>
+      <c r="C38" s="797"/>
+      <c r="D38" s="804"/>
+      <c r="E38" s="804"/>
+      <c r="F38" s="808"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="814" t="s">
-        <v>609</v>
-      </c>
-      <c r="C39" s="815"/>
-      <c r="D39" s="821"/>
-      <c r="E39" s="821"/>
-      <c r="F39" s="808"/>
+      <c r="B39" s="813" t="s">
+        <v>598</v>
+      </c>
+      <c r="C39" s="814"/>
+      <c r="D39" s="820"/>
+      <c r="E39" s="820"/>
+      <c r="F39" s="807"/>
     </row>
     <row r="40" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="341" t="s">
@@ -7258,34 +7487,34 @@
       <c r="C40" s="347"/>
       <c r="D40" s="354"/>
       <c r="E40" s="354"/>
-      <c r="F40" s="801"/>
+      <c r="F40" s="800"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="338" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="C41" s="345"/>
       <c r="D41" s="350"/>
       <c r="E41" s="350"/>
-      <c r="F41" s="800"/>
+      <c r="F41" s="799"/>
     </row>
     <row r="42" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="369" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
       <c r="C42" s="345"/>
       <c r="D42" s="350"/>
       <c r="E42" s="350"/>
-      <c r="F42" s="800"/>
+      <c r="F42" s="799"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="814" t="s">
-        <v>609</v>
+      <c r="B43" s="813" t="s">
+        <v>598</v>
       </c>
       <c r="C43" s="360"/>
       <c r="D43" s="355"/>
       <c r="E43" s="359"/>
-      <c r="F43" s="801"/>
+      <c r="F43" s="800"/>
     </row>
     <row r="46" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B46" s="327" t="s">
@@ -7312,10 +7541,10 @@
       <c r="D49" s="342" t="s">
         <v>265</v>
       </c>
-      <c r="E49" s="926" t="s">
+      <c r="E49" s="927" t="s">
         <v>517</v>
       </c>
-      <c r="F49" s="927"/>
+      <c r="F49" s="928"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="333" t="s">
@@ -7368,7 +7597,7 @@
       <c r="C54" s="346"/>
       <c r="D54" s="351"/>
       <c r="E54" s="352"/>
-      <c r="F54" s="800"/>
+      <c r="F54" s="799"/>
     </row>
     <row r="55" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="340" t="s">
@@ -7377,34 +7606,34 @@
       <c r="C55" s="347"/>
       <c r="D55" s="353"/>
       <c r="E55" s="353"/>
-      <c r="F55" s="801"/>
+      <c r="F55" s="800"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" s="338" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="C56" s="345"/>
-      <c r="D56" s="799"/>
-      <c r="E56" s="806"/>
-      <c r="F56" s="807"/>
+      <c r="D56" s="798"/>
+      <c r="E56" s="805"/>
+      <c r="F56" s="806"/>
     </row>
     <row r="57" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="817" t="s">
-        <v>607</v>
-      </c>
-      <c r="C57" s="798"/>
-      <c r="D57" s="805"/>
-      <c r="E57" s="805"/>
-      <c r="F57" s="809"/>
+      <c r="B57" s="816" t="s">
+        <v>596</v>
+      </c>
+      <c r="C57" s="797"/>
+      <c r="D57" s="804"/>
+      <c r="E57" s="804"/>
+      <c r="F57" s="808"/>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B58" s="813" t="s">
-        <v>609</v>
-      </c>
-      <c r="C58" s="815"/>
-      <c r="D58" s="821"/>
-      <c r="E58" s="821"/>
-      <c r="F58" s="808"/>
+      <c r="B58" s="812" t="s">
+        <v>598</v>
+      </c>
+      <c r="C58" s="814"/>
+      <c r="D58" s="820"/>
+      <c r="E58" s="820"/>
+      <c r="F58" s="807"/>
     </row>
     <row r="59" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="340" t="s">
@@ -7413,16 +7642,16 @@
       <c r="C59" s="347"/>
       <c r="D59" s="354"/>
       <c r="E59" s="354"/>
-      <c r="F59" s="801"/>
+      <c r="F59" s="800"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="338" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="C60" s="345"/>
       <c r="D60" s="350"/>
       <c r="E60" s="350"/>
-      <c r="F60" s="800"/>
+      <c r="F60" s="799"/>
     </row>
     <row r="61" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="369" t="s">
@@ -7431,16 +7660,16 @@
       <c r="C61" s="345"/>
       <c r="D61" s="350"/>
       <c r="E61" s="350"/>
-      <c r="F61" s="800"/>
+      <c r="F61" s="799"/>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B62" s="802" t="s">
-        <v>609</v>
+      <c r="B62" s="801" t="s">
+        <v>598</v>
       </c>
       <c r="C62" s="360"/>
       <c r="D62" s="364"/>
       <c r="E62" s="361"/>
-      <c r="F62" s="801"/>
+      <c r="F62" s="800"/>
     </row>
     <row r="65" spans="2:6" ht="21" x14ac:dyDescent="0.4">
       <c r="B65" s="327" t="s">
@@ -7467,10 +7696,10 @@
       <c r="D68" s="342" t="s">
         <v>265</v>
       </c>
-      <c r="E68" s="926" t="s">
+      <c r="E68" s="927" t="s">
         <v>517</v>
       </c>
-      <c r="F68" s="927"/>
+      <c r="F68" s="928"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="504" t="s">
@@ -7523,7 +7752,7 @@
       <c r="C73" s="346"/>
       <c r="D73" s="351"/>
       <c r="E73" s="352"/>
-      <c r="F73" s="800"/>
+      <c r="F73" s="799"/>
     </row>
     <row r="74" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B74" s="340" t="s">
@@ -7532,34 +7761,34 @@
       <c r="C74" s="347"/>
       <c r="D74" s="353"/>
       <c r="E74" s="353"/>
-      <c r="F74" s="801"/>
+      <c r="F74" s="800"/>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B75" s="816" t="s">
-        <v>606</v>
-      </c>
-      <c r="C75" s="812"/>
+      <c r="B75" s="815" t="s">
+        <v>595</v>
+      </c>
+      <c r="C75" s="811"/>
       <c r="D75" s="350"/>
       <c r="E75" s="350"/>
-      <c r="F75" s="800"/>
+      <c r="F75" s="799"/>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B76" s="817" t="s">
-        <v>607</v>
-      </c>
-      <c r="C76" s="798"/>
-      <c r="D76" s="805"/>
-      <c r="E76" s="805"/>
-      <c r="F76" s="809"/>
+      <c r="B76" s="816" t="s">
+        <v>596</v>
+      </c>
+      <c r="C76" s="797"/>
+      <c r="D76" s="804"/>
+      <c r="E76" s="804"/>
+      <c r="F76" s="808"/>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B77" s="813" t="s">
-        <v>579</v>
-      </c>
-      <c r="C77" s="815"/>
-      <c r="D77" s="821"/>
-      <c r="E77" s="821"/>
-      <c r="F77" s="810"/>
+      <c r="B77" s="812" t="s">
+        <v>568</v>
+      </c>
+      <c r="C77" s="814"/>
+      <c r="D77" s="820"/>
+      <c r="E77" s="820"/>
+      <c r="F77" s="809"/>
     </row>
     <row r="78" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B78" s="340" t="s">
@@ -7568,34 +7797,34 @@
       <c r="C78" s="347"/>
       <c r="D78" s="354"/>
       <c r="E78" s="354"/>
-      <c r="F78" s="801"/>
+      <c r="F78" s="800"/>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="338" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="C79" s="345"/>
       <c r="D79" s="350"/>
       <c r="E79" s="350"/>
-      <c r="F79" s="800"/>
+      <c r="F79" s="799"/>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="369" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
       <c r="C80" s="345"/>
       <c r="D80" s="350"/>
       <c r="E80" s="350"/>
-      <c r="F80" s="800"/>
+      <c r="F80" s="799"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B81" s="802" t="s">
-        <v>609</v>
+      <c r="B81" s="801" t="s">
+        <v>598</v>
       </c>
       <c r="C81" s="360"/>
       <c r="D81" s="364"/>
       <c r="E81" s="361"/>
-      <c r="F81" s="801"/>
+      <c r="F81" s="800"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -7645,8 +7874,8 @@
       </c>
       <c r="C2" s="373"/>
       <c r="D2" s="373"/>
-      <c r="E2" s="921"/>
-      <c r="F2" s="921"/>
+      <c r="E2" s="924"/>
+      <c r="F2" s="924"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="372"/>
@@ -7678,13 +7907,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="370"/>
-      <c r="B6" s="918" t="s">
+      <c r="B6" s="925" t="s">
         <v>439</v>
       </c>
-      <c r="C6" s="918"/>
-      <c r="D6" s="918"/>
-      <c r="E6" s="918"/>
-      <c r="F6" s="918"/>
+      <c r="C6" s="925"/>
+      <c r="D6" s="925"/>
+      <c r="E6" s="925"/>
+      <c r="F6" s="925"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="370"/>
@@ -7699,14 +7928,14 @@
       <c r="B8" s="399" t="s">
         <v>471</v>
       </c>
-      <c r="C8" s="928" t="s">
+      <c r="C8" s="929" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="929"/>
-      <c r="E8" s="928" t="s">
+      <c r="D8" s="930"/>
+      <c r="E8" s="929" t="s">
         <v>233</v>
       </c>
-      <c r="F8" s="929"/>
+      <c r="F8" s="930"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="370"/>
@@ -7842,11 +8071,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="370"/>
-      <c r="B22" s="922"/>
-      <c r="C22" s="922"/>
-      <c r="D22" s="922"/>
-      <c r="E22" s="922"/>
-      <c r="F22" s="922"/>
+      <c r="B22" s="919"/>
+      <c r="C22" s="919"/>
+      <c r="D22" s="919"/>
+      <c r="E22" s="919"/>
+      <c r="F22" s="919"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="370"/>
@@ -7918,20 +8147,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="930" t="s">
+      <c r="B2" s="931" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="931" t="s">
+      <c r="C2" s="932" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="931" t="s">
+      <c r="D2" s="932" t="s">
         <v>168</v>
       </c>
       <c r="E2" s="424" t="s">
         <v>275</v>
       </c>
       <c r="F2" s="424" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="G2" s="424" t="s">
         <v>277</v>
@@ -7959,9 +8188,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="930"/>
-      <c r="C3" s="932"/>
-      <c r="D3" s="932"/>
+      <c r="B3" s="931"/>
+      <c r="C3" s="933"/>
+      <c r="D3" s="933"/>
       <c r="E3" s="439" t="s">
         <v>283</v>
       </c>
@@ -7994,7 +8223,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="933" t="s">
+      <c r="B4" s="934" t="s">
         <v>286</v>
       </c>
       <c r="C4" s="425" t="s">
@@ -8013,7 +8242,7 @@
       <c r="N4" s="427"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="933"/>
+      <c r="B5" s="934"/>
       <c r="C5" s="425" t="s">
         <v>83</v>
       </c>
@@ -8030,7 +8259,7 @@
       <c r="N5" s="427"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="934"/>
+      <c r="B6" s="935"/>
       <c r="C6" s="435" t="s">
         <v>276</v>
       </c>
@@ -8145,43 +8374,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="938" t="s">
+      <c r="A1" s="948" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="939"/>
+      <c r="B1" s="949"/>
       <c r="C1" s="455"/>
-      <c r="D1" s="949" t="s">
+      <c r="D1" s="939" t="s">
         <v>287</v>
       </c>
-      <c r="E1" s="950"/>
-      <c r="F1" s="950"/>
-      <c r="G1" s="950"/>
-      <c r="H1" s="950"/>
-      <c r="I1" s="951"/>
-      <c r="J1" s="940" t="s">
+      <c r="E1" s="940"/>
+      <c r="F1" s="940"/>
+      <c r="G1" s="940"/>
+      <c r="H1" s="940"/>
+      <c r="I1" s="941"/>
+      <c r="J1" s="950" t="s">
         <v>288</v>
       </c>
-      <c r="K1" s="941"/>
-      <c r="L1" s="941"/>
-      <c r="M1" s="941"/>
-      <c r="N1" s="942"/>
-      <c r="O1" s="943" t="s">
+      <c r="K1" s="951"/>
+      <c r="L1" s="951"/>
+      <c r="M1" s="951"/>
+      <c r="N1" s="952"/>
+      <c r="O1" s="953" t="s">
         <v>289</v>
       </c>
-      <c r="P1" s="944"/>
-      <c r="Q1" s="945"/>
+      <c r="P1" s="954"/>
+      <c r="Q1" s="955"/>
       <c r="R1" s="442" t="s">
         <v>71</v>
       </c>
       <c r="S1" s="443"/>
-      <c r="T1" s="937" t="s">
+      <c r="T1" s="947" t="s">
         <v>482</v>
       </c>
-      <c r="U1" s="937"/>
-      <c r="V1" s="937"/>
-      <c r="W1" s="937"/>
-      <c r="X1" s="937"/>
-      <c r="Y1" s="937"/>
+      <c r="U1" s="947"/>
+      <c r="V1" s="947"/>
+      <c r="W1" s="947"/>
+      <c r="X1" s="947"/>
+      <c r="Y1" s="947"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="445" t="s">
@@ -8193,18 +8422,18 @@
       <c r="C2" s="446" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="954" t="s">
+      <c r="D2" s="944" t="s">
         <v>291</v>
       </c>
-      <c r="E2" s="953"/>
-      <c r="F2" s="953" t="s">
+      <c r="E2" s="943"/>
+      <c r="F2" s="943" t="s">
         <v>292</v>
       </c>
-      <c r="G2" s="953"/>
-      <c r="H2" s="952" t="s">
+      <c r="G2" s="943"/>
+      <c r="H2" s="942" t="s">
         <v>293</v>
       </c>
-      <c r="I2" s="952"/>
+      <c r="I2" s="942"/>
       <c r="J2" s="447">
         <v>0</v>
       </c>
@@ -8235,18 +8464,18 @@
       <c r="S2" s="681" t="s">
         <v>81</v>
       </c>
-      <c r="T2" s="935" t="s">
+      <c r="T2" s="945" t="s">
         <v>451</v>
       </c>
-      <c r="U2" s="935"/>
-      <c r="V2" s="936" t="s">
+      <c r="U2" s="945"/>
+      <c r="V2" s="946" t="s">
         <v>468</v>
       </c>
-      <c r="W2" s="936"/>
-      <c r="X2" s="936" t="s">
+      <c r="W2" s="946"/>
+      <c r="X2" s="946" t="s">
         <v>469</v>
       </c>
-      <c r="Y2" s="936"/>
+      <c r="Y2" s="946"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="450"/>
@@ -8272,13 +8501,13 @@
       <c r="I3" s="665" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="946" t="s">
+      <c r="J3" s="936" t="s">
         <v>298</v>
       </c>
-      <c r="K3" s="947"/>
-      <c r="L3" s="947"/>
-      <c r="M3" s="947"/>
-      <c r="N3" s="948"/>
+      <c r="K3" s="937"/>
+      <c r="L3" s="937"/>
+      <c r="M3" s="937"/>
+      <c r="N3" s="938"/>
       <c r="O3" s="458"/>
       <c r="P3" s="458"/>
       <c r="Q3" s="458"/>
@@ -9507,11 +9736,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:X4"/>
   <mergeCells count="12">
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -9519,6 +9743,11 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9559,25 +9788,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="836" t="s">
+      <c r="A1" s="864" t="s">
         <v>299</v>
       </c>
-      <c r="B1" s="837"/>
-      <c r="C1" s="837"/>
-      <c r="D1" s="837"/>
-      <c r="E1" s="837"/>
-      <c r="F1" s="837"/>
+      <c r="B1" s="865"/>
+      <c r="C1" s="865"/>
+      <c r="D1" s="865"/>
+      <c r="E1" s="865"/>
+      <c r="F1" s="865"/>
       <c r="G1" s="472"/>
-      <c r="H1" s="961" t="s">
+      <c r="H1" s="960" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="962"/>
-      <c r="J1" s="962"/>
+      <c r="I1" s="961"/>
+      <c r="J1" s="961"/>
       <c r="K1" s="474"/>
       <c r="L1" s="464"/>
       <c r="M1" s="474"/>
       <c r="N1" s="465"/>
-      <c r="O1" s="959" t="s">
+      <c r="O1" s="958" t="s">
         <v>300</v>
       </c>
       <c r="P1" s="466"/>
@@ -9589,26 +9818,26 @@
       <c r="T1" s="464"/>
       <c r="U1" s="474"/>
       <c r="V1" s="465"/>
-      <c r="W1" s="959" t="s">
+      <c r="W1" s="958" t="s">
         <v>302</v>
       </c>
       <c r="X1" s="466"/>
-      <c r="Y1" s="963" t="s">
+      <c r="Y1" s="962" t="s">
         <v>303</v>
       </c>
-      <c r="Z1" s="963"/>
-      <c r="AA1" s="963"/>
-      <c r="AB1" s="963"/>
-      <c r="AC1" s="963"/>
-      <c r="AD1" s="964"/>
-      <c r="AE1" s="959" t="s">
+      <c r="Z1" s="962"/>
+      <c r="AA1" s="962"/>
+      <c r="AB1" s="962"/>
+      <c r="AC1" s="962"/>
+      <c r="AD1" s="963"/>
+      <c r="AE1" s="958" t="s">
         <v>304</v>
       </c>
-      <c r="AF1" s="958" t="s">
+      <c r="AF1" s="957" t="s">
         <v>467</v>
       </c>
-      <c r="AG1" s="937"/>
-      <c r="AH1" s="937"/>
+      <c r="AG1" s="947"/>
+      <c r="AH1" s="947"/>
       <c r="AI1" s="688"/>
       <c r="AJ1" s="688"/>
       <c r="AK1" s="688"/>
@@ -9667,56 +9896,56 @@
       <c r="C2" s="473" t="s">
         <v>306</v>
       </c>
-      <c r="D2" s="957" t="s">
+      <c r="D2" s="956" t="s">
         <v>472</v>
       </c>
-      <c r="E2" s="957"/>
-      <c r="F2" s="957" t="s">
+      <c r="E2" s="956"/>
+      <c r="F2" s="956" t="s">
         <v>473</v>
       </c>
-      <c r="G2" s="957"/>
+      <c r="G2" s="956"/>
       <c r="H2" s="468"/>
-      <c r="I2" s="955" t="s">
+      <c r="I2" s="964" t="s">
         <v>178</v>
       </c>
-      <c r="J2" s="955"/>
-      <c r="K2" s="955" t="s">
+      <c r="J2" s="964"/>
+      <c r="K2" s="964" t="s">
         <v>179</v>
       </c>
-      <c r="L2" s="955"/>
-      <c r="M2" s="955" t="s">
+      <c r="L2" s="964"/>
+      <c r="M2" s="964" t="s">
         <v>180</v>
       </c>
-      <c r="N2" s="956"/>
-      <c r="O2" s="960"/>
+      <c r="N2" s="965"/>
+      <c r="O2" s="959"/>
       <c r="P2" s="469"/>
-      <c r="Q2" s="955" t="s">
+      <c r="Q2" s="964" t="s">
         <v>178</v>
       </c>
-      <c r="R2" s="955"/>
-      <c r="S2" s="955" t="s">
+      <c r="R2" s="964"/>
+      <c r="S2" s="964" t="s">
         <v>179</v>
       </c>
-      <c r="T2" s="955"/>
-      <c r="U2" s="955" t="s">
+      <c r="T2" s="964"/>
+      <c r="U2" s="964" t="s">
         <v>180</v>
       </c>
-      <c r="V2" s="956"/>
-      <c r="W2" s="960"/>
+      <c r="V2" s="965"/>
+      <c r="W2" s="959"/>
       <c r="X2" s="469"/>
-      <c r="Y2" s="955" t="s">
+      <c r="Y2" s="964" t="s">
         <v>178</v>
       </c>
-      <c r="Z2" s="955"/>
-      <c r="AA2" s="955" t="s">
+      <c r="Z2" s="964"/>
+      <c r="AA2" s="964" t="s">
         <v>179</v>
       </c>
-      <c r="AB2" s="955"/>
-      <c r="AC2" s="955" t="s">
+      <c r="AB2" s="964"/>
+      <c r="AC2" s="964" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="956"/>
-      <c r="AE2" s="960"/>
+      <c r="AD2" s="965"/>
+      <c r="AE2" s="959"/>
       <c r="AF2" s="682" t="s">
         <v>451</v>
       </c>
@@ -10602,6 +10831,8 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:AH4"/>
   <mergeCells count="18">
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AE1:AE2"/>
@@ -10618,8 +10849,6 @@
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="U2:V2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10746,7 +10975,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="498" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="B18" s="499" t="s">
         <v>325</v>
@@ -10838,9 +11067,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="965"/>
-      <c r="B1" s="867"/>
-      <c r="C1" s="867"/>
+      <c r="A1" s="984"/>
+      <c r="B1" s="854"/>
+      <c r="C1" s="854"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="740"/>
@@ -10855,21 +11084,21 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="973" t="s">
+      <c r="A3" s="988" t="s">
         <v>332</v>
       </c>
-      <c r="B3" s="975" t="s">
+      <c r="B3" s="990" t="s">
         <v>440</v>
       </c>
-      <c r="C3" s="976"/>
-      <c r="D3" s="971" t="s">
+      <c r="C3" s="991"/>
+      <c r="D3" s="976" t="s">
         <v>441</v>
       </c>
-      <c r="E3" s="972"/>
-      <c r="F3" s="971" t="s">
+      <c r="E3" s="977"/>
+      <c r="F3" s="976" t="s">
         <v>475</v>
       </c>
-      <c r="G3" s="972"/>
+      <c r="G3" s="977"/>
       <c r="I3" s="738" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
@@ -10880,14 +11109,14 @@
       <c r="K3" s="720"/>
       <c r="L3" s="720"/>
       <c r="N3" s="705"/>
-      <c r="O3" s="987" t="s">
+      <c r="O3" s="973" t="s">
         <v>333</v>
       </c>
-      <c r="P3" s="987"/>
-      <c r="Q3" s="987" t="s">
+      <c r="P3" s="973"/>
+      <c r="Q3" s="973" t="s">
         <v>334</v>
       </c>
-      <c r="R3" s="987"/>
+      <c r="R3" s="973"/>
       <c r="S3" s="705"/>
       <c r="T3" s="713" t="s">
         <v>335</v>
@@ -10895,7 +11124,7 @@
       <c r="U3" s="705"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="974"/>
+      <c r="A4" s="989"/>
       <c r="B4" s="512" t="s">
         <v>336</v>
       </c>
@@ -11154,14 +11383,14 @@
       <c r="K10" s="720"/>
       <c r="L10" s="720"/>
       <c r="N10" s="713"/>
-      <c r="O10" s="987" t="s">
+      <c r="O10" s="973" t="s">
         <v>336</v>
       </c>
-      <c r="P10" s="987"/>
-      <c r="Q10" s="987" t="s">
+      <c r="P10" s="973"/>
+      <c r="Q10" s="973" t="s">
         <v>343</v>
       </c>
-      <c r="R10" s="987"/>
+      <c r="R10" s="973"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I11" s="738" t="str">
@@ -11225,7 +11454,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="973" t="s">
+      <c r="A13" s="988" t="s">
         <v>344</v>
       </c>
       <c r="B13" s="511" t="str">
@@ -11271,7 +11500,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="974"/>
+      <c r="A14" s="989"/>
       <c r="B14" s="514" t="s">
         <v>337</v>
       </c>
@@ -11401,34 +11630,34 @@
       <c r="A21" s="502" t="s">
         <v>349</v>
       </c>
-      <c r="B21" s="988" t="s">
+      <c r="B21" s="978" t="s">
         <v>494</v>
       </c>
-      <c r="C21" s="989"/>
-      <c r="D21" s="989"/>
-      <c r="E21" s="989"/>
-      <c r="F21" s="989"/>
-      <c r="G21" s="989"/>
+      <c r="C21" s="979"/>
+      <c r="D21" s="979"/>
+      <c r="E21" s="979"/>
+      <c r="F21" s="979"/>
+      <c r="G21" s="979"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="516" t="s">
         <v>313</v>
       </c>
-      <c r="B22" s="977" t="str">
+      <c r="B22" s="980" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="978"/>
-      <c r="D22" s="977" t="str">
+      <c r="C22" s="981"/>
+      <c r="D22" s="980" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="978"/>
-      <c r="F22" s="977" t="str">
+      <c r="E22" s="981"/>
+      <c r="F22" s="980" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="978"/>
+      <c r="G22" s="981"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="517"/>
@@ -11855,21 +12084,21 @@
       <c r="A41" s="519" t="s">
         <v>359</v>
       </c>
-      <c r="B41" s="967" t="str">
+      <c r="B41" s="986" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="968"/>
-      <c r="D41" s="969" t="str">
+      <c r="C41" s="987"/>
+      <c r="D41" s="974" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="970"/>
-      <c r="F41" s="969" t="str">
+      <c r="E41" s="975"/>
+      <c r="F41" s="974" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G41" s="970"/>
+      <c r="G41" s="975"/>
       <c r="N41" s="705"/>
       <c r="O41" s="732" t="s">
         <v>445</v>
@@ -12083,11 +12312,11 @@
       <c r="F53" s="710" t="s">
         <v>500</v>
       </c>
-      <c r="H53" s="990" t="s">
+      <c r="H53" s="966" t="s">
         <v>487</v>
       </c>
-      <c r="I53" s="990"/>
-      <c r="J53" s="990"/>
+      <c r="I53" s="966"/>
+      <c r="J53" s="966"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="701" t="s">
@@ -12257,11 +12486,11 @@
       <c r="F63" s="710" t="s">
         <v>500</v>
       </c>
-      <c r="H63" s="990" t="s">
+      <c r="H63" s="966" t="s">
         <v>501</v>
       </c>
-      <c r="I63" s="990"/>
-      <c r="J63" s="990"/>
+      <c r="I63" s="966"/>
+      <c r="J63" s="966"/>
       <c r="L63" s="708"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -12448,12 +12677,12 @@
       <c r="A74" s="623" t="s">
         <v>358</v>
       </c>
-      <c r="B74" s="966" t="s">
+      <c r="B74" s="985" t="s">
         <v>442</v>
       </c>
-      <c r="C74" s="966"/>
-      <c r="D74" s="966"/>
-      <c r="E74" s="966"/>
+      <c r="C74" s="985"/>
+      <c r="D74" s="985"/>
+      <c r="E74" s="985"/>
       <c r="I74" s="709"/>
       <c r="J74" s="709"/>
       <c r="K74" s="709"/>
@@ -12769,36 +12998,36 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="981" t="str">
+      <c r="B85" s="971" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="982"/>
-      <c r="D85" s="981" t="str">
+      <c r="C85" s="972"/>
+      <c r="D85" s="971" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="982"/>
-      <c r="F85" s="981" t="str">
+      <c r="E85" s="972"/>
+      <c r="F85" s="971" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="982"/>
+      <c r="G85" s="972"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="503"/>
-      <c r="B86" s="926" t="s">
+      <c r="B86" s="927" t="s">
         <v>266</v>
       </c>
-      <c r="C86" s="927"/>
-      <c r="D86" s="926" t="s">
+      <c r="C86" s="928"/>
+      <c r="D86" s="927" t="s">
         <v>266</v>
       </c>
-      <c r="E86" s="927"/>
-      <c r="F86" s="926" t="s">
+      <c r="E86" s="928"/>
+      <c r="F86" s="927" t="s">
         <v>266</v>
       </c>
-      <c r="G86" s="927"/>
+      <c r="G86" s="928"/>
       <c r="N86" s="713" t="s">
         <v>385</v>
       </c>
@@ -13079,36 +13308,36 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="981" t="str">
+      <c r="B101" s="971" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="982"/>
-      <c r="D101" s="981" t="str">
+      <c r="C101" s="972"/>
+      <c r="D101" s="971" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="982"/>
-      <c r="F101" s="981" t="str">
+      <c r="E101" s="972"/>
+      <c r="F101" s="971" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="982"/>
+      <c r="G101" s="972"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="503"/>
-      <c r="B102" s="926" t="s">
+      <c r="B102" s="927" t="s">
         <v>266</v>
       </c>
-      <c r="C102" s="927"/>
-      <c r="D102" s="926" t="s">
+      <c r="C102" s="928"/>
+      <c r="D102" s="927" t="s">
         <v>266</v>
       </c>
-      <c r="E102" s="927"/>
-      <c r="F102" s="926" t="s">
+      <c r="E102" s="928"/>
+      <c r="F102" s="927" t="s">
         <v>266</v>
       </c>
-      <c r="G102" s="927"/>
+      <c r="G102" s="928"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="504" t="s">
@@ -13389,36 +13618,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="983" t="str">
+      <c r="B116" s="967" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="984"/>
-      <c r="D116" s="983" t="str">
+      <c r="C116" s="968"/>
+      <c r="D116" s="967" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="984"/>
-      <c r="F116" s="983" t="str">
+      <c r="E116" s="968"/>
+      <c r="F116" s="967" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="984"/>
+      <c r="G116" s="968"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="542"/>
-      <c r="B117" s="985" t="s">
+      <c r="B117" s="969" t="s">
         <v>266</v>
       </c>
-      <c r="C117" s="986"/>
-      <c r="D117" s="985" t="s">
+      <c r="C117" s="970"/>
+      <c r="D117" s="969" t="s">
         <v>266</v>
       </c>
-      <c r="E117" s="986"/>
-      <c r="F117" s="985" t="s">
+      <c r="E117" s="970"/>
+      <c r="F117" s="969" t="s">
         <v>266</v>
       </c>
-      <c r="G117" s="986"/>
+      <c r="G117" s="970"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="543" t="s">
@@ -13721,12 +13950,12 @@
       <c r="A129" s="546" t="s">
         <v>344</v>
       </c>
-      <c r="B129" s="979" t="str">
+      <c r="B129" s="982" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="980"/>
-      <c r="D129" s="980"/>
+      <c r="C129" s="983"/>
+      <c r="D129" s="983"/>
       <c r="N129" s="713" t="s">
         <v>385</v>
       </c>
@@ -13948,7 +14177,7 @@
     </row>
     <row r="150" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="556" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="B150" s="556" t="s">
         <v>63</v>
@@ -13967,7 +14196,7 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" s="556" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="B151" s="556" t="s">
         <v>63</v>
@@ -14502,22 +14731,16 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="39">
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -14531,16 +14754,22 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17940,66 +18169,66 @@
       <c r="AQ3" s="6"/>
     </row>
     <row r="4" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="825" t="s">
+      <c r="A4" s="824" t="s">
         <v>497</v>
       </c>
-      <c r="B4" s="826"/>
-      <c r="C4" s="826"/>
-      <c r="D4" s="826"/>
-      <c r="E4" s="826"/>
-      <c r="F4" s="827"/>
-      <c r="G4" s="827"/>
-      <c r="H4" s="827"/>
-      <c r="I4" s="827"/>
-      <c r="J4" s="827"/>
-      <c r="K4" s="827"/>
-      <c r="L4" s="827"/>
-      <c r="M4" s="827"/>
-      <c r="N4" s="827"/>
-      <c r="O4" s="827"/>
-      <c r="P4" s="827"/>
-      <c r="Q4" s="827"/>
-      <c r="R4" s="827"/>
-      <c r="S4" s="827"/>
-      <c r="T4" s="827"/>
-      <c r="U4" s="827"/>
-      <c r="V4" s="827"/>
-      <c r="W4" s="827"/>
-      <c r="X4" s="827"/>
-      <c r="Y4" s="827"/>
-      <c r="Z4" s="827"/>
-      <c r="AA4" s="827"/>
-      <c r="AB4" s="827"/>
-      <c r="AC4" s="827"/>
-      <c r="AD4" s="827"/>
-      <c r="AE4" s="827"/>
-      <c r="AF4" s="827"/>
-      <c r="AG4" s="827"/>
-      <c r="AH4" s="827"/>
-      <c r="AI4" s="827"/>
-      <c r="AJ4" s="827"/>
-      <c r="AK4" s="827"/>
-      <c r="AL4" s="827"/>
-      <c r="AM4" s="827"/>
-      <c r="AN4" s="827"/>
-      <c r="AO4" s="827"/>
-      <c r="AP4" s="827"/>
-      <c r="AQ4" s="827"/>
+      <c r="B4" s="825"/>
+      <c r="C4" s="825"/>
+      <c r="D4" s="825"/>
+      <c r="E4" s="825"/>
+      <c r="F4" s="826"/>
+      <c r="G4" s="826"/>
+      <c r="H4" s="826"/>
+      <c r="I4" s="826"/>
+      <c r="J4" s="826"/>
+      <c r="K4" s="826"/>
+      <c r="L4" s="826"/>
+      <c r="M4" s="826"/>
+      <c r="N4" s="826"/>
+      <c r="O4" s="826"/>
+      <c r="P4" s="826"/>
+      <c r="Q4" s="826"/>
+      <c r="R4" s="826"/>
+      <c r="S4" s="826"/>
+      <c r="T4" s="826"/>
+      <c r="U4" s="826"/>
+      <c r="V4" s="826"/>
+      <c r="W4" s="826"/>
+      <c r="X4" s="826"/>
+      <c r="Y4" s="826"/>
+      <c r="Z4" s="826"/>
+      <c r="AA4" s="826"/>
+      <c r="AB4" s="826"/>
+      <c r="AC4" s="826"/>
+      <c r="AD4" s="826"/>
+      <c r="AE4" s="826"/>
+      <c r="AF4" s="826"/>
+      <c r="AG4" s="826"/>
+      <c r="AH4" s="826"/>
+      <c r="AI4" s="826"/>
+      <c r="AJ4" s="826"/>
+      <c r="AK4" s="826"/>
+      <c r="AL4" s="826"/>
+      <c r="AM4" s="826"/>
+      <c r="AN4" s="826"/>
+      <c r="AO4" s="826"/>
+      <c r="AP4" s="826"/>
+      <c r="AQ4" s="826"/>
     </row>
     <row r="5" spans="1:43" s="7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="828" t="s">
+      <c r="A5" s="827" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="828" t="s">
+      <c r="B5" s="827" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="795" t="s">
-        <v>580</v>
-      </c>
-      <c r="D5" s="828" t="s">
+      <c r="C5" s="794" t="s">
+        <v>569</v>
+      </c>
+      <c r="D5" s="827" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="828" t="s">
+      <c r="E5" s="827" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="12" t="s">
@@ -18024,34 +18253,34 @@
         <v>35</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="S5" s="16" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
       <c r="T5" s="16" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
       <c r="U5" s="16" t="s">
-        <v>603</v>
+        <v>592</v>
       </c>
       <c r="V5" s="16" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
       <c r="W5" s="16" t="s">
         <v>37</v>
@@ -18059,10 +18288,10 @@
       <c r="X5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="Y5" s="830" t="s">
-        <v>605</v>
-      </c>
-      <c r="Z5" s="830" t="s">
+      <c r="Y5" s="829" t="s">
+        <v>594</v>
+      </c>
+      <c r="Z5" s="829" t="s">
         <v>39</v>
       </c>
       <c r="AA5" s="16" t="s">
@@ -18092,7 +18321,7 @@
       <c r="AI5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="AJ5" s="830" t="s">
+      <c r="AJ5" s="829" t="s">
         <v>48</v>
       </c>
       <c r="AK5" s="16" t="s">
@@ -18101,28 +18330,28 @@
       <c r="AL5" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="AM5" s="828" t="s">
+      <c r="AM5" s="827" t="s">
         <v>51</v>
       </c>
-      <c r="AN5" s="828" t="s">
+      <c r="AN5" s="827" t="s">
         <v>52</v>
       </c>
-      <c r="AO5" s="828" t="s">
+      <c r="AO5" s="827" t="s">
         <v>53</v>
       </c>
-      <c r="AP5" s="828" t="s">
+      <c r="AP5" s="827" t="s">
         <v>54</v>
       </c>
-      <c r="AQ5" s="828" t="s">
+      <c r="AQ5" s="827" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:43" s="9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="829"/>
-      <c r="B6" s="829"/>
-      <c r="C6" s="796"/>
-      <c r="D6" s="829"/>
-      <c r="E6" s="829"/>
+      <c r="A6" s="828"/>
+      <c r="B6" s="828"/>
+      <c r="C6" s="795"/>
+      <c r="D6" s="828"/>
+      <c r="E6" s="828"/>
       <c r="F6" s="14" t="s">
         <v>56</v>
       </c>
@@ -18180,8 +18409,8 @@
       <c r="X6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Y6" s="831"/>
-      <c r="Z6" s="831"/>
+      <c r="Y6" s="830"/>
+      <c r="Z6" s="830"/>
       <c r="AA6" s="9" t="s">
         <v>57</v>
       </c>
@@ -18209,18 +18438,18 @@
       <c r="AI6" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AJ6" s="831"/>
+      <c r="AJ6" s="830"/>
       <c r="AK6" s="9" t="s">
         <v>57</v>
       </c>
       <c r="AL6" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AM6" s="829"/>
-      <c r="AN6" s="829"/>
-      <c r="AO6" s="829"/>
-      <c r="AP6" s="829"/>
-      <c r="AQ6" s="829"/>
+      <c r="AM6" s="828"/>
+      <c r="AN6" s="828"/>
+      <c r="AO6" s="828"/>
+      <c r="AP6" s="828"/>
+      <c r="AQ6" s="828"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="AE7" s="8"/>
@@ -18234,7 +18463,7 @@
     <row r="9" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A9" s="662"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="822"/>
+      <c r="C9" s="821"/>
       <c r="D9" s="662"/>
       <c r="E9" s="662"/>
       <c r="F9" s="662"/>
@@ -58390,36 +58619,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="753" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="776"/>
-      <c r="B1" s="776"/>
-      <c r="C1" s="776"/>
-      <c r="D1" s="777"/>
-      <c r="E1" s="778"/>
-      <c r="F1" s="778"/>
-      <c r="G1" s="779"/>
-      <c r="H1" s="780"/>
-      <c r="I1" s="780"/>
-      <c r="J1" s="781"/>
-      <c r="K1" s="782"/>
-      <c r="L1" s="782"/>
-      <c r="M1" s="783"/>
-      <c r="N1" s="784"/>
-      <c r="O1" s="784"/>
-      <c r="P1" s="785"/>
-      <c r="Q1" s="786"/>
-      <c r="R1" s="786"/>
-      <c r="S1" s="787"/>
-      <c r="T1" s="788"/>
-      <c r="U1" s="788"/>
-      <c r="V1" s="789"/>
-      <c r="W1" s="790"/>
-      <c r="X1" s="790"/>
-      <c r="Y1" s="791"/>
-      <c r="Z1" s="792"/>
-      <c r="AA1" s="792"/>
-      <c r="AB1" s="793"/>
-      <c r="AC1" s="794"/>
-      <c r="AD1" s="794"/>
+      <c r="A1" s="775"/>
+      <c r="B1" s="775"/>
+      <c r="C1" s="775"/>
+      <c r="D1" s="776"/>
+      <c r="E1" s="777"/>
+      <c r="F1" s="777"/>
+      <c r="G1" s="778"/>
+      <c r="H1" s="779"/>
+      <c r="I1" s="779"/>
+      <c r="J1" s="780"/>
+      <c r="K1" s="781"/>
+      <c r="L1" s="781"/>
+      <c r="M1" s="782"/>
+      <c r="N1" s="783"/>
+      <c r="O1" s="783"/>
+      <c r="P1" s="784"/>
+      <c r="Q1" s="785"/>
+      <c r="R1" s="785"/>
+      <c r="S1" s="786"/>
+      <c r="T1" s="787"/>
+      <c r="U1" s="787"/>
+      <c r="V1" s="788"/>
+      <c r="W1" s="789"/>
+      <c r="X1" s="789"/>
+      <c r="Y1" s="790"/>
+      <c r="Z1" s="791"/>
+      <c r="AA1" s="791"/>
+      <c r="AB1" s="792"/>
+      <c r="AC1" s="793"/>
+      <c r="AD1" s="793"/>
     </row>
     <row r="2" spans="1:30" s="752" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="742"/>
@@ -58483,20 +58712,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="58.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="832" t="s">
+      <c r="A1" s="831" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="834" t="s">
+      <c r="B1" s="833" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="823" t="s">
-        <v>584</v>
+      <c r="C1" s="822" t="s">
+        <v>573</v>
       </c>
       <c r="D1" s="766" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
       <c r="E1" s="766" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="F1" s="661" t="s">
         <v>502</v>
@@ -58536,8 +58765,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="833"/>
-      <c r="B2" s="835"/>
+      <c r="A2" s="832"/>
+      <c r="B2" s="834"/>
       <c r="C2" s="9" t="s">
         <v>57</v>
       </c>
@@ -58702,123 +58931,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="658" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="836" t="s">
+      <c r="A1" s="864" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="837"/>
-      <c r="C1" s="837"/>
-      <c r="D1" s="837"/>
-      <c r="E1" s="837"/>
-      <c r="F1" s="837"/>
-      <c r="G1" s="837"/>
-      <c r="H1" s="838" t="s">
+      <c r="B1" s="865"/>
+      <c r="C1" s="865"/>
+      <c r="D1" s="865"/>
+      <c r="E1" s="865"/>
+      <c r="F1" s="865"/>
+      <c r="G1" s="865"/>
+      <c r="H1" s="866" t="s">
         <v>451</v>
       </c>
-      <c r="I1" s="839"/>
-      <c r="J1" s="839"/>
-      <c r="K1" s="839"/>
-      <c r="L1" s="839"/>
-      <c r="M1" s="840"/>
-      <c r="N1" s="841" t="s">
+      <c r="I1" s="867"/>
+      <c r="J1" s="867"/>
+      <c r="K1" s="867"/>
+      <c r="L1" s="867"/>
+      <c r="M1" s="868"/>
+      <c r="N1" s="869" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="842"/>
-      <c r="P1" s="842"/>
-      <c r="Q1" s="842"/>
-      <c r="R1" s="842"/>
-      <c r="S1" s="842"/>
-      <c r="T1" s="842"/>
-      <c r="U1" s="842"/>
-      <c r="V1" s="843" t="s">
+      <c r="O1" s="847"/>
+      <c r="P1" s="847"/>
+      <c r="Q1" s="847"/>
+      <c r="R1" s="847"/>
+      <c r="S1" s="847"/>
+      <c r="T1" s="847"/>
+      <c r="U1" s="847"/>
+      <c r="V1" s="870" t="s">
         <v>73</v>
       </c>
-      <c r="W1" s="844"/>
-      <c r="X1" s="845"/>
-      <c r="Y1" s="845"/>
-      <c r="Z1" s="846"/>
-      <c r="AA1" s="847" t="s">
+      <c r="W1" s="871"/>
+      <c r="X1" s="872"/>
+      <c r="Y1" s="872"/>
+      <c r="Z1" s="873"/>
+      <c r="AA1" s="874" t="s">
         <v>74</v>
       </c>
-      <c r="AB1" s="848"/>
-      <c r="AC1" s="848"/>
-      <c r="AD1" s="848"/>
-      <c r="AE1" s="848"/>
-      <c r="AF1" s="848"/>
-      <c r="AG1" s="848"/>
-      <c r="AH1" s="848"/>
-      <c r="AI1" s="848"/>
-      <c r="AJ1" s="848"/>
-      <c r="AK1" s="848"/>
-      <c r="AL1" s="848"/>
-      <c r="AM1" s="848"/>
+      <c r="AB1" s="875"/>
+      <c r="AC1" s="875"/>
+      <c r="AD1" s="875"/>
+      <c r="AE1" s="875"/>
+      <c r="AF1" s="875"/>
+      <c r="AG1" s="875"/>
+      <c r="AH1" s="875"/>
+      <c r="AI1" s="875"/>
+      <c r="AJ1" s="875"/>
+      <c r="AK1" s="875"/>
+      <c r="AL1" s="875"/>
+      <c r="AM1" s="875"/>
       <c r="AN1" s="52"/>
       <c r="AO1" s="53"/>
-      <c r="AP1" s="860" t="s">
+      <c r="AP1" s="846" t="s">
         <v>75</v>
       </c>
-      <c r="AQ1" s="842"/>
-      <c r="AR1" s="842"/>
-      <c r="AS1" s="842"/>
-      <c r="AT1" s="842"/>
-      <c r="AU1" s="842"/>
-      <c r="AV1" s="842"/>
-      <c r="AW1" s="861"/>
-      <c r="AX1" s="868" t="s">
-        <v>581</v>
-      </c>
-      <c r="AY1" s="869"/>
-      <c r="AZ1" s="869"/>
-      <c r="BA1" s="869"/>
-      <c r="BB1" s="869"/>
-      <c r="BC1" s="870"/>
-      <c r="BD1" s="871" t="s">
+      <c r="AQ1" s="847"/>
+      <c r="AR1" s="847"/>
+      <c r="AS1" s="847"/>
+      <c r="AT1" s="847"/>
+      <c r="AU1" s="847"/>
+      <c r="AV1" s="847"/>
+      <c r="AW1" s="848"/>
+      <c r="AX1" s="855" t="s">
+        <v>570</v>
+      </c>
+      <c r="AY1" s="856"/>
+      <c r="AZ1" s="856"/>
+      <c r="BA1" s="856"/>
+      <c r="BB1" s="856"/>
+      <c r="BC1" s="857"/>
+      <c r="BD1" s="858" t="s">
         <v>76</v>
       </c>
-      <c r="BE1" s="872"/>
-      <c r="BF1" s="872"/>
-      <c r="BG1" s="872"/>
-      <c r="BH1" s="872"/>
-      <c r="BI1" s="873"/>
-      <c r="BJ1" s="874" t="s">
+      <c r="BE1" s="859"/>
+      <c r="BF1" s="859"/>
+      <c r="BG1" s="859"/>
+      <c r="BH1" s="859"/>
+      <c r="BI1" s="860"/>
+      <c r="BJ1" s="861" t="s">
         <v>77</v>
       </c>
-      <c r="BK1" s="875"/>
-      <c r="BL1" s="875"/>
-      <c r="BM1" s="875"/>
-      <c r="BN1" s="875"/>
-      <c r="BO1" s="875"/>
-      <c r="BP1" s="876"/>
-      <c r="BQ1" s="849" t="s">
+      <c r="BK1" s="862"/>
+      <c r="BL1" s="862"/>
+      <c r="BM1" s="862"/>
+      <c r="BN1" s="862"/>
+      <c r="BO1" s="862"/>
+      <c r="BP1" s="863"/>
+      <c r="BQ1" s="835" t="s">
         <v>78</v>
       </c>
-      <c r="BR1" s="850"/>
-      <c r="BS1" s="850"/>
-      <c r="BT1" s="850"/>
-      <c r="BU1" s="850"/>
-      <c r="BV1" s="850"/>
+      <c r="BR1" s="836"/>
+      <c r="BS1" s="836"/>
+      <c r="BT1" s="836"/>
+      <c r="BU1" s="836"/>
+      <c r="BV1" s="836"/>
       <c r="BW1" s="53"/>
       <c r="BX1" s="54"/>
-      <c r="BY1" s="851" t="s">
+      <c r="BY1" s="837" t="s">
         <v>79</v>
       </c>
-      <c r="BZ1" s="852"/>
-      <c r="CA1" s="852"/>
-      <c r="CB1" s="852"/>
-      <c r="CC1" s="852"/>
-      <c r="CD1" s="852"/>
-      <c r="CE1" s="852"/>
-      <c r="CF1" s="853"/>
-      <c r="CG1" s="853"/>
-      <c r="CH1" s="853"/>
-      <c r="CI1" s="853"/>
-      <c r="CJ1" s="853"/>
-      <c r="CK1" s="853"/>
-      <c r="CL1" s="853"/>
-      <c r="CM1" s="853"/>
-      <c r="CN1" s="853"/>
-      <c r="CO1" s="853"/>
-      <c r="CP1" s="853"/>
-      <c r="CQ1" s="853"/>
+      <c r="BZ1" s="838"/>
+      <c r="CA1" s="838"/>
+      <c r="CB1" s="838"/>
+      <c r="CC1" s="838"/>
+      <c r="CD1" s="838"/>
+      <c r="CE1" s="838"/>
+      <c r="CF1" s="839"/>
+      <c r="CG1" s="839"/>
+      <c r="CH1" s="839"/>
+      <c r="CI1" s="839"/>
+      <c r="CJ1" s="839"/>
+      <c r="CK1" s="839"/>
+      <c r="CL1" s="839"/>
+      <c r="CM1" s="839"/>
+      <c r="CN1" s="839"/>
+      <c r="CO1" s="839"/>
+      <c r="CP1" s="839"/>
+      <c r="CQ1" s="839"/>
     </row>
     <row r="2" spans="1:95" s="658" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -58842,18 +59071,18 @@
       <c r="G2" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="854" t="s">
+      <c r="H2" s="840" t="s">
         <v>452</v>
       </c>
-      <c r="I2" s="855"/>
-      <c r="J2" s="855" t="s">
+      <c r="I2" s="841"/>
+      <c r="J2" s="841" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="855"/>
-      <c r="L2" s="855" t="s">
+      <c r="K2" s="841"/>
+      <c r="L2" s="841" t="s">
         <v>88</v>
       </c>
-      <c r="M2" s="856"/>
+      <c r="M2" s="842"/>
       <c r="N2" s="57" t="s">
         <v>80</v>
       </c>
@@ -58962,36 +59191,36 @@
       <c r="AW2" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="AX2" s="857" t="s">
+      <c r="AX2" s="843" t="s">
         <v>115</v>
       </c>
-      <c r="AY2" s="858"/>
-      <c r="AZ2" s="858"/>
-      <c r="BA2" s="858" t="s">
+      <c r="AY2" s="844"/>
+      <c r="AZ2" s="844"/>
+      <c r="BA2" s="844" t="s">
         <v>116</v>
       </c>
-      <c r="BB2" s="858"/>
-      <c r="BC2" s="859"/>
-      <c r="BD2" s="862" t="s">
+      <c r="BB2" s="844"/>
+      <c r="BC2" s="845"/>
+      <c r="BD2" s="849" t="s">
         <v>115</v>
       </c>
-      <c r="BE2" s="863"/>
-      <c r="BF2" s="863"/>
-      <c r="BG2" s="863" t="s">
+      <c r="BE2" s="850"/>
+      <c r="BF2" s="850"/>
+      <c r="BG2" s="850" t="s">
         <v>116</v>
       </c>
-      <c r="BH2" s="863"/>
-      <c r="BI2" s="864"/>
-      <c r="BJ2" s="865" t="s">
+      <c r="BH2" s="850"/>
+      <c r="BI2" s="851"/>
+      <c r="BJ2" s="852" t="s">
         <v>115</v>
       </c>
-      <c r="BK2" s="866"/>
-      <c r="BL2" s="866"/>
-      <c r="BM2" s="866" t="s">
+      <c r="BK2" s="853"/>
+      <c r="BL2" s="853"/>
+      <c r="BM2" s="853" t="s">
         <v>116</v>
       </c>
-      <c r="BN2" s="867"/>
-      <c r="BO2" s="867"/>
+      <c r="BN2" s="854"/>
+      <c r="BO2" s="854"/>
       <c r="BP2" s="69" t="s">
         <v>117</v>
       </c>
@@ -59624,6 +59853,11 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -59639,11 +59873,6 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -59655,7 +59884,7 @@
   <sheetPr codeName="Feuil6"/>
   <dimension ref="A1:CZ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="BP5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -59727,127 +59956,127 @@
         <v>157</v>
       </c>
       <c r="L1" s="145"/>
-      <c r="M1" s="877" t="s">
+      <c r="M1" s="899" t="s">
         <v>158</v>
       </c>
-      <c r="N1" s="878" t="s">
+      <c r="N1" s="900" t="s">
         <v>507</v>
       </c>
-      <c r="O1" s="879"/>
-      <c r="P1" s="879"/>
-      <c r="Q1" s="879"/>
-      <c r="R1" s="880" t="s">
+      <c r="O1" s="901"/>
+      <c r="P1" s="901"/>
+      <c r="Q1" s="901"/>
+      <c r="R1" s="902" t="s">
         <v>451</v>
       </c>
-      <c r="S1" s="881"/>
-      <c r="T1" s="881"/>
-      <c r="U1" s="881"/>
-      <c r="V1" s="881"/>
-      <c r="W1" s="881"/>
-      <c r="X1" s="882"/>
-      <c r="Y1" s="883" t="s">
+      <c r="S1" s="895"/>
+      <c r="T1" s="895"/>
+      <c r="U1" s="895"/>
+      <c r="V1" s="895"/>
+      <c r="W1" s="895"/>
+      <c r="X1" s="903"/>
+      <c r="Y1" s="889" t="s">
         <v>459</v>
       </c>
-      <c r="Z1" s="872"/>
-      <c r="AA1" s="886" t="s">
+      <c r="Z1" s="859"/>
+      <c r="AA1" s="905" t="s">
         <v>159</v>
       </c>
-      <c r="AB1" s="897" t="s">
+      <c r="AB1" s="877" t="s">
         <v>160</v>
       </c>
-      <c r="AC1" s="893" t="s">
+      <c r="AC1" s="891" t="s">
         <v>161</v>
       </c>
-      <c r="AD1" s="894"/>
-      <c r="AE1" s="894"/>
-      <c r="AF1" s="895"/>
-      <c r="AG1" s="896" t="s">
+      <c r="AD1" s="892"/>
+      <c r="AE1" s="892"/>
+      <c r="AF1" s="893"/>
+      <c r="AG1" s="894" t="s">
         <v>162</v>
       </c>
-      <c r="AH1" s="881"/>
-      <c r="AI1" s="881"/>
-      <c r="AJ1" s="881"/>
-      <c r="AK1" s="881"/>
-      <c r="AL1" s="881"/>
-      <c r="AM1" s="881"/>
-      <c r="AN1" s="881"/>
-      <c r="AO1" s="897" t="s">
+      <c r="AH1" s="895"/>
+      <c r="AI1" s="895"/>
+      <c r="AJ1" s="895"/>
+      <c r="AK1" s="895"/>
+      <c r="AL1" s="895"/>
+      <c r="AM1" s="895"/>
+      <c r="AN1" s="895"/>
+      <c r="AO1" s="877" t="s">
         <v>163</v>
       </c>
-      <c r="AP1" s="883" t="s">
+      <c r="AP1" s="889" t="s">
         <v>458</v>
       </c>
-      <c r="AQ1" s="872"/>
-      <c r="AR1" s="872"/>
-      <c r="AS1" s="873"/>
-      <c r="AT1" s="900" t="s">
+      <c r="AQ1" s="859"/>
+      <c r="AR1" s="859"/>
+      <c r="AS1" s="860"/>
+      <c r="AT1" s="897" t="s">
         <v>164</v>
       </c>
-      <c r="AU1" s="901"/>
-      <c r="AV1" s="901"/>
-      <c r="AW1" s="901"/>
-      <c r="AX1" s="901"/>
-      <c r="AY1" s="901"/>
-      <c r="AZ1" s="901"/>
-      <c r="BA1" s="901"/>
-      <c r="BB1" s="901"/>
-      <c r="BC1" s="901"/>
-      <c r="BD1" s="901"/>
-      <c r="BE1" s="901"/>
-      <c r="BF1" s="901"/>
-      <c r="BG1" s="901"/>
-      <c r="BH1" s="901"/>
-      <c r="BI1" s="901"/>
-      <c r="BJ1" s="901"/>
-      <c r="BK1" s="901"/>
-      <c r="BL1" s="901"/>
-      <c r="BM1" s="901"/>
-      <c r="BN1" s="901"/>
-      <c r="BO1" s="901"/>
-      <c r="BP1" s="901"/>
-      <c r="BQ1" s="901"/>
-      <c r="BR1" s="901"/>
-      <c r="BS1" s="901"/>
-      <c r="BT1" s="901"/>
-      <c r="BU1" s="901"/>
-      <c r="BV1" s="901"/>
-      <c r="BW1" s="897" t="s">
+      <c r="AU1" s="898"/>
+      <c r="AV1" s="898"/>
+      <c r="AW1" s="898"/>
+      <c r="AX1" s="898"/>
+      <c r="AY1" s="898"/>
+      <c r="AZ1" s="898"/>
+      <c r="BA1" s="898"/>
+      <c r="BB1" s="898"/>
+      <c r="BC1" s="898"/>
+      <c r="BD1" s="898"/>
+      <c r="BE1" s="898"/>
+      <c r="BF1" s="898"/>
+      <c r="BG1" s="898"/>
+      <c r="BH1" s="898"/>
+      <c r="BI1" s="898"/>
+      <c r="BJ1" s="898"/>
+      <c r="BK1" s="898"/>
+      <c r="BL1" s="898"/>
+      <c r="BM1" s="898"/>
+      <c r="BN1" s="898"/>
+      <c r="BO1" s="898"/>
+      <c r="BP1" s="898"/>
+      <c r="BQ1" s="898"/>
+      <c r="BR1" s="898"/>
+      <c r="BS1" s="898"/>
+      <c r="BT1" s="898"/>
+      <c r="BU1" s="898"/>
+      <c r="BV1" s="898"/>
+      <c r="BW1" s="877" t="s">
         <v>165</v>
       </c>
-      <c r="BX1" s="883" t="s">
+      <c r="BX1" s="889" t="s">
         <v>457</v>
       </c>
-      <c r="BY1" s="872"/>
-      <c r="BZ1" s="872"/>
-      <c r="CA1" s="873"/>
-      <c r="CB1" s="908" t="s">
+      <c r="BY1" s="859"/>
+      <c r="BZ1" s="859"/>
+      <c r="CA1" s="860"/>
+      <c r="CB1" s="888" t="s">
         <v>474</v>
       </c>
-      <c r="CC1" s="891" t="s">
+      <c r="CC1" s="890" t="s">
         <v>74</v>
       </c>
-      <c r="CD1" s="891"/>
-      <c r="CE1" s="891"/>
-      <c r="CF1" s="891"/>
-      <c r="CG1" s="891"/>
-      <c r="CH1" s="891"/>
-      <c r="CI1" s="891"/>
-      <c r="CJ1" s="891"/>
-      <c r="CK1" s="891"/>
-      <c r="CL1" s="891"/>
-      <c r="CM1" s="891"/>
-      <c r="CN1" s="891"/>
+      <c r="CD1" s="890"/>
+      <c r="CE1" s="890"/>
+      <c r="CF1" s="890"/>
+      <c r="CG1" s="890"/>
+      <c r="CH1" s="890"/>
+      <c r="CI1" s="890"/>
+      <c r="CJ1" s="890"/>
+      <c r="CK1" s="890"/>
+      <c r="CL1" s="890"/>
+      <c r="CM1" s="890"/>
+      <c r="CN1" s="890"/>
       <c r="CO1" s="146"/>
-      <c r="CP1" s="904" t="s">
+      <c r="CP1" s="876" t="s">
         <v>78</v>
       </c>
-      <c r="CQ1" s="842"/>
-      <c r="CR1" s="842"/>
-      <c r="CS1" s="842"/>
-      <c r="CT1" s="842"/>
-      <c r="CU1" s="842"/>
-      <c r="CV1" s="842"/>
-      <c r="CW1" s="861"/>
+      <c r="CQ1" s="847"/>
+      <c r="CR1" s="847"/>
+      <c r="CS1" s="847"/>
+      <c r="CT1" s="847"/>
+      <c r="CU1" s="847"/>
+      <c r="CV1" s="847"/>
+      <c r="CW1" s="848"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="147" t="s">
@@ -59886,7 +60115,7 @@
       <c r="L2" s="151" t="s">
         <v>81</v>
       </c>
-      <c r="M2" s="877"/>
+      <c r="M2" s="899"/>
       <c r="N2" s="152" t="s">
         <v>170</v>
       </c>
@@ -59902,22 +60131,22 @@
       <c r="R2" s="157" t="s">
         <v>173</v>
       </c>
-      <c r="S2" s="888" t="s">
+      <c r="S2" s="907" t="s">
         <v>452</v>
       </c>
-      <c r="T2" s="867"/>
-      <c r="U2" s="889" t="s">
+      <c r="T2" s="854"/>
+      <c r="U2" s="908" t="s">
         <v>87</v>
       </c>
-      <c r="V2" s="889"/>
-      <c r="W2" s="889" t="s">
+      <c r="V2" s="908"/>
+      <c r="W2" s="908" t="s">
         <v>88</v>
       </c>
-      <c r="X2" s="890"/>
-      <c r="Y2" s="884"/>
-      <c r="Z2" s="885"/>
-      <c r="AA2" s="887"/>
-      <c r="AB2" s="898"/>
+      <c r="X2" s="909"/>
+      <c r="Y2" s="904"/>
+      <c r="Z2" s="884"/>
+      <c r="AA2" s="906"/>
+      <c r="AB2" s="878"/>
       <c r="AC2" s="153" t="s">
         <v>174</v>
       </c>
@@ -59930,81 +60159,81 @@
       <c r="AF2" s="153" t="s">
         <v>177</v>
       </c>
-      <c r="AG2" s="899" t="s">
+      <c r="AG2" s="896" t="s">
         <v>178</v>
       </c>
-      <c r="AH2" s="892"/>
-      <c r="AI2" s="892" t="s">
+      <c r="AH2" s="881"/>
+      <c r="AI2" s="881" t="s">
         <v>179</v>
       </c>
-      <c r="AJ2" s="892"/>
-      <c r="AK2" s="892" t="s">
+      <c r="AJ2" s="881"/>
+      <c r="AK2" s="881" t="s">
         <v>180</v>
       </c>
-      <c r="AL2" s="892"/>
+      <c r="AL2" s="881"/>
       <c r="AM2" s="154" t="s">
         <v>181</v>
       </c>
       <c r="AN2" s="154" t="s">
         <v>182</v>
       </c>
-      <c r="AO2" s="898"/>
-      <c r="AP2" s="991" t="s">
-        <v>606</v>
-      </c>
-      <c r="AQ2" s="885"/>
-      <c r="AR2" s="992" t="s">
-        <v>607</v>
-      </c>
-      <c r="AS2" s="902"/>
-      <c r="AT2" s="892" t="s">
+      <c r="AO2" s="878"/>
+      <c r="AP2" s="883" t="s">
+        <v>595</v>
+      </c>
+      <c r="AQ2" s="884"/>
+      <c r="AR2" s="885" t="s">
+        <v>596</v>
+      </c>
+      <c r="AS2" s="886"/>
+      <c r="AT2" s="881" t="s">
         <v>183</v>
       </c>
-      <c r="AU2" s="892"/>
-      <c r="AV2" s="903" t="s">
+      <c r="AU2" s="881"/>
+      <c r="AV2" s="882" t="s">
         <v>184</v>
       </c>
-      <c r="AW2" s="903"/>
-      <c r="AX2" s="903" t="s">
+      <c r="AW2" s="882"/>
+      <c r="AX2" s="882" t="s">
         <v>185</v>
       </c>
-      <c r="AY2" s="903"/>
+      <c r="AY2" s="882"/>
       <c r="AZ2" s="154" t="s">
         <v>186</v>
       </c>
       <c r="BA2" s="154" t="s">
         <v>187</v>
       </c>
-      <c r="BB2" s="892" t="s">
+      <c r="BB2" s="881" t="s">
         <v>188</v>
       </c>
-      <c r="BC2" s="892"/>
-      <c r="BD2" s="903" t="s">
+      <c r="BC2" s="881"/>
+      <c r="BD2" s="882" t="s">
         <v>189</v>
       </c>
-      <c r="BE2" s="903"/>
-      <c r="BF2" s="903" t="s">
+      <c r="BE2" s="882"/>
+      <c r="BF2" s="882" t="s">
         <v>190</v>
       </c>
-      <c r="BG2" s="903"/>
+      <c r="BG2" s="882"/>
       <c r="BH2" s="154" t="s">
         <v>191</v>
       </c>
       <c r="BI2" s="154" t="s">
         <v>192</v>
       </c>
-      <c r="BJ2" s="892" t="s">
+      <c r="BJ2" s="881" t="s">
         <v>193</v>
       </c>
-      <c r="BK2" s="892"/>
-      <c r="BL2" s="903" t="s">
+      <c r="BK2" s="881"/>
+      <c r="BL2" s="882" t="s">
         <v>194</v>
       </c>
-      <c r="BM2" s="903"/>
-      <c r="BN2" s="903" t="s">
+      <c r="BM2" s="882"/>
+      <c r="BN2" s="882" t="s">
         <v>195</v>
       </c>
-      <c r="BO2" s="903"/>
+      <c r="BO2" s="882"/>
       <c r="BP2" s="154" t="s">
         <v>196</v>
       </c>
@@ -60026,16 +60255,16 @@
       <c r="BV2" s="154" t="s">
         <v>202</v>
       </c>
-      <c r="BW2" s="898"/>
-      <c r="BX2" s="991" t="s">
-        <v>606</v>
-      </c>
-      <c r="BY2" s="885"/>
-      <c r="BZ2" s="992" t="s">
-        <v>607</v>
-      </c>
-      <c r="CA2" s="902"/>
-      <c r="CB2" s="908"/>
+      <c r="BW2" s="878"/>
+      <c r="BX2" s="883" t="s">
+        <v>595</v>
+      </c>
+      <c r="BY2" s="884"/>
+      <c r="BZ2" s="885" t="s">
+        <v>596</v>
+      </c>
+      <c r="CA2" s="886"/>
+      <c r="CB2" s="888"/>
       <c r="CC2" s="138" t="s">
         <v>96</v>
       </c>
@@ -60075,22 +60304,22 @@
       <c r="CO2" s="140" t="s">
         <v>460</v>
       </c>
-      <c r="CP2" s="907" t="s">
+      <c r="CP2" s="887" t="s">
         <v>204</v>
       </c>
-      <c r="CQ2" s="905"/>
-      <c r="CR2" s="905" t="s">
+      <c r="CQ2" s="879"/>
+      <c r="CR2" s="879" t="s">
         <v>205</v>
       </c>
-      <c r="CS2" s="905"/>
-      <c r="CT2" s="905" t="s">
+      <c r="CS2" s="879"/>
+      <c r="CT2" s="879" t="s">
         <v>206</v>
       </c>
-      <c r="CU2" s="905"/>
-      <c r="CV2" s="905" t="s">
+      <c r="CU2" s="879"/>
+      <c r="CV2" s="879" t="s">
         <v>207</v>
       </c>
-      <c r="CW2" s="906"/>
+      <c r="CW2" s="880"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="168"/>
@@ -60955,6 +61184,29 @@
     </sortState>
   </autoFilter>
   <mergeCells count="39">
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="CC1:CN1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AN1"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
     <mergeCell ref="CP1:CW1"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="CV2:CW2"/>
@@ -60971,29 +61223,6 @@
     <mergeCell ref="CT2:CU2"/>
     <mergeCell ref="CB1:CB2"/>
     <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CC1:CN1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AN1"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -61037,110 +61266,105 @@
       <c r="K1" s="144"/>
       <c r="L1" s="145"/>
       <c r="M1" s="695"/>
-      <c r="N1" s="912"/>
-      <c r="O1" s="913"/>
-      <c r="P1" s="913"/>
-      <c r="Q1" s="913"/>
-      <c r="R1" s="880"/>
-      <c r="S1" s="881"/>
-      <c r="T1" s="881"/>
-      <c r="U1" s="881"/>
-      <c r="V1" s="881"/>
-      <c r="W1" s="881"/>
-      <c r="X1" s="882"/>
-      <c r="Y1" s="883"/>
-      <c r="Z1" s="872"/>
+      <c r="N1" s="910"/>
+      <c r="O1" s="911"/>
+      <c r="P1" s="911"/>
+      <c r="Q1" s="911"/>
+      <c r="R1" s="902"/>
+      <c r="S1" s="895"/>
+      <c r="T1" s="895"/>
+      <c r="U1" s="895"/>
+      <c r="V1" s="895"/>
+      <c r="W1" s="895"/>
+      <c r="X1" s="903"/>
+      <c r="Y1" s="889"/>
+      <c r="Z1" s="859"/>
       <c r="AA1" s="696"/>
       <c r="AB1" s="694"/>
-      <c r="AC1" s="893"/>
-      <c r="AD1" s="894"/>
-      <c r="AE1" s="894"/>
-      <c r="AF1" s="895"/>
-      <c r="AG1" s="896"/>
-      <c r="AH1" s="881"/>
-      <c r="AI1" s="881"/>
-      <c r="AJ1" s="881"/>
-      <c r="AK1" s="881"/>
-      <c r="AL1" s="881"/>
-      <c r="AM1" s="881"/>
-      <c r="AN1" s="881"/>
+      <c r="AC1" s="891"/>
+      <c r="AD1" s="892"/>
+      <c r="AE1" s="892"/>
+      <c r="AF1" s="893"/>
+      <c r="AG1" s="894"/>
+      <c r="AH1" s="895"/>
+      <c r="AI1" s="895"/>
+      <c r="AJ1" s="895"/>
+      <c r="AK1" s="895"/>
+      <c r="AL1" s="895"/>
+      <c r="AM1" s="895"/>
+      <c r="AN1" s="895"/>
       <c r="AO1" s="694"/>
-      <c r="AP1" s="883"/>
-      <c r="AQ1" s="872"/>
-      <c r="AR1" s="872"/>
-      <c r="AS1" s="873"/>
-      <c r="AT1" s="900"/>
-      <c r="AU1" s="901"/>
-      <c r="AV1" s="901"/>
-      <c r="AW1" s="901"/>
-      <c r="AX1" s="901"/>
-      <c r="AY1" s="901"/>
-      <c r="AZ1" s="901"/>
-      <c r="BA1" s="901"/>
-      <c r="BB1" s="901"/>
-      <c r="BC1" s="901"/>
-      <c r="BD1" s="901"/>
-      <c r="BE1" s="901"/>
-      <c r="BF1" s="901"/>
-      <c r="BG1" s="901"/>
-      <c r="BH1" s="901"/>
-      <c r="BI1" s="901"/>
-      <c r="BJ1" s="901"/>
-      <c r="BK1" s="901"/>
-      <c r="BL1" s="901"/>
-      <c r="BM1" s="901"/>
-      <c r="BN1" s="901"/>
-      <c r="BO1" s="901"/>
-      <c r="BP1" s="901"/>
-      <c r="BQ1" s="901"/>
-      <c r="BR1" s="901"/>
-      <c r="BS1" s="901"/>
-      <c r="BT1" s="901"/>
-      <c r="BU1" s="901"/>
-      <c r="BV1" s="901"/>
+      <c r="AP1" s="889"/>
+      <c r="AQ1" s="859"/>
+      <c r="AR1" s="859"/>
+      <c r="AS1" s="860"/>
+      <c r="AT1" s="897"/>
+      <c r="AU1" s="898"/>
+      <c r="AV1" s="898"/>
+      <c r="AW1" s="898"/>
+      <c r="AX1" s="898"/>
+      <c r="AY1" s="898"/>
+      <c r="AZ1" s="898"/>
+      <c r="BA1" s="898"/>
+      <c r="BB1" s="898"/>
+      <c r="BC1" s="898"/>
+      <c r="BD1" s="898"/>
+      <c r="BE1" s="898"/>
+      <c r="BF1" s="898"/>
+      <c r="BG1" s="898"/>
+      <c r="BH1" s="898"/>
+      <c r="BI1" s="898"/>
+      <c r="BJ1" s="898"/>
+      <c r="BK1" s="898"/>
+      <c r="BL1" s="898"/>
+      <c r="BM1" s="898"/>
+      <c r="BN1" s="898"/>
+      <c r="BO1" s="898"/>
+      <c r="BP1" s="898"/>
+      <c r="BQ1" s="898"/>
+      <c r="BR1" s="898"/>
+      <c r="BS1" s="898"/>
+      <c r="BT1" s="898"/>
+      <c r="BU1" s="898"/>
+      <c r="BV1" s="898"/>
       <c r="BW1" s="694"/>
-      <c r="BX1" s="883"/>
-      <c r="BY1" s="872"/>
-      <c r="BZ1" s="872"/>
-      <c r="CA1" s="873"/>
-      <c r="CB1" s="891"/>
-      <c r="CC1" s="891"/>
-      <c r="CD1" s="891"/>
-      <c r="CE1" s="891"/>
-      <c r="CF1" s="891"/>
-      <c r="CG1" s="891"/>
-      <c r="CH1" s="891"/>
-      <c r="CI1" s="891"/>
-      <c r="CJ1" s="891"/>
-      <c r="CK1" s="891"/>
-      <c r="CL1" s="891"/>
-      <c r="CM1" s="891"/>
+      <c r="BX1" s="889"/>
+      <c r="BY1" s="859"/>
+      <c r="BZ1" s="859"/>
+      <c r="CA1" s="860"/>
+      <c r="CB1" s="890"/>
+      <c r="CC1" s="890"/>
+      <c r="CD1" s="890"/>
+      <c r="CE1" s="890"/>
+      <c r="CF1" s="890"/>
+      <c r="CG1" s="890"/>
+      <c r="CH1" s="890"/>
+      <c r="CI1" s="890"/>
+      <c r="CJ1" s="890"/>
+      <c r="CK1" s="890"/>
+      <c r="CL1" s="890"/>
+      <c r="CM1" s="890"/>
       <c r="CN1" s="693"/>
-      <c r="CO1" s="904"/>
-      <c r="CP1" s="842"/>
-      <c r="CQ1" s="842"/>
-      <c r="CR1" s="842"/>
-      <c r="CS1" s="842"/>
-      <c r="CT1" s="842"/>
-      <c r="CU1" s="842"/>
-      <c r="CV1" s="861"/>
-      <c r="CW1" s="909"/>
-      <c r="CX1" s="910"/>
-      <c r="CY1" s="910"/>
-      <c r="CZ1" s="911"/>
-      <c r="DA1" s="910"/>
-      <c r="DB1" s="910"/>
-      <c r="DC1" s="911"/>
-      <c r="DD1" s="910"/>
-      <c r="DE1" s="910"/>
+      <c r="CO1" s="876"/>
+      <c r="CP1" s="847"/>
+      <c r="CQ1" s="847"/>
+      <c r="CR1" s="847"/>
+      <c r="CS1" s="847"/>
+      <c r="CT1" s="847"/>
+      <c r="CU1" s="847"/>
+      <c r="CV1" s="848"/>
+      <c r="CW1" s="912"/>
+      <c r="CX1" s="913"/>
+      <c r="CY1" s="913"/>
+      <c r="CZ1" s="914"/>
+      <c r="DA1" s="913"/>
+      <c r="DB1" s="913"/>
+      <c r="DC1" s="914"/>
+      <c r="DD1" s="913"/>
+      <c r="DE1" s="913"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="CZ1:DB1"/>
     <mergeCell ref="DC1:DE1"/>
@@ -61149,6 +61373,11 @@
     <mergeCell ref="AG1:AN1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CB1:CM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -61188,18 +61417,18 @@
       <c r="E1" s="143"/>
       <c r="F1" s="143"/>
       <c r="G1" s="143"/>
-      <c r="H1" s="915" t="s">
-        <v>589</v>
-      </c>
-      <c r="I1" s="915"/>
-      <c r="J1" s="915"/>
-      <c r="K1" s="915"/>
-      <c r="L1" s="914" t="s">
-        <v>590</v>
-      </c>
-      <c r="M1" s="914"/>
-      <c r="N1" s="914"/>
-      <c r="O1" s="914"/>
+      <c r="H1" s="916" t="s">
+        <v>578</v>
+      </c>
+      <c r="I1" s="916"/>
+      <c r="J1" s="916"/>
+      <c r="K1" s="916"/>
+      <c r="L1" s="915" t="s">
+        <v>579</v>
+      </c>
+      <c r="M1" s="915"/>
+      <c r="N1" s="915"/>
+      <c r="O1" s="915"/>
     </row>
     <row r="2" spans="1:15" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="444" t="s">
@@ -61233,19 +61462,19 @@
         <v>26</v>
       </c>
       <c r="K2" s="140" t="s">
-        <v>588</v>
-      </c>
-      <c r="L2" s="824" t="s">
-        <v>587</v>
-      </c>
-      <c r="M2" s="824" t="s">
+        <v>577</v>
+      </c>
+      <c r="L2" s="823" t="s">
+        <v>576</v>
+      </c>
+      <c r="M2" s="823" t="s">
         <v>242</v>
       </c>
-      <c r="N2" s="824" t="s">
+      <c r="N2" s="823" t="s">
         <v>249</v>
       </c>
-      <c r="O2" s="824" t="s">
-        <v>591</v>
+      <c r="O2" s="823" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -61374,10 +61603,10 @@
       <c r="B2" s="203" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="921" t="s">
+      <c r="C2" s="924" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="921"/>
+      <c r="D2" s="924"/>
       <c r="E2" s="201"/>
       <c r="F2" s="201"/>
       <c r="G2" s="201"/>
@@ -61525,7 +61754,7 @@
       <c r="S6" s="201"/>
       <c r="T6" s="201"/>
       <c r="U6" s="214" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="V6" s="372"/>
       <c r="W6" s="372"/>
@@ -61536,40 +61765,40 @@
       <c r="Z6" s="372"/>
       <c r="AA6" s="372"/>
       <c r="AB6" s="377" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="200"/>
-      <c r="B7" s="918"/>
-      <c r="C7" s="918"/>
-      <c r="D7" s="918"/>
+      <c r="B7" s="925"/>
+      <c r="C7" s="925"/>
+      <c r="D7" s="925"/>
       <c r="E7" s="201"/>
       <c r="F7" s="201"/>
       <c r="G7" s="201"/>
       <c r="H7" s="201"/>
       <c r="I7" s="201"/>
-      <c r="J7" s="918"/>
-      <c r="K7" s="918"/>
-      <c r="L7" s="918"/>
+      <c r="J7" s="925"/>
+      <c r="K7" s="925"/>
+      <c r="L7" s="925"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="201"/>
       <c r="P7" s="202" t="s">
         <v>231</v>
       </c>
-      <c r="Q7" s="918"/>
-      <c r="R7" s="918"/>
-      <c r="S7" s="918"/>
+      <c r="Q7" s="925"/>
+      <c r="R7" s="925"/>
+      <c r="S7" s="925"/>
       <c r="T7" s="201"/>
       <c r="U7" s="215"/>
       <c r="V7" s="372"/>
       <c r="W7" s="372" t="s">
         <v>231</v>
       </c>
-      <c r="X7" s="918"/>
-      <c r="Y7" s="918"/>
-      <c r="Z7" s="918"/>
+      <c r="X7" s="925"/>
+      <c r="Y7" s="925"/>
+      <c r="Z7" s="925"/>
       <c r="AA7" s="372"/>
       <c r="AB7" s="215"/>
     </row>
@@ -61608,54 +61837,54 @@
       <c r="B9" s="216" t="s">
         <v>437</v>
       </c>
-      <c r="C9" s="919" t="s">
+      <c r="C9" s="920" t="s">
         <v>232</v>
       </c>
-      <c r="D9" s="920"/>
-      <c r="E9" s="919" t="s">
+      <c r="D9" s="921"/>
+      <c r="E9" s="920" t="s">
         <v>233</v>
       </c>
-      <c r="F9" s="920"/>
+      <c r="F9" s="921"/>
       <c r="G9" s="201"/>
       <c r="H9" s="201"/>
       <c r="I9" s="201"/>
       <c r="J9" s="216" t="s">
         <v>437</v>
       </c>
-      <c r="K9" s="919" t="s">
+      <c r="K9" s="920" t="s">
         <v>232</v>
       </c>
-      <c r="L9" s="920"/>
-      <c r="M9" s="919" t="s">
+      <c r="L9" s="921"/>
+      <c r="M9" s="920" t="s">
         <v>233</v>
       </c>
-      <c r="N9" s="920"/>
+      <c r="N9" s="921"/>
       <c r="O9" s="201"/>
       <c r="P9" s="201"/>
       <c r="Q9" s="216" t="s">
         <v>437</v>
       </c>
-      <c r="R9" s="919" t="s">
+      <c r="R9" s="920" t="s">
         <v>232</v>
       </c>
-      <c r="S9" s="920"/>
-      <c r="T9" s="919" t="s">
+      <c r="S9" s="921"/>
+      <c r="T9" s="920" t="s">
         <v>233</v>
       </c>
-      <c r="U9" s="920"/>
+      <c r="U9" s="921"/>
       <c r="V9" s="372"/>
       <c r="W9" s="372"/>
       <c r="X9" s="216" t="s">
         <v>437</v>
       </c>
-      <c r="Y9" s="919" t="s">
+      <c r="Y9" s="920" t="s">
         <v>232</v>
       </c>
-      <c r="Z9" s="920"/>
-      <c r="AA9" s="919" t="s">
+      <c r="Z9" s="921"/>
+      <c r="AA9" s="920" t="s">
         <v>233</v>
       </c>
-      <c r="AB9" s="920"/>
+      <c r="AB9" s="921"/>
     </row>
     <row r="10" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="200"/>
@@ -61695,7 +61924,7 @@
       <c r="O10" s="201"/>
       <c r="P10" s="201"/>
       <c r="Q10" s="217" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="R10" s="218" t="s">
         <v>59</v>
@@ -61712,7 +61941,7 @@
       <c r="V10" s="372"/>
       <c r="W10" s="372"/>
       <c r="X10" s="217" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="Y10" s="218" t="s">
         <v>59</v>
@@ -61734,10 +61963,10 @@
       </c>
       <c r="C11" s="221"/>
       <c r="D11" s="221"/>
-      <c r="E11" s="916" t="s">
+      <c r="E11" s="917" t="s">
         <v>237</v>
       </c>
-      <c r="F11" s="917"/>
+      <c r="F11" s="918"/>
       <c r="G11" s="222"/>
       <c r="H11" s="222"/>
       <c r="I11" s="222"/>
@@ -61746,10 +61975,10 @@
       </c>
       <c r="K11" s="201"/>
       <c r="L11" s="201"/>
-      <c r="M11" s="923" t="s">
+      <c r="M11" s="922" t="s">
         <v>237</v>
       </c>
-      <c r="N11" s="924"/>
+      <c r="N11" s="923"/>
       <c r="O11" s="222"/>
       <c r="P11" s="222"/>
       <c r="Q11" s="220" t="s">
@@ -61757,10 +61986,10 @@
       </c>
       <c r="R11" s="221"/>
       <c r="S11" s="221"/>
-      <c r="T11" s="916" t="s">
+      <c r="T11" s="917" t="s">
         <v>237</v>
       </c>
-      <c r="U11" s="917"/>
+      <c r="U11" s="918"/>
       <c r="V11" s="372"/>
       <c r="W11" s="372"/>
       <c r="X11" s="220" t="s">
@@ -61768,10 +61997,10 @@
       </c>
       <c r="Y11" s="221"/>
       <c r="Z11" s="221"/>
-      <c r="AA11" s="916" t="s">
+      <c r="AA11" s="917" t="s">
         <v>237</v>
       </c>
-      <c r="AB11" s="917"/>
+      <c r="AB11" s="918"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="200"/>
@@ -61814,7 +62043,7 @@
     <row r="13" spans="1:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="200"/>
       <c r="B13" s="321" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="C13" s="301"/>
       <c r="D13" s="283"/>
@@ -61824,7 +62053,7 @@
       <c r="H13" s="222"/>
       <c r="I13" s="222"/>
       <c r="J13" s="321" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="K13" s="301"/>
       <c r="L13" s="283"/>
@@ -61833,7 +62062,7 @@
       <c r="O13" s="222"/>
       <c r="P13" s="222"/>
       <c r="Q13" s="321" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="R13" s="301"/>
       <c r="S13" s="283"/>
@@ -61842,7 +62071,7 @@
       <c r="V13" s="372"/>
       <c r="W13" s="372"/>
       <c r="X13" s="321" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="Y13" s="301"/>
       <c r="Z13" s="283"/>
@@ -62076,10 +62305,10 @@
       </c>
       <c r="C20" s="302"/>
       <c r="D20" s="249"/>
-      <c r="E20" s="916" t="s">
+      <c r="E20" s="917" t="s">
         <v>243</v>
       </c>
-      <c r="F20" s="917"/>
+      <c r="F20" s="918"/>
       <c r="G20" s="230"/>
       <c r="H20" s="230"/>
       <c r="I20" s="201"/>
@@ -62088,10 +62317,10 @@
       </c>
       <c r="K20" s="302"/>
       <c r="L20" s="249"/>
-      <c r="M20" s="916" t="s">
+      <c r="M20" s="917" t="s">
         <v>243</v>
       </c>
-      <c r="N20" s="917"/>
+      <c r="N20" s="918"/>
       <c r="O20" s="240"/>
       <c r="P20" s="240"/>
       <c r="Q20" s="220" t="s">
@@ -62099,10 +62328,10 @@
       </c>
       <c r="R20" s="302"/>
       <c r="S20" s="249"/>
-      <c r="T20" s="916" t="s">
+      <c r="T20" s="917" t="s">
         <v>243</v>
       </c>
-      <c r="U20" s="917"/>
+      <c r="U20" s="918"/>
       <c r="V20" s="277"/>
       <c r="W20" s="277"/>
       <c r="X20" s="220" t="s">
@@ -62110,10 +62339,10 @@
       </c>
       <c r="Y20" s="302"/>
       <c r="Z20" s="249"/>
-      <c r="AA20" s="916" t="s">
+      <c r="AA20" s="917" t="s">
         <v>243</v>
       </c>
-      <c r="AB20" s="917"/>
+      <c r="AB20" s="918"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="200"/>
@@ -62456,10 +62685,10 @@
       </c>
       <c r="C30" s="302"/>
       <c r="D30" s="249"/>
-      <c r="E30" s="916" t="s">
+      <c r="E30" s="917" t="s">
         <v>243</v>
       </c>
-      <c r="F30" s="917"/>
+      <c r="F30" s="918"/>
       <c r="G30" s="230"/>
       <c r="H30" s="230"/>
       <c r="I30" s="201"/>
@@ -62468,10 +62697,10 @@
       </c>
       <c r="K30" s="302"/>
       <c r="L30" s="249"/>
-      <c r="M30" s="916" t="s">
-        <v>576</v>
-      </c>
-      <c r="N30" s="917"/>
+      <c r="M30" s="917" t="s">
+        <v>565</v>
+      </c>
+      <c r="N30" s="918"/>
       <c r="O30" s="240"/>
       <c r="P30" s="240"/>
       <c r="Q30" s="220" t="s">
@@ -62479,10 +62708,10 @@
       </c>
       <c r="R30" s="302"/>
       <c r="S30" s="249"/>
-      <c r="T30" s="916" t="s">
+      <c r="T30" s="917" t="s">
         <v>243</v>
       </c>
-      <c r="U30" s="917"/>
+      <c r="U30" s="918"/>
       <c r="V30" s="277"/>
       <c r="W30" s="277"/>
       <c r="X30" s="220" t="s">
@@ -62490,10 +62719,10 @@
       </c>
       <c r="Y30" s="302"/>
       <c r="Z30" s="249"/>
-      <c r="AA30" s="916" t="s">
+      <c r="AA30" s="917" t="s">
         <v>243</v>
       </c>
-      <c r="AB30" s="917"/>
+      <c r="AB30" s="918"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="262"/>
@@ -62931,11 +63160,11 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="200"/>
-      <c r="B42" s="922"/>
-      <c r="C42" s="922"/>
-      <c r="D42" s="922"/>
-      <c r="E42" s="922"/>
-      <c r="F42" s="922"/>
+      <c r="B42" s="919"/>
+      <c r="C42" s="919"/>
+      <c r="D42" s="919"/>
+      <c r="E42" s="919"/>
+      <c r="F42" s="919"/>
       <c r="G42" s="240"/>
       <c r="H42" s="201"/>
       <c r="I42" s="240"/>
@@ -63122,6 +63351,21 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="26">
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -63133,21 +63377,6 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA20:AB20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
fix line 37 in summary legal compliance
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368" activeTab="1"/>
+    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="616">
   <si>
     <t>Acronym</t>
   </si>
@@ -2436,6 +2436,9 @@
       <t>. Member States have to report the treatment for each of their treatment plant in categories "primary", "secondary", "Other" (for more stringent treatment) and details for more stringent in categories "Nremoval", "Premoval", "UV", "Chlorination", "ozonation", "sand filtration", "microfiltration"  and "other". In sheet "distance to compliance" these information are used to calculate if, for a waste water treatment plant, the equipment reported (in place) meet UWWTD requirements. This is the case only if all equipment for this level of treatment (secondary or more stringent) are reported. In sheet "summary installation in place" these information are used to calculate if, for a waste water treatment plant, the equipment reported (in place) meet the specific level of treatment (secondary respectively more stringent), with no consideration of  UWWTD requirements, i.e. including cases in which it is not required by the UWWTD.</t>
     </r>
   </si>
+  <si>
+    <t>Glossary</t>
+  </si>
 </sst>
 </file>
 
@@ -2448,7 +2451,7 @@
     <numFmt numFmtId="167" formatCode="yyyy\/mm\/dd"/>
     <numFmt numFmtId="168" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="51" x14ac:knownFonts="1">
+  <fonts count="53" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2783,6 +2786,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="49">
@@ -3932,7 +3948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1002">
+  <cellXfs count="1005">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -5889,9 +5905,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="48" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5910,6 +5923,7 @@
     <xf numFmtId="49" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5941,45 +5955,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6016,6 +5991,9 @@
     <xf numFmtId="3" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6064,6 +6042,111 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6076,21 +6159,12 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6106,65 +6180,11 @@
     <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6175,12 +6195,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6193,26 +6207,26 @@
     <xf numFmtId="0" fontId="25" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6242,6 +6256,33 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6275,34 +6316,10 @@
     <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6327,8 +6344,57 @@
     <xf numFmtId="3" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6342,18 +6408,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6366,47 +6420,18 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="51" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6720,8 +6745,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6731,7 +6756,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="832"/>
+      <c r="A1" s="831"/>
       <c r="B1" s="824"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6754,20 +6779,22 @@
       <c r="A6" s="769"/>
       <c r="B6" s="772"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="769"/>
-      <c r="B7" s="772"/>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="1001" t="s">
+        <v>615</v>
+      </c>
+      <c r="B7" s="1002"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="826" t="s">
+      <c r="A8" s="1003" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="824" t="s">
+      <c r="B8" s="1004" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="827" t="s">
+      <c r="A9" s="826" t="s">
         <v>461</v>
       </c>
       <c r="B9" s="772" t="s">
@@ -6775,7 +6802,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="828" t="s">
+      <c r="A10" s="827" t="s">
         <v>522</v>
       </c>
       <c r="B10" s="772" t="s">
@@ -6783,7 +6810,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="828" t="s">
+      <c r="A11" s="827" t="s">
         <v>523</v>
       </c>
       <c r="B11" s="772" t="s">
@@ -6791,7 +6818,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="828" t="s">
+      <c r="A12" s="827" t="s">
         <v>524</v>
       </c>
       <c r="B12" s="770" t="s">
@@ -6799,7 +6826,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="828" t="s">
+      <c r="A13" s="827" t="s">
         <v>525</v>
       </c>
       <c r="B13" s="770" t="s">
@@ -6807,7 +6834,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="828" t="s">
+      <c r="A14" s="827" t="s">
         <v>526</v>
       </c>
       <c r="B14" s="770" t="s">
@@ -6815,7 +6842,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="828" t="s">
+      <c r="A15" s="827" t="s">
         <v>527</v>
       </c>
       <c r="B15" s="770" t="s">
@@ -6823,7 +6850,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="828" t="s">
+      <c r="A16" s="827" t="s">
         <v>528</v>
       </c>
       <c r="B16" s="770" t="s">
@@ -6831,7 +6858,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="828" t="s">
+      <c r="A17" s="827" t="s">
         <v>529</v>
       </c>
       <c r="B17" s="770" t="s">
@@ -6839,7 +6866,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="828" t="s">
+      <c r="A18" s="827" t="s">
         <v>530</v>
       </c>
       <c r="B18" s="770" t="s">
@@ -6847,7 +6874,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="828" t="s">
+      <c r="A19" s="827" t="s">
         <v>531</v>
       </c>
       <c r="B19" s="770" t="s">
@@ -6855,7 +6882,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="828" t="s">
+      <c r="A20" s="827" t="s">
         <v>600</v>
       </c>
       <c r="B20" s="770" t="s">
@@ -6863,7 +6890,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="828" t="s">
+      <c r="A21" s="827" t="s">
         <v>533</v>
       </c>
       <c r="B21" s="770" t="s">
@@ -6871,7 +6898,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="828" t="s">
+      <c r="A22" s="827" t="s">
         <v>534</v>
       </c>
       <c r="B22" s="770" t="s">
@@ -6879,7 +6906,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="828" t="s">
+      <c r="A23" s="827" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="770" t="s">
@@ -6887,7 +6914,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="828" t="s">
+      <c r="A24" s="827" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="770" t="s">
@@ -6895,7 +6922,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="828" t="s">
+      <c r="A25" s="827" t="s">
         <v>538</v>
       </c>
       <c r="B25" s="770" t="s">
@@ -6903,7 +6930,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="828" t="s">
+      <c r="A26" s="827" t="s">
         <v>540</v>
       </c>
       <c r="B26" s="770" t="s">
@@ -6911,7 +6938,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="828" t="s">
+      <c r="A27" s="827" t="s">
         <v>541</v>
       </c>
       <c r="B27" s="770" t="s">
@@ -6919,7 +6946,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="828" t="s">
+      <c r="A28" s="827" t="s">
         <v>542</v>
       </c>
       <c r="B28" s="770" t="s">
@@ -6927,7 +6954,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="828" t="s">
+      <c r="A29" s="827" t="s">
         <v>496</v>
       </c>
       <c r="B29" s="772" t="s">
@@ -6935,7 +6962,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="828" t="s">
+      <c r="A30" s="827" t="s">
         <v>223</v>
       </c>
       <c r="B30" s="770" t="s">
@@ -6943,7 +6970,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="828" t="s">
+      <c r="A31" s="827" t="s">
         <v>490</v>
       </c>
       <c r="B31" s="770" t="s">
@@ -6951,7 +6978,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="828" t="s">
+      <c r="A32" s="827" t="s">
         <v>492</v>
       </c>
       <c r="B32" s="770" t="s">
@@ -6959,7 +6986,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="828" t="s">
+      <c r="A33" s="827" t="s">
         <v>543</v>
       </c>
       <c r="B33" s="770" t="s">
@@ -6967,7 +6994,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="828" t="s">
+      <c r="A34" s="827" t="s">
         <v>544</v>
       </c>
       <c r="B34" s="770" t="s">
@@ -6975,7 +7002,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="828" t="s">
+      <c r="A35" s="827" t="s">
         <v>545</v>
       </c>
       <c r="B35" s="770" t="s">
@@ -6983,7 +7010,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="828" t="s">
+      <c r="A36" s="827" t="s">
         <v>547</v>
       </c>
       <c r="B36" s="770" t="s">
@@ -6991,7 +7018,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="828">
+      <c r="A37" s="827">
         <v>1</v>
       </c>
       <c r="B37" s="770" t="s">
@@ -6999,7 +7026,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="828" t="s">
+      <c r="A38" s="827" t="s">
         <v>548</v>
       </c>
       <c r="B38" s="770" t="s">
@@ -7007,7 +7034,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="828">
+      <c r="A39" s="827">
         <v>2</v>
       </c>
       <c r="B39" s="770" t="s">
@@ -7015,7 +7042,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="828" t="s">
+      <c r="A40" s="827" t="s">
         <v>549</v>
       </c>
       <c r="B40" s="770" t="s">
@@ -7023,7 +7050,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="828" t="s">
+      <c r="A41" s="827" t="s">
         <v>550</v>
       </c>
       <c r="B41" s="770" t="s">
@@ -7031,7 +7058,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="829" t="s">
+      <c r="A42" s="828" t="s">
         <v>552</v>
       </c>
       <c r="B42" s="825" t="s">
@@ -7039,7 +7066,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="828" t="s">
+      <c r="A43" s="827" t="s">
         <v>554</v>
       </c>
       <c r="B43" s="825" t="s">
@@ -7047,7 +7074,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="828" t="s">
+      <c r="A44" s="827" t="s">
         <v>556</v>
       </c>
       <c r="B44" s="770" t="s">
@@ -7055,7 +7082,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="829" t="s">
+      <c r="A45" s="828" t="s">
         <v>557</v>
       </c>
       <c r="B45" s="770" t="s">
@@ -7063,7 +7090,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="829" t="s">
+      <c r="A46" s="828" t="s">
         <v>92</v>
       </c>
       <c r="B46" s="770" t="s">
@@ -7071,7 +7098,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="829" t="s">
+      <c r="A47" s="828" t="s">
         <v>558</v>
       </c>
       <c r="B47" s="825" t="s">
@@ -7079,7 +7106,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="829" t="s">
+      <c r="A48" s="828" t="s">
         <v>559</v>
       </c>
       <c r="B48" s="825" t="s">
@@ -7087,7 +7114,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="829" t="s">
+      <c r="A49" s="828" t="s">
         <v>561</v>
       </c>
       <c r="B49" s="825" t="s">
@@ -7095,7 +7122,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="830" t="s">
+      <c r="A50" s="829" t="s">
         <v>114</v>
       </c>
       <c r="B50" s="772" t="s">
@@ -7103,7 +7130,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="829" t="s">
+      <c r="A51" s="828" t="s">
         <v>507</v>
       </c>
       <c r="B51" s="772" t="s">
@@ -7111,7 +7138,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="829" t="s">
+      <c r="A52" s="828" t="s">
         <v>517</v>
       </c>
       <c r="B52" s="825" t="s">
@@ -7119,7 +7146,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="829" t="s">
+      <c r="A53" s="828" t="s">
         <v>563</v>
       </c>
       <c r="B53" s="825" t="s">
@@ -7127,15 +7154,15 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="829" t="s">
+      <c r="A54" s="828" t="s">
         <v>511</v>
       </c>
-      <c r="B54" s="831" t="s">
+      <c r="B54" s="830" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A55" s="829" t="s">
+      <c r="A55" s="828" t="s">
         <v>564</v>
       </c>
       <c r="B55" s="825" t="s">
@@ -7143,7 +7170,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="829" t="s">
+      <c r="A56" s="828" t="s">
         <v>607</v>
       </c>
       <c r="B56" s="825" t="s">
@@ -7151,11 +7178,11 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="829"/>
+      <c r="A57" s="828"/>
       <c r="B57" s="825"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="829"/>
+      <c r="A58" s="828"/>
       <c r="B58" s="825"/>
     </row>
   </sheetData>
@@ -7875,8 +7902,8 @@
       </c>
       <c r="C2" s="373"/>
       <c r="D2" s="373"/>
-      <c r="E2" s="931"/>
-      <c r="F2" s="931"/>
+      <c r="E2" s="933"/>
+      <c r="F2" s="933"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="372"/>
@@ -7908,13 +7935,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="370"/>
-      <c r="B6" s="928" t="s">
+      <c r="B6" s="934" t="s">
         <v>439</v>
       </c>
-      <c r="C6" s="928"/>
-      <c r="D6" s="928"/>
-      <c r="E6" s="928"/>
-      <c r="F6" s="928"/>
+      <c r="C6" s="934"/>
+      <c r="D6" s="934"/>
+      <c r="E6" s="934"/>
+      <c r="F6" s="934"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="370"/>
@@ -8072,11 +8099,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="370"/>
-      <c r="B22" s="932"/>
-      <c r="C22" s="932"/>
-      <c r="D22" s="932"/>
-      <c r="E22" s="932"/>
-      <c r="F22" s="932"/>
+      <c r="B22" s="928"/>
+      <c r="C22" s="928"/>
+      <c r="D22" s="928"/>
+      <c r="E22" s="928"/>
+      <c r="F22" s="928"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="370"/>
@@ -8375,43 +8402,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="948" t="s">
+      <c r="A1" s="957" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="949"/>
+      <c r="B1" s="958"/>
       <c r="C1" s="455"/>
-      <c r="D1" s="959" t="s">
+      <c r="D1" s="948" t="s">
         <v>287</v>
       </c>
-      <c r="E1" s="960"/>
-      <c r="F1" s="960"/>
-      <c r="G1" s="960"/>
-      <c r="H1" s="960"/>
-      <c r="I1" s="961"/>
-      <c r="J1" s="950" t="s">
+      <c r="E1" s="949"/>
+      <c r="F1" s="949"/>
+      <c r="G1" s="949"/>
+      <c r="H1" s="949"/>
+      <c r="I1" s="950"/>
+      <c r="J1" s="959" t="s">
         <v>288</v>
       </c>
-      <c r="K1" s="951"/>
-      <c r="L1" s="951"/>
-      <c r="M1" s="951"/>
-      <c r="N1" s="952"/>
-      <c r="O1" s="953" t="s">
+      <c r="K1" s="960"/>
+      <c r="L1" s="960"/>
+      <c r="M1" s="960"/>
+      <c r="N1" s="961"/>
+      <c r="O1" s="962" t="s">
         <v>289</v>
       </c>
-      <c r="P1" s="954"/>
-      <c r="Q1" s="955"/>
+      <c r="P1" s="963"/>
+      <c r="Q1" s="964"/>
       <c r="R1" s="442" t="s">
         <v>71</v>
       </c>
       <c r="S1" s="443"/>
-      <c r="T1" s="947" t="s">
+      <c r="T1" s="956" t="s">
         <v>482</v>
       </c>
-      <c r="U1" s="947"/>
-      <c r="V1" s="947"/>
-      <c r="W1" s="947"/>
-      <c r="X1" s="947"/>
-      <c r="Y1" s="947"/>
+      <c r="U1" s="956"/>
+      <c r="V1" s="956"/>
+      <c r="W1" s="956"/>
+      <c r="X1" s="956"/>
+      <c r="Y1" s="956"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="445" t="s">
@@ -8423,18 +8450,18 @@
       <c r="C2" s="446" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="964" t="s">
+      <c r="D2" s="953" t="s">
         <v>291</v>
       </c>
-      <c r="E2" s="963"/>
-      <c r="F2" s="963" t="s">
+      <c r="E2" s="952"/>
+      <c r="F2" s="952" t="s">
         <v>292</v>
       </c>
-      <c r="G2" s="963"/>
-      <c r="H2" s="962" t="s">
+      <c r="G2" s="952"/>
+      <c r="H2" s="951" t="s">
         <v>293</v>
       </c>
-      <c r="I2" s="962"/>
+      <c r="I2" s="951"/>
       <c r="J2" s="447">
         <v>0</v>
       </c>
@@ -8465,18 +8492,18 @@
       <c r="S2" s="681" t="s">
         <v>81</v>
       </c>
-      <c r="T2" s="945" t="s">
+      <c r="T2" s="954" t="s">
         <v>451</v>
       </c>
-      <c r="U2" s="945"/>
-      <c r="V2" s="946" t="s">
+      <c r="U2" s="954"/>
+      <c r="V2" s="955" t="s">
         <v>468</v>
       </c>
-      <c r="W2" s="946"/>
-      <c r="X2" s="946" t="s">
+      <c r="W2" s="955"/>
+      <c r="X2" s="955" t="s">
         <v>469</v>
       </c>
-      <c r="Y2" s="946"/>
+      <c r="Y2" s="955"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="450"/>
@@ -8502,13 +8529,13 @@
       <c r="I3" s="665" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="956" t="s">
+      <c r="J3" s="945" t="s">
         <v>298</v>
       </c>
-      <c r="K3" s="957"/>
-      <c r="L3" s="957"/>
-      <c r="M3" s="957"/>
-      <c r="N3" s="958"/>
+      <c r="K3" s="946"/>
+      <c r="L3" s="946"/>
+      <c r="M3" s="946"/>
+      <c r="N3" s="947"/>
       <c r="O3" s="458"/>
       <c r="P3" s="458"/>
       <c r="Q3" s="458"/>
@@ -9737,11 +9764,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:X4"/>
   <mergeCells count="12">
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -9749,6 +9771,11 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9789,25 +9816,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="844" t="s">
+      <c r="A1" s="873" t="s">
         <v>299</v>
       </c>
-      <c r="B1" s="845"/>
-      <c r="C1" s="845"/>
-      <c r="D1" s="845"/>
-      <c r="E1" s="845"/>
-      <c r="F1" s="845"/>
+      <c r="B1" s="874"/>
+      <c r="C1" s="874"/>
+      <c r="D1" s="874"/>
+      <c r="E1" s="874"/>
+      <c r="F1" s="874"/>
       <c r="G1" s="472"/>
-      <c r="H1" s="970" t="s">
+      <c r="H1" s="971" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="971"/>
-      <c r="J1" s="971"/>
+      <c r="I1" s="972"/>
+      <c r="J1" s="972"/>
       <c r="K1" s="474"/>
       <c r="L1" s="464"/>
       <c r="M1" s="474"/>
       <c r="N1" s="465"/>
-      <c r="O1" s="968" t="s">
+      <c r="O1" s="969" t="s">
         <v>300</v>
       </c>
       <c r="P1" s="466"/>
@@ -9819,26 +9846,26 @@
       <c r="T1" s="464"/>
       <c r="U1" s="474"/>
       <c r="V1" s="465"/>
-      <c r="W1" s="968" t="s">
+      <c r="W1" s="969" t="s">
         <v>302</v>
       </c>
       <c r="X1" s="466"/>
-      <c r="Y1" s="972" t="s">
+      <c r="Y1" s="973" t="s">
         <v>303</v>
       </c>
-      <c r="Z1" s="972"/>
-      <c r="AA1" s="972"/>
-      <c r="AB1" s="972"/>
-      <c r="AC1" s="972"/>
-      <c r="AD1" s="973"/>
-      <c r="AE1" s="968" t="s">
+      <c r="Z1" s="973"/>
+      <c r="AA1" s="973"/>
+      <c r="AB1" s="973"/>
+      <c r="AC1" s="973"/>
+      <c r="AD1" s="974"/>
+      <c r="AE1" s="969" t="s">
         <v>304</v>
       </c>
-      <c r="AF1" s="967" t="s">
+      <c r="AF1" s="968" t="s">
         <v>467</v>
       </c>
-      <c r="AG1" s="947"/>
-      <c r="AH1" s="947"/>
+      <c r="AG1" s="956"/>
+      <c r="AH1" s="956"/>
       <c r="AI1" s="688"/>
       <c r="AJ1" s="688"/>
       <c r="AK1" s="688"/>
@@ -9897,14 +9924,14 @@
       <c r="C2" s="473" t="s">
         <v>306</v>
       </c>
-      <c r="D2" s="966" t="s">
+      <c r="D2" s="967" t="s">
         <v>472</v>
       </c>
-      <c r="E2" s="966"/>
-      <c r="F2" s="966" t="s">
+      <c r="E2" s="967"/>
+      <c r="F2" s="967" t="s">
         <v>473</v>
       </c>
-      <c r="G2" s="966"/>
+      <c r="G2" s="967"/>
       <c r="H2" s="468"/>
       <c r="I2" s="965" t="s">
         <v>178</v>
@@ -9917,8 +9944,8 @@
       <c r="M2" s="965" t="s">
         <v>180</v>
       </c>
-      <c r="N2" s="974"/>
-      <c r="O2" s="969"/>
+      <c r="N2" s="966"/>
+      <c r="O2" s="970"/>
       <c r="P2" s="469"/>
       <c r="Q2" s="965" t="s">
         <v>178</v>
@@ -9931,8 +9958,8 @@
       <c r="U2" s="965" t="s">
         <v>180</v>
       </c>
-      <c r="V2" s="974"/>
-      <c r="W2" s="969"/>
+      <c r="V2" s="966"/>
+      <c r="W2" s="970"/>
       <c r="X2" s="469"/>
       <c r="Y2" s="965" t="s">
         <v>178</v>
@@ -9945,8 +9972,8 @@
       <c r="AC2" s="965" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="974"/>
-      <c r="AE2" s="969"/>
+      <c r="AD2" s="966"/>
+      <c r="AE2" s="970"/>
       <c r="AF2" s="682" t="s">
         <v>451</v>
       </c>
@@ -10832,11 +10859,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:AH4"/>
   <mergeCells count="18">
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="A1:F1"/>
@@ -10850,6 +10872,11 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11068,9 +11095,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="975"/>
-      <c r="B1" s="875"/>
-      <c r="C1" s="875"/>
+      <c r="A1" s="993"/>
+      <c r="B1" s="863"/>
+      <c r="C1" s="863"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="740"/>
@@ -11085,21 +11112,21 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="983" t="s">
+      <c r="A3" s="997" t="s">
         <v>332</v>
       </c>
-      <c r="B3" s="985" t="s">
+      <c r="B3" s="999" t="s">
         <v>440</v>
       </c>
-      <c r="C3" s="986"/>
-      <c r="D3" s="981" t="s">
+      <c r="C3" s="1000"/>
+      <c r="D3" s="985" t="s">
         <v>441</v>
       </c>
-      <c r="E3" s="982"/>
-      <c r="F3" s="981" t="s">
+      <c r="E3" s="986"/>
+      <c r="F3" s="985" t="s">
         <v>475</v>
       </c>
-      <c r="G3" s="982"/>
+      <c r="G3" s="986"/>
       <c r="I3" s="738" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
@@ -11110,14 +11137,14 @@
       <c r="K3" s="720"/>
       <c r="L3" s="720"/>
       <c r="N3" s="705"/>
-      <c r="O3" s="997" t="s">
+      <c r="O3" s="982" t="s">
         <v>333</v>
       </c>
-      <c r="P3" s="997"/>
-      <c r="Q3" s="997" t="s">
+      <c r="P3" s="982"/>
+      <c r="Q3" s="982" t="s">
         <v>334</v>
       </c>
-      <c r="R3" s="997"/>
+      <c r="R3" s="982"/>
       <c r="S3" s="705"/>
       <c r="T3" s="713" t="s">
         <v>335</v>
@@ -11125,7 +11152,7 @@
       <c r="U3" s="705"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="984"/>
+      <c r="A4" s="998"/>
       <c r="B4" s="512" t="s">
         <v>336</v>
       </c>
@@ -11384,14 +11411,14 @@
       <c r="K10" s="720"/>
       <c r="L10" s="720"/>
       <c r="N10" s="713"/>
-      <c r="O10" s="997" t="s">
+      <c r="O10" s="982" t="s">
         <v>336</v>
       </c>
-      <c r="P10" s="997"/>
-      <c r="Q10" s="997" t="s">
+      <c r="P10" s="982"/>
+      <c r="Q10" s="982" t="s">
         <v>343</v>
       </c>
-      <c r="R10" s="997"/>
+      <c r="R10" s="982"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I11" s="738" t="str">
@@ -11455,7 +11482,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="983" t="s">
+      <c r="A13" s="997" t="s">
         <v>344</v>
       </c>
       <c r="B13" s="511" t="str">
@@ -11501,7 +11528,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="984"/>
+      <c r="A14" s="998"/>
       <c r="B14" s="514" t="s">
         <v>337</v>
       </c>
@@ -11631,34 +11658,34 @@
       <c r="A21" s="502" t="s">
         <v>349</v>
       </c>
-      <c r="B21" s="998" t="s">
+      <c r="B21" s="987" t="s">
         <v>494</v>
       </c>
-      <c r="C21" s="999"/>
-      <c r="D21" s="999"/>
-      <c r="E21" s="999"/>
-      <c r="F21" s="999"/>
-      <c r="G21" s="999"/>
+      <c r="C21" s="988"/>
+      <c r="D21" s="988"/>
+      <c r="E21" s="988"/>
+      <c r="F21" s="988"/>
+      <c r="G21" s="988"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="516" t="s">
         <v>313</v>
       </c>
-      <c r="B22" s="987" t="str">
+      <c r="B22" s="989" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="988"/>
-      <c r="D22" s="987" t="str">
+      <c r="C22" s="990"/>
+      <c r="D22" s="989" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="988"/>
-      <c r="F22" s="987" t="str">
+      <c r="E22" s="990"/>
+      <c r="F22" s="989" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="988"/>
+      <c r="G22" s="990"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="517"/>
@@ -12085,21 +12112,21 @@
       <c r="A41" s="519" t="s">
         <v>359</v>
       </c>
-      <c r="B41" s="977" t="str">
+      <c r="B41" s="995" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="978"/>
-      <c r="D41" s="979" t="str">
+      <c r="C41" s="996"/>
+      <c r="D41" s="983" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="980"/>
-      <c r="F41" s="979" t="str">
+      <c r="E41" s="984"/>
+      <c r="F41" s="983" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G41" s="980"/>
+      <c r="G41" s="984"/>
       <c r="N41" s="705"/>
       <c r="O41" s="732" t="s">
         <v>445</v>
@@ -12313,11 +12340,11 @@
       <c r="F53" s="710" t="s">
         <v>500</v>
       </c>
-      <c r="H53" s="1000" t="s">
+      <c r="H53" s="975" t="s">
         <v>487</v>
       </c>
-      <c r="I53" s="1000"/>
-      <c r="J53" s="1000"/>
+      <c r="I53" s="975"/>
+      <c r="J53" s="975"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="701" t="s">
@@ -12487,11 +12514,11 @@
       <c r="F63" s="710" t="s">
         <v>500</v>
       </c>
-      <c r="H63" s="1000" t="s">
+      <c r="H63" s="975" t="s">
         <v>501</v>
       </c>
-      <c r="I63" s="1000"/>
-      <c r="J63" s="1000"/>
+      <c r="I63" s="975"/>
+      <c r="J63" s="975"/>
       <c r="L63" s="708"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -12678,12 +12705,12 @@
       <c r="A74" s="623" t="s">
         <v>358</v>
       </c>
-      <c r="B74" s="976" t="s">
+      <c r="B74" s="994" t="s">
         <v>442</v>
       </c>
-      <c r="C74" s="976"/>
-      <c r="D74" s="976"/>
-      <c r="E74" s="976"/>
+      <c r="C74" s="994"/>
+      <c r="D74" s="994"/>
+      <c r="E74" s="994"/>
       <c r="I74" s="709"/>
       <c r="J74" s="709"/>
       <c r="K74" s="709"/>
@@ -12999,21 +13026,21 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="991" t="str">
+      <c r="B85" s="980" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="992"/>
-      <c r="D85" s="991" t="str">
+      <c r="C85" s="981"/>
+      <c r="D85" s="980" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="992"/>
-      <c r="F85" s="991" t="str">
+      <c r="E85" s="981"/>
+      <c r="F85" s="980" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="992"/>
+      <c r="G85" s="981"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="503"/>
@@ -13309,21 +13336,21 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="991" t="str">
+      <c r="B101" s="980" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="992"/>
-      <c r="D101" s="991" t="str">
+      <c r="C101" s="981"/>
+      <c r="D101" s="980" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="992"/>
-      <c r="F101" s="991" t="str">
+      <c r="E101" s="981"/>
+      <c r="F101" s="980" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="992"/>
+      <c r="G101" s="981"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="503"/>
@@ -13619,36 +13646,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="993" t="str">
+      <c r="B116" s="976" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="994"/>
-      <c r="D116" s="993" t="str">
+      <c r="C116" s="977"/>
+      <c r="D116" s="976" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="994"/>
-      <c r="F116" s="993" t="str">
+      <c r="E116" s="977"/>
+      <c r="F116" s="976" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="994"/>
+      <c r="G116" s="977"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="542"/>
-      <c r="B117" s="995" t="s">
+      <c r="B117" s="978" t="s">
         <v>266</v>
       </c>
-      <c r="C117" s="996"/>
-      <c r="D117" s="995" t="s">
+      <c r="C117" s="979"/>
+      <c r="D117" s="978" t="s">
         <v>266</v>
       </c>
-      <c r="E117" s="996"/>
-      <c r="F117" s="995" t="s">
+      <c r="E117" s="979"/>
+      <c r="F117" s="978" t="s">
         <v>266</v>
       </c>
-      <c r="G117" s="996"/>
+      <c r="G117" s="979"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="543" t="s">
@@ -13951,12 +13978,12 @@
       <c r="A129" s="546" t="s">
         <v>344</v>
       </c>
-      <c r="B129" s="989" t="str">
+      <c r="B129" s="991" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="990"/>
-      <c r="D129" s="990"/>
+      <c r="C129" s="992"/>
+      <c r="D129" s="992"/>
       <c r="N129" s="713" t="s">
         <v>385</v>
       </c>
@@ -14732,22 +14759,16 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="39">
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -14761,16 +14782,22 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18061,7 +18088,7 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:AQ10000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="AA8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -18453,16 +18480,16 @@
       <c r="AQ6" s="837"/>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="AD7" s="1001"/>
+      <c r="AD7" s="832"/>
       <c r="AE7" s="8"/>
-      <c r="AG7" s="1001"/>
+      <c r="AG7" s="832"/>
       <c r="AH7" s="8"/>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C8" s="755"/>
-      <c r="AD8" s="1001"/>
+      <c r="AD8" s="832"/>
       <c r="AE8" s="625"/>
-      <c r="AG8" s="1001"/>
+      <c r="AG8" s="832"/>
       <c r="AH8" s="625"/>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.3">
@@ -18514,7 +18541,7 @@
       <c r="A10" s="428" t="s">
         <v>64</v>
       </c>
-      <c r="AD10" s="1001"/>
+      <c r="AD10" s="832"/>
       <c r="AE10" s="8"/>
       <c r="AH10" s="8"/>
     </row>
@@ -18522,7 +18549,7 @@
       <c r="A11" s="428" t="s">
         <v>65</v>
       </c>
-      <c r="AD11" s="1001"/>
+      <c r="AD11" s="832"/>
       <c r="AE11" s="8"/>
       <c r="AH11" s="8"/>
     </row>
@@ -58938,123 +58965,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="658" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="844" t="s">
+      <c r="A1" s="873" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="845"/>
-      <c r="C1" s="845"/>
-      <c r="D1" s="845"/>
-      <c r="E1" s="845"/>
-      <c r="F1" s="845"/>
-      <c r="G1" s="845"/>
-      <c r="H1" s="846" t="s">
+      <c r="B1" s="874"/>
+      <c r="C1" s="874"/>
+      <c r="D1" s="874"/>
+      <c r="E1" s="874"/>
+      <c r="F1" s="874"/>
+      <c r="G1" s="874"/>
+      <c r="H1" s="875" t="s">
         <v>451</v>
       </c>
-      <c r="I1" s="847"/>
-      <c r="J1" s="847"/>
-      <c r="K1" s="847"/>
-      <c r="L1" s="847"/>
-      <c r="M1" s="848"/>
-      <c r="N1" s="849" t="s">
+      <c r="I1" s="876"/>
+      <c r="J1" s="876"/>
+      <c r="K1" s="876"/>
+      <c r="L1" s="876"/>
+      <c r="M1" s="877"/>
+      <c r="N1" s="878" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="850"/>
-      <c r="P1" s="850"/>
-      <c r="Q1" s="850"/>
-      <c r="R1" s="850"/>
-      <c r="S1" s="850"/>
-      <c r="T1" s="850"/>
-      <c r="U1" s="850"/>
-      <c r="V1" s="851" t="s">
+      <c r="O1" s="856"/>
+      <c r="P1" s="856"/>
+      <c r="Q1" s="856"/>
+      <c r="R1" s="856"/>
+      <c r="S1" s="856"/>
+      <c r="T1" s="856"/>
+      <c r="U1" s="856"/>
+      <c r="V1" s="879" t="s">
         <v>73</v>
       </c>
-      <c r="W1" s="852"/>
-      <c r="X1" s="853"/>
-      <c r="Y1" s="853"/>
-      <c r="Z1" s="854"/>
-      <c r="AA1" s="855" t="s">
+      <c r="W1" s="880"/>
+      <c r="X1" s="881"/>
+      <c r="Y1" s="881"/>
+      <c r="Z1" s="882"/>
+      <c r="AA1" s="883" t="s">
         <v>74</v>
       </c>
-      <c r="AB1" s="856"/>
-      <c r="AC1" s="856"/>
-      <c r="AD1" s="856"/>
-      <c r="AE1" s="856"/>
-      <c r="AF1" s="856"/>
-      <c r="AG1" s="856"/>
-      <c r="AH1" s="856"/>
-      <c r="AI1" s="856"/>
-      <c r="AJ1" s="856"/>
-      <c r="AK1" s="856"/>
-      <c r="AL1" s="856"/>
-      <c r="AM1" s="856"/>
+      <c r="AB1" s="884"/>
+      <c r="AC1" s="884"/>
+      <c r="AD1" s="884"/>
+      <c r="AE1" s="884"/>
+      <c r="AF1" s="884"/>
+      <c r="AG1" s="884"/>
+      <c r="AH1" s="884"/>
+      <c r="AI1" s="884"/>
+      <c r="AJ1" s="884"/>
+      <c r="AK1" s="884"/>
+      <c r="AL1" s="884"/>
+      <c r="AM1" s="884"/>
       <c r="AN1" s="52"/>
       <c r="AO1" s="53"/>
-      <c r="AP1" s="868" t="s">
+      <c r="AP1" s="855" t="s">
         <v>75</v>
       </c>
-      <c r="AQ1" s="850"/>
-      <c r="AR1" s="850"/>
-      <c r="AS1" s="850"/>
-      <c r="AT1" s="850"/>
-      <c r="AU1" s="850"/>
-      <c r="AV1" s="850"/>
-      <c r="AW1" s="869"/>
-      <c r="AX1" s="876" t="s">
+      <c r="AQ1" s="856"/>
+      <c r="AR1" s="856"/>
+      <c r="AS1" s="856"/>
+      <c r="AT1" s="856"/>
+      <c r="AU1" s="856"/>
+      <c r="AV1" s="856"/>
+      <c r="AW1" s="857"/>
+      <c r="AX1" s="864" t="s">
         <v>570</v>
       </c>
-      <c r="AY1" s="877"/>
-      <c r="AZ1" s="877"/>
-      <c r="BA1" s="877"/>
-      <c r="BB1" s="877"/>
-      <c r="BC1" s="878"/>
-      <c r="BD1" s="879" t="s">
+      <c r="AY1" s="865"/>
+      <c r="AZ1" s="865"/>
+      <c r="BA1" s="865"/>
+      <c r="BB1" s="865"/>
+      <c r="BC1" s="866"/>
+      <c r="BD1" s="867" t="s">
         <v>76</v>
       </c>
-      <c r="BE1" s="880"/>
-      <c r="BF1" s="880"/>
-      <c r="BG1" s="880"/>
-      <c r="BH1" s="880"/>
-      <c r="BI1" s="881"/>
-      <c r="BJ1" s="882" t="s">
+      <c r="BE1" s="868"/>
+      <c r="BF1" s="868"/>
+      <c r="BG1" s="868"/>
+      <c r="BH1" s="868"/>
+      <c r="BI1" s="869"/>
+      <c r="BJ1" s="870" t="s">
         <v>77</v>
       </c>
-      <c r="BK1" s="883"/>
-      <c r="BL1" s="883"/>
-      <c r="BM1" s="883"/>
-      <c r="BN1" s="883"/>
-      <c r="BO1" s="883"/>
-      <c r="BP1" s="884"/>
-      <c r="BQ1" s="857" t="s">
+      <c r="BK1" s="871"/>
+      <c r="BL1" s="871"/>
+      <c r="BM1" s="871"/>
+      <c r="BN1" s="871"/>
+      <c r="BO1" s="871"/>
+      <c r="BP1" s="872"/>
+      <c r="BQ1" s="844" t="s">
         <v>78</v>
       </c>
-      <c r="BR1" s="858"/>
-      <c r="BS1" s="858"/>
-      <c r="BT1" s="858"/>
-      <c r="BU1" s="858"/>
-      <c r="BV1" s="858"/>
+      <c r="BR1" s="845"/>
+      <c r="BS1" s="845"/>
+      <c r="BT1" s="845"/>
+      <c r="BU1" s="845"/>
+      <c r="BV1" s="845"/>
       <c r="BW1" s="53"/>
       <c r="BX1" s="54"/>
-      <c r="BY1" s="859" t="s">
+      <c r="BY1" s="846" t="s">
         <v>79</v>
       </c>
-      <c r="BZ1" s="860"/>
-      <c r="CA1" s="860"/>
-      <c r="CB1" s="860"/>
-      <c r="CC1" s="860"/>
-      <c r="CD1" s="860"/>
-      <c r="CE1" s="860"/>
-      <c r="CF1" s="861"/>
-      <c r="CG1" s="861"/>
-      <c r="CH1" s="861"/>
-      <c r="CI1" s="861"/>
-      <c r="CJ1" s="861"/>
-      <c r="CK1" s="861"/>
-      <c r="CL1" s="861"/>
-      <c r="CM1" s="861"/>
-      <c r="CN1" s="861"/>
-      <c r="CO1" s="861"/>
-      <c r="CP1" s="861"/>
-      <c r="CQ1" s="861"/>
+      <c r="BZ1" s="847"/>
+      <c r="CA1" s="847"/>
+      <c r="CB1" s="847"/>
+      <c r="CC1" s="847"/>
+      <c r="CD1" s="847"/>
+      <c r="CE1" s="847"/>
+      <c r="CF1" s="848"/>
+      <c r="CG1" s="848"/>
+      <c r="CH1" s="848"/>
+      <c r="CI1" s="848"/>
+      <c r="CJ1" s="848"/>
+      <c r="CK1" s="848"/>
+      <c r="CL1" s="848"/>
+      <c r="CM1" s="848"/>
+      <c r="CN1" s="848"/>
+      <c r="CO1" s="848"/>
+      <c r="CP1" s="848"/>
+      <c r="CQ1" s="848"/>
     </row>
     <row r="2" spans="1:95" s="658" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -59078,18 +59105,18 @@
       <c r="G2" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="862" t="s">
+      <c r="H2" s="849" t="s">
         <v>452</v>
       </c>
-      <c r="I2" s="863"/>
-      <c r="J2" s="863" t="s">
+      <c r="I2" s="850"/>
+      <c r="J2" s="850" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="863"/>
-      <c r="L2" s="863" t="s">
+      <c r="K2" s="850"/>
+      <c r="L2" s="850" t="s">
         <v>88</v>
       </c>
-      <c r="M2" s="864"/>
+      <c r="M2" s="851"/>
       <c r="N2" s="57" t="s">
         <v>80</v>
       </c>
@@ -59198,36 +59225,36 @@
       <c r="AW2" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="AX2" s="865" t="s">
+      <c r="AX2" s="852" t="s">
         <v>115</v>
       </c>
-      <c r="AY2" s="866"/>
-      <c r="AZ2" s="866"/>
-      <c r="BA2" s="866" t="s">
+      <c r="AY2" s="853"/>
+      <c r="AZ2" s="853"/>
+      <c r="BA2" s="853" t="s">
         <v>116</v>
       </c>
-      <c r="BB2" s="866"/>
-      <c r="BC2" s="867"/>
-      <c r="BD2" s="870" t="s">
+      <c r="BB2" s="853"/>
+      <c r="BC2" s="854"/>
+      <c r="BD2" s="858" t="s">
         <v>115</v>
       </c>
-      <c r="BE2" s="871"/>
-      <c r="BF2" s="871"/>
-      <c r="BG2" s="871" t="s">
+      <c r="BE2" s="859"/>
+      <c r="BF2" s="859"/>
+      <c r="BG2" s="859" t="s">
         <v>116</v>
       </c>
-      <c r="BH2" s="871"/>
-      <c r="BI2" s="872"/>
-      <c r="BJ2" s="873" t="s">
+      <c r="BH2" s="859"/>
+      <c r="BI2" s="860"/>
+      <c r="BJ2" s="861" t="s">
         <v>115</v>
       </c>
-      <c r="BK2" s="874"/>
-      <c r="BL2" s="874"/>
-      <c r="BM2" s="874" t="s">
+      <c r="BK2" s="862"/>
+      <c r="BL2" s="862"/>
+      <c r="BM2" s="862" t="s">
         <v>116</v>
       </c>
-      <c r="BN2" s="875"/>
-      <c r="BO2" s="875"/>
+      <c r="BN2" s="863"/>
+      <c r="BO2" s="863"/>
       <c r="BP2" s="69" t="s">
         <v>117</v>
       </c>
@@ -59860,6 +59887,11 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -59875,11 +59907,6 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -59963,100 +59990,100 @@
         <v>157</v>
       </c>
       <c r="L1" s="145"/>
-      <c r="M1" s="885" t="s">
+      <c r="M1" s="908" t="s">
         <v>158</v>
       </c>
-      <c r="N1" s="886" t="s">
+      <c r="N1" s="909" t="s">
         <v>507</v>
       </c>
-      <c r="O1" s="887"/>
-      <c r="P1" s="887"/>
-      <c r="Q1" s="887"/>
-      <c r="R1" s="888" t="s">
+      <c r="O1" s="910"/>
+      <c r="P1" s="910"/>
+      <c r="Q1" s="910"/>
+      <c r="R1" s="911" t="s">
         <v>451</v>
       </c>
-      <c r="S1" s="889"/>
-      <c r="T1" s="889"/>
-      <c r="U1" s="889"/>
-      <c r="V1" s="889"/>
-      <c r="W1" s="889"/>
-      <c r="X1" s="890"/>
-      <c r="Y1" s="891" t="s">
+      <c r="S1" s="904"/>
+      <c r="T1" s="904"/>
+      <c r="U1" s="904"/>
+      <c r="V1" s="904"/>
+      <c r="W1" s="904"/>
+      <c r="X1" s="912"/>
+      <c r="Y1" s="898" t="s">
         <v>459</v>
       </c>
-      <c r="Z1" s="880"/>
-      <c r="AA1" s="894" t="s">
+      <c r="Z1" s="868"/>
+      <c r="AA1" s="914" t="s">
         <v>159</v>
       </c>
-      <c r="AB1" s="906" t="s">
+      <c r="AB1" s="886" t="s">
         <v>160</v>
       </c>
-      <c r="AC1" s="902" t="s">
+      <c r="AC1" s="900" t="s">
         <v>161</v>
       </c>
-      <c r="AD1" s="903"/>
-      <c r="AE1" s="903"/>
-      <c r="AF1" s="904"/>
-      <c r="AG1" s="905" t="s">
+      <c r="AD1" s="901"/>
+      <c r="AE1" s="901"/>
+      <c r="AF1" s="902"/>
+      <c r="AG1" s="903" t="s">
         <v>162</v>
       </c>
-      <c r="AH1" s="889"/>
-      <c r="AI1" s="889"/>
-      <c r="AJ1" s="889"/>
-      <c r="AK1" s="889"/>
-      <c r="AL1" s="889"/>
-      <c r="AM1" s="889"/>
-      <c r="AN1" s="889"/>
-      <c r="AO1" s="906" t="s">
+      <c r="AH1" s="904"/>
+      <c r="AI1" s="904"/>
+      <c r="AJ1" s="904"/>
+      <c r="AK1" s="904"/>
+      <c r="AL1" s="904"/>
+      <c r="AM1" s="904"/>
+      <c r="AN1" s="904"/>
+      <c r="AO1" s="886" t="s">
         <v>163</v>
       </c>
-      <c r="AP1" s="891" t="s">
+      <c r="AP1" s="898" t="s">
         <v>458</v>
       </c>
-      <c r="AQ1" s="880"/>
-      <c r="AR1" s="880"/>
-      <c r="AS1" s="881"/>
-      <c r="AT1" s="909" t="s">
+      <c r="AQ1" s="868"/>
+      <c r="AR1" s="868"/>
+      <c r="AS1" s="869"/>
+      <c r="AT1" s="906" t="s">
         <v>164</v>
       </c>
-      <c r="AU1" s="910"/>
-      <c r="AV1" s="910"/>
-      <c r="AW1" s="910"/>
-      <c r="AX1" s="910"/>
-      <c r="AY1" s="910"/>
-      <c r="AZ1" s="910"/>
-      <c r="BA1" s="910"/>
-      <c r="BB1" s="910"/>
-      <c r="BC1" s="910"/>
-      <c r="BD1" s="910"/>
-      <c r="BE1" s="910"/>
-      <c r="BF1" s="910"/>
-      <c r="BG1" s="910"/>
-      <c r="BH1" s="910"/>
-      <c r="BI1" s="910"/>
-      <c r="BJ1" s="910"/>
-      <c r="BK1" s="910"/>
-      <c r="BL1" s="910"/>
-      <c r="BM1" s="910"/>
-      <c r="BN1" s="910"/>
-      <c r="BO1" s="910"/>
-      <c r="BP1" s="910"/>
-      <c r="BQ1" s="910"/>
-      <c r="BR1" s="910"/>
-      <c r="BS1" s="910"/>
-      <c r="BT1" s="910"/>
-      <c r="BU1" s="910"/>
-      <c r="BV1" s="910"/>
-      <c r="BW1" s="906" t="s">
+      <c r="AU1" s="907"/>
+      <c r="AV1" s="907"/>
+      <c r="AW1" s="907"/>
+      <c r="AX1" s="907"/>
+      <c r="AY1" s="907"/>
+      <c r="AZ1" s="907"/>
+      <c r="BA1" s="907"/>
+      <c r="BB1" s="907"/>
+      <c r="BC1" s="907"/>
+      <c r="BD1" s="907"/>
+      <c r="BE1" s="907"/>
+      <c r="BF1" s="907"/>
+      <c r="BG1" s="907"/>
+      <c r="BH1" s="907"/>
+      <c r="BI1" s="907"/>
+      <c r="BJ1" s="907"/>
+      <c r="BK1" s="907"/>
+      <c r="BL1" s="907"/>
+      <c r="BM1" s="907"/>
+      <c r="BN1" s="907"/>
+      <c r="BO1" s="907"/>
+      <c r="BP1" s="907"/>
+      <c r="BQ1" s="907"/>
+      <c r="BR1" s="907"/>
+      <c r="BS1" s="907"/>
+      <c r="BT1" s="907"/>
+      <c r="BU1" s="907"/>
+      <c r="BV1" s="907"/>
+      <c r="BW1" s="886" t="s">
         <v>165</v>
       </c>
-      <c r="BX1" s="891" t="s">
+      <c r="BX1" s="898" t="s">
         <v>457</v>
       </c>
-      <c r="BY1" s="880"/>
-      <c r="BZ1" s="880"/>
-      <c r="CA1" s="881"/>
-      <c r="CB1" s="918" t="s">
+      <c r="BY1" s="868"/>
+      <c r="BZ1" s="868"/>
+      <c r="CA1" s="869"/>
+      <c r="CB1" s="897" t="s">
         <v>474</v>
       </c>
       <c r="CC1" s="899" t="s">
@@ -60074,16 +60101,16 @@
       <c r="CM1" s="899"/>
       <c r="CN1" s="899"/>
       <c r="CO1" s="146"/>
-      <c r="CP1" s="914" t="s">
+      <c r="CP1" s="885" t="s">
         <v>78</v>
       </c>
-      <c r="CQ1" s="850"/>
-      <c r="CR1" s="850"/>
-      <c r="CS1" s="850"/>
-      <c r="CT1" s="850"/>
-      <c r="CU1" s="850"/>
-      <c r="CV1" s="850"/>
-      <c r="CW1" s="869"/>
+      <c r="CQ1" s="856"/>
+      <c r="CR1" s="856"/>
+      <c r="CS1" s="856"/>
+      <c r="CT1" s="856"/>
+      <c r="CU1" s="856"/>
+      <c r="CV1" s="856"/>
+      <c r="CW1" s="857"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="147" t="s">
@@ -60122,7 +60149,7 @@
       <c r="L2" s="151" t="s">
         <v>81</v>
       </c>
-      <c r="M2" s="885"/>
+      <c r="M2" s="908"/>
       <c r="N2" s="152" t="s">
         <v>170</v>
       </c>
@@ -60138,22 +60165,22 @@
       <c r="R2" s="157" t="s">
         <v>173</v>
       </c>
-      <c r="S2" s="896" t="s">
+      <c r="S2" s="916" t="s">
         <v>452</v>
       </c>
-      <c r="T2" s="875"/>
-      <c r="U2" s="897" t="s">
+      <c r="T2" s="863"/>
+      <c r="U2" s="917" t="s">
         <v>87</v>
       </c>
-      <c r="V2" s="897"/>
-      <c r="W2" s="897" t="s">
+      <c r="V2" s="917"/>
+      <c r="W2" s="917" t="s">
         <v>88</v>
       </c>
-      <c r="X2" s="898"/>
-      <c r="Y2" s="892"/>
+      <c r="X2" s="918"/>
+      <c r="Y2" s="913"/>
       <c r="Z2" s="893"/>
-      <c r="AA2" s="895"/>
-      <c r="AB2" s="907"/>
+      <c r="AA2" s="915"/>
+      <c r="AB2" s="887"/>
       <c r="AC2" s="153" t="s">
         <v>174</v>
       </c>
@@ -60166,81 +60193,81 @@
       <c r="AF2" s="153" t="s">
         <v>177</v>
       </c>
-      <c r="AG2" s="908" t="s">
+      <c r="AG2" s="905" t="s">
         <v>178</v>
       </c>
-      <c r="AH2" s="900"/>
-      <c r="AI2" s="900" t="s">
+      <c r="AH2" s="890"/>
+      <c r="AI2" s="890" t="s">
         <v>179</v>
       </c>
-      <c r="AJ2" s="900"/>
-      <c r="AK2" s="900" t="s">
+      <c r="AJ2" s="890"/>
+      <c r="AK2" s="890" t="s">
         <v>180</v>
       </c>
-      <c r="AL2" s="900"/>
+      <c r="AL2" s="890"/>
       <c r="AM2" s="154" t="s">
         <v>181</v>
       </c>
       <c r="AN2" s="154" t="s">
         <v>182</v>
       </c>
-      <c r="AO2" s="907"/>
-      <c r="AP2" s="901" t="s">
+      <c r="AO2" s="887"/>
+      <c r="AP2" s="892" t="s">
         <v>595</v>
       </c>
       <c r="AQ2" s="893"/>
-      <c r="AR2" s="911" t="s">
+      <c r="AR2" s="894" t="s">
         <v>596</v>
       </c>
-      <c r="AS2" s="912"/>
-      <c r="AT2" s="900" t="s">
+      <c r="AS2" s="895"/>
+      <c r="AT2" s="890" t="s">
         <v>183</v>
       </c>
-      <c r="AU2" s="900"/>
-      <c r="AV2" s="913" t="s">
+      <c r="AU2" s="890"/>
+      <c r="AV2" s="891" t="s">
         <v>184</v>
       </c>
-      <c r="AW2" s="913"/>
-      <c r="AX2" s="913" t="s">
+      <c r="AW2" s="891"/>
+      <c r="AX2" s="891" t="s">
         <v>185</v>
       </c>
-      <c r="AY2" s="913"/>
+      <c r="AY2" s="891"/>
       <c r="AZ2" s="154" t="s">
         <v>186</v>
       </c>
       <c r="BA2" s="154" t="s">
         <v>187</v>
       </c>
-      <c r="BB2" s="900" t="s">
+      <c r="BB2" s="890" t="s">
         <v>188</v>
       </c>
-      <c r="BC2" s="900"/>
-      <c r="BD2" s="913" t="s">
+      <c r="BC2" s="890"/>
+      <c r="BD2" s="891" t="s">
         <v>189</v>
       </c>
-      <c r="BE2" s="913"/>
-      <c r="BF2" s="913" t="s">
+      <c r="BE2" s="891"/>
+      <c r="BF2" s="891" t="s">
         <v>190</v>
       </c>
-      <c r="BG2" s="913"/>
+      <c r="BG2" s="891"/>
       <c r="BH2" s="154" t="s">
         <v>191</v>
       </c>
       <c r="BI2" s="154" t="s">
         <v>192</v>
       </c>
-      <c r="BJ2" s="900" t="s">
+      <c r="BJ2" s="890" t="s">
         <v>193</v>
       </c>
-      <c r="BK2" s="900"/>
-      <c r="BL2" s="913" t="s">
+      <c r="BK2" s="890"/>
+      <c r="BL2" s="891" t="s">
         <v>194</v>
       </c>
-      <c r="BM2" s="913"/>
-      <c r="BN2" s="913" t="s">
+      <c r="BM2" s="891"/>
+      <c r="BN2" s="891" t="s">
         <v>195</v>
       </c>
-      <c r="BO2" s="913"/>
+      <c r="BO2" s="891"/>
       <c r="BP2" s="154" t="s">
         <v>196</v>
       </c>
@@ -60262,16 +60289,16 @@
       <c r="BV2" s="154" t="s">
         <v>202</v>
       </c>
-      <c r="BW2" s="907"/>
-      <c r="BX2" s="901" t="s">
+      <c r="BW2" s="887"/>
+      <c r="BX2" s="892" t="s">
         <v>595</v>
       </c>
       <c r="BY2" s="893"/>
-      <c r="BZ2" s="911" t="s">
+      <c r="BZ2" s="894" t="s">
         <v>596</v>
       </c>
-      <c r="CA2" s="912"/>
-      <c r="CB2" s="918"/>
+      <c r="CA2" s="895"/>
+      <c r="CB2" s="897"/>
       <c r="CC2" s="138" t="s">
         <v>96</v>
       </c>
@@ -60311,22 +60338,22 @@
       <c r="CO2" s="140" t="s">
         <v>460</v>
       </c>
-      <c r="CP2" s="917" t="s">
+      <c r="CP2" s="896" t="s">
         <v>204</v>
       </c>
-      <c r="CQ2" s="915"/>
-      <c r="CR2" s="915" t="s">
+      <c r="CQ2" s="888"/>
+      <c r="CR2" s="888" t="s">
         <v>205</v>
       </c>
-      <c r="CS2" s="915"/>
-      <c r="CT2" s="915" t="s">
+      <c r="CS2" s="888"/>
+      <c r="CT2" s="888" t="s">
         <v>206</v>
       </c>
-      <c r="CU2" s="915"/>
-      <c r="CV2" s="915" t="s">
+      <c r="CU2" s="888"/>
+      <c r="CV2" s="888" t="s">
         <v>207</v>
       </c>
-      <c r="CW2" s="916"/>
+      <c r="CW2" s="889"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="168"/>
@@ -61191,6 +61218,29 @@
     </sortState>
   </autoFilter>
   <mergeCells count="39">
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="CC1:CN1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AN1"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
     <mergeCell ref="CP1:CW1"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="CV2:CW2"/>
@@ -61207,29 +61257,6 @@
     <mergeCell ref="CT2:CU2"/>
     <mergeCell ref="CB1:CB2"/>
     <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CC1:CN1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AN1"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -61273,72 +61300,72 @@
       <c r="K1" s="144"/>
       <c r="L1" s="145"/>
       <c r="M1" s="695"/>
-      <c r="N1" s="922"/>
-      <c r="O1" s="923"/>
-      <c r="P1" s="923"/>
-      <c r="Q1" s="923"/>
-      <c r="R1" s="888"/>
-      <c r="S1" s="889"/>
-      <c r="T1" s="889"/>
-      <c r="U1" s="889"/>
-      <c r="V1" s="889"/>
-      <c r="W1" s="889"/>
-      <c r="X1" s="890"/>
-      <c r="Y1" s="891"/>
-      <c r="Z1" s="880"/>
+      <c r="N1" s="919"/>
+      <c r="O1" s="920"/>
+      <c r="P1" s="920"/>
+      <c r="Q1" s="920"/>
+      <c r="R1" s="911"/>
+      <c r="S1" s="904"/>
+      <c r="T1" s="904"/>
+      <c r="U1" s="904"/>
+      <c r="V1" s="904"/>
+      <c r="W1" s="904"/>
+      <c r="X1" s="912"/>
+      <c r="Y1" s="898"/>
+      <c r="Z1" s="868"/>
       <c r="AA1" s="696"/>
       <c r="AB1" s="694"/>
-      <c r="AC1" s="902"/>
-      <c r="AD1" s="903"/>
-      <c r="AE1" s="903"/>
-      <c r="AF1" s="904"/>
-      <c r="AG1" s="905"/>
-      <c r="AH1" s="889"/>
-      <c r="AI1" s="889"/>
-      <c r="AJ1" s="889"/>
-      <c r="AK1" s="889"/>
-      <c r="AL1" s="889"/>
-      <c r="AM1" s="889"/>
-      <c r="AN1" s="889"/>
+      <c r="AC1" s="900"/>
+      <c r="AD1" s="901"/>
+      <c r="AE1" s="901"/>
+      <c r="AF1" s="902"/>
+      <c r="AG1" s="903"/>
+      <c r="AH1" s="904"/>
+      <c r="AI1" s="904"/>
+      <c r="AJ1" s="904"/>
+      <c r="AK1" s="904"/>
+      <c r="AL1" s="904"/>
+      <c r="AM1" s="904"/>
+      <c r="AN1" s="904"/>
       <c r="AO1" s="694"/>
-      <c r="AP1" s="891"/>
-      <c r="AQ1" s="880"/>
-      <c r="AR1" s="880"/>
-      <c r="AS1" s="881"/>
-      <c r="AT1" s="909"/>
-      <c r="AU1" s="910"/>
-      <c r="AV1" s="910"/>
-      <c r="AW1" s="910"/>
-      <c r="AX1" s="910"/>
-      <c r="AY1" s="910"/>
-      <c r="AZ1" s="910"/>
-      <c r="BA1" s="910"/>
-      <c r="BB1" s="910"/>
-      <c r="BC1" s="910"/>
-      <c r="BD1" s="910"/>
-      <c r="BE1" s="910"/>
-      <c r="BF1" s="910"/>
-      <c r="BG1" s="910"/>
-      <c r="BH1" s="910"/>
-      <c r="BI1" s="910"/>
-      <c r="BJ1" s="910"/>
-      <c r="BK1" s="910"/>
-      <c r="BL1" s="910"/>
-      <c r="BM1" s="910"/>
-      <c r="BN1" s="910"/>
-      <c r="BO1" s="910"/>
-      <c r="BP1" s="910"/>
-      <c r="BQ1" s="910"/>
-      <c r="BR1" s="910"/>
-      <c r="BS1" s="910"/>
-      <c r="BT1" s="910"/>
-      <c r="BU1" s="910"/>
-      <c r="BV1" s="910"/>
+      <c r="AP1" s="898"/>
+      <c r="AQ1" s="868"/>
+      <c r="AR1" s="868"/>
+      <c r="AS1" s="869"/>
+      <c r="AT1" s="906"/>
+      <c r="AU1" s="907"/>
+      <c r="AV1" s="907"/>
+      <c r="AW1" s="907"/>
+      <c r="AX1" s="907"/>
+      <c r="AY1" s="907"/>
+      <c r="AZ1" s="907"/>
+      <c r="BA1" s="907"/>
+      <c r="BB1" s="907"/>
+      <c r="BC1" s="907"/>
+      <c r="BD1" s="907"/>
+      <c r="BE1" s="907"/>
+      <c r="BF1" s="907"/>
+      <c r="BG1" s="907"/>
+      <c r="BH1" s="907"/>
+      <c r="BI1" s="907"/>
+      <c r="BJ1" s="907"/>
+      <c r="BK1" s="907"/>
+      <c r="BL1" s="907"/>
+      <c r="BM1" s="907"/>
+      <c r="BN1" s="907"/>
+      <c r="BO1" s="907"/>
+      <c r="BP1" s="907"/>
+      <c r="BQ1" s="907"/>
+      <c r="BR1" s="907"/>
+      <c r="BS1" s="907"/>
+      <c r="BT1" s="907"/>
+      <c r="BU1" s="907"/>
+      <c r="BV1" s="907"/>
       <c r="BW1" s="694"/>
-      <c r="BX1" s="891"/>
-      <c r="BY1" s="880"/>
-      <c r="BZ1" s="880"/>
-      <c r="CA1" s="881"/>
+      <c r="BX1" s="898"/>
+      <c r="BY1" s="868"/>
+      <c r="BZ1" s="868"/>
+      <c r="CA1" s="869"/>
       <c r="CB1" s="899"/>
       <c r="CC1" s="899"/>
       <c r="CD1" s="899"/>
@@ -61352,31 +61379,26 @@
       <c r="CL1" s="899"/>
       <c r="CM1" s="899"/>
       <c r="CN1" s="693"/>
-      <c r="CO1" s="914"/>
-      <c r="CP1" s="850"/>
-      <c r="CQ1" s="850"/>
-      <c r="CR1" s="850"/>
-      <c r="CS1" s="850"/>
-      <c r="CT1" s="850"/>
-      <c r="CU1" s="850"/>
-      <c r="CV1" s="869"/>
-      <c r="CW1" s="919"/>
-      <c r="CX1" s="920"/>
-      <c r="CY1" s="920"/>
-      <c r="CZ1" s="921"/>
-      <c r="DA1" s="920"/>
-      <c r="DB1" s="920"/>
-      <c r="DC1" s="921"/>
-      <c r="DD1" s="920"/>
-      <c r="DE1" s="920"/>
+      <c r="CO1" s="885"/>
+      <c r="CP1" s="856"/>
+      <c r="CQ1" s="856"/>
+      <c r="CR1" s="856"/>
+      <c r="CS1" s="856"/>
+      <c r="CT1" s="856"/>
+      <c r="CU1" s="856"/>
+      <c r="CV1" s="857"/>
+      <c r="CW1" s="921"/>
+      <c r="CX1" s="922"/>
+      <c r="CY1" s="922"/>
+      <c r="CZ1" s="923"/>
+      <c r="DA1" s="922"/>
+      <c r="DB1" s="922"/>
+      <c r="DC1" s="923"/>
+      <c r="DD1" s="922"/>
+      <c r="DE1" s="922"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="CZ1:DB1"/>
     <mergeCell ref="DC1:DE1"/>
@@ -61385,6 +61407,11 @@
     <mergeCell ref="AG1:AN1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CB1:CM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -61610,10 +61637,10 @@
       <c r="B2" s="203" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="931" t="s">
+      <c r="C2" s="933" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="931"/>
+      <c r="D2" s="933"/>
       <c r="E2" s="201"/>
       <c r="F2" s="201"/>
       <c r="G2" s="201"/>
@@ -61777,35 +61804,35 @@
     </row>
     <row r="7" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="200"/>
-      <c r="B7" s="928"/>
-      <c r="C7" s="928"/>
-      <c r="D7" s="928"/>
+      <c r="B7" s="934"/>
+      <c r="C7" s="934"/>
+      <c r="D7" s="934"/>
       <c r="E7" s="201"/>
       <c r="F7" s="201"/>
       <c r="G7" s="201"/>
       <c r="H7" s="201"/>
       <c r="I7" s="201"/>
-      <c r="J7" s="928"/>
-      <c r="K7" s="928"/>
-      <c r="L7" s="928"/>
+      <c r="J7" s="934"/>
+      <c r="K7" s="934"/>
+      <c r="L7" s="934"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="201"/>
       <c r="P7" s="202" t="s">
         <v>231</v>
       </c>
-      <c r="Q7" s="928"/>
-      <c r="R7" s="928"/>
-      <c r="S7" s="928"/>
+      <c r="Q7" s="934"/>
+      <c r="R7" s="934"/>
+      <c r="S7" s="934"/>
       <c r="T7" s="201"/>
       <c r="U7" s="215"/>
       <c r="V7" s="372"/>
       <c r="W7" s="372" t="s">
         <v>231</v>
       </c>
-      <c r="X7" s="928"/>
-      <c r="Y7" s="928"/>
-      <c r="Z7" s="928"/>
+      <c r="X7" s="934"/>
+      <c r="Y7" s="934"/>
+      <c r="Z7" s="934"/>
       <c r="AA7" s="372"/>
       <c r="AB7" s="215"/>
     </row>
@@ -61982,10 +62009,10 @@
       </c>
       <c r="K11" s="201"/>
       <c r="L11" s="201"/>
-      <c r="M11" s="933" t="s">
+      <c r="M11" s="931" t="s">
         <v>237</v>
       </c>
-      <c r="N11" s="934"/>
+      <c r="N11" s="932"/>
       <c r="O11" s="222"/>
       <c r="P11" s="222"/>
       <c r="Q11" s="220" t="s">
@@ -63167,11 +63194,11 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="200"/>
-      <c r="B42" s="932"/>
-      <c r="C42" s="932"/>
-      <c r="D42" s="932"/>
-      <c r="E42" s="932"/>
-      <c r="F42" s="932"/>
+      <c r="B42" s="928"/>
+      <c r="C42" s="928"/>
+      <c r="D42" s="928"/>
+      <c r="E42" s="928"/>
+      <c r="F42" s="928"/>
       <c r="G42" s="240"/>
       <c r="H42" s="201"/>
       <c r="I42" s="240"/>
@@ -63358,6 +63385,21 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="26">
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -63369,21 +63411,6 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA20:AB20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
update druapl core and add a column on RCA sheet in register
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="660" yWindow="480" windowWidth="13740" windowHeight="7368" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Glossary" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="643">
   <si>
     <t>Acronym</t>
   </si>
@@ -3994,7 +3994,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1003">
+  <cellXfs count="1002">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -5970,15 +5970,6 @@
     </xf>
     <xf numFmtId="0" fontId="53" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6001,6 +5992,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6037,9 +6067,6 @@
     <xf numFmtId="3" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6088,41 +6115,92 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6133,104 +6211,26 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6238,15 +6238,6 @@
     <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6259,26 +6250,26 @@
     <xf numFmtId="0" fontId="25" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6308,6 +6299,39 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -6334,39 +6358,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6396,80 +6387,86 @@
     <xf numFmtId="3" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7238,8 +7235,8 @@
       <c r="B3" s="323" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="937"/>
-      <c r="D3" s="937"/>
+      <c r="C3" s="934"/>
+      <c r="D3" s="934"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C4" s="324"/>
@@ -7272,10 +7269,10 @@
       <c r="D10" s="331" t="s">
         <v>252</v>
       </c>
-      <c r="E10" s="938" t="s">
+      <c r="E10" s="935" t="s">
         <v>495</v>
       </c>
-      <c r="F10" s="939"/>
+      <c r="F10" s="936"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="332" t="s">
@@ -7430,10 +7427,10 @@
       <c r="D30" s="341" t="s">
         <v>252</v>
       </c>
-      <c r="E30" s="938" t="s">
+      <c r="E30" s="935" t="s">
         <v>495</v>
       </c>
-      <c r="F30" s="939"/>
+      <c r="F30" s="936"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="332" t="s">
@@ -7585,10 +7582,10 @@
       <c r="D49" s="341" t="s">
         <v>252</v>
       </c>
-      <c r="E49" s="938" t="s">
+      <c r="E49" s="935" t="s">
         <v>495</v>
       </c>
-      <c r="F49" s="939"/>
+      <c r="F49" s="936"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="332" t="s">
@@ -7740,10 +7737,10 @@
       <c r="D68" s="341" t="s">
         <v>252</v>
       </c>
-      <c r="E68" s="938" t="s">
+      <c r="E68" s="935" t="s">
         <v>495</v>
       </c>
-      <c r="F68" s="939"/>
+      <c r="F68" s="936"/>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="503" t="s">
@@ -7918,8 +7915,8 @@
       </c>
       <c r="C2" s="372"/>
       <c r="D2" s="372"/>
-      <c r="E2" s="935"/>
-      <c r="F2" s="935"/>
+      <c r="E2" s="930"/>
+      <c r="F2" s="930"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="371"/>
@@ -7951,13 +7948,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="369"/>
-      <c r="B6" s="936" t="s">
+      <c r="B6" s="927" t="s">
         <v>420</v>
       </c>
-      <c r="C6" s="936"/>
-      <c r="D6" s="936"/>
-      <c r="E6" s="936"/>
-      <c r="F6" s="936"/>
+      <c r="C6" s="927"/>
+      <c r="D6" s="927"/>
+      <c r="E6" s="927"/>
+      <c r="F6" s="927"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="369"/>
@@ -7972,14 +7969,14 @@
       <c r="B8" s="398" t="s">
         <v>451</v>
       </c>
-      <c r="C8" s="940" t="s">
+      <c r="C8" s="937" t="s">
         <v>220</v>
       </c>
-      <c r="D8" s="941"/>
-      <c r="E8" s="940" t="s">
+      <c r="D8" s="938"/>
+      <c r="E8" s="937" t="s">
         <v>221</v>
       </c>
-      <c r="F8" s="941"/>
+      <c r="F8" s="938"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="369"/>
@@ -8115,11 +8112,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="369"/>
-      <c r="B22" s="930"/>
-      <c r="C22" s="930"/>
-      <c r="D22" s="930"/>
-      <c r="E22" s="930"/>
-      <c r="F22" s="930"/>
+      <c r="B22" s="931"/>
+      <c r="C22" s="931"/>
+      <c r="D22" s="931"/>
+      <c r="E22" s="931"/>
+      <c r="F22" s="931"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="369"/>
@@ -8191,13 +8188,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="942" t="s">
+      <c r="B2" s="939" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="943" t="s">
+      <c r="C2" s="940" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="943" t="s">
+      <c r="D2" s="940" t="s">
         <v>158</v>
       </c>
       <c r="E2" s="423" t="s">
@@ -8232,9 +8229,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="942"/>
-      <c r="C3" s="944"/>
-      <c r="D3" s="944"/>
+      <c r="B3" s="939"/>
+      <c r="C3" s="941"/>
+      <c r="D3" s="941"/>
       <c r="E3" s="438" t="s">
         <v>269</v>
       </c>
@@ -8267,7 +8264,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="945" t="s">
+      <c r="B4" s="942" t="s">
         <v>272</v>
       </c>
       <c r="C4" s="424" t="s">
@@ -8286,7 +8283,7 @@
       <c r="N4" s="426"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="945"/>
+      <c r="B5" s="942"/>
       <c r="C5" s="424" t="s">
         <v>82</v>
       </c>
@@ -8303,7 +8300,7 @@
       <c r="N5" s="426"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="946"/>
+      <c r="B6" s="943"/>
       <c r="C6" s="434" t="s">
         <v>262</v>
       </c>
@@ -8418,43 +8415,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="959" t="s">
+      <c r="A1" s="947" t="s">
         <v>638</v>
       </c>
-      <c r="B1" s="960"/>
+      <c r="B1" s="948"/>
       <c r="C1" s="454"/>
-      <c r="D1" s="950" t="s">
+      <c r="D1" s="958" t="s">
         <v>273</v>
       </c>
-      <c r="E1" s="951"/>
-      <c r="F1" s="951"/>
-      <c r="G1" s="951"/>
-      <c r="H1" s="951"/>
-      <c r="I1" s="952"/>
-      <c r="J1" s="961" t="s">
+      <c r="E1" s="959"/>
+      <c r="F1" s="959"/>
+      <c r="G1" s="959"/>
+      <c r="H1" s="959"/>
+      <c r="I1" s="960"/>
+      <c r="J1" s="949" t="s">
         <v>624</v>
       </c>
-      <c r="K1" s="962"/>
-      <c r="L1" s="962"/>
-      <c r="M1" s="962"/>
-      <c r="N1" s="963"/>
-      <c r="O1" s="964" t="s">
+      <c r="K1" s="950"/>
+      <c r="L1" s="950"/>
+      <c r="M1" s="950"/>
+      <c r="N1" s="951"/>
+      <c r="O1" s="952" t="s">
         <v>274</v>
       </c>
-      <c r="P1" s="965"/>
-      <c r="Q1" s="966"/>
+      <c r="P1" s="953"/>
+      <c r="Q1" s="954"/>
       <c r="R1" s="441" t="s">
         <v>70</v>
       </c>
       <c r="S1" s="442"/>
-      <c r="T1" s="958" t="s">
+      <c r="T1" s="946" t="s">
         <v>462</v>
       </c>
-      <c r="U1" s="958"/>
-      <c r="V1" s="958"/>
-      <c r="W1" s="958"/>
-      <c r="X1" s="958"/>
-      <c r="Y1" s="958"/>
+      <c r="U1" s="946"/>
+      <c r="V1" s="946"/>
+      <c r="W1" s="946"/>
+      <c r="X1" s="946"/>
+      <c r="Y1" s="946"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="444" t="s">
@@ -8466,18 +8463,18 @@
       <c r="C2" s="445" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="955" t="s">
+      <c r="D2" s="963" t="s">
         <v>275</v>
       </c>
-      <c r="E2" s="954"/>
-      <c r="F2" s="954" t="s">
+      <c r="E2" s="962"/>
+      <c r="F2" s="962" t="s">
         <v>276</v>
       </c>
-      <c r="G2" s="954"/>
-      <c r="H2" s="953" t="s">
+      <c r="G2" s="962"/>
+      <c r="H2" s="961" t="s">
         <v>277</v>
       </c>
-      <c r="I2" s="953"/>
+      <c r="I2" s="961"/>
       <c r="J2" s="446">
         <v>0</v>
       </c>
@@ -8508,18 +8505,18 @@
       <c r="S2" s="675" t="s">
         <v>80</v>
       </c>
-      <c r="T2" s="956" t="s">
+      <c r="T2" s="944" t="s">
         <v>432</v>
       </c>
-      <c r="U2" s="956"/>
-      <c r="V2" s="957" t="s">
+      <c r="U2" s="944"/>
+      <c r="V2" s="945" t="s">
         <v>448</v>
       </c>
-      <c r="W2" s="957"/>
-      <c r="X2" s="957" t="s">
+      <c r="W2" s="945"/>
+      <c r="X2" s="945" t="s">
         <v>449</v>
       </c>
-      <c r="Y2" s="957"/>
+      <c r="Y2" s="945"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="449"/>
@@ -8545,13 +8542,13 @@
       <c r="I3" s="659" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="947" t="s">
+      <c r="J3" s="955" t="s">
         <v>282</v>
       </c>
-      <c r="K3" s="948"/>
-      <c r="L3" s="948"/>
-      <c r="M3" s="948"/>
-      <c r="N3" s="949"/>
+      <c r="K3" s="956"/>
+      <c r="L3" s="956"/>
+      <c r="M3" s="956"/>
+      <c r="N3" s="957"/>
       <c r="O3" s="457"/>
       <c r="P3" s="457"/>
       <c r="Q3" s="457"/>
@@ -9480,6 +9477,11 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:X4"/>
   <mergeCells count="12">
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -9487,11 +9489,6 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9532,25 +9529,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="873" t="s">
+      <c r="A1" s="841" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="874"/>
-      <c r="C1" s="874"/>
-      <c r="D1" s="874"/>
-      <c r="E1" s="874"/>
-      <c r="F1" s="874"/>
+      <c r="B1" s="842"/>
+      <c r="C1" s="842"/>
+      <c r="D1" s="842"/>
+      <c r="E1" s="842"/>
+      <c r="F1" s="842"/>
       <c r="G1" s="471"/>
-      <c r="H1" s="973" t="s">
+      <c r="H1" s="970" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="974"/>
-      <c r="J1" s="974"/>
+      <c r="I1" s="971"/>
+      <c r="J1" s="971"/>
       <c r="K1" s="473"/>
       <c r="L1" s="463"/>
       <c r="M1" s="473"/>
       <c r="N1" s="464"/>
-      <c r="O1" s="971" t="s">
+      <c r="O1" s="968" t="s">
         <v>284</v>
       </c>
       <c r="P1" s="465"/>
@@ -9562,26 +9559,26 @@
       <c r="T1" s="463"/>
       <c r="U1" s="473"/>
       <c r="V1" s="464"/>
-      <c r="W1" s="971" t="s">
+      <c r="W1" s="968" t="s">
         <v>286</v>
       </c>
       <c r="X1" s="465"/>
-      <c r="Y1" s="975" t="s">
+      <c r="Y1" s="972" t="s">
         <v>287</v>
       </c>
-      <c r="Z1" s="975"/>
-      <c r="AA1" s="975"/>
-      <c r="AB1" s="975"/>
-      <c r="AC1" s="975"/>
-      <c r="AD1" s="976"/>
-      <c r="AE1" s="971" t="s">
+      <c r="Z1" s="972"/>
+      <c r="AA1" s="972"/>
+      <c r="AB1" s="972"/>
+      <c r="AC1" s="972"/>
+      <c r="AD1" s="973"/>
+      <c r="AE1" s="968" t="s">
         <v>288</v>
       </c>
-      <c r="AF1" s="970" t="s">
+      <c r="AF1" s="967" t="s">
         <v>447</v>
       </c>
-      <c r="AG1" s="958"/>
-      <c r="AH1" s="958"/>
+      <c r="AG1" s="946"/>
+      <c r="AH1" s="946"/>
       <c r="AI1" s="682"/>
       <c r="AJ1" s="682"/>
       <c r="AK1" s="682"/>
@@ -9640,56 +9637,56 @@
       <c r="C2" s="472" t="s">
         <v>290</v>
       </c>
-      <c r="D2" s="969" t="s">
+      <c r="D2" s="966" t="s">
         <v>452</v>
       </c>
-      <c r="E2" s="969"/>
-      <c r="F2" s="969" t="s">
+      <c r="E2" s="966"/>
+      <c r="F2" s="966" t="s">
         <v>453</v>
       </c>
-      <c r="G2" s="969"/>
+      <c r="G2" s="966"/>
       <c r="H2" s="467"/>
-      <c r="I2" s="967" t="s">
+      <c r="I2" s="964" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="967"/>
-      <c r="K2" s="967" t="s">
+      <c r="J2" s="964"/>
+      <c r="K2" s="964" t="s">
         <v>167</v>
       </c>
-      <c r="L2" s="967"/>
-      <c r="M2" s="967" t="s">
+      <c r="L2" s="964"/>
+      <c r="M2" s="964" t="s">
         <v>168</v>
       </c>
-      <c r="N2" s="968"/>
-      <c r="O2" s="972"/>
+      <c r="N2" s="965"/>
+      <c r="O2" s="969"/>
       <c r="P2" s="468"/>
-      <c r="Q2" s="967" t="s">
+      <c r="Q2" s="964" t="s">
         <v>166</v>
       </c>
-      <c r="R2" s="967"/>
-      <c r="S2" s="967" t="s">
+      <c r="R2" s="964"/>
+      <c r="S2" s="964" t="s">
         <v>167</v>
       </c>
-      <c r="T2" s="967"/>
-      <c r="U2" s="967" t="s">
+      <c r="T2" s="964"/>
+      <c r="U2" s="964" t="s">
         <v>168</v>
       </c>
-      <c r="V2" s="968"/>
-      <c r="W2" s="972"/>
+      <c r="V2" s="965"/>
+      <c r="W2" s="969"/>
       <c r="X2" s="468"/>
-      <c r="Y2" s="967" t="s">
+      <c r="Y2" s="964" t="s">
         <v>166</v>
       </c>
-      <c r="Z2" s="967"/>
-      <c r="AA2" s="967" t="s">
+      <c r="Z2" s="964"/>
+      <c r="AA2" s="964" t="s">
         <v>167</v>
       </c>
-      <c r="AB2" s="967"/>
-      <c r="AC2" s="967" t="s">
+      <c r="AB2" s="964"/>
+      <c r="AC2" s="964" t="s">
         <v>168</v>
       </c>
-      <c r="AD2" s="968"/>
-      <c r="AE2" s="972"/>
+      <c r="AD2" s="965"/>
+      <c r="AE2" s="969"/>
       <c r="AF2" s="676" t="s">
         <v>432</v>
       </c>
@@ -10575,11 +10572,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:AH4"/>
   <mergeCells count="18">
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AE1:AE2"/>
@@ -10593,6 +10585,11 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10816,11 +10813,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="995" t="s">
+      <c r="A1" s="974" t="s">
         <v>629</v>
       </c>
-      <c r="B1" s="863"/>
-      <c r="C1" s="863"/>
+      <c r="B1" s="872"/>
+      <c r="C1" s="872"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="734"/>
@@ -10835,21 +10832,21 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="999" t="s">
+      <c r="A3" s="982" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="1001" t="s">
+      <c r="B3" s="984" t="s">
         <v>421</v>
       </c>
-      <c r="C3" s="1002"/>
-      <c r="D3" s="987" t="s">
+      <c r="C3" s="985"/>
+      <c r="D3" s="980" t="s">
         <v>422</v>
       </c>
-      <c r="E3" s="988"/>
-      <c r="F3" s="987" t="s">
+      <c r="E3" s="981"/>
+      <c r="F3" s="980" t="s">
         <v>455</v>
       </c>
-      <c r="G3" s="988"/>
+      <c r="G3" s="981"/>
       <c r="I3" s="732" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
@@ -10860,14 +10857,14 @@
       <c r="K3" s="714"/>
       <c r="L3" s="714"/>
       <c r="N3" s="699"/>
-      <c r="O3" s="984" t="s">
+      <c r="O3" s="996" t="s">
         <v>317</v>
       </c>
-      <c r="P3" s="984"/>
-      <c r="Q3" s="984" t="s">
+      <c r="P3" s="996"/>
+      <c r="Q3" s="996" t="s">
         <v>318</v>
       </c>
-      <c r="R3" s="984"/>
+      <c r="R3" s="996"/>
       <c r="S3" s="699"/>
       <c r="T3" s="707" t="s">
         <v>319</v>
@@ -10875,7 +10872,7 @@
       <c r="U3" s="699"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1000"/>
+      <c r="A4" s="983"/>
       <c r="B4" s="511" t="s">
         <v>320</v>
       </c>
@@ -11134,14 +11131,14 @@
       <c r="K10" s="714"/>
       <c r="L10" s="714"/>
       <c r="N10" s="707"/>
-      <c r="O10" s="984" t="s">
+      <c r="O10" s="996" t="s">
         <v>320</v>
       </c>
-      <c r="P10" s="984"/>
-      <c r="Q10" s="984" t="s">
+      <c r="P10" s="996"/>
+      <c r="Q10" s="996" t="s">
         <v>327</v>
       </c>
-      <c r="R10" s="984"/>
+      <c r="R10" s="996"/>
     </row>
     <row r="11" spans="1:21" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A11" s="831" t="s">
@@ -11208,7 +11205,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="999" t="s">
+      <c r="A13" s="982" t="s">
         <v>328</v>
       </c>
       <c r="B13" s="510" t="str">
@@ -11254,7 +11251,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="1000"/>
+      <c r="A14" s="983"/>
       <c r="B14" s="513" t="s">
         <v>321</v>
       </c>
@@ -11389,34 +11386,34 @@
       <c r="A21" s="501" t="s">
         <v>333</v>
       </c>
-      <c r="B21" s="989" t="s">
+      <c r="B21" s="997" t="s">
         <v>474</v>
       </c>
-      <c r="C21" s="990"/>
-      <c r="D21" s="990"/>
-      <c r="E21" s="990"/>
-      <c r="F21" s="990"/>
-      <c r="G21" s="990"/>
+      <c r="C21" s="998"/>
+      <c r="D21" s="998"/>
+      <c r="E21" s="998"/>
+      <c r="F21" s="998"/>
+      <c r="G21" s="998"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="515" t="s">
         <v>297</v>
       </c>
-      <c r="B22" s="991" t="str">
+      <c r="B22" s="986" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="992"/>
-      <c r="D22" s="991" t="str">
+      <c r="C22" s="987"/>
+      <c r="D22" s="986" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="992"/>
-      <c r="F22" s="991" t="str">
+      <c r="E22" s="987"/>
+      <c r="F22" s="986" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="992"/>
+      <c r="G22" s="987"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="516"/>
@@ -11843,21 +11840,21 @@
       <c r="A41" s="518" t="s">
         <v>343</v>
       </c>
-      <c r="B41" s="997" t="str">
+      <c r="B41" s="976" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="998"/>
-      <c r="D41" s="985" t="str">
+      <c r="C41" s="977"/>
+      <c r="D41" s="978" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="986"/>
-      <c r="F41" s="985" t="str">
+      <c r="E41" s="979"/>
+      <c r="F41" s="978" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G41" s="986"/>
+      <c r="G41" s="979"/>
       <c r="N41" s="699"/>
       <c r="O41" s="726" t="s">
         <v>426</v>
@@ -12076,11 +12073,11 @@
       <c r="F53" s="704" t="s">
         <v>480</v>
       </c>
-      <c r="H53" s="977" t="s">
+      <c r="H53" s="999" t="s">
         <v>467</v>
       </c>
-      <c r="I53" s="977"/>
-      <c r="J53" s="977"/>
+      <c r="I53" s="999"/>
+      <c r="J53" s="999"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="695" t="s">
@@ -12250,11 +12247,11 @@
       <c r="F63" s="704" t="s">
         <v>480</v>
       </c>
-      <c r="H63" s="977" t="s">
+      <c r="H63" s="999" t="s">
         <v>481</v>
       </c>
-      <c r="I63" s="977"/>
-      <c r="J63" s="977"/>
+      <c r="I63" s="999"/>
+      <c r="J63" s="999"/>
       <c r="L63" s="702"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -12441,12 +12438,12 @@
       <c r="A74" s="831" t="s">
         <v>633</v>
       </c>
-      <c r="B74" s="996" t="s">
+      <c r="B74" s="975" t="s">
         <v>423</v>
       </c>
-      <c r="C74" s="996"/>
-      <c r="D74" s="996"/>
-      <c r="E74" s="996"/>
+      <c r="C74" s="975"/>
+      <c r="D74" s="975"/>
+      <c r="E74" s="975"/>
       <c r="I74" s="703"/>
       <c r="J74" s="703"/>
       <c r="K74" s="703"/>
@@ -12762,36 +12759,36 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="982" t="str">
+      <c r="B85" s="990" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="983"/>
-      <c r="D85" s="982" t="str">
+      <c r="C85" s="991"/>
+      <c r="D85" s="990" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="983"/>
-      <c r="F85" s="982" t="str">
+      <c r="E85" s="991"/>
+      <c r="F85" s="990" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="983"/>
+      <c r="G85" s="991"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="502"/>
-      <c r="B86" s="938" t="s">
+      <c r="B86" s="935" t="s">
         <v>253</v>
       </c>
-      <c r="C86" s="939"/>
-      <c r="D86" s="938" t="s">
+      <c r="C86" s="936"/>
+      <c r="D86" s="935" t="s">
         <v>253</v>
       </c>
-      <c r="E86" s="939"/>
-      <c r="F86" s="938" t="s">
+      <c r="E86" s="936"/>
+      <c r="F86" s="935" t="s">
         <v>253</v>
       </c>
-      <c r="G86" s="939"/>
+      <c r="G86" s="936"/>
       <c r="N86" s="707" t="s">
         <v>369</v>
       </c>
@@ -13078,36 +13075,36 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="982" t="str">
+      <c r="B101" s="990" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="983"/>
-      <c r="D101" s="982" t="str">
+      <c r="C101" s="991"/>
+      <c r="D101" s="990" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="983"/>
-      <c r="F101" s="982" t="str">
+      <c r="E101" s="991"/>
+      <c r="F101" s="990" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="983"/>
+      <c r="G101" s="991"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="502"/>
-      <c r="B102" s="938" t="s">
+      <c r="B102" s="935" t="s">
         <v>253</v>
       </c>
-      <c r="C102" s="939"/>
-      <c r="D102" s="938" t="s">
+      <c r="C102" s="936"/>
+      <c r="D102" s="935" t="s">
         <v>253</v>
       </c>
-      <c r="E102" s="939"/>
-      <c r="F102" s="938" t="s">
+      <c r="E102" s="936"/>
+      <c r="F102" s="935" t="s">
         <v>253</v>
       </c>
-      <c r="G102" s="939"/>
+      <c r="G102" s="936"/>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="503" t="s">
@@ -13393,36 +13390,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="978" t="str">
+      <c r="B116" s="992" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="979"/>
-      <c r="D116" s="978" t="str">
+      <c r="C116" s="993"/>
+      <c r="D116" s="992" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="979"/>
-      <c r="F116" s="978" t="str">
+      <c r="E116" s="993"/>
+      <c r="F116" s="992" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="979"/>
+      <c r="G116" s="993"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="541"/>
-      <c r="B117" s="980" t="s">
+      <c r="B117" s="994" t="s">
         <v>253</v>
       </c>
-      <c r="C117" s="981"/>
-      <c r="D117" s="980" t="s">
+      <c r="C117" s="995"/>
+      <c r="D117" s="994" t="s">
         <v>253</v>
       </c>
-      <c r="E117" s="981"/>
-      <c r="F117" s="980" t="s">
+      <c r="E117" s="995"/>
+      <c r="F117" s="994" t="s">
         <v>253</v>
       </c>
-      <c r="G117" s="981"/>
+      <c r="G117" s="995"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="542" t="s">
@@ -13725,12 +13722,12 @@
       <c r="A129" s="545" t="s">
         <v>328</v>
       </c>
-      <c r="B129" s="993" t="str">
+      <c r="B129" s="988" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="994"/>
-      <c r="D129" s="994"/>
+      <c r="C129" s="989"/>
+      <c r="D129" s="989"/>
       <c r="N129" s="707" t="s">
         <v>369</v>
       </c>
@@ -14506,16 +14503,22 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="39">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -14529,22 +14532,16 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17841,13 +17838,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:AQ10000"/>
+  <dimension ref="A1:AR10000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="AA8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="AG8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AG8" sqref="AG8"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:AR4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17886,7 +17883,7 @@
     <col min="42" max="43" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
@@ -17901,13 +17898,13 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="E2" s="427" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="6"/>
@@ -17951,67 +17948,68 @@
       <c r="AP3" s="6"/>
       <c r="AQ3" s="6"/>
     </row>
-    <row r="4" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="833" t="s">
+    <row r="4" spans="1:44" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1000" t="s">
         <v>477</v>
       </c>
-      <c r="B4" s="834"/>
-      <c r="C4" s="834"/>
-      <c r="D4" s="834"/>
-      <c r="E4" s="834"/>
-      <c r="F4" s="835"/>
-      <c r="G4" s="835"/>
-      <c r="H4" s="835"/>
-      <c r="I4" s="835"/>
-      <c r="J4" s="835"/>
-      <c r="K4" s="835"/>
-      <c r="L4" s="835"/>
-      <c r="M4" s="835"/>
-      <c r="N4" s="835"/>
-      <c r="O4" s="835"/>
-      <c r="P4" s="835"/>
-      <c r="Q4" s="835"/>
-      <c r="R4" s="835"/>
-      <c r="S4" s="835"/>
-      <c r="T4" s="835"/>
-      <c r="U4" s="835"/>
-      <c r="V4" s="835"/>
-      <c r="W4" s="835"/>
-      <c r="X4" s="835"/>
-      <c r="Y4" s="835"/>
-      <c r="Z4" s="835"/>
-      <c r="AA4" s="835"/>
-      <c r="AB4" s="835"/>
-      <c r="AC4" s="835"/>
-      <c r="AD4" s="835"/>
-      <c r="AE4" s="835"/>
-      <c r="AF4" s="835"/>
-      <c r="AG4" s="835"/>
-      <c r="AH4" s="835"/>
-      <c r="AI4" s="835"/>
-      <c r="AJ4" s="835"/>
-      <c r="AK4" s="835"/>
-      <c r="AL4" s="835"/>
-      <c r="AM4" s="835"/>
-      <c r="AN4" s="835"/>
-      <c r="AO4" s="835"/>
-      <c r="AP4" s="835"/>
-      <c r="AQ4" s="835"/>
-    </row>
-    <row r="5" spans="1:43" s="7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="836" t="s">
+      <c r="B4" s="1001"/>
+      <c r="C4" s="1001"/>
+      <c r="D4" s="1001"/>
+      <c r="E4" s="1001"/>
+      <c r="F4" s="1001"/>
+      <c r="G4" s="1001"/>
+      <c r="H4" s="1001"/>
+      <c r="I4" s="1001"/>
+      <c r="J4" s="1001"/>
+      <c r="K4" s="1001"/>
+      <c r="L4" s="1001"/>
+      <c r="M4" s="1001"/>
+      <c r="N4" s="1001"/>
+      <c r="O4" s="1001"/>
+      <c r="P4" s="1001"/>
+      <c r="Q4" s="1001"/>
+      <c r="R4" s="1001"/>
+      <c r="S4" s="1001"/>
+      <c r="T4" s="1001"/>
+      <c r="U4" s="1001"/>
+      <c r="V4" s="1001"/>
+      <c r="W4" s="1001"/>
+      <c r="X4" s="1001"/>
+      <c r="Y4" s="1001"/>
+      <c r="Z4" s="1001"/>
+      <c r="AA4" s="1001"/>
+      <c r="AB4" s="1001"/>
+      <c r="AC4" s="1001"/>
+      <c r="AD4" s="1001"/>
+      <c r="AE4" s="1001"/>
+      <c r="AF4" s="1001"/>
+      <c r="AG4" s="1001"/>
+      <c r="AH4" s="1001"/>
+      <c r="AI4" s="1001"/>
+      <c r="AJ4" s="1001"/>
+      <c r="AK4" s="1001"/>
+      <c r="AL4" s="1001"/>
+      <c r="AM4" s="1001"/>
+      <c r="AN4" s="1001"/>
+      <c r="AO4" s="1001"/>
+      <c r="AP4" s="1001"/>
+      <c r="AQ4" s="1001"/>
+      <c r="AR4" s="1001"/>
+    </row>
+    <row r="5" spans="1:44" s="7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="833" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="836" t="s">
+      <c r="B5" s="833" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="786" t="s">
         <v>546</v>
       </c>
-      <c r="D5" s="836" t="s">
+      <c r="D5" s="833" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="836" t="s">
+      <c r="E5" s="833" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="12" t="s">
@@ -18071,10 +18069,10 @@
       <c r="X5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="838" t="s">
+      <c r="Y5" s="835" t="s">
         <v>570</v>
       </c>
-      <c r="Z5" s="838" t="s">
+      <c r="Z5" s="835" t="s">
         <v>38</v>
       </c>
       <c r="AA5" s="16" t="s">
@@ -18104,7 +18102,7 @@
       <c r="AI5" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="AJ5" s="838" t="s">
+      <c r="AJ5" s="835" t="s">
         <v>47</v>
       </c>
       <c r="AK5" s="16" t="s">
@@ -18113,28 +18111,31 @@
       <c r="AL5" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="AM5" s="836" t="s">
+      <c r="AM5" s="833" t="s">
         <v>50</v>
       </c>
-      <c r="AN5" s="836" t="s">
+      <c r="AN5" s="833" t="s">
         <v>51</v>
       </c>
-      <c r="AO5" s="836" t="s">
+      <c r="AO5" s="833" t="s">
         <v>52</v>
       </c>
-      <c r="AP5" s="836" t="s">
+      <c r="AP5" s="833" t="s">
         <v>53</v>
       </c>
-      <c r="AQ5" s="836" t="s">
+      <c r="AQ5" s="833" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:43" s="9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="837"/>
-      <c r="B6" s="837"/>
+      <c r="AR5" s="833" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" s="9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="834"/>
+      <c r="B6" s="834"/>
       <c r="C6" s="787"/>
-      <c r="D6" s="837"/>
-      <c r="E6" s="837"/>
+      <c r="D6" s="834"/>
+      <c r="E6" s="834"/>
       <c r="F6" s="14" t="s">
         <v>55</v>
       </c>
@@ -18192,8 +18193,8 @@
       <c r="X6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="Y6" s="839"/>
-      <c r="Z6" s="839"/>
+      <c r="Y6" s="836"/>
+      <c r="Z6" s="836"/>
       <c r="AA6" s="9" t="s">
         <v>56</v>
       </c>
@@ -18221,33 +18222,34 @@
       <c r="AI6" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="AJ6" s="839"/>
+      <c r="AJ6" s="836"/>
       <c r="AK6" s="9" t="s">
         <v>56</v>
       </c>
       <c r="AL6" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="AM6" s="837"/>
-      <c r="AN6" s="837"/>
-      <c r="AO6" s="837"/>
-      <c r="AP6" s="837"/>
-      <c r="AQ6" s="837"/>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="AM6" s="834"/>
+      <c r="AN6" s="834"/>
+      <c r="AO6" s="834"/>
+      <c r="AP6" s="834"/>
+      <c r="AQ6" s="834"/>
+      <c r="AR6" s="834"/>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="AD7" s="822"/>
       <c r="AE7" s="8"/>
       <c r="AG7" s="822"/>
       <c r="AH7" s="8"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="C8" s="749"/>
       <c r="AD8" s="822"/>
       <c r="AE8" s="623"/>
       <c r="AG8" s="822"/>
       <c r="AH8" s="623"/>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" s="656"/>
       <c r="B9" s="2"/>
       <c r="C9" s="813"/>
@@ -18292,7 +18294,7 @@
       <c r="AP9" s="656"/>
       <c r="AQ9" s="656"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" s="427" t="s">
         <v>63</v>
       </c>
@@ -18300,7 +18302,7 @@
       <c r="AE10" s="8"/>
       <c r="AH10" s="8"/>
     </row>
-    <row r="11" spans="1:43" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="427" t="s">
         <v>64</v>
       </c>
@@ -18308,23 +18310,23 @@
       <c r="AE11" s="8"/>
       <c r="AH11" s="8"/>
     </row>
-    <row r="12" spans="1:43" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AE12" s="8"/>
       <c r="AH12" s="8"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="AE13" s="8"/>
       <c r="AH13" s="8"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="AE14" s="8"/>
       <c r="AH14" s="8"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="AE15" s="8"/>
       <c r="AH15" s="8"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="AE16" s="8"/>
       <c r="AH16" s="8"/>
     </row>
@@ -58271,8 +58273,9 @@
       <sortCondition descending="1" ref="B7"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="13">
-    <mergeCell ref="A4:AQ4"/>
+  <mergeCells count="14">
+    <mergeCell ref="AR5:AR6"/>
+    <mergeCell ref="A4:AR4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="D5:D6"/>
@@ -58503,10 +58506,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="58.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="840" t="s">
+      <c r="A1" s="837" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="842" t="s">
+      <c r="B1" s="839" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="814" t="s">
@@ -58556,8 +58559,8 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="841"/>
-      <c r="B2" s="843"/>
+      <c r="A2" s="838"/>
+      <c r="B2" s="840"/>
       <c r="C2" s="9" t="s">
         <v>56</v>
       </c>
@@ -58724,123 +58727,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="652" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="873" t="s">
+      <c r="A1" s="841" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="874"/>
-      <c r="C1" s="874"/>
-      <c r="D1" s="874"/>
-      <c r="E1" s="874"/>
-      <c r="F1" s="874"/>
-      <c r="G1" s="874"/>
-      <c r="H1" s="875" t="s">
+      <c r="B1" s="842"/>
+      <c r="C1" s="842"/>
+      <c r="D1" s="842"/>
+      <c r="E1" s="842"/>
+      <c r="F1" s="842"/>
+      <c r="G1" s="842"/>
+      <c r="H1" s="843" t="s">
         <v>432</v>
       </c>
-      <c r="I1" s="876"/>
-      <c r="J1" s="876"/>
-      <c r="K1" s="876"/>
-      <c r="L1" s="876"/>
-      <c r="M1" s="877"/>
-      <c r="N1" s="878" t="s">
+      <c r="I1" s="844"/>
+      <c r="J1" s="844"/>
+      <c r="K1" s="844"/>
+      <c r="L1" s="844"/>
+      <c r="M1" s="845"/>
+      <c r="N1" s="846" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="856"/>
-      <c r="P1" s="856"/>
-      <c r="Q1" s="856"/>
-      <c r="R1" s="856"/>
-      <c r="S1" s="856"/>
-      <c r="T1" s="856"/>
-      <c r="U1" s="856"/>
-      <c r="V1" s="879" t="s">
+      <c r="O1" s="847"/>
+      <c r="P1" s="847"/>
+      <c r="Q1" s="847"/>
+      <c r="R1" s="847"/>
+      <c r="S1" s="847"/>
+      <c r="T1" s="847"/>
+      <c r="U1" s="847"/>
+      <c r="V1" s="848" t="s">
         <v>72</v>
       </c>
-      <c r="W1" s="880"/>
-      <c r="X1" s="881"/>
-      <c r="Y1" s="881"/>
-      <c r="Z1" s="882"/>
-      <c r="AA1" s="883" t="s">
+      <c r="W1" s="849"/>
+      <c r="X1" s="850"/>
+      <c r="Y1" s="850"/>
+      <c r="Z1" s="851"/>
+      <c r="AA1" s="852" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="884"/>
-      <c r="AC1" s="884"/>
-      <c r="AD1" s="884"/>
-      <c r="AE1" s="884"/>
-      <c r="AF1" s="884"/>
-      <c r="AG1" s="884"/>
-      <c r="AH1" s="884"/>
-      <c r="AI1" s="884"/>
-      <c r="AJ1" s="884"/>
-      <c r="AK1" s="884"/>
-      <c r="AL1" s="884"/>
-      <c r="AM1" s="884"/>
+      <c r="AB1" s="853"/>
+      <c r="AC1" s="853"/>
+      <c r="AD1" s="853"/>
+      <c r="AE1" s="853"/>
+      <c r="AF1" s="853"/>
+      <c r="AG1" s="853"/>
+      <c r="AH1" s="853"/>
+      <c r="AI1" s="853"/>
+      <c r="AJ1" s="853"/>
+      <c r="AK1" s="853"/>
+      <c r="AL1" s="853"/>
+      <c r="AM1" s="853"/>
       <c r="AN1" s="52"/>
       <c r="AO1" s="53"/>
-      <c r="AP1" s="855" t="s">
+      <c r="AP1" s="865" t="s">
         <v>74</v>
       </c>
-      <c r="AQ1" s="856"/>
-      <c r="AR1" s="856"/>
-      <c r="AS1" s="856"/>
-      <c r="AT1" s="856"/>
-      <c r="AU1" s="856"/>
-      <c r="AV1" s="856"/>
-      <c r="AW1" s="857"/>
-      <c r="AX1" s="864" t="s">
+      <c r="AQ1" s="847"/>
+      <c r="AR1" s="847"/>
+      <c r="AS1" s="847"/>
+      <c r="AT1" s="847"/>
+      <c r="AU1" s="847"/>
+      <c r="AV1" s="847"/>
+      <c r="AW1" s="866"/>
+      <c r="AX1" s="873" t="s">
         <v>547</v>
       </c>
-      <c r="AY1" s="865"/>
-      <c r="AZ1" s="865"/>
-      <c r="BA1" s="865"/>
-      <c r="BB1" s="865"/>
-      <c r="BC1" s="866"/>
-      <c r="BD1" s="867" t="s">
+      <c r="AY1" s="874"/>
+      <c r="AZ1" s="874"/>
+      <c r="BA1" s="874"/>
+      <c r="BB1" s="874"/>
+      <c r="BC1" s="875"/>
+      <c r="BD1" s="876" t="s">
         <v>75</v>
       </c>
-      <c r="BE1" s="868"/>
-      <c r="BF1" s="868"/>
-      <c r="BG1" s="868"/>
-      <c r="BH1" s="868"/>
-      <c r="BI1" s="869"/>
-      <c r="BJ1" s="870" t="s">
+      <c r="BE1" s="877"/>
+      <c r="BF1" s="877"/>
+      <c r="BG1" s="877"/>
+      <c r="BH1" s="877"/>
+      <c r="BI1" s="878"/>
+      <c r="BJ1" s="879" t="s">
         <v>76</v>
       </c>
-      <c r="BK1" s="871"/>
-      <c r="BL1" s="871"/>
-      <c r="BM1" s="871"/>
-      <c r="BN1" s="871"/>
-      <c r="BO1" s="871"/>
-      <c r="BP1" s="872"/>
-      <c r="BQ1" s="844" t="s">
+      <c r="BK1" s="880"/>
+      <c r="BL1" s="880"/>
+      <c r="BM1" s="880"/>
+      <c r="BN1" s="880"/>
+      <c r="BO1" s="880"/>
+      <c r="BP1" s="881"/>
+      <c r="BQ1" s="854" t="s">
         <v>77</v>
       </c>
-      <c r="BR1" s="845"/>
-      <c r="BS1" s="845"/>
-      <c r="BT1" s="845"/>
-      <c r="BU1" s="845"/>
-      <c r="BV1" s="845"/>
+      <c r="BR1" s="855"/>
+      <c r="BS1" s="855"/>
+      <c r="BT1" s="855"/>
+      <c r="BU1" s="855"/>
+      <c r="BV1" s="855"/>
       <c r="BW1" s="53"/>
       <c r="BX1" s="54"/>
-      <c r="BY1" s="846" t="s">
+      <c r="BY1" s="856" t="s">
         <v>78</v>
       </c>
-      <c r="BZ1" s="847"/>
-      <c r="CA1" s="847"/>
-      <c r="CB1" s="847"/>
-      <c r="CC1" s="847"/>
-      <c r="CD1" s="847"/>
-      <c r="CE1" s="847"/>
-      <c r="CF1" s="848"/>
-      <c r="CG1" s="848"/>
-      <c r="CH1" s="848"/>
-      <c r="CI1" s="848"/>
-      <c r="CJ1" s="848"/>
-      <c r="CK1" s="848"/>
-      <c r="CL1" s="848"/>
-      <c r="CM1" s="848"/>
-      <c r="CN1" s="848"/>
-      <c r="CO1" s="848"/>
-      <c r="CP1" s="848"/>
-      <c r="CQ1" s="848"/>
+      <c r="BZ1" s="857"/>
+      <c r="CA1" s="857"/>
+      <c r="CB1" s="857"/>
+      <c r="CC1" s="857"/>
+      <c r="CD1" s="857"/>
+      <c r="CE1" s="857"/>
+      <c r="CF1" s="858"/>
+      <c r="CG1" s="858"/>
+      <c r="CH1" s="858"/>
+      <c r="CI1" s="858"/>
+      <c r="CJ1" s="858"/>
+      <c r="CK1" s="858"/>
+      <c r="CL1" s="858"/>
+      <c r="CM1" s="858"/>
+      <c r="CN1" s="858"/>
+      <c r="CO1" s="858"/>
+      <c r="CP1" s="858"/>
+      <c r="CQ1" s="858"/>
     </row>
     <row r="2" spans="1:95" s="652" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -58864,18 +58867,18 @@
       <c r="G2" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="849" t="s">
+      <c r="H2" s="859" t="s">
         <v>433</v>
       </c>
-      <c r="I2" s="850"/>
-      <c r="J2" s="850" t="s">
+      <c r="I2" s="860"/>
+      <c r="J2" s="860" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="850"/>
-      <c r="L2" s="850" t="s">
+      <c r="K2" s="860"/>
+      <c r="L2" s="860" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="851"/>
+      <c r="M2" s="861"/>
       <c r="N2" s="57" t="s">
         <v>79</v>
       </c>
@@ -58984,36 +58987,36 @@
       <c r="AW2" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="AX2" s="852" t="s">
+      <c r="AX2" s="862" t="s">
         <v>112</v>
       </c>
-      <c r="AY2" s="853"/>
-      <c r="AZ2" s="853"/>
-      <c r="BA2" s="853" t="s">
+      <c r="AY2" s="863"/>
+      <c r="AZ2" s="863"/>
+      <c r="BA2" s="863" t="s">
         <v>113</v>
       </c>
-      <c r="BB2" s="853"/>
-      <c r="BC2" s="854"/>
-      <c r="BD2" s="858" t="s">
+      <c r="BB2" s="863"/>
+      <c r="BC2" s="864"/>
+      <c r="BD2" s="867" t="s">
         <v>112</v>
       </c>
-      <c r="BE2" s="859"/>
-      <c r="BF2" s="859"/>
-      <c r="BG2" s="859" t="s">
+      <c r="BE2" s="868"/>
+      <c r="BF2" s="868"/>
+      <c r="BG2" s="868" t="s">
         <v>113</v>
       </c>
-      <c r="BH2" s="859"/>
-      <c r="BI2" s="860"/>
-      <c r="BJ2" s="861" t="s">
+      <c r="BH2" s="868"/>
+      <c r="BI2" s="869"/>
+      <c r="BJ2" s="870" t="s">
         <v>112</v>
       </c>
-      <c r="BK2" s="862"/>
-      <c r="BL2" s="862"/>
-      <c r="BM2" s="862" t="s">
+      <c r="BK2" s="871"/>
+      <c r="BL2" s="871"/>
+      <c r="BM2" s="871" t="s">
         <v>113</v>
       </c>
-      <c r="BN2" s="863"/>
-      <c r="BO2" s="863"/>
+      <c r="BN2" s="872"/>
+      <c r="BO2" s="872"/>
       <c r="BP2" s="69" t="s">
         <v>114</v>
       </c>
@@ -59663,11 +59666,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -59683,6 +59681,11 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -59766,131 +59769,131 @@
       <c r="H1" s="142"/>
       <c r="I1" s="142"/>
       <c r="J1" s="142"/>
-      <c r="K1" s="885" t="s">
+      <c r="K1" s="911" t="s">
         <v>613</v>
       </c>
-      <c r="L1" s="886"/>
-      <c r="M1" s="910" t="s">
+      <c r="L1" s="912"/>
+      <c r="M1" s="882" t="s">
         <v>150</v>
       </c>
-      <c r="N1" s="911" t="s">
+      <c r="N1" s="883" t="s">
         <v>487</v>
       </c>
-      <c r="O1" s="912"/>
-      <c r="P1" s="912"/>
-      <c r="Q1" s="912"/>
-      <c r="R1" s="913" t="s">
+      <c r="O1" s="884"/>
+      <c r="P1" s="884"/>
+      <c r="Q1" s="884"/>
+      <c r="R1" s="885" t="s">
         <v>432</v>
       </c>
-      <c r="S1" s="906"/>
-      <c r="T1" s="906"/>
-      <c r="U1" s="906"/>
-      <c r="V1" s="906"/>
-      <c r="W1" s="906"/>
-      <c r="X1" s="914"/>
-      <c r="Y1" s="900" t="s">
+      <c r="S1" s="886"/>
+      <c r="T1" s="886"/>
+      <c r="U1" s="886"/>
+      <c r="V1" s="886"/>
+      <c r="W1" s="886"/>
+      <c r="X1" s="887"/>
+      <c r="Y1" s="888" t="s">
         <v>440</v>
       </c>
-      <c r="Z1" s="868"/>
-      <c r="AA1" s="916" t="s">
+      <c r="Z1" s="877"/>
+      <c r="AA1" s="891" t="s">
         <v>151</v>
       </c>
-      <c r="AB1" s="888" t="s">
+      <c r="AB1" s="903" t="s">
         <v>152</v>
       </c>
-      <c r="AC1" s="902" t="s">
+      <c r="AC1" s="899" t="s">
         <v>153</v>
       </c>
-      <c r="AD1" s="903"/>
-      <c r="AE1" s="903"/>
-      <c r="AF1" s="904"/>
-      <c r="AG1" s="905" t="s">
+      <c r="AD1" s="900"/>
+      <c r="AE1" s="900"/>
+      <c r="AF1" s="901"/>
+      <c r="AG1" s="902" t="s">
         <v>609</v>
       </c>
-      <c r="AH1" s="906"/>
-      <c r="AI1" s="906"/>
-      <c r="AJ1" s="906"/>
-      <c r="AK1" s="906"/>
-      <c r="AL1" s="906"/>
-      <c r="AM1" s="906"/>
-      <c r="AN1" s="906"/>
-      <c r="AO1" s="888" t="s">
+      <c r="AH1" s="886"/>
+      <c r="AI1" s="886"/>
+      <c r="AJ1" s="886"/>
+      <c r="AK1" s="886"/>
+      <c r="AL1" s="886"/>
+      <c r="AM1" s="886"/>
+      <c r="AN1" s="886"/>
+      <c r="AO1" s="903" t="s">
         <v>154</v>
       </c>
-      <c r="AP1" s="900" t="s">
+      <c r="AP1" s="888" t="s">
         <v>439</v>
       </c>
-      <c r="AQ1" s="868"/>
-      <c r="AR1" s="868"/>
-      <c r="AS1" s="869"/>
-      <c r="AT1" s="908" t="s">
+      <c r="AQ1" s="877"/>
+      <c r="AR1" s="877"/>
+      <c r="AS1" s="878"/>
+      <c r="AT1" s="906" t="s">
         <v>610</v>
       </c>
-      <c r="AU1" s="909"/>
-      <c r="AV1" s="909"/>
-      <c r="AW1" s="909"/>
-      <c r="AX1" s="909"/>
-      <c r="AY1" s="909"/>
-      <c r="AZ1" s="909"/>
-      <c r="BA1" s="909"/>
-      <c r="BB1" s="909"/>
-      <c r="BC1" s="909"/>
-      <c r="BD1" s="909"/>
-      <c r="BE1" s="909"/>
-      <c r="BF1" s="909"/>
-      <c r="BG1" s="909"/>
-      <c r="BH1" s="909"/>
-      <c r="BI1" s="909"/>
-      <c r="BJ1" s="909"/>
-      <c r="BK1" s="909"/>
-      <c r="BL1" s="909"/>
-      <c r="BM1" s="909"/>
-      <c r="BN1" s="909"/>
-      <c r="BO1" s="909"/>
-      <c r="BP1" s="909"/>
-      <c r="BQ1" s="909"/>
-      <c r="BR1" s="909"/>
-      <c r="BS1" s="909"/>
-      <c r="BT1" s="909"/>
-      <c r="BU1" s="909"/>
-      <c r="BV1" s="909"/>
-      <c r="BW1" s="888" t="s">
+      <c r="AU1" s="907"/>
+      <c r="AV1" s="907"/>
+      <c r="AW1" s="907"/>
+      <c r="AX1" s="907"/>
+      <c r="AY1" s="907"/>
+      <c r="AZ1" s="907"/>
+      <c r="BA1" s="907"/>
+      <c r="BB1" s="907"/>
+      <c r="BC1" s="907"/>
+      <c r="BD1" s="907"/>
+      <c r="BE1" s="907"/>
+      <c r="BF1" s="907"/>
+      <c r="BG1" s="907"/>
+      <c r="BH1" s="907"/>
+      <c r="BI1" s="907"/>
+      <c r="BJ1" s="907"/>
+      <c r="BK1" s="907"/>
+      <c r="BL1" s="907"/>
+      <c r="BM1" s="907"/>
+      <c r="BN1" s="907"/>
+      <c r="BO1" s="907"/>
+      <c r="BP1" s="907"/>
+      <c r="BQ1" s="907"/>
+      <c r="BR1" s="907"/>
+      <c r="BS1" s="907"/>
+      <c r="BT1" s="907"/>
+      <c r="BU1" s="907"/>
+      <c r="BV1" s="907"/>
+      <c r="BW1" s="903" t="s">
         <v>155</v>
       </c>
-      <c r="BX1" s="900" t="s">
+      <c r="BX1" s="888" t="s">
         <v>438</v>
       </c>
-      <c r="BY1" s="868"/>
-      <c r="BZ1" s="868"/>
-      <c r="CA1" s="869"/>
-      <c r="CB1" s="899" t="s">
+      <c r="BY1" s="877"/>
+      <c r="BZ1" s="877"/>
+      <c r="CA1" s="878"/>
+      <c r="CB1" s="917" t="s">
         <v>454</v>
       </c>
-      <c r="CC1" s="901" t="s">
+      <c r="CC1" s="896" t="s">
         <v>73</v>
       </c>
-      <c r="CD1" s="901"/>
-      <c r="CE1" s="901"/>
-      <c r="CF1" s="901"/>
-      <c r="CG1" s="901"/>
-      <c r="CH1" s="901"/>
-      <c r="CI1" s="901"/>
-      <c r="CJ1" s="901"/>
-      <c r="CK1" s="901"/>
-      <c r="CL1" s="901"/>
-      <c r="CM1" s="901"/>
-      <c r="CN1" s="901"/>
+      <c r="CD1" s="896"/>
+      <c r="CE1" s="896"/>
+      <c r="CF1" s="896"/>
+      <c r="CG1" s="896"/>
+      <c r="CH1" s="896"/>
+      <c r="CI1" s="896"/>
+      <c r="CJ1" s="896"/>
+      <c r="CK1" s="896"/>
+      <c r="CL1" s="896"/>
+      <c r="CM1" s="896"/>
+      <c r="CN1" s="896"/>
       <c r="CO1" s="145"/>
-      <c r="CP1" s="887" t="s">
+      <c r="CP1" s="913" t="s">
         <v>77</v>
       </c>
-      <c r="CQ1" s="856"/>
-      <c r="CR1" s="856"/>
-      <c r="CS1" s="856"/>
-      <c r="CT1" s="856"/>
-      <c r="CU1" s="856"/>
-      <c r="CV1" s="856"/>
-      <c r="CW1" s="857"/>
+      <c r="CQ1" s="847"/>
+      <c r="CR1" s="847"/>
+      <c r="CS1" s="847"/>
+      <c r="CT1" s="847"/>
+      <c r="CU1" s="847"/>
+      <c r="CV1" s="847"/>
+      <c r="CW1" s="866"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="146" t="s">
@@ -59929,7 +59932,7 @@
       <c r="L2" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="910"/>
+      <c r="M2" s="882"/>
       <c r="N2" s="151" t="s">
         <v>160</v>
       </c>
@@ -59945,22 +59948,22 @@
       <c r="R2" s="156" t="s">
         <v>163</v>
       </c>
-      <c r="S2" s="918" t="s">
+      <c r="S2" s="893" t="s">
         <v>433</v>
       </c>
-      <c r="T2" s="863"/>
-      <c r="U2" s="919" t="s">
+      <c r="T2" s="872"/>
+      <c r="U2" s="894" t="s">
         <v>86</v>
       </c>
-      <c r="V2" s="919"/>
-      <c r="W2" s="919" t="s">
+      <c r="V2" s="894"/>
+      <c r="W2" s="894" t="s">
         <v>87</v>
       </c>
-      <c r="X2" s="920"/>
-      <c r="Y2" s="915"/>
-      <c r="Z2" s="895"/>
-      <c r="AA2" s="917"/>
-      <c r="AB2" s="889"/>
+      <c r="X2" s="895"/>
+      <c r="Y2" s="889"/>
+      <c r="Z2" s="890"/>
+      <c r="AA2" s="892"/>
+      <c r="AB2" s="904"/>
       <c r="AC2" s="152" t="s">
         <v>164</v>
       </c>
@@ -59973,81 +59976,81 @@
       <c r="AF2" s="152" t="s">
         <v>607</v>
       </c>
-      <c r="AG2" s="907" t="s">
+      <c r="AG2" s="905" t="s">
         <v>593</v>
       </c>
-      <c r="AH2" s="892"/>
-      <c r="AI2" s="892" t="s">
+      <c r="AH2" s="897"/>
+      <c r="AI2" s="897" t="s">
         <v>167</v>
       </c>
-      <c r="AJ2" s="892"/>
-      <c r="AK2" s="892" t="s">
+      <c r="AJ2" s="897"/>
+      <c r="AK2" s="897" t="s">
         <v>168</v>
       </c>
-      <c r="AL2" s="892"/>
+      <c r="AL2" s="897"/>
       <c r="AM2" s="153" t="s">
         <v>169</v>
       </c>
       <c r="AN2" s="153" t="s">
         <v>170</v>
       </c>
-      <c r="AO2" s="889"/>
-      <c r="AP2" s="894" t="s">
+      <c r="AO2" s="904"/>
+      <c r="AP2" s="898" t="s">
         <v>571</v>
       </c>
-      <c r="AQ2" s="895"/>
-      <c r="AR2" s="896" t="s">
+      <c r="AQ2" s="890"/>
+      <c r="AR2" s="908" t="s">
         <v>572</v>
       </c>
-      <c r="AS2" s="897"/>
-      <c r="AT2" s="892" t="s">
+      <c r="AS2" s="909"/>
+      <c r="AT2" s="897" t="s">
         <v>171</v>
       </c>
-      <c r="AU2" s="892"/>
-      <c r="AV2" s="893" t="s">
+      <c r="AU2" s="897"/>
+      <c r="AV2" s="910" t="s">
         <v>172</v>
       </c>
-      <c r="AW2" s="893"/>
-      <c r="AX2" s="893" t="s">
+      <c r="AW2" s="910"/>
+      <c r="AX2" s="910" t="s">
         <v>173</v>
       </c>
-      <c r="AY2" s="893"/>
+      <c r="AY2" s="910"/>
       <c r="AZ2" s="153" t="s">
         <v>174</v>
       </c>
       <c r="BA2" s="153" t="s">
         <v>175</v>
       </c>
-      <c r="BB2" s="892" t="s">
+      <c r="BB2" s="897" t="s">
         <v>176</v>
       </c>
-      <c r="BC2" s="892"/>
-      <c r="BD2" s="893" t="s">
+      <c r="BC2" s="897"/>
+      <c r="BD2" s="910" t="s">
         <v>177</v>
       </c>
-      <c r="BE2" s="893"/>
-      <c r="BF2" s="893" t="s">
+      <c r="BE2" s="910"/>
+      <c r="BF2" s="910" t="s">
         <v>178</v>
       </c>
-      <c r="BG2" s="893"/>
+      <c r="BG2" s="910"/>
       <c r="BH2" s="153" t="s">
         <v>179</v>
       </c>
       <c r="BI2" s="153" t="s">
         <v>180</v>
       </c>
-      <c r="BJ2" s="892" t="s">
+      <c r="BJ2" s="897" t="s">
         <v>181</v>
       </c>
-      <c r="BK2" s="892"/>
-      <c r="BL2" s="893" t="s">
+      <c r="BK2" s="897"/>
+      <c r="BL2" s="910" t="s">
         <v>182</v>
       </c>
-      <c r="BM2" s="893"/>
-      <c r="BN2" s="893" t="s">
+      <c r="BM2" s="910"/>
+      <c r="BN2" s="910" t="s">
         <v>183</v>
       </c>
-      <c r="BO2" s="893"/>
+      <c r="BO2" s="910"/>
       <c r="BP2" s="153" t="s">
         <v>184</v>
       </c>
@@ -60069,16 +60072,16 @@
       <c r="BV2" s="153" t="s">
         <v>190</v>
       </c>
-      <c r="BW2" s="889"/>
-      <c r="BX2" s="894" t="s">
+      <c r="BW2" s="904"/>
+      <c r="BX2" s="898" t="s">
         <v>571</v>
       </c>
-      <c r="BY2" s="895"/>
-      <c r="BZ2" s="896" t="s">
+      <c r="BY2" s="890"/>
+      <c r="BZ2" s="908" t="s">
         <v>572</v>
       </c>
-      <c r="CA2" s="897"/>
-      <c r="CB2" s="899"/>
+      <c r="CA2" s="909"/>
+      <c r="CB2" s="917"/>
       <c r="CC2" s="137" t="s">
         <v>94</v>
       </c>
@@ -60118,22 +60121,22 @@
       <c r="CO2" s="139" t="s">
         <v>590</v>
       </c>
-      <c r="CP2" s="898" t="s">
+      <c r="CP2" s="916" t="s">
         <v>192</v>
       </c>
-      <c r="CQ2" s="890"/>
-      <c r="CR2" s="890" t="s">
+      <c r="CQ2" s="914"/>
+      <c r="CR2" s="914" t="s">
         <v>193</v>
       </c>
-      <c r="CS2" s="890"/>
-      <c r="CT2" s="890" t="s">
+      <c r="CS2" s="914"/>
+      <c r="CT2" s="914" t="s">
         <v>194</v>
       </c>
-      <c r="CU2" s="890"/>
-      <c r="CV2" s="890" t="s">
+      <c r="CU2" s="914"/>
+      <c r="CV2" s="914" t="s">
         <v>195</v>
       </c>
-      <c r="CW2" s="891"/>
+      <c r="CW2" s="915"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="167"/>
@@ -61010,14 +61013,22 @@
     </sortState>
   </autoFilter>
   <mergeCells count="40">
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="CP1:CW1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CB1:CB2"/>
     <mergeCell ref="BX1:CA1"/>
     <mergeCell ref="CC1:CN1"/>
     <mergeCell ref="AK2:AL2"/>
@@ -61034,22 +61045,14 @@
     <mergeCell ref="AT2:AU2"/>
     <mergeCell ref="AV2:AW2"/>
     <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="CP1:CW1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CB1:CB2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -61097,101 +61100,106 @@
       <c r="O1" s="922"/>
       <c r="P1" s="922"/>
       <c r="Q1" s="922"/>
-      <c r="R1" s="913"/>
-      <c r="S1" s="906"/>
-      <c r="T1" s="906"/>
-      <c r="U1" s="906"/>
-      <c r="V1" s="906"/>
-      <c r="W1" s="906"/>
-      <c r="X1" s="914"/>
-      <c r="Y1" s="900"/>
-      <c r="Z1" s="868"/>
+      <c r="R1" s="885"/>
+      <c r="S1" s="886"/>
+      <c r="T1" s="886"/>
+      <c r="U1" s="886"/>
+      <c r="V1" s="886"/>
+      <c r="W1" s="886"/>
+      <c r="X1" s="887"/>
+      <c r="Y1" s="888"/>
+      <c r="Z1" s="877"/>
       <c r="AA1" s="690"/>
       <c r="AB1" s="688"/>
-      <c r="AC1" s="902"/>
-      <c r="AD1" s="903"/>
-      <c r="AE1" s="903"/>
-      <c r="AF1" s="904"/>
-      <c r="AG1" s="905"/>
-      <c r="AH1" s="906"/>
-      <c r="AI1" s="906"/>
-      <c r="AJ1" s="906"/>
-      <c r="AK1" s="906"/>
-      <c r="AL1" s="906"/>
-      <c r="AM1" s="906"/>
-      <c r="AN1" s="906"/>
+      <c r="AC1" s="899"/>
+      <c r="AD1" s="900"/>
+      <c r="AE1" s="900"/>
+      <c r="AF1" s="901"/>
+      <c r="AG1" s="902"/>
+      <c r="AH1" s="886"/>
+      <c r="AI1" s="886"/>
+      <c r="AJ1" s="886"/>
+      <c r="AK1" s="886"/>
+      <c r="AL1" s="886"/>
+      <c r="AM1" s="886"/>
+      <c r="AN1" s="886"/>
       <c r="AO1" s="688"/>
-      <c r="AP1" s="900"/>
-      <c r="AQ1" s="868"/>
-      <c r="AR1" s="868"/>
-      <c r="AS1" s="869"/>
-      <c r="AT1" s="908"/>
-      <c r="AU1" s="909"/>
-      <c r="AV1" s="909"/>
-      <c r="AW1" s="909"/>
-      <c r="AX1" s="909"/>
-      <c r="AY1" s="909"/>
-      <c r="AZ1" s="909"/>
-      <c r="BA1" s="909"/>
-      <c r="BB1" s="909"/>
-      <c r="BC1" s="909"/>
-      <c r="BD1" s="909"/>
-      <c r="BE1" s="909"/>
-      <c r="BF1" s="909"/>
-      <c r="BG1" s="909"/>
-      <c r="BH1" s="909"/>
-      <c r="BI1" s="909"/>
-      <c r="BJ1" s="909"/>
-      <c r="BK1" s="909"/>
-      <c r="BL1" s="909"/>
-      <c r="BM1" s="909"/>
-      <c r="BN1" s="909"/>
-      <c r="BO1" s="909"/>
-      <c r="BP1" s="909"/>
-      <c r="BQ1" s="909"/>
-      <c r="BR1" s="909"/>
-      <c r="BS1" s="909"/>
-      <c r="BT1" s="909"/>
-      <c r="BU1" s="909"/>
-      <c r="BV1" s="909"/>
+      <c r="AP1" s="888"/>
+      <c r="AQ1" s="877"/>
+      <c r="AR1" s="877"/>
+      <c r="AS1" s="878"/>
+      <c r="AT1" s="906"/>
+      <c r="AU1" s="907"/>
+      <c r="AV1" s="907"/>
+      <c r="AW1" s="907"/>
+      <c r="AX1" s="907"/>
+      <c r="AY1" s="907"/>
+      <c r="AZ1" s="907"/>
+      <c r="BA1" s="907"/>
+      <c r="BB1" s="907"/>
+      <c r="BC1" s="907"/>
+      <c r="BD1" s="907"/>
+      <c r="BE1" s="907"/>
+      <c r="BF1" s="907"/>
+      <c r="BG1" s="907"/>
+      <c r="BH1" s="907"/>
+      <c r="BI1" s="907"/>
+      <c r="BJ1" s="907"/>
+      <c r="BK1" s="907"/>
+      <c r="BL1" s="907"/>
+      <c r="BM1" s="907"/>
+      <c r="BN1" s="907"/>
+      <c r="BO1" s="907"/>
+      <c r="BP1" s="907"/>
+      <c r="BQ1" s="907"/>
+      <c r="BR1" s="907"/>
+      <c r="BS1" s="907"/>
+      <c r="BT1" s="907"/>
+      <c r="BU1" s="907"/>
+      <c r="BV1" s="907"/>
       <c r="BW1" s="688"/>
-      <c r="BX1" s="900"/>
-      <c r="BY1" s="868"/>
-      <c r="BZ1" s="868"/>
-      <c r="CA1" s="869"/>
-      <c r="CB1" s="901"/>
-      <c r="CC1" s="901"/>
-      <c r="CD1" s="901"/>
-      <c r="CE1" s="901"/>
-      <c r="CF1" s="901"/>
-      <c r="CG1" s="901"/>
-      <c r="CH1" s="901"/>
-      <c r="CI1" s="901"/>
-      <c r="CJ1" s="901"/>
-      <c r="CK1" s="901"/>
-      <c r="CL1" s="901"/>
-      <c r="CM1" s="901"/>
+      <c r="BX1" s="888"/>
+      <c r="BY1" s="877"/>
+      <c r="BZ1" s="877"/>
+      <c r="CA1" s="878"/>
+      <c r="CB1" s="896"/>
+      <c r="CC1" s="896"/>
+      <c r="CD1" s="896"/>
+      <c r="CE1" s="896"/>
+      <c r="CF1" s="896"/>
+      <c r="CG1" s="896"/>
+      <c r="CH1" s="896"/>
+      <c r="CI1" s="896"/>
+      <c r="CJ1" s="896"/>
+      <c r="CK1" s="896"/>
+      <c r="CL1" s="896"/>
+      <c r="CM1" s="896"/>
       <c r="CN1" s="687"/>
-      <c r="CO1" s="887"/>
-      <c r="CP1" s="856"/>
-      <c r="CQ1" s="856"/>
-      <c r="CR1" s="856"/>
-      <c r="CS1" s="856"/>
-      <c r="CT1" s="856"/>
-      <c r="CU1" s="856"/>
-      <c r="CV1" s="857"/>
-      <c r="CW1" s="923"/>
-      <c r="CX1" s="924"/>
-      <c r="CY1" s="924"/>
-      <c r="CZ1" s="925"/>
-      <c r="DA1" s="924"/>
-      <c r="DB1" s="924"/>
-      <c r="DC1" s="925"/>
-      <c r="DD1" s="924"/>
-      <c r="DE1" s="924"/>
+      <c r="CO1" s="913"/>
+      <c r="CP1" s="847"/>
+      <c r="CQ1" s="847"/>
+      <c r="CR1" s="847"/>
+      <c r="CS1" s="847"/>
+      <c r="CT1" s="847"/>
+      <c r="CU1" s="847"/>
+      <c r="CV1" s="866"/>
+      <c r="CW1" s="918"/>
+      <c r="CX1" s="919"/>
+      <c r="CY1" s="919"/>
+      <c r="CZ1" s="920"/>
+      <c r="DA1" s="919"/>
+      <c r="DB1" s="919"/>
+      <c r="DC1" s="920"/>
+      <c r="DD1" s="919"/>
+      <c r="DE1" s="919"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="CZ1:DB1"/>
     <mergeCell ref="DC1:DE1"/>
@@ -61200,11 +61208,6 @@
     <mergeCell ref="AG1:AN1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CB1:CM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -61244,18 +61247,18 @@
       <c r="E1" s="142"/>
       <c r="F1" s="142"/>
       <c r="G1" s="142"/>
-      <c r="H1" s="927" t="s">
+      <c r="H1" s="924" t="s">
         <v>555</v>
       </c>
-      <c r="I1" s="927"/>
-      <c r="J1" s="927"/>
-      <c r="K1" s="927"/>
-      <c r="L1" s="926" t="s">
+      <c r="I1" s="924"/>
+      <c r="J1" s="924"/>
+      <c r="K1" s="924"/>
+      <c r="L1" s="923" t="s">
         <v>556</v>
       </c>
-      <c r="M1" s="926"/>
-      <c r="N1" s="926"/>
-      <c r="O1" s="926"/>
+      <c r="M1" s="923"/>
+      <c r="N1" s="923"/>
+      <c r="O1" s="923"/>
     </row>
     <row r="2" spans="1:15" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="443" t="s">
@@ -61374,7 +61377,7 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -61430,10 +61433,10 @@
       <c r="B2" s="202" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="935" t="s">
+      <c r="C2" s="930" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="935"/>
+      <c r="D2" s="930"/>
       <c r="E2" s="200"/>
       <c r="F2" s="200"/>
       <c r="G2" s="200"/>
@@ -61597,35 +61600,35 @@
     </row>
     <row r="7" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="199"/>
-      <c r="B7" s="936"/>
-      <c r="C7" s="936"/>
-      <c r="D7" s="936"/>
+      <c r="B7" s="927"/>
+      <c r="C7" s="927"/>
+      <c r="D7" s="927"/>
       <c r="E7" s="200"/>
       <c r="F7" s="200"/>
       <c r="G7" s="200"/>
       <c r="H7" s="200"/>
       <c r="I7" s="200"/>
-      <c r="J7" s="936"/>
-      <c r="K7" s="936"/>
-      <c r="L7" s="936"/>
+      <c r="J7" s="927"/>
+      <c r="K7" s="927"/>
+      <c r="L7" s="927"/>
       <c r="M7" s="200"/>
       <c r="N7" s="200"/>
       <c r="O7" s="200"/>
       <c r="P7" s="201" t="s">
         <v>219</v>
       </c>
-      <c r="Q7" s="936"/>
-      <c r="R7" s="936"/>
-      <c r="S7" s="936"/>
+      <c r="Q7" s="927"/>
+      <c r="R7" s="927"/>
+      <c r="S7" s="927"/>
       <c r="T7" s="200"/>
       <c r="U7" s="214"/>
       <c r="V7" s="371"/>
       <c r="W7" s="371" t="s">
         <v>219</v>
       </c>
-      <c r="X7" s="936"/>
-      <c r="Y7" s="936"/>
-      <c r="Z7" s="936"/>
+      <c r="X7" s="927"/>
+      <c r="Y7" s="927"/>
+      <c r="Z7" s="927"/>
       <c r="AA7" s="371"/>
       <c r="AB7" s="214"/>
     </row>
@@ -61664,54 +61667,54 @@
       <c r="B9" s="215" t="s">
         <v>418</v>
       </c>
-      <c r="C9" s="931" t="s">
+      <c r="C9" s="928" t="s">
         <v>220</v>
       </c>
-      <c r="D9" s="932"/>
-      <c r="E9" s="931" t="s">
+      <c r="D9" s="929"/>
+      <c r="E9" s="928" t="s">
         <v>221</v>
       </c>
-      <c r="F9" s="932"/>
+      <c r="F9" s="929"/>
       <c r="G9" s="200"/>
       <c r="H9" s="200"/>
       <c r="I9" s="200"/>
       <c r="J9" s="215" t="s">
         <v>418</v>
       </c>
-      <c r="K9" s="931" t="s">
+      <c r="K9" s="928" t="s">
         <v>220</v>
       </c>
-      <c r="L9" s="932"/>
-      <c r="M9" s="931" t="s">
+      <c r="L9" s="929"/>
+      <c r="M9" s="928" t="s">
         <v>221</v>
       </c>
-      <c r="N9" s="932"/>
+      <c r="N9" s="929"/>
       <c r="O9" s="200"/>
       <c r="P9" s="200"/>
       <c r="Q9" s="215" t="s">
         <v>418</v>
       </c>
-      <c r="R9" s="931" t="s">
+      <c r="R9" s="928" t="s">
         <v>220</v>
       </c>
-      <c r="S9" s="932"/>
-      <c r="T9" s="931" t="s">
+      <c r="S9" s="929"/>
+      <c r="T9" s="928" t="s">
         <v>221</v>
       </c>
-      <c r="U9" s="932"/>
+      <c r="U9" s="929"/>
       <c r="V9" s="371"/>
       <c r="W9" s="371"/>
       <c r="X9" s="215" t="s">
         <v>418</v>
       </c>
-      <c r="Y9" s="931" t="s">
+      <c r="Y9" s="928" t="s">
         <v>220</v>
       </c>
-      <c r="Z9" s="932"/>
-      <c r="AA9" s="931" t="s">
+      <c r="Z9" s="929"/>
+      <c r="AA9" s="928" t="s">
         <v>221</v>
       </c>
-      <c r="AB9" s="932"/>
+      <c r="AB9" s="929"/>
     </row>
     <row r="10" spans="1:28" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="199"/>
@@ -61790,10 +61793,10 @@
       </c>
       <c r="C11" s="220"/>
       <c r="D11" s="220"/>
-      <c r="E11" s="928" t="s">
+      <c r="E11" s="925" t="s">
         <v>225</v>
       </c>
-      <c r="F11" s="929"/>
+      <c r="F11" s="926"/>
       <c r="G11" s="221"/>
       <c r="H11" s="221"/>
       <c r="I11" s="221"/>
@@ -61802,10 +61805,10 @@
       </c>
       <c r="K11" s="200"/>
       <c r="L11" s="200"/>
-      <c r="M11" s="933" t="s">
+      <c r="M11" s="932" t="s">
         <v>225</v>
       </c>
-      <c r="N11" s="934"/>
+      <c r="N11" s="933"/>
       <c r="O11" s="221"/>
       <c r="P11" s="221"/>
       <c r="Q11" s="219" t="s">
@@ -61813,10 +61816,10 @@
       </c>
       <c r="R11" s="220"/>
       <c r="S11" s="220"/>
-      <c r="T11" s="928" t="s">
+      <c r="T11" s="925" t="s">
         <v>225</v>
       </c>
-      <c r="U11" s="929"/>
+      <c r="U11" s="926"/>
       <c r="V11" s="371"/>
       <c r="W11" s="371"/>
       <c r="X11" s="219" t="s">
@@ -61824,10 +61827,10 @@
       </c>
       <c r="Y11" s="220"/>
       <c r="Z11" s="220"/>
-      <c r="AA11" s="928" t="s">
+      <c r="AA11" s="925" t="s">
         <v>225</v>
       </c>
-      <c r="AB11" s="929"/>
+      <c r="AB11" s="926"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="199"/>
@@ -62132,10 +62135,10 @@
       </c>
       <c r="C20" s="301"/>
       <c r="D20" s="248"/>
-      <c r="E20" s="928" t="s">
+      <c r="E20" s="925" t="s">
         <v>231</v>
       </c>
-      <c r="F20" s="929"/>
+      <c r="F20" s="926"/>
       <c r="G20" s="229"/>
       <c r="H20" s="229"/>
       <c r="I20" s="200"/>
@@ -62144,10 +62147,10 @@
       </c>
       <c r="K20" s="301"/>
       <c r="L20" s="248"/>
-      <c r="M20" s="928" t="s">
+      <c r="M20" s="925" t="s">
         <v>231</v>
       </c>
-      <c r="N20" s="929"/>
+      <c r="N20" s="926"/>
       <c r="O20" s="239"/>
       <c r="P20" s="239"/>
       <c r="Q20" s="219" t="s">
@@ -62155,10 +62158,10 @@
       </c>
       <c r="R20" s="301"/>
       <c r="S20" s="248"/>
-      <c r="T20" s="928" t="s">
+      <c r="T20" s="925" t="s">
         <v>231</v>
       </c>
-      <c r="U20" s="929"/>
+      <c r="U20" s="926"/>
       <c r="V20" s="276"/>
       <c r="W20" s="276"/>
       <c r="X20" s="219" t="s">
@@ -62166,10 +62169,10 @@
       </c>
       <c r="Y20" s="301"/>
       <c r="Z20" s="248"/>
-      <c r="AA20" s="928" t="s">
+      <c r="AA20" s="925" t="s">
         <v>231</v>
       </c>
-      <c r="AB20" s="929"/>
+      <c r="AB20" s="926"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="199"/>
@@ -62512,10 +62515,10 @@
       </c>
       <c r="C30" s="301"/>
       <c r="D30" s="248"/>
-      <c r="E30" s="928" t="s">
+      <c r="E30" s="925" t="s">
         <v>231</v>
       </c>
-      <c r="F30" s="929"/>
+      <c r="F30" s="926"/>
       <c r="G30" s="229"/>
       <c r="H30" s="229"/>
       <c r="I30" s="200"/>
@@ -62524,10 +62527,10 @@
       </c>
       <c r="K30" s="301"/>
       <c r="L30" s="248"/>
-      <c r="M30" s="928" t="s">
+      <c r="M30" s="925" t="s">
         <v>543</v>
       </c>
-      <c r="N30" s="929"/>
+      <c r="N30" s="926"/>
       <c r="O30" s="239"/>
       <c r="P30" s="239"/>
       <c r="Q30" s="219" t="s">
@@ -62535,10 +62538,10 @@
       </c>
       <c r="R30" s="301"/>
       <c r="S30" s="248"/>
-      <c r="T30" s="928" t="s">
+      <c r="T30" s="925" t="s">
         <v>231</v>
       </c>
-      <c r="U30" s="929"/>
+      <c r="U30" s="926"/>
       <c r="V30" s="276"/>
       <c r="W30" s="276"/>
       <c r="X30" s="219" t="s">
@@ -62546,10 +62549,10 @@
       </c>
       <c r="Y30" s="301"/>
       <c r="Z30" s="248"/>
-      <c r="AA30" s="928" t="s">
+      <c r="AA30" s="925" t="s">
         <v>231</v>
       </c>
-      <c r="AB30" s="929"/>
+      <c r="AB30" s="926"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="261"/>
@@ -62987,11 +62990,11 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="199"/>
-      <c r="B42" s="930"/>
-      <c r="C42" s="930"/>
-      <c r="D42" s="930"/>
-      <c r="E42" s="930"/>
-      <c r="F42" s="930"/>
+      <c r="B42" s="931"/>
+      <c r="C42" s="931"/>
+      <c r="D42" s="931"/>
+      <c r="E42" s="931"/>
+      <c r="F42" s="931"/>
       <c r="G42" s="239"/>
       <c r="H42" s="200"/>
       <c r="I42" s="239"/>
@@ -63178,21 +63181,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="26">
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -63204,6 +63192,21 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA20:AB20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add column in register's rca sheet
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2020_register_model_20210212.xlsx
@@ -41,7 +41,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">Agglomerationout!$A$5:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">breach_list!$B$7:$N$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Glossary!$A$2:$B$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Information on sensitive area'!$A$7:$AQ$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Information on sensitive area'!$A$7:$AS$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'New agglomerations'!$A$5:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">'New treatment plants'!$A$4:$F$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Nuts2_level analyse'!$A$4:$AH$4</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="644">
   <si>
     <t>Acronym</t>
   </si>
@@ -2476,6 +2476,9 @@
   </si>
   <si>
     <t>(2) 0: collection but no treatment, 1: primary treatment, 2: secondary treatment, 3: more stringent treatment</t>
+  </si>
+  <si>
+    <t>Total load of agglomerations (p.e.)</t>
   </si>
 </sst>
 </file>
@@ -3994,7 +3997,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1002">
+  <cellXfs count="1003">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -5994,45 +5997,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -6067,6 +6031,9 @@
     <xf numFmtId="3" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6115,6 +6082,117 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6127,21 +6205,12 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6157,71 +6226,11 @@
     <xf numFmtId="3" fontId="7" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="18" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6232,12 +6241,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6250,26 +6253,26 @@
     <xf numFmtId="0" fontId="25" fillId="20" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6299,6 +6302,33 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6331,39 +6361,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6387,6 +6384,64 @@
     <xf numFmtId="3" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -6399,18 +6454,6 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6423,52 +6466,13 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="30" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7915,8 +7919,8 @@
       </c>
       <c r="C2" s="372"/>
       <c r="D2" s="372"/>
-      <c r="E2" s="930"/>
-      <c r="F2" s="930"/>
+      <c r="E2" s="932"/>
+      <c r="F2" s="932"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="371"/>
@@ -7948,13 +7952,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="369"/>
-      <c r="B6" s="927" t="s">
+      <c r="B6" s="933" t="s">
         <v>420</v>
       </c>
-      <c r="C6" s="927"/>
-      <c r="D6" s="927"/>
-      <c r="E6" s="927"/>
-      <c r="F6" s="927"/>
+      <c r="C6" s="933"/>
+      <c r="D6" s="933"/>
+      <c r="E6" s="933"/>
+      <c r="F6" s="933"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="369"/>
@@ -8112,11 +8116,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="369"/>
-      <c r="B22" s="931"/>
-      <c r="C22" s="931"/>
-      <c r="D22" s="931"/>
-      <c r="E22" s="931"/>
-      <c r="F22" s="931"/>
+      <c r="B22" s="927"/>
+      <c r="C22" s="927"/>
+      <c r="D22" s="927"/>
+      <c r="E22" s="927"/>
+      <c r="F22" s="927"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="369"/>
@@ -8415,43 +8419,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="947" t="s">
+      <c r="A1" s="956" t="s">
         <v>638</v>
       </c>
-      <c r="B1" s="948"/>
+      <c r="B1" s="957"/>
       <c r="C1" s="454"/>
-      <c r="D1" s="958" t="s">
+      <c r="D1" s="947" t="s">
         <v>273</v>
       </c>
-      <c r="E1" s="959"/>
-      <c r="F1" s="959"/>
-      <c r="G1" s="959"/>
-      <c r="H1" s="959"/>
-      <c r="I1" s="960"/>
-      <c r="J1" s="949" t="s">
+      <c r="E1" s="948"/>
+      <c r="F1" s="948"/>
+      <c r="G1" s="948"/>
+      <c r="H1" s="948"/>
+      <c r="I1" s="949"/>
+      <c r="J1" s="958" t="s">
         <v>624</v>
       </c>
-      <c r="K1" s="950"/>
-      <c r="L1" s="950"/>
-      <c r="M1" s="950"/>
-      <c r="N1" s="951"/>
-      <c r="O1" s="952" t="s">
+      <c r="K1" s="959"/>
+      <c r="L1" s="959"/>
+      <c r="M1" s="959"/>
+      <c r="N1" s="960"/>
+      <c r="O1" s="961" t="s">
         <v>274</v>
       </c>
-      <c r="P1" s="953"/>
-      <c r="Q1" s="954"/>
+      <c r="P1" s="962"/>
+      <c r="Q1" s="963"/>
       <c r="R1" s="441" t="s">
         <v>70</v>
       </c>
       <c r="S1" s="442"/>
-      <c r="T1" s="946" t="s">
+      <c r="T1" s="955" t="s">
         <v>462</v>
       </c>
-      <c r="U1" s="946"/>
-      <c r="V1" s="946"/>
-      <c r="W1" s="946"/>
-      <c r="X1" s="946"/>
-      <c r="Y1" s="946"/>
+      <c r="U1" s="955"/>
+      <c r="V1" s="955"/>
+      <c r="W1" s="955"/>
+      <c r="X1" s="955"/>
+      <c r="Y1" s="955"/>
     </row>
     <row r="2" spans="1:25" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="444" t="s">
@@ -8463,18 +8467,18 @@
       <c r="C2" s="445" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="963" t="s">
+      <c r="D2" s="952" t="s">
         <v>275</v>
       </c>
-      <c r="E2" s="962"/>
-      <c r="F2" s="962" t="s">
+      <c r="E2" s="951"/>
+      <c r="F2" s="951" t="s">
         <v>276</v>
       </c>
-      <c r="G2" s="962"/>
-      <c r="H2" s="961" t="s">
+      <c r="G2" s="951"/>
+      <c r="H2" s="950" t="s">
         <v>277</v>
       </c>
-      <c r="I2" s="961"/>
+      <c r="I2" s="950"/>
       <c r="J2" s="446">
         <v>0</v>
       </c>
@@ -8505,18 +8509,18 @@
       <c r="S2" s="675" t="s">
         <v>80</v>
       </c>
-      <c r="T2" s="944" t="s">
+      <c r="T2" s="953" t="s">
         <v>432</v>
       </c>
-      <c r="U2" s="944"/>
-      <c r="V2" s="945" t="s">
+      <c r="U2" s="953"/>
+      <c r="V2" s="954" t="s">
         <v>448</v>
       </c>
-      <c r="W2" s="945"/>
-      <c r="X2" s="945" t="s">
+      <c r="W2" s="954"/>
+      <c r="X2" s="954" t="s">
         <v>449</v>
       </c>
-      <c r="Y2" s="945"/>
+      <c r="Y2" s="954"/>
     </row>
     <row r="3" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="449"/>
@@ -8542,13 +8546,13 @@
       <c r="I3" s="659" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="955" t="s">
+      <c r="J3" s="944" t="s">
         <v>282</v>
       </c>
-      <c r="K3" s="956"/>
-      <c r="L3" s="956"/>
-      <c r="M3" s="956"/>
-      <c r="N3" s="957"/>
+      <c r="K3" s="945"/>
+      <c r="L3" s="945"/>
+      <c r="M3" s="945"/>
+      <c r="N3" s="946"/>
       <c r="O3" s="457"/>
       <c r="P3" s="457"/>
       <c r="Q3" s="457"/>
@@ -9477,11 +9481,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:X4"/>
   <mergeCells count="12">
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
@@ -9489,6 +9488,11 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9529,25 +9533,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="841" t="s">
+      <c r="A1" s="870" t="s">
         <v>283</v>
       </c>
-      <c r="B1" s="842"/>
-      <c r="C1" s="842"/>
-      <c r="D1" s="842"/>
-      <c r="E1" s="842"/>
-      <c r="F1" s="842"/>
+      <c r="B1" s="871"/>
+      <c r="C1" s="871"/>
+      <c r="D1" s="871"/>
+      <c r="E1" s="871"/>
+      <c r="F1" s="871"/>
       <c r="G1" s="471"/>
-      <c r="H1" s="970" t="s">
+      <c r="H1" s="968" t="s">
         <v>151</v>
       </c>
-      <c r="I1" s="971"/>
-      <c r="J1" s="971"/>
+      <c r="I1" s="969"/>
+      <c r="J1" s="969"/>
       <c r="K1" s="473"/>
       <c r="L1" s="463"/>
       <c r="M1" s="473"/>
       <c r="N1" s="464"/>
-      <c r="O1" s="968" t="s">
+      <c r="O1" s="966" t="s">
         <v>284</v>
       </c>
       <c r="P1" s="465"/>
@@ -9559,26 +9563,26 @@
       <c r="T1" s="463"/>
       <c r="U1" s="473"/>
       <c r="V1" s="464"/>
-      <c r="W1" s="968" t="s">
+      <c r="W1" s="966" t="s">
         <v>286</v>
       </c>
       <c r="X1" s="465"/>
-      <c r="Y1" s="972" t="s">
+      <c r="Y1" s="970" t="s">
         <v>287</v>
       </c>
-      <c r="Z1" s="972"/>
-      <c r="AA1" s="972"/>
-      <c r="AB1" s="972"/>
-      <c r="AC1" s="972"/>
-      <c r="AD1" s="973"/>
-      <c r="AE1" s="968" t="s">
+      <c r="Z1" s="970"/>
+      <c r="AA1" s="970"/>
+      <c r="AB1" s="970"/>
+      <c r="AC1" s="970"/>
+      <c r="AD1" s="971"/>
+      <c r="AE1" s="966" t="s">
         <v>288</v>
       </c>
-      <c r="AF1" s="967" t="s">
+      <c r="AF1" s="965" t="s">
         <v>447</v>
       </c>
-      <c r="AG1" s="946"/>
-      <c r="AH1" s="946"/>
+      <c r="AG1" s="955"/>
+      <c r="AH1" s="955"/>
       <c r="AI1" s="682"/>
       <c r="AJ1" s="682"/>
       <c r="AK1" s="682"/>
@@ -9637,56 +9641,56 @@
       <c r="C2" s="472" t="s">
         <v>290</v>
       </c>
-      <c r="D2" s="966" t="s">
+      <c r="D2" s="964" t="s">
         <v>452</v>
       </c>
-      <c r="E2" s="966"/>
-      <c r="F2" s="966" t="s">
+      <c r="E2" s="964"/>
+      <c r="F2" s="964" t="s">
         <v>453</v>
       </c>
-      <c r="G2" s="966"/>
+      <c r="G2" s="964"/>
       <c r="H2" s="467"/>
-      <c r="I2" s="964" t="s">
+      <c r="I2" s="972" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="964"/>
-      <c r="K2" s="964" t="s">
+      <c r="J2" s="972"/>
+      <c r="K2" s="972" t="s">
         <v>167</v>
       </c>
-      <c r="L2" s="964"/>
-      <c r="M2" s="964" t="s">
+      <c r="L2" s="972"/>
+      <c r="M2" s="972" t="s">
         <v>168</v>
       </c>
-      <c r="N2" s="965"/>
-      <c r="O2" s="969"/>
+      <c r="N2" s="973"/>
+      <c r="O2" s="967"/>
       <c r="P2" s="468"/>
-      <c r="Q2" s="964" t="s">
+      <c r="Q2" s="972" t="s">
         <v>166</v>
       </c>
-      <c r="R2" s="964"/>
-      <c r="S2" s="964" t="s">
+      <c r="R2" s="972"/>
+      <c r="S2" s="972" t="s">
         <v>167</v>
       </c>
-      <c r="T2" s="964"/>
-      <c r="U2" s="964" t="s">
+      <c r="T2" s="972"/>
+      <c r="U2" s="972" t="s">
         <v>168</v>
       </c>
-      <c r="V2" s="965"/>
-      <c r="W2" s="969"/>
+      <c r="V2" s="973"/>
+      <c r="W2" s="967"/>
       <c r="X2" s="468"/>
-      <c r="Y2" s="964" t="s">
+      <c r="Y2" s="972" t="s">
         <v>166</v>
       </c>
-      <c r="Z2" s="964"/>
-      <c r="AA2" s="964" t="s">
+      <c r="Z2" s="972"/>
+      <c r="AA2" s="972" t="s">
         <v>167</v>
       </c>
-      <c r="AB2" s="964"/>
-      <c r="AC2" s="964" t="s">
+      <c r="AB2" s="972"/>
+      <c r="AC2" s="972" t="s">
         <v>168</v>
       </c>
-      <c r="AD2" s="965"/>
-      <c r="AE2" s="969"/>
+      <c r="AD2" s="973"/>
+      <c r="AE2" s="967"/>
       <c r="AF2" s="676" t="s">
         <v>432</v>
       </c>
@@ -10572,6 +10576,8 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A4:AH4"/>
   <mergeCells count="18">
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AE1:AE2"/>
@@ -10588,8 +10594,6 @@
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="U2:V2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10813,11 +10817,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="974" t="s">
+      <c r="A1" s="992" t="s">
         <v>629</v>
       </c>
-      <c r="B1" s="872"/>
-      <c r="C1" s="872"/>
+      <c r="B1" s="860"/>
+      <c r="C1" s="860"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I2" s="734"/>
@@ -10832,21 +10836,21 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="982" t="s">
+      <c r="A3" s="996" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="984" t="s">
+      <c r="B3" s="998" t="s">
         <v>421</v>
       </c>
-      <c r="C3" s="985"/>
-      <c r="D3" s="980" t="s">
+      <c r="C3" s="999"/>
+      <c r="D3" s="984" t="s">
         <v>422</v>
       </c>
-      <c r="E3" s="981"/>
-      <c r="F3" s="980" t="s">
+      <c r="E3" s="985"/>
+      <c r="F3" s="984" t="s">
         <v>455</v>
       </c>
-      <c r="G3" s="981"/>
+      <c r="G3" s="985"/>
       <c r="I3" s="732" t="str">
         <f>$B$3</f>
         <v xml:space="preserve">[#current_year#] </v>
@@ -10857,14 +10861,14 @@
       <c r="K3" s="714"/>
       <c r="L3" s="714"/>
       <c r="N3" s="699"/>
-      <c r="O3" s="996" t="s">
+      <c r="O3" s="981" t="s">
         <v>317</v>
       </c>
-      <c r="P3" s="996"/>
-      <c r="Q3" s="996" t="s">
+      <c r="P3" s="981"/>
+      <c r="Q3" s="981" t="s">
         <v>318</v>
       </c>
-      <c r="R3" s="996"/>
+      <c r="R3" s="981"/>
       <c r="S3" s="699"/>
       <c r="T3" s="707" t="s">
         <v>319</v>
@@ -10872,7 +10876,7 @@
       <c r="U3" s="699"/>
     </row>
     <row r="4" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="983"/>
+      <c r="A4" s="997"/>
       <c r="B4" s="511" t="s">
         <v>320</v>
       </c>
@@ -11131,14 +11135,14 @@
       <c r="K10" s="714"/>
       <c r="L10" s="714"/>
       <c r="N10" s="707"/>
-      <c r="O10" s="996" t="s">
+      <c r="O10" s="981" t="s">
         <v>320</v>
       </c>
-      <c r="P10" s="996"/>
-      <c r="Q10" s="996" t="s">
+      <c r="P10" s="981"/>
+      <c r="Q10" s="981" t="s">
         <v>327</v>
       </c>
-      <c r="R10" s="996"/>
+      <c r="R10" s="981"/>
     </row>
     <row r="11" spans="1:21" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A11" s="831" t="s">
@@ -11205,7 +11209,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="982" t="s">
+      <c r="A13" s="996" t="s">
         <v>328</v>
       </c>
       <c r="B13" s="510" t="str">
@@ -11251,7 +11255,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="983"/>
+      <c r="A14" s="997"/>
       <c r="B14" s="513" t="s">
         <v>321</v>
       </c>
@@ -11386,34 +11390,34 @@
       <c r="A21" s="501" t="s">
         <v>333</v>
       </c>
-      <c r="B21" s="997" t="s">
+      <c r="B21" s="986" t="s">
         <v>474</v>
       </c>
-      <c r="C21" s="998"/>
-      <c r="D21" s="998"/>
-      <c r="E21" s="998"/>
-      <c r="F21" s="998"/>
-      <c r="G21" s="998"/>
+      <c r="C21" s="987"/>
+      <c r="D21" s="987"/>
+      <c r="E21" s="987"/>
+      <c r="F21" s="987"/>
+      <c r="G21" s="987"/>
     </row>
     <row r="22" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="515" t="s">
         <v>297</v>
       </c>
-      <c r="B22" s="986" t="str">
+      <c r="B22" s="988" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C22" s="987"/>
-      <c r="D22" s="986" t="str">
+      <c r="C22" s="989"/>
+      <c r="D22" s="988" t="str">
         <f>D3</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E22" s="987"/>
-      <c r="F22" s="986" t="str">
+      <c r="E22" s="989"/>
+      <c r="F22" s="988" t="str">
         <f>F3</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G22" s="987"/>
+      <c r="G22" s="989"/>
     </row>
     <row r="23" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="516"/>
@@ -11840,21 +11844,21 @@
       <c r="A41" s="518" t="s">
         <v>343</v>
       </c>
-      <c r="B41" s="976" t="str">
+      <c r="B41" s="994" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C41" s="977"/>
-      <c r="D41" s="978" t="str">
+      <c r="C41" s="995"/>
+      <c r="D41" s="982" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E41" s="979"/>
-      <c r="F41" s="978" t="str">
+      <c r="E41" s="983"/>
+      <c r="F41" s="982" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G41" s="979"/>
+      <c r="G41" s="983"/>
       <c r="N41" s="699"/>
       <c r="O41" s="726" t="s">
         <v>426</v>
@@ -12073,11 +12077,11 @@
       <c r="F53" s="704" t="s">
         <v>480</v>
       </c>
-      <c r="H53" s="999" t="s">
+      <c r="H53" s="974" t="s">
         <v>467</v>
       </c>
-      <c r="I53" s="999"/>
-      <c r="J53" s="999"/>
+      <c r="I53" s="974"/>
+      <c r="J53" s="974"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="695" t="s">
@@ -12247,11 +12251,11 @@
       <c r="F63" s="704" t="s">
         <v>480</v>
       </c>
-      <c r="H63" s="999" t="s">
+      <c r="H63" s="974" t="s">
         <v>481</v>
       </c>
-      <c r="I63" s="999"/>
-      <c r="J63" s="999"/>
+      <c r="I63" s="974"/>
+      <c r="J63" s="974"/>
       <c r="L63" s="702"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -12438,12 +12442,12 @@
       <c r="A74" s="831" t="s">
         <v>633</v>
       </c>
-      <c r="B74" s="975" t="s">
+      <c r="B74" s="993" t="s">
         <v>423</v>
       </c>
-      <c r="C74" s="975"/>
-      <c r="D74" s="975"/>
-      <c r="E74" s="975"/>
+      <c r="C74" s="993"/>
+      <c r="D74" s="993"/>
+      <c r="E74" s="993"/>
       <c r="I74" s="703"/>
       <c r="J74" s="703"/>
       <c r="K74" s="703"/>
@@ -12759,21 +12763,21 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="990" t="str">
+      <c r="B85" s="979" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C85" s="991"/>
-      <c r="D85" s="990" t="str">
+      <c r="C85" s="980"/>
+      <c r="D85" s="979" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E85" s="991"/>
-      <c r="F85" s="990" t="str">
+      <c r="E85" s="980"/>
+      <c r="F85" s="979" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G85" s="991"/>
+      <c r="G85" s="980"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="502"/>
@@ -13075,21 +13079,21 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B101" s="990" t="str">
+      <c r="B101" s="979" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C101" s="991"/>
-      <c r="D101" s="990" t="str">
+      <c r="C101" s="980"/>
+      <c r="D101" s="979" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E101" s="991"/>
-      <c r="F101" s="990" t="str">
+      <c r="E101" s="980"/>
+      <c r="F101" s="979" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G101" s="991"/>
+      <c r="G101" s="980"/>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="502"/>
@@ -13390,36 +13394,36 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B116" s="992" t="str">
+      <c r="B116" s="975" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C116" s="993"/>
-      <c r="D116" s="992" t="str">
+      <c r="C116" s="976"/>
+      <c r="D116" s="975" t="str">
         <f>C13</f>
         <v>[#previous_year#]</v>
       </c>
-      <c r="E116" s="993"/>
-      <c r="F116" s="992" t="str">
+      <c r="E116" s="976"/>
+      <c r="F116" s="975" t="str">
         <f>D13</f>
         <v>[#previous_year_n2#]</v>
       </c>
-      <c r="G116" s="993"/>
+      <c r="G116" s="976"/>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="541"/>
-      <c r="B117" s="994" t="s">
+      <c r="B117" s="977" t="s">
         <v>253</v>
       </c>
-      <c r="C117" s="995"/>
-      <c r="D117" s="994" t="s">
+      <c r="C117" s="978"/>
+      <c r="D117" s="977" t="s">
         <v>253</v>
       </c>
-      <c r="E117" s="995"/>
-      <c r="F117" s="994" t="s">
+      <c r="E117" s="978"/>
+      <c r="F117" s="977" t="s">
         <v>253</v>
       </c>
-      <c r="G117" s="995"/>
+      <c r="G117" s="978"/>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="542" t="s">
@@ -13722,12 +13726,12 @@
       <c r="A129" s="545" t="s">
         <v>328</v>
       </c>
-      <c r="B129" s="988" t="str">
+      <c r="B129" s="990" t="str">
         <f>B3</f>
         <v xml:space="preserve">[#current_year#] </v>
       </c>
-      <c r="C129" s="989"/>
-      <c r="D129" s="989"/>
+      <c r="C129" s="991"/>
+      <c r="D129" s="991"/>
       <c r="N129" s="707" t="s">
         <v>369</v>
       </c>
@@ -14503,22 +14507,16 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="39">
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="F116:G116"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="F102:G102"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
     <mergeCell ref="B129:D129"/>
     <mergeCell ref="B85:C85"/>
     <mergeCell ref="D85:E85"/>
@@ -14532,16 +14530,22 @@
     <mergeCell ref="D116:E116"/>
     <mergeCell ref="B117:C117"/>
     <mergeCell ref="D117:E117"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="F102:G102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17838,13 +17842,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:AR10000"/>
+  <dimension ref="A1:AS10000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="AG8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="AN8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:AR4"/>
+      <selection pane="bottomRight" activeCell="AT17" sqref="AT17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17881,9 +17885,11 @@
     <col min="40" max="40" width="18.44140625" customWidth="1"/>
     <col min="41" max="41" width="19.44140625" customWidth="1"/>
     <col min="42" max="43" width="18.21875" customWidth="1"/>
+    <col min="44" max="44" width="10.21875" customWidth="1"/>
+    <col min="45" max="45" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
@@ -17898,13 +17904,13 @@
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="E2" s="427" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="6"/>
@@ -17948,7 +17954,7 @@
       <c r="AP3" s="6"/>
       <c r="AQ3" s="6"/>
     </row>
-    <row r="4" spans="1:44" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:45" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1000" t="s">
         <v>477</v>
       </c>
@@ -17995,8 +18001,9 @@
       <c r="AP4" s="1001"/>
       <c r="AQ4" s="1001"/>
       <c r="AR4" s="1001"/>
-    </row>
-    <row r="5" spans="1:44" s="7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AS4" s="1001"/>
+    </row>
+    <row r="5" spans="1:45" s="7" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="833" t="s">
         <v>25</v>
       </c>
@@ -18129,8 +18136,11 @@
       <c r="AR5" s="833" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="6" spans="1:44" s="9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AS5" s="833" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" s="9" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="834"/>
       <c r="B6" s="834"/>
       <c r="C6" s="787"/>
@@ -18235,21 +18245,24 @@
       <c r="AP6" s="834"/>
       <c r="AQ6" s="834"/>
       <c r="AR6" s="834"/>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AS6" s="834"/>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AD7" s="822"/>
       <c r="AE7" s="8"/>
       <c r="AG7" s="822"/>
       <c r="AH7" s="8"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="C8" s="749"/>
       <c r="AD8" s="822"/>
       <c r="AE8" s="623"/>
       <c r="AG8" s="822"/>
       <c r="AH8" s="623"/>
-    </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AR8" s="1002"/>
+      <c r="AS8" s="1002"/>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A9" s="656"/>
       <c r="B9" s="2"/>
       <c r="C9" s="813"/>
@@ -18293,104 +18306,126 @@
       <c r="AO9" s="656"/>
       <c r="AP9" s="656"/>
       <c r="AQ9" s="656"/>
-    </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AR9" s="1002"/>
+      <c r="AS9" s="1002"/>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A10" s="427" t="s">
         <v>63</v>
       </c>
       <c r="AD10" s="822"/>
       <c r="AE10" s="8"/>
       <c r="AH10" s="8"/>
-    </row>
-    <row r="11" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AR10" s="1002"/>
+      <c r="AS10" s="1002"/>
+    </row>
+    <row r="11" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="427" t="s">
         <v>64</v>
       </c>
       <c r="AD11" s="822"/>
       <c r="AE11" s="8"/>
       <c r="AH11" s="8"/>
-    </row>
-    <row r="12" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AR11" s="1002"/>
+      <c r="AS11" s="1002"/>
+    </row>
+    <row r="12" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AE12" s="8"/>
       <c r="AH12" s="8"/>
-    </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AR12" s="1002"/>
+      <c r="AS12" s="1002"/>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AE13" s="8"/>
       <c r="AH13" s="8"/>
-    </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AR13" s="1002"/>
+      <c r="AS13" s="1002"/>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AE14" s="8"/>
       <c r="AH14" s="8"/>
-    </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AR14" s="1002"/>
+      <c r="AS14" s="1002"/>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AE15" s="8"/>
       <c r="AH15" s="8"/>
-    </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AR15" s="1002"/>
+      <c r="AS15" s="1002"/>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
       <c r="AE16" s="8"/>
       <c r="AH16" s="8"/>
-    </row>
-    <row r="17" spans="31:34" x14ac:dyDescent="0.3">
+      <c r="AR16" s="1002"/>
+      <c r="AS16" s="1002"/>
+    </row>
+    <row r="17" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE17" s="8"/>
       <c r="AH17" s="8"/>
-    </row>
-    <row r="18" spans="31:34" x14ac:dyDescent="0.3">
+      <c r="AR17" s="1002"/>
+      <c r="AS17" s="1002"/>
+    </row>
+    <row r="18" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE18" s="8"/>
       <c r="AH18" s="8"/>
-    </row>
-    <row r="19" spans="31:34" x14ac:dyDescent="0.3">
+      <c r="AR18" s="1002"/>
+      <c r="AS18" s="1002"/>
+    </row>
+    <row r="19" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE19" s="8"/>
       <c r="AH19" s="8"/>
-    </row>
-    <row r="20" spans="31:34" x14ac:dyDescent="0.3">
+      <c r="AR19" s="1002"/>
+      <c r="AS19" s="1002"/>
+    </row>
+    <row r="20" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE20" s="8"/>
       <c r="AH20" s="8"/>
     </row>
-    <row r="21" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="21" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE21" s="8"/>
       <c r="AH21" s="8"/>
     </row>
-    <row r="22" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="22" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE22" s="8"/>
       <c r="AH22" s="8"/>
     </row>
-    <row r="23" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="23" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE23" s="8"/>
       <c r="AH23" s="8"/>
     </row>
-    <row r="24" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="24" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE24" s="8"/>
       <c r="AH24" s="8"/>
     </row>
-    <row r="25" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="25" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE25" s="8"/>
       <c r="AH25" s="8"/>
     </row>
-    <row r="26" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="26" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE26" s="8"/>
       <c r="AH26" s="8"/>
     </row>
-    <row r="27" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="27" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE27" s="8"/>
       <c r="AH27" s="8"/>
     </row>
-    <row r="28" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="28" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE28" s="8"/>
       <c r="AH28" s="8"/>
     </row>
-    <row r="29" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="29" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE29" s="8"/>
       <c r="AH29" s="8"/>
     </row>
-    <row r="30" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="30" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE30" s="8"/>
       <c r="AH30" s="8"/>
     </row>
-    <row r="31" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="31" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE31" s="8"/>
       <c r="AH31" s="8"/>
     </row>
-    <row r="32" spans="31:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="31:45" x14ac:dyDescent="0.3">
       <c r="AE32" s="8"/>
       <c r="AH32" s="8"/>
     </row>
@@ -58268,14 +58303,9 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A7:AQ7">
-    <sortState ref="B8:AQ8">
-      <sortCondition descending="1" ref="B7"/>
-    </sortState>
-  </autoFilter>
-  <mergeCells count="14">
+  <autoFilter ref="A7:AS7"/>
+  <mergeCells count="15">
     <mergeCell ref="AR5:AR6"/>
-    <mergeCell ref="A4:AR4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="D5:D6"/>
@@ -58288,6 +58318,8 @@
     <mergeCell ref="AO5:AO6"/>
     <mergeCell ref="AP5:AP6"/>
     <mergeCell ref="AQ5:AQ6"/>
+    <mergeCell ref="A4:AS4"/>
+    <mergeCell ref="AS5:AS6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -58727,123 +58759,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:95" s="652" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="841" t="s">
+      <c r="A1" s="870" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="842"/>
-      <c r="C1" s="842"/>
-      <c r="D1" s="842"/>
-      <c r="E1" s="842"/>
-      <c r="F1" s="842"/>
-      <c r="G1" s="842"/>
-      <c r="H1" s="843" t="s">
+      <c r="B1" s="871"/>
+      <c r="C1" s="871"/>
+      <c r="D1" s="871"/>
+      <c r="E1" s="871"/>
+      <c r="F1" s="871"/>
+      <c r="G1" s="871"/>
+      <c r="H1" s="872" t="s">
         <v>432</v>
       </c>
-      <c r="I1" s="844"/>
-      <c r="J1" s="844"/>
-      <c r="K1" s="844"/>
-      <c r="L1" s="844"/>
-      <c r="M1" s="845"/>
-      <c r="N1" s="846" t="s">
+      <c r="I1" s="873"/>
+      <c r="J1" s="873"/>
+      <c r="K1" s="873"/>
+      <c r="L1" s="873"/>
+      <c r="M1" s="874"/>
+      <c r="N1" s="875" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="847"/>
-      <c r="P1" s="847"/>
-      <c r="Q1" s="847"/>
-      <c r="R1" s="847"/>
-      <c r="S1" s="847"/>
-      <c r="T1" s="847"/>
-      <c r="U1" s="847"/>
-      <c r="V1" s="848" t="s">
+      <c r="O1" s="853"/>
+      <c r="P1" s="853"/>
+      <c r="Q1" s="853"/>
+      <c r="R1" s="853"/>
+      <c r="S1" s="853"/>
+      <c r="T1" s="853"/>
+      <c r="U1" s="853"/>
+      <c r="V1" s="876" t="s">
         <v>72</v>
       </c>
-      <c r="W1" s="849"/>
-      <c r="X1" s="850"/>
-      <c r="Y1" s="850"/>
-      <c r="Z1" s="851"/>
-      <c r="AA1" s="852" t="s">
+      <c r="W1" s="877"/>
+      <c r="X1" s="878"/>
+      <c r="Y1" s="878"/>
+      <c r="Z1" s="879"/>
+      <c r="AA1" s="880" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="853"/>
-      <c r="AC1" s="853"/>
-      <c r="AD1" s="853"/>
-      <c r="AE1" s="853"/>
-      <c r="AF1" s="853"/>
-      <c r="AG1" s="853"/>
-      <c r="AH1" s="853"/>
-      <c r="AI1" s="853"/>
-      <c r="AJ1" s="853"/>
-      <c r="AK1" s="853"/>
-      <c r="AL1" s="853"/>
-      <c r="AM1" s="853"/>
+      <c r="AB1" s="881"/>
+      <c r="AC1" s="881"/>
+      <c r="AD1" s="881"/>
+      <c r="AE1" s="881"/>
+      <c r="AF1" s="881"/>
+      <c r="AG1" s="881"/>
+      <c r="AH1" s="881"/>
+      <c r="AI1" s="881"/>
+      <c r="AJ1" s="881"/>
+      <c r="AK1" s="881"/>
+      <c r="AL1" s="881"/>
+      <c r="AM1" s="881"/>
       <c r="AN1" s="52"/>
       <c r="AO1" s="53"/>
-      <c r="AP1" s="865" t="s">
+      <c r="AP1" s="852" t="s">
         <v>74</v>
       </c>
-      <c r="AQ1" s="847"/>
-      <c r="AR1" s="847"/>
-      <c r="AS1" s="847"/>
-      <c r="AT1" s="847"/>
-      <c r="AU1" s="847"/>
-      <c r="AV1" s="847"/>
-      <c r="AW1" s="866"/>
-      <c r="AX1" s="873" t="s">
+      <c r="AQ1" s="853"/>
+      <c r="AR1" s="853"/>
+      <c r="AS1" s="853"/>
+      <c r="AT1" s="853"/>
+      <c r="AU1" s="853"/>
+      <c r="AV1" s="853"/>
+      <c r="AW1" s="854"/>
+      <c r="AX1" s="861" t="s">
         <v>547</v>
       </c>
-      <c r="AY1" s="874"/>
-      <c r="AZ1" s="874"/>
-      <c r="BA1" s="874"/>
-      <c r="BB1" s="874"/>
-      <c r="BC1" s="875"/>
-      <c r="BD1" s="876" t="s">
+      <c r="AY1" s="862"/>
+      <c r="AZ1" s="862"/>
+      <c r="BA1" s="862"/>
+      <c r="BB1" s="862"/>
+      <c r="BC1" s="863"/>
+      <c r="BD1" s="864" t="s">
         <v>75</v>
       </c>
-      <c r="BE1" s="877"/>
-      <c r="BF1" s="877"/>
-      <c r="BG1" s="877"/>
-      <c r="BH1" s="877"/>
-      <c r="BI1" s="878"/>
-      <c r="BJ1" s="879" t="s">
+      <c r="BE1" s="865"/>
+      <c r="BF1" s="865"/>
+      <c r="BG1" s="865"/>
+      <c r="BH1" s="865"/>
+      <c r="BI1" s="866"/>
+      <c r="BJ1" s="867" t="s">
         <v>76</v>
       </c>
-      <c r="BK1" s="880"/>
-      <c r="BL1" s="880"/>
-      <c r="BM1" s="880"/>
-      <c r="BN1" s="880"/>
-      <c r="BO1" s="880"/>
-      <c r="BP1" s="881"/>
-      <c r="BQ1" s="854" t="s">
+      <c r="BK1" s="868"/>
+      <c r="BL1" s="868"/>
+      <c r="BM1" s="868"/>
+      <c r="BN1" s="868"/>
+      <c r="BO1" s="868"/>
+      <c r="BP1" s="869"/>
+      <c r="BQ1" s="841" t="s">
         <v>77</v>
       </c>
-      <c r="BR1" s="855"/>
-      <c r="BS1" s="855"/>
-      <c r="BT1" s="855"/>
-      <c r="BU1" s="855"/>
-      <c r="BV1" s="855"/>
+      <c r="BR1" s="842"/>
+      <c r="BS1" s="842"/>
+      <c r="BT1" s="842"/>
+      <c r="BU1" s="842"/>
+      <c r="BV1" s="842"/>
       <c r="BW1" s="53"/>
       <c r="BX1" s="54"/>
-      <c r="BY1" s="856" t="s">
+      <c r="BY1" s="843" t="s">
         <v>78</v>
       </c>
-      <c r="BZ1" s="857"/>
-      <c r="CA1" s="857"/>
-      <c r="CB1" s="857"/>
-      <c r="CC1" s="857"/>
-      <c r="CD1" s="857"/>
-      <c r="CE1" s="857"/>
-      <c r="CF1" s="858"/>
-      <c r="CG1" s="858"/>
-      <c r="CH1" s="858"/>
-      <c r="CI1" s="858"/>
-      <c r="CJ1" s="858"/>
-      <c r="CK1" s="858"/>
-      <c r="CL1" s="858"/>
-      <c r="CM1" s="858"/>
-      <c r="CN1" s="858"/>
-      <c r="CO1" s="858"/>
-      <c r="CP1" s="858"/>
-      <c r="CQ1" s="858"/>
+      <c r="BZ1" s="844"/>
+      <c r="CA1" s="844"/>
+      <c r="CB1" s="844"/>
+      <c r="CC1" s="844"/>
+      <c r="CD1" s="844"/>
+      <c r="CE1" s="844"/>
+      <c r="CF1" s="845"/>
+      <c r="CG1" s="845"/>
+      <c r="CH1" s="845"/>
+      <c r="CI1" s="845"/>
+      <c r="CJ1" s="845"/>
+      <c r="CK1" s="845"/>
+      <c r="CL1" s="845"/>
+      <c r="CM1" s="845"/>
+      <c r="CN1" s="845"/>
+      <c r="CO1" s="845"/>
+      <c r="CP1" s="845"/>
+      <c r="CQ1" s="845"/>
     </row>
     <row r="2" spans="1:95" s="652" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
@@ -58867,18 +58899,18 @@
       <c r="G2" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="859" t="s">
+      <c r="H2" s="846" t="s">
         <v>433</v>
       </c>
-      <c r="I2" s="860"/>
-      <c r="J2" s="860" t="s">
+      <c r="I2" s="847"/>
+      <c r="J2" s="847" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="860"/>
-      <c r="L2" s="860" t="s">
+      <c r="K2" s="847"/>
+      <c r="L2" s="847" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="861"/>
+      <c r="M2" s="848"/>
       <c r="N2" s="57" t="s">
         <v>79</v>
       </c>
@@ -58987,36 +59019,36 @@
       <c r="AW2" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="AX2" s="862" t="s">
+      <c r="AX2" s="849" t="s">
         <v>112</v>
       </c>
-      <c r="AY2" s="863"/>
-      <c r="AZ2" s="863"/>
-      <c r="BA2" s="863" t="s">
+      <c r="AY2" s="850"/>
+      <c r="AZ2" s="850"/>
+      <c r="BA2" s="850" t="s">
         <v>113</v>
       </c>
-      <c r="BB2" s="863"/>
-      <c r="BC2" s="864"/>
-      <c r="BD2" s="867" t="s">
+      <c r="BB2" s="850"/>
+      <c r="BC2" s="851"/>
+      <c r="BD2" s="855" t="s">
         <v>112</v>
       </c>
-      <c r="BE2" s="868"/>
-      <c r="BF2" s="868"/>
-      <c r="BG2" s="868" t="s">
+      <c r="BE2" s="856"/>
+      <c r="BF2" s="856"/>
+      <c r="BG2" s="856" t="s">
         <v>113</v>
       </c>
-      <c r="BH2" s="868"/>
-      <c r="BI2" s="869"/>
-      <c r="BJ2" s="870" t="s">
+      <c r="BH2" s="856"/>
+      <c r="BI2" s="857"/>
+      <c r="BJ2" s="858" t="s">
         <v>112</v>
       </c>
-      <c r="BK2" s="871"/>
-      <c r="BL2" s="871"/>
-      <c r="BM2" s="871" t="s">
+      <c r="BK2" s="859"/>
+      <c r="BL2" s="859"/>
+      <c r="BM2" s="859" t="s">
         <v>113</v>
       </c>
-      <c r="BN2" s="872"/>
-      <c r="BO2" s="872"/>
+      <c r="BN2" s="860"/>
+      <c r="BO2" s="860"/>
       <c r="BP2" s="69" t="s">
         <v>114</v>
       </c>
@@ -59666,6 +59698,11 @@
     </sortState>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AM1"/>
     <mergeCell ref="BQ1:BV1"/>
     <mergeCell ref="BY1:CQ1"/>
     <mergeCell ref="H2:I2"/>
@@ -59681,11 +59718,6 @@
     <mergeCell ref="AX1:BC1"/>
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BP1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -59769,36 +59801,36 @@
       <c r="H1" s="142"/>
       <c r="I1" s="142"/>
       <c r="J1" s="142"/>
-      <c r="K1" s="911" t="s">
+      <c r="K1" s="882" t="s">
         <v>613</v>
       </c>
-      <c r="L1" s="912"/>
-      <c r="M1" s="882" t="s">
+      <c r="L1" s="883"/>
+      <c r="M1" s="907" t="s">
         <v>150</v>
       </c>
-      <c r="N1" s="883" t="s">
+      <c r="N1" s="908" t="s">
         <v>487</v>
       </c>
-      <c r="O1" s="884"/>
-      <c r="P1" s="884"/>
-      <c r="Q1" s="884"/>
-      <c r="R1" s="885" t="s">
+      <c r="O1" s="909"/>
+      <c r="P1" s="909"/>
+      <c r="Q1" s="909"/>
+      <c r="R1" s="910" t="s">
         <v>432</v>
       </c>
-      <c r="S1" s="886"/>
-      <c r="T1" s="886"/>
-      <c r="U1" s="886"/>
-      <c r="V1" s="886"/>
-      <c r="W1" s="886"/>
-      <c r="X1" s="887"/>
-      <c r="Y1" s="888" t="s">
+      <c r="S1" s="903"/>
+      <c r="T1" s="903"/>
+      <c r="U1" s="903"/>
+      <c r="V1" s="903"/>
+      <c r="W1" s="903"/>
+      <c r="X1" s="911"/>
+      <c r="Y1" s="897" t="s">
         <v>440</v>
       </c>
-      <c r="Z1" s="877"/>
-      <c r="AA1" s="891" t="s">
+      <c r="Z1" s="865"/>
+      <c r="AA1" s="913" t="s">
         <v>151</v>
       </c>
-      <c r="AB1" s="903" t="s">
+      <c r="AB1" s="885" t="s">
         <v>152</v>
       </c>
       <c r="AC1" s="899" t="s">
@@ -59810,90 +59842,90 @@
       <c r="AG1" s="902" t="s">
         <v>609</v>
       </c>
-      <c r="AH1" s="886"/>
-      <c r="AI1" s="886"/>
-      <c r="AJ1" s="886"/>
-      <c r="AK1" s="886"/>
-      <c r="AL1" s="886"/>
-      <c r="AM1" s="886"/>
-      <c r="AN1" s="886"/>
-      <c r="AO1" s="903" t="s">
+      <c r="AH1" s="903"/>
+      <c r="AI1" s="903"/>
+      <c r="AJ1" s="903"/>
+      <c r="AK1" s="903"/>
+      <c r="AL1" s="903"/>
+      <c r="AM1" s="903"/>
+      <c r="AN1" s="903"/>
+      <c r="AO1" s="885" t="s">
         <v>154</v>
       </c>
-      <c r="AP1" s="888" t="s">
+      <c r="AP1" s="897" t="s">
         <v>439</v>
       </c>
-      <c r="AQ1" s="877"/>
-      <c r="AR1" s="877"/>
-      <c r="AS1" s="878"/>
-      <c r="AT1" s="906" t="s">
+      <c r="AQ1" s="865"/>
+      <c r="AR1" s="865"/>
+      <c r="AS1" s="866"/>
+      <c r="AT1" s="905" t="s">
         <v>610</v>
       </c>
-      <c r="AU1" s="907"/>
-      <c r="AV1" s="907"/>
-      <c r="AW1" s="907"/>
-      <c r="AX1" s="907"/>
-      <c r="AY1" s="907"/>
-      <c r="AZ1" s="907"/>
-      <c r="BA1" s="907"/>
-      <c r="BB1" s="907"/>
-      <c r="BC1" s="907"/>
-      <c r="BD1" s="907"/>
-      <c r="BE1" s="907"/>
-      <c r="BF1" s="907"/>
-      <c r="BG1" s="907"/>
-      <c r="BH1" s="907"/>
-      <c r="BI1" s="907"/>
-      <c r="BJ1" s="907"/>
-      <c r="BK1" s="907"/>
-      <c r="BL1" s="907"/>
-      <c r="BM1" s="907"/>
-      <c r="BN1" s="907"/>
-      <c r="BO1" s="907"/>
-      <c r="BP1" s="907"/>
-      <c r="BQ1" s="907"/>
-      <c r="BR1" s="907"/>
-      <c r="BS1" s="907"/>
-      <c r="BT1" s="907"/>
-      <c r="BU1" s="907"/>
-      <c r="BV1" s="907"/>
-      <c r="BW1" s="903" t="s">
+      <c r="AU1" s="906"/>
+      <c r="AV1" s="906"/>
+      <c r="AW1" s="906"/>
+      <c r="AX1" s="906"/>
+      <c r="AY1" s="906"/>
+      <c r="AZ1" s="906"/>
+      <c r="BA1" s="906"/>
+      <c r="BB1" s="906"/>
+      <c r="BC1" s="906"/>
+      <c r="BD1" s="906"/>
+      <c r="BE1" s="906"/>
+      <c r="BF1" s="906"/>
+      <c r="BG1" s="906"/>
+      <c r="BH1" s="906"/>
+      <c r="BI1" s="906"/>
+      <c r="BJ1" s="906"/>
+      <c r="BK1" s="906"/>
+      <c r="BL1" s="906"/>
+      <c r="BM1" s="906"/>
+      <c r="BN1" s="906"/>
+      <c r="BO1" s="906"/>
+      <c r="BP1" s="906"/>
+      <c r="BQ1" s="906"/>
+      <c r="BR1" s="906"/>
+      <c r="BS1" s="906"/>
+      <c r="BT1" s="906"/>
+      <c r="BU1" s="906"/>
+      <c r="BV1" s="906"/>
+      <c r="BW1" s="885" t="s">
         <v>155</v>
       </c>
-      <c r="BX1" s="888" t="s">
+      <c r="BX1" s="897" t="s">
         <v>438</v>
       </c>
-      <c r="BY1" s="877"/>
-      <c r="BZ1" s="877"/>
-      <c r="CA1" s="878"/>
-      <c r="CB1" s="917" t="s">
+      <c r="BY1" s="865"/>
+      <c r="BZ1" s="865"/>
+      <c r="CA1" s="866"/>
+      <c r="CB1" s="896" t="s">
         <v>454</v>
       </c>
-      <c r="CC1" s="896" t="s">
+      <c r="CC1" s="898" t="s">
         <v>73</v>
       </c>
-      <c r="CD1" s="896"/>
-      <c r="CE1" s="896"/>
-      <c r="CF1" s="896"/>
-      <c r="CG1" s="896"/>
-      <c r="CH1" s="896"/>
-      <c r="CI1" s="896"/>
-      <c r="CJ1" s="896"/>
-      <c r="CK1" s="896"/>
-      <c r="CL1" s="896"/>
-      <c r="CM1" s="896"/>
-      <c r="CN1" s="896"/>
+      <c r="CD1" s="898"/>
+      <c r="CE1" s="898"/>
+      <c r="CF1" s="898"/>
+      <c r="CG1" s="898"/>
+      <c r="CH1" s="898"/>
+      <c r="CI1" s="898"/>
+      <c r="CJ1" s="898"/>
+      <c r="CK1" s="898"/>
+      <c r="CL1" s="898"/>
+      <c r="CM1" s="898"/>
+      <c r="CN1" s="898"/>
       <c r="CO1" s="145"/>
-      <c r="CP1" s="913" t="s">
+      <c r="CP1" s="884" t="s">
         <v>77</v>
       </c>
-      <c r="CQ1" s="847"/>
-      <c r="CR1" s="847"/>
-      <c r="CS1" s="847"/>
-      <c r="CT1" s="847"/>
-      <c r="CU1" s="847"/>
-      <c r="CV1" s="847"/>
-      <c r="CW1" s="866"/>
+      <c r="CQ1" s="853"/>
+      <c r="CR1" s="853"/>
+      <c r="CS1" s="853"/>
+      <c r="CT1" s="853"/>
+      <c r="CU1" s="853"/>
+      <c r="CV1" s="853"/>
+      <c r="CW1" s="854"/>
     </row>
     <row r="2" spans="1:104" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="146" t="s">
@@ -59932,7 +59964,7 @@
       <c r="L2" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="882"/>
+      <c r="M2" s="907"/>
       <c r="N2" s="151" t="s">
         <v>160</v>
       </c>
@@ -59948,22 +59980,22 @@
       <c r="R2" s="156" t="s">
         <v>163</v>
       </c>
-      <c r="S2" s="893" t="s">
+      <c r="S2" s="915" t="s">
         <v>433</v>
       </c>
-      <c r="T2" s="872"/>
-      <c r="U2" s="894" t="s">
+      <c r="T2" s="860"/>
+      <c r="U2" s="916" t="s">
         <v>86</v>
       </c>
-      <c r="V2" s="894"/>
-      <c r="W2" s="894" t="s">
+      <c r="V2" s="916"/>
+      <c r="W2" s="916" t="s">
         <v>87</v>
       </c>
-      <c r="X2" s="895"/>
-      <c r="Y2" s="889"/>
-      <c r="Z2" s="890"/>
-      <c r="AA2" s="892"/>
-      <c r="AB2" s="904"/>
+      <c r="X2" s="917"/>
+      <c r="Y2" s="912"/>
+      <c r="Z2" s="892"/>
+      <c r="AA2" s="914"/>
+      <c r="AB2" s="886"/>
       <c r="AC2" s="152" t="s">
         <v>164</v>
       </c>
@@ -59976,81 +60008,81 @@
       <c r="AF2" s="152" t="s">
         <v>607</v>
       </c>
-      <c r="AG2" s="905" t="s">
+      <c r="AG2" s="904" t="s">
         <v>593</v>
       </c>
-      <c r="AH2" s="897"/>
-      <c r="AI2" s="897" t="s">
+      <c r="AH2" s="889"/>
+      <c r="AI2" s="889" t="s">
         <v>167</v>
       </c>
-      <c r="AJ2" s="897"/>
-      <c r="AK2" s="897" t="s">
+      <c r="AJ2" s="889"/>
+      <c r="AK2" s="889" t="s">
         <v>168</v>
       </c>
-      <c r="AL2" s="897"/>
+      <c r="AL2" s="889"/>
       <c r="AM2" s="153" t="s">
         <v>169</v>
       </c>
       <c r="AN2" s="153" t="s">
         <v>170</v>
       </c>
-      <c r="AO2" s="904"/>
-      <c r="AP2" s="898" t="s">
+      <c r="AO2" s="886"/>
+      <c r="AP2" s="891" t="s">
         <v>571</v>
       </c>
-      <c r="AQ2" s="890"/>
-      <c r="AR2" s="908" t="s">
+      <c r="AQ2" s="892"/>
+      <c r="AR2" s="893" t="s">
         <v>572</v>
       </c>
-      <c r="AS2" s="909"/>
-      <c r="AT2" s="897" t="s">
+      <c r="AS2" s="894"/>
+      <c r="AT2" s="889" t="s">
         <v>171</v>
       </c>
-      <c r="AU2" s="897"/>
-      <c r="AV2" s="910" t="s">
+      <c r="AU2" s="889"/>
+      <c r="AV2" s="890" t="s">
         <v>172</v>
       </c>
-      <c r="AW2" s="910"/>
-      <c r="AX2" s="910" t="s">
+      <c r="AW2" s="890"/>
+      <c r="AX2" s="890" t="s">
         <v>173</v>
       </c>
-      <c r="AY2" s="910"/>
+      <c r="AY2" s="890"/>
       <c r="AZ2" s="153" t="s">
         <v>174</v>
       </c>
       <c r="BA2" s="153" t="s">
         <v>175</v>
       </c>
-      <c r="BB2" s="897" t="s">
+      <c r="BB2" s="889" t="s">
         <v>176</v>
       </c>
-      <c r="BC2" s="897"/>
-      <c r="BD2" s="910" t="s">
+      <c r="BC2" s="889"/>
+      <c r="BD2" s="890" t="s">
         <v>177</v>
       </c>
-      <c r="BE2" s="910"/>
-      <c r="BF2" s="910" t="s">
+      <c r="BE2" s="890"/>
+      <c r="BF2" s="890" t="s">
         <v>178</v>
       </c>
-      <c r="BG2" s="910"/>
+      <c r="BG2" s="890"/>
       <c r="BH2" s="153" t="s">
         <v>179</v>
       </c>
       <c r="BI2" s="153" t="s">
         <v>180</v>
       </c>
-      <c r="BJ2" s="897" t="s">
+      <c r="BJ2" s="889" t="s">
         <v>181</v>
       </c>
-      <c r="BK2" s="897"/>
-      <c r="BL2" s="910" t="s">
+      <c r="BK2" s="889"/>
+      <c r="BL2" s="890" t="s">
         <v>182</v>
       </c>
-      <c r="BM2" s="910"/>
-      <c r="BN2" s="910" t="s">
+      <c r="BM2" s="890"/>
+      <c r="BN2" s="890" t="s">
         <v>183</v>
       </c>
-      <c r="BO2" s="910"/>
+      <c r="BO2" s="890"/>
       <c r="BP2" s="153" t="s">
         <v>184</v>
       </c>
@@ -60072,16 +60104,16 @@
       <c r="BV2" s="153" t="s">
         <v>190</v>
       </c>
-      <c r="BW2" s="904"/>
-      <c r="BX2" s="898" t="s">
+      <c r="BW2" s="886"/>
+      <c r="BX2" s="891" t="s">
         <v>571</v>
       </c>
-      <c r="BY2" s="890"/>
-      <c r="BZ2" s="908" t="s">
+      <c r="BY2" s="892"/>
+      <c r="BZ2" s="893" t="s">
         <v>572</v>
       </c>
-      <c r="CA2" s="909"/>
-      <c r="CB2" s="917"/>
+      <c r="CA2" s="894"/>
+      <c r="CB2" s="896"/>
       <c r="CC2" s="137" t="s">
         <v>94</v>
       </c>
@@ -60121,22 +60153,22 @@
       <c r="CO2" s="139" t="s">
         <v>590</v>
       </c>
-      <c r="CP2" s="916" t="s">
+      <c r="CP2" s="895" t="s">
         <v>192</v>
       </c>
-      <c r="CQ2" s="914"/>
-      <c r="CR2" s="914" t="s">
+      <c r="CQ2" s="887"/>
+      <c r="CR2" s="887" t="s">
         <v>193</v>
       </c>
-      <c r="CS2" s="914"/>
-      <c r="CT2" s="914" t="s">
+      <c r="CS2" s="887"/>
+      <c r="CT2" s="887" t="s">
         <v>194</v>
       </c>
-      <c r="CU2" s="914"/>
-      <c r="CV2" s="914" t="s">
+      <c r="CU2" s="887"/>
+      <c r="CV2" s="887" t="s">
         <v>195</v>
       </c>
-      <c r="CW2" s="915"/>
+      <c r="CW2" s="888"/>
     </row>
     <row r="3" spans="1:104" s="1" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="167"/>
@@ -61013,6 +61045,30 @@
     </sortState>
   </autoFilter>
   <mergeCells count="40">
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CC1:CN1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AN1"/>
+    <mergeCell ref="AO1:AO2"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="BW1:BW2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="CP1:CW1"/>
     <mergeCell ref="AB1:AB2"/>
@@ -61029,30 +61085,6 @@
     <mergeCell ref="CR2:CS2"/>
     <mergeCell ref="CT2:CU2"/>
     <mergeCell ref="CB1:CB2"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CC1:CN1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AG1:AN1"/>
-    <mergeCell ref="AO1:AO2"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AT1:BV1"/>
-    <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -61096,19 +61128,19 @@
       <c r="K1" s="143"/>
       <c r="L1" s="144"/>
       <c r="M1" s="689"/>
-      <c r="N1" s="921"/>
-      <c r="O1" s="922"/>
-      <c r="P1" s="922"/>
-      <c r="Q1" s="922"/>
-      <c r="R1" s="885"/>
-      <c r="S1" s="886"/>
-      <c r="T1" s="886"/>
-      <c r="U1" s="886"/>
-      <c r="V1" s="886"/>
-      <c r="W1" s="886"/>
-      <c r="X1" s="887"/>
-      <c r="Y1" s="888"/>
-      <c r="Z1" s="877"/>
+      <c r="N1" s="918"/>
+      <c r="O1" s="919"/>
+      <c r="P1" s="919"/>
+      <c r="Q1" s="919"/>
+      <c r="R1" s="910"/>
+      <c r="S1" s="903"/>
+      <c r="T1" s="903"/>
+      <c r="U1" s="903"/>
+      <c r="V1" s="903"/>
+      <c r="W1" s="903"/>
+      <c r="X1" s="911"/>
+      <c r="Y1" s="897"/>
+      <c r="Z1" s="865"/>
       <c r="AA1" s="690"/>
       <c r="AB1" s="688"/>
       <c r="AC1" s="899"/>
@@ -61116,90 +61148,85 @@
       <c r="AE1" s="900"/>
       <c r="AF1" s="901"/>
       <c r="AG1" s="902"/>
-      <c r="AH1" s="886"/>
-      <c r="AI1" s="886"/>
-      <c r="AJ1" s="886"/>
-      <c r="AK1" s="886"/>
-      <c r="AL1" s="886"/>
-      <c r="AM1" s="886"/>
-      <c r="AN1" s="886"/>
+      <c r="AH1" s="903"/>
+      <c r="AI1" s="903"/>
+      <c r="AJ1" s="903"/>
+      <c r="AK1" s="903"/>
+      <c r="AL1" s="903"/>
+      <c r="AM1" s="903"/>
+      <c r="AN1" s="903"/>
       <c r="AO1" s="688"/>
-      <c r="AP1" s="888"/>
-      <c r="AQ1" s="877"/>
-      <c r="AR1" s="877"/>
-      <c r="AS1" s="878"/>
-      <c r="AT1" s="906"/>
-      <c r="AU1" s="907"/>
-      <c r="AV1" s="907"/>
-      <c r="AW1" s="907"/>
-      <c r="AX1" s="907"/>
-      <c r="AY1" s="907"/>
-      <c r="AZ1" s="907"/>
-      <c r="BA1" s="907"/>
-      <c r="BB1" s="907"/>
-      <c r="BC1" s="907"/>
-      <c r="BD1" s="907"/>
-      <c r="BE1" s="907"/>
-      <c r="BF1" s="907"/>
-      <c r="BG1" s="907"/>
-      <c r="BH1" s="907"/>
-      <c r="BI1" s="907"/>
-      <c r="BJ1" s="907"/>
-      <c r="BK1" s="907"/>
-      <c r="BL1" s="907"/>
-      <c r="BM1" s="907"/>
-      <c r="BN1" s="907"/>
-      <c r="BO1" s="907"/>
-      <c r="BP1" s="907"/>
-      <c r="BQ1" s="907"/>
-      <c r="BR1" s="907"/>
-      <c r="BS1" s="907"/>
-      <c r="BT1" s="907"/>
-      <c r="BU1" s="907"/>
-      <c r="BV1" s="907"/>
+      <c r="AP1" s="897"/>
+      <c r="AQ1" s="865"/>
+      <c r="AR1" s="865"/>
+      <c r="AS1" s="866"/>
+      <c r="AT1" s="905"/>
+      <c r="AU1" s="906"/>
+      <c r="AV1" s="906"/>
+      <c r="AW1" s="906"/>
+      <c r="AX1" s="906"/>
+      <c r="AY1" s="906"/>
+      <c r="AZ1" s="906"/>
+      <c r="BA1" s="906"/>
+      <c r="BB1" s="906"/>
+      <c r="BC1" s="906"/>
+      <c r="BD1" s="906"/>
+      <c r="BE1" s="906"/>
+      <c r="BF1" s="906"/>
+      <c r="BG1" s="906"/>
+      <c r="BH1" s="906"/>
+      <c r="BI1" s="906"/>
+      <c r="BJ1" s="906"/>
+      <c r="BK1" s="906"/>
+      <c r="BL1" s="906"/>
+      <c r="BM1" s="906"/>
+      <c r="BN1" s="906"/>
+      <c r="BO1" s="906"/>
+      <c r="BP1" s="906"/>
+      <c r="BQ1" s="906"/>
+      <c r="BR1" s="906"/>
+      <c r="BS1" s="906"/>
+      <c r="BT1" s="906"/>
+      <c r="BU1" s="906"/>
+      <c r="BV1" s="906"/>
       <c r="BW1" s="688"/>
-      <c r="BX1" s="888"/>
-      <c r="BY1" s="877"/>
-      <c r="BZ1" s="877"/>
-      <c r="CA1" s="878"/>
-      <c r="CB1" s="896"/>
-      <c r="CC1" s="896"/>
-      <c r="CD1" s="896"/>
-      <c r="CE1" s="896"/>
-      <c r="CF1" s="896"/>
-      <c r="CG1" s="896"/>
-      <c r="CH1" s="896"/>
-      <c r="CI1" s="896"/>
-      <c r="CJ1" s="896"/>
-      <c r="CK1" s="896"/>
-      <c r="CL1" s="896"/>
-      <c r="CM1" s="896"/>
+      <c r="BX1" s="897"/>
+      <c r="BY1" s="865"/>
+      <c r="BZ1" s="865"/>
+      <c r="CA1" s="866"/>
+      <c r="CB1" s="898"/>
+      <c r="CC1" s="898"/>
+      <c r="CD1" s="898"/>
+      <c r="CE1" s="898"/>
+      <c r="CF1" s="898"/>
+      <c r="CG1" s="898"/>
+      <c r="CH1" s="898"/>
+      <c r="CI1" s="898"/>
+      <c r="CJ1" s="898"/>
+      <c r="CK1" s="898"/>
+      <c r="CL1" s="898"/>
+      <c r="CM1" s="898"/>
       <c r="CN1" s="687"/>
-      <c r="CO1" s="913"/>
-      <c r="CP1" s="847"/>
-      <c r="CQ1" s="847"/>
-      <c r="CR1" s="847"/>
-      <c r="CS1" s="847"/>
-      <c r="CT1" s="847"/>
-      <c r="CU1" s="847"/>
-      <c r="CV1" s="866"/>
-      <c r="CW1" s="918"/>
-      <c r="CX1" s="919"/>
-      <c r="CY1" s="919"/>
-      <c r="CZ1" s="920"/>
-      <c r="DA1" s="919"/>
-      <c r="DB1" s="919"/>
-      <c r="DC1" s="920"/>
-      <c r="DD1" s="919"/>
-      <c r="DE1" s="919"/>
+      <c r="CO1" s="884"/>
+      <c r="CP1" s="853"/>
+      <c r="CQ1" s="853"/>
+      <c r="CR1" s="853"/>
+      <c r="CS1" s="853"/>
+      <c r="CT1" s="853"/>
+      <c r="CU1" s="853"/>
+      <c r="CV1" s="854"/>
+      <c r="CW1" s="920"/>
+      <c r="CX1" s="921"/>
+      <c r="CY1" s="921"/>
+      <c r="CZ1" s="922"/>
+      <c r="DA1" s="921"/>
+      <c r="DB1" s="921"/>
+      <c r="DC1" s="922"/>
+      <c r="DD1" s="921"/>
+      <c r="DE1" s="921"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="BX1:CA1"/>
-    <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CW1:CY1"/>
     <mergeCell ref="CZ1:DB1"/>
     <mergeCell ref="DC1:DE1"/>
@@ -61208,6 +61235,11 @@
     <mergeCell ref="AG1:AN1"/>
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="BX1:CA1"/>
+    <mergeCell ref="CB1:CM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -61433,10 +61465,10 @@
       <c r="B2" s="202" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="930" t="s">
+      <c r="C2" s="932" t="s">
         <v>216</v>
       </c>
-      <c r="D2" s="930"/>
+      <c r="D2" s="932"/>
       <c r="E2" s="200"/>
       <c r="F2" s="200"/>
       <c r="G2" s="200"/>
@@ -61600,35 +61632,35 @@
     </row>
     <row r="7" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="199"/>
-      <c r="B7" s="927"/>
-      <c r="C7" s="927"/>
-      <c r="D7" s="927"/>
+      <c r="B7" s="933"/>
+      <c r="C7" s="933"/>
+      <c r="D7" s="933"/>
       <c r="E7" s="200"/>
       <c r="F7" s="200"/>
       <c r="G7" s="200"/>
       <c r="H7" s="200"/>
       <c r="I7" s="200"/>
-      <c r="J7" s="927"/>
-      <c r="K7" s="927"/>
-      <c r="L7" s="927"/>
+      <c r="J7" s="933"/>
+      <c r="K7" s="933"/>
+      <c r="L7" s="933"/>
       <c r="M7" s="200"/>
       <c r="N7" s="200"/>
       <c r="O7" s="200"/>
       <c r="P7" s="201" t="s">
         <v>219</v>
       </c>
-      <c r="Q7" s="927"/>
-      <c r="R7" s="927"/>
-      <c r="S7" s="927"/>
+      <c r="Q7" s="933"/>
+      <c r="R7" s="933"/>
+      <c r="S7" s="933"/>
       <c r="T7" s="200"/>
       <c r="U7" s="214"/>
       <c r="V7" s="371"/>
       <c r="W7" s="371" t="s">
         <v>219</v>
       </c>
-      <c r="X7" s="927"/>
-      <c r="Y7" s="927"/>
-      <c r="Z7" s="927"/>
+      <c r="X7" s="933"/>
+      <c r="Y7" s="933"/>
+      <c r="Z7" s="933"/>
       <c r="AA7" s="371"/>
       <c r="AB7" s="214"/>
     </row>
@@ -61805,10 +61837,10 @@
       </c>
       <c r="K11" s="200"/>
       <c r="L11" s="200"/>
-      <c r="M11" s="932" t="s">
+      <c r="M11" s="930" t="s">
         <v>225</v>
       </c>
-      <c r="N11" s="933"/>
+      <c r="N11" s="931"/>
       <c r="O11" s="221"/>
       <c r="P11" s="221"/>
       <c r="Q11" s="219" t="s">
@@ -62990,11 +63022,11 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" s="199"/>
-      <c r="B42" s="931"/>
-      <c r="C42" s="931"/>
-      <c r="D42" s="931"/>
-      <c r="E42" s="931"/>
-      <c r="F42" s="931"/>
+      <c r="B42" s="927"/>
+      <c r="C42" s="927"/>
+      <c r="D42" s="927"/>
+      <c r="E42" s="927"/>
+      <c r="F42" s="927"/>
       <c r="G42" s="239"/>
       <c r="H42" s="200"/>
       <c r="I42" s="239"/>
@@ -63181,6 +63213,21 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="26">
+    <mergeCell ref="AA30:AB30"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -63192,21 +63239,6 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="AA30:AB30"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AA20:AB20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>